<commit_message>
more data in json
</commit_message>
<xml_diff>
--- a/data/summary.xlsx
+++ b/data/summary.xlsx
@@ -491,7 +491,8 @@
       <c r="E2" t="inlineStr"/>
       <c r="F2" t="inlineStr">
         <is>
-          <t>LLM stands for "Language Model" and it is a crucial component in Artificial Intelligence (AI) research. The main purpose of an LLM is to generate natural-sounding text or speech by predicting the next word, phrase or sentence based on the context provided. This allows AI systems to communicate with humans more effectively, understand and respond to their queries, and perform tasks that require language understanding and generation. \nIn AI research, LLM's are used in various ways such as natural language processing, machine translation, speech recognition, text summarization, chatbots, and personal assistants</t>
+          <t>LLM stands for "Language Model" and it is a crucial component in Artificial Intelligence (AI) research. The main purpose of an LLM is to generate natural-sounding text or speech by predicting the next word, phrase or sentence based on the context provided. This allows AI systems to communicate with humans more effectively, understand and respond to their queries, and perform tasks that require language understanding and generation. 
+In AI research, LLM's are used in various ways such as natural language processing, machine translation, speech recognition, text summarization, chatbots, and personal assistants</t>
         </is>
       </c>
     </row>
@@ -535,7 +536,8 @@
       <c r="E4" t="inlineStr"/>
       <c r="F4" t="inlineStr">
         <is>
-          <t>In recent years, there has been a significant increase in the adoption and development of large language models (LLM) for various natural language processing tasks. These include machine translation, text classification, summarization, question answering, etc. The use of LLMs in artificial intelligence (AI) research has led to improved performance on many NLP tasks due to their ability to capture long-range dependencies and contextual information from large amounts of data.\n\nLLMs have shown great potential for learning effective representations by pretraining on massive amounts of unlabeled text, which can then be fine-tuned for specific downstream</t>
+          <t>In recent years, there has been a significant increase in the adoption and development of large language models (LLM) for various natural language processing tasks. These include machine translation, text classification, summarization, question answering, etc. The use of LLMs in artificial intelligence (AI) research has led to improved performance on many NLP tasks due to their ability to capture long-range dependencies and contextual information from large amounts of data.
+LLMs have shown great potential for learning effective representations by pretraining on massive amounts of unlabeled text, which can then be fine-tuned for specific downstream</t>
         </is>
       </c>
     </row>
@@ -557,7 +559,8 @@
       <c r="E5" t="inlineStr"/>
       <c r="F5" t="inlineStr">
         <is>
-          <t>In artificial intelligence (AI) research, legal language models (LLMs) are used to analyze and interpret legal documents. They can help automate tasks such as extracting information from contracts or identifying relevant case law for specific situations. This technology has the potential to improve efficiency in various aspects of the legal industry by reducing reliance on manual processes that may be time-consuming, costly, and prone to human error.\n\nLLMs can also assist with tasks like summarizing large amounts of information or generating new documents based on existing ones. For example, an LLM could generate a summary report for a</t>
+          <t>In artificial intelligence (AI) research, legal language models (LLMs) are used to analyze and interpret legal documents. They can help automate tasks such as extracting information from contracts or identifying relevant case law for specific situations. This technology has the potential to improve efficiency in various aspects of the legal industry by reducing reliance on manual processes that may be time-consuming, costly, and prone to human error.
+LLMs can also assist with tasks like summarizing large amounts of information or generating new documents based on existing ones. For example, an LLM could generate a summary report for a</t>
         </is>
       </c>
     </row>
@@ -579,7 +582,8 @@
       <c r="E6" t="inlineStr"/>
       <c r="F6" t="inlineStr">
         <is>
-          <t>In recent years, large language models (LLM) have become an essential part of artificial intelligence (AI) research. These deep neural networks are trained on massive amounts of text data to learn how words and phrases relate to each other contextually. LLMs can be used for various tasks such as question answering, machine translation, summarization, and natural language understanding. They have shown significant improvements in performance compared to traditional approaches due to their ability to capture complex relationships between different parts of the input text.\n\nOne example of an important contribution from LLMs is GPT-4, a transformer-based model developed by</t>
+          <t>In recent years, large language models (LLM) have become an essential part of artificial intelligence (AI) research. These deep neural networks are trained on massive amounts of text data to learn how words and phrases relate to each other contextually. LLMs can be used for various tasks such as question answering, machine translation, summarization, and natural language understanding. They have shown significant improvements in performance compared to traditional approaches due to their ability to capture complex relationships between different parts of the input text.
+One example of an important contribution from LLMs is GPT-4, a transformer-based model developed by</t>
         </is>
       </c>
     </row>
@@ -645,7 +649,8 @@
       <c r="E9" t="inlineStr"/>
       <c r="F9" t="inlineStr">
         <is>
-          <t>explain use of LLM's in AI research\nExplain the role of LLMs in Natural Language Processing (NLP) and how they are used in various applications.</t>
+          <t>explain use of LLM's in AI research
+Explain the role of LLMs in Natural Language Processing (NLP) and how they are used in various applications.</t>
         </is>
       </c>
     </row>
@@ -689,7 +694,8 @@
       <c r="E11" t="inlineStr"/>
       <c r="F11" t="inlineStr">
         <is>
-          <t>- [x] explain what a neural network is and how it works. \n- [] describe some applications for NN,s (e.g., image recognition) that are not related to language processing or natural langauge understanding but could be used with the same framework as NLP systems?</t>
+          <t>- [x] explain what a neural network is and how it works. 
+- [] describe some applications for NN,s (e.g., image recognition) that are not related to language processing or natural langauge understanding but could be used with the same framework as NLP systems?</t>
         </is>
       </c>
     </row>
@@ -799,7 +805,65 @@
       <c r="E16" t="inlineStr"/>
       <c r="F16" t="inlineStr">
         <is>
-          <t>explain use of LLM's in AI research\nI am not sure what you mean by that. I think it is a good idea to have an open-ended question, but the answer should be clear and specific enough for me so my understanding can move forward with your argumentation\n\n## [](#header-2)Questions about "AI" in ML:\n### Amy Jones(@AmyJones):  \n&gt; I think that'll make a lot of difference. It is an interesting field, and it has been around for quite some time now... but the biggest thing to me right away was how much more people are using machine learning in AI than they used before\n\n### Amit(@Amit):  \n&gt; I think that's true! But there were a lot of other things too. For example, we haven’t had as many examples where the data is not available to be accessed by anyone... but it was an interesting field and one which has been around for quite some time now\n\n### Alex(@alex):  \n&gt; I think that's true! But there were a lot of other things too. For example, we haven’t had as many examples where the data is not available to be accessed by anyone... but it was an interesting field and one which has been around for quite some time now\n\n### Alexander(@alexander):  \n&gt; I think that's true! But there were a lot of other things too. For example, we haven’t had as many examples where the data is not available to be accessed by anyone... but it was an interesting field and one which has been around for quite some time now\n\n### Alexander(@alexander):  \n&gt; I think that's true! But there were a lot of other things too. For example, we haven’t had as many examples where the data is not available to be accessed by anyone... but it was an interesting field and one which has been around for quite some time now\n\n### Alexander(@alexander):  \n&gt; I think that's true! But there were a lot of other things too. For example, we haven’t had as many examples where the data is not available to be accessed by anyone... but it was an interesting field and one which has been around for quite some time now\n\n### Alexander(@alexander):  \n&gt; I think that's true! But there were a lot of other things too. For example, we haven’t had as many examples where the data is not available to be accessed by anyone... but it was an interesting field and one which has been around for quite some time now\n\n### Alexander(@alexander):  \n&gt; I think that's true! But there were a lot of other things too. For example, we haven’t had as many examples where the data is not available to be accessed by anyone... but it was an interesting field and one which has been around for quite some time now\n\n### Alexander(@alexander):  \n&gt; I think that's true! But there were a lot of other things too. For example, we haven’t had as many examples where the data is not available to be accessed by anyone... but it was an interesting field and one which has been around for quite some time now\n\n### Alexander(@alexander):  \n&gt; I think that's true! But there were a lot of other things too. For example, we haven’t had as many examples where the data is not available to be accessed by anyone... but it was an interesting field and one which has been around for quite some time now\n\n### Alexander(@alexander):  \n&gt; I think that's true! But there were a lot of other things too. For example, we haven’t had as many examples where the data is not available to be accessed by anyone... but it was an interesting field and one which has been around for quite some time now\n\n### Alexander(@alexander):  \n&gt; I think that's true! But there were a lot of other things too. For example, we haven’t had as many examples where the data is not available to be accessed by anyone... but it was an interesting field and one which has been around for quite some time now\n\n### Alexander(@alexander):  \n&gt; I think that's true! But there were a lot of other things too. For example, we haven’t had as many examples where the data is not available to be accessed by anyone... but it was an interesting field and one which has been around for quite some time now\n\n### Alexander(@alexander):  \n&gt; I think that's true! But there were a lot of other things too. For example, we haven’t had as many examples where the data is not available to be accessed by anyone... but it was an interesting field and one which has been around for quite some time now\n\n### Alexander(@alexander):  \n&gt; I think that's true! But there were a lot of other things too. For example, we haven’t had as many examples where the data is not available to be accessed by anyone... but it was an interesting field and one which has been around for quite some time now\n\n### Alexander(@alexander):  \n&gt; I think that's true! But there were a lot of other things too. For example, we haven’t had as many examples where the data is not available to be accessed by anyone... but it was an interesting field and one which has been around for quite some time now\n\n### Alexander(@alexander):  \n&gt; I think that's true! But there were a lot of other things too. For example, we haven’t had as many examples where the data is not available to be accessed by anyone... but it was an interesting field and one which has been around for quite some time now\n\n### Alexander(@alexander):  \n&gt; I think that's true! But there were a lot of other things too. For example, we haven’t had as many examples where the data is not available to be accessed by anyone... but it was an interesting field and one which has been around for quite some time now\n\n### Alexander(@alexander):  \n&gt; I think that's true! But there were a lot of other things too. For example, we haven’t had as many examples where the data is not available to be accessed by anyone... but it was an interesting field and one which has been around for quite some time now\n\n### Alexander(@alexander):  \n&gt; I think that's true! But there were a lot of other things too. For example, we haven’t had as many examples where the data is not available to be accessed by anyone... but it was an interesting field and one which has been around for quite some time now\n\n### Alexander(@alexander):  \n&gt; I think that's true! But there were a lot of other things too. For example, we haven’t had as many examples where the data is not available to be accessed by anyone... but it was an interesting field and one which has been around for quite some time now\n\n### Alexander(@alexander):  \n&gt; I think that's true! But there were a lot of other things too. For example, we haven’t had as many examples where the data is not available to be accessed by anyone... but it was an interesting field and one which has been around for quite some time now\n\n### Alexander(@alexander):  \n&gt; I think that's true! But there were a lot of other things too. For example, we haven’t had as many examples where the data is not available to be accessed by anyone... but it was an interesting field and one which has been around for quite some time now\n\n### Alexander(@alexander):  \n&gt; I think that's true! But there were a lot of other things too. For example, we haven’t had as many examples where the data is not available to be accessed by anyone... but it was an interesting field and one which has been around for quite some time now\n\n### Alexander(@alexander):  \n&gt; I think that's true! But there were a lot of other things too. For example, we haven’t had as many examples where the data is not available to be accessed by anyone... but it was an interesting field and one which has been around for quite some time now\n\n### Alexander(@alexander):  \n&gt; I think that's true! But there were a lot of other things too. For example, we haven’t had as many examples where the data is not available to be accessed by anyone... but it was an interesting field and one which has been around for quite some time now\n\n### Alexander(@alexander):  \n&gt; I think that's true! But there were a lot of other things too. For example, we haven’t had as many examples where the data is not available to be accessed by anyone... but it was an interesting field and one which has been around for quite some time now\n\n### Alexander(@alexander):  \n&gt; I think that's true! But there were</t>
+          <t>explain use of LLM's in AI research
+I am not sure what you mean by that. I think it is a good idea to have an open-ended question, but the answer should be clear and specific enough for me so my understanding can move forward with your argumentation
+## [](#header-2)Questions about "AI" in ML:
+### Amy Jones(@AmyJones):  
+&gt; I think that'll make a lot of difference. It is an interesting field, and it has been around for quite some time now... but the biggest thing to me right away was how much more people are using machine learning in AI than they used before
+### Amit(@Amit):  
+&gt; I think that's true! But there were a lot of other things too. For example, we haven’t had as many examples where the data is not available to be accessed by anyone... but it was an interesting field and one which has been around for quite some time now
+### Alex(@alex):  
+&gt; I think that's true! But there were a lot of other things too. For example, we haven’t had as many examples where the data is not available to be accessed by anyone... but it was an interesting field and one which has been around for quite some time now
+### Alexander(@alexander):  
+&gt; I think that's true! But there were a lot of other things too. For example, we haven’t had as many examples where the data is not available to be accessed by anyone... but it was an interesting field and one which has been around for quite some time now
+### Alexander(@alexander):  
+&gt; I think that's true! But there were a lot of other things too. For example, we haven’t had as many examples where the data is not available to be accessed by anyone... but it was an interesting field and one which has been around for quite some time now
+### Alexander(@alexander):  
+&gt; I think that's true! But there were a lot of other things too. For example, we haven’t had as many examples where the data is not available to be accessed by anyone... but it was an interesting field and one which has been around for quite some time now
+### Alexander(@alexander):  
+&gt; I think that's true! But there were a lot of other things too. For example, we haven’t had as many examples where the data is not available to be accessed by anyone... but it was an interesting field and one which has been around for quite some time now
+### Alexander(@alexander):  
+&gt; I think that's true! But there were a lot of other things too. For example, we haven’t had as many examples where the data is not available to be accessed by anyone... but it was an interesting field and one which has been around for quite some time now
+### Alexander(@alexander):  
+&gt; I think that's true! But there were a lot of other things too. For example, we haven’t had as many examples where the data is not available to be accessed by anyone... but it was an interesting field and one which has been around for quite some time now
+### Alexander(@alexander):  
+&gt; I think that's true! But there were a lot of other things too. For example, we haven’t had as many examples where the data is not available to be accessed by anyone... but it was an interesting field and one which has been around for quite some time now
+### Alexander(@alexander):  
+&gt; I think that's true! But there were a lot of other things too. For example, we haven’t had as many examples where the data is not available to be accessed by anyone... but it was an interesting field and one which has been around for quite some time now
+### Alexander(@alexander):  
+&gt; I think that's true! But there were a lot of other things too. For example, we haven’t had as many examples where the data is not available to be accessed by anyone... but it was an interesting field and one which has been around for quite some time now
+### Alexander(@alexander):  
+&gt; I think that's true! But there were a lot of other things too. For example, we haven’t had as many examples where the data is not available to be accessed by anyone... but it was an interesting field and one which has been around for quite some time now
+### Alexander(@alexander):  
+&gt; I think that's true! But there were a lot of other things too. For example, we haven’t had as many examples where the data is not available to be accessed by anyone... but it was an interesting field and one which has been around for quite some time now
+### Alexander(@alexander):  
+&gt; I think that's true! But there were a lot of other things too. For example, we haven’t had as many examples where the data is not available to be accessed by anyone... but it was an interesting field and one which has been around for quite some time now
+### Alexander(@alexander):  
+&gt; I think that's true! But there were a lot of other things too. For example, we haven’t had as many examples where the data is not available to be accessed by anyone... but it was an interesting field and one which has been around for quite some time now
+### Alexander(@alexander):  
+&gt; I think that's true! But there were a lot of other things too. For example, we haven’t had as many examples where the data is not available to be accessed by anyone... but it was an interesting field and one which has been around for quite some time now
+### Alexander(@alexander):  
+&gt; I think that's true! But there were a lot of other things too. For example, we haven’t had as many examples where the data is not available to be accessed by anyone... but it was an interesting field and one which has been around for quite some time now
+### Alexander(@alexander):  
+&gt; I think that's true! But there were a lot of other things too. For example, we haven’t had as many examples where the data is not available to be accessed by anyone... but it was an interesting field and one which has been around for quite some time now
+### Alexander(@alexander):  
+&gt; I think that's true! But there were a lot of other things too. For example, we haven’t had as many examples where the data is not available to be accessed by anyone... but it was an interesting field and one which has been around for quite some time now
+### Alexander(@alexander):  
+&gt; I think that's true! But there were a lot of other things too. For example, we haven’t had as many examples where the data is not available to be accessed by anyone... but it was an interesting field and one which has been around for quite some time now
+### Alexander(@alexander):  
+&gt; I think that's true! But there were a lot of other things too. For example, we haven’t had as many examples where the data is not available to be accessed by anyone... but it was an interesting field and one which has been around for quite some time now
+### Alexander(@alexander):  
+&gt; I think that's true! But there were a lot of other things too. For example, we haven’t had as many examples where the data is not available to be accessed by anyone... but it was an interesting field and one which has been around for quite some time now
+### Alexander(@alexander):  
+&gt; I think that's true! But there were a lot of other things too. For example, we haven’t had as many examples where the data is not available to be accessed by anyone... but it was an interesting field and one which has been around for quite some time now
+### Alexander(@alexander):  
+&gt; I think that's true! But there were a lot of other things too. For example, we haven’t had as many examples where the data is not available to be accessed by anyone... but it was an interesting field and one which has been around for quite some time now
+### Alexander(@alexander):  
+&gt; I think that's true! But there were a lot of other things too. For example, we haven’t had as many examples where the data is not available to be accessed by anyone... but it was an interesting field and one which has been around for quite some time now
+### Alexander(@alexander):  
+&gt; I think that's true! But there were a lot of other things too. For example, we haven’t had as many examples where the data is not available to be accessed by anyone... but it was an interesting field and one which has been around for quite some time now
+### Alexander(@alexander):  
+&gt; I think that's true! But there were</t>
         </is>
       </c>
     </row>
@@ -1175,7 +1239,11 @@
       <c r="E2" t="inlineStr"/>
       <c r="F2" t="inlineStr">
         <is>
-          <t>To solve this equation, we can use algebraic techniques. Here's one way to approach it:\n- First, let's simplify both sides of the equation by combining like terms on each side: \n- On the left hand side, we have a binomial expression that can be expanded using the Binomial Theorem: (a+b)^x = a^x + xab^(x-1) for any real number x. Applying this to our problem, we get: \n8^X + 2^X = 130\n- Now, let's combine like terms on the right</t>
+          <t>To solve this equation, we can use algebraic techniques. Here's one way to approach it:
+- First, let's simplify both sides of the equation by combining like terms on each side: 
+- On the left hand side, we have a binomial expression that can be expanded using the Binomial Theorem: (a+b)^x = a^x + xab^(x-1) for any real number x. Applying this to our problem, we get: 
+8^X + 2^X = 130
+- Now, let's combine like terms on the right</t>
         </is>
       </c>
     </row>
@@ -1197,7 +1265,10 @@
       <c r="E3" t="inlineStr"/>
       <c r="F3" t="inlineStr">
         <is>
-          <t>To solve for x in the equation 8^x + 2^x = 130, we can follow these steps:\n1. First, let's simplify the expression on the left-hand side of the equation by combining like terms: (8^x) + (2^x) = 8*2^(x+1).\n2. Next, we can factor out a common term from both sides of the equation to get rid of any unnecessary multiplication: (8*2^(x+1)) - 130 = 0.\n3. Now that we have factored the</t>
+          <t>To solve for x in the equation 8^x + 2^x = 130, we can follow these steps:
+1. First, let's simplify the expression on the left-hand side of the equation by combining like terms: (8^x) + (2^x) = 8*2^(x+1).
+2. Next, we can factor out a common term from both sides of the equation to get rid of any unnecessary multiplication: (8*2^(x+1)) - 130 = 0.
+3. Now that we have factored the</t>
         </is>
       </c>
     </row>
@@ -1219,7 +1290,10 @@
       <c r="E4" t="inlineStr"/>
       <c r="F4" t="inlineStr">
         <is>
-          <t>To solve for x in the equation 8^x + 2^x = 130, we need to find a common base between the two exponents. In this case, it's 4 (i.e., 8 and 2 are both divisible by 2). So, let's rewrite the equation as:\n\n(4)^(x+1) + (4)^x = 130\n\nNow, we can subtract the second term from both sides of the equation to isolate it on one side. This gives us:\n\n(4)^(x+</t>
+          <t>To solve for x in the equation 8^x + 2^x = 130, we need to find a common base between the two exponents. In this case, it's 4 (i.e., 8 and 2 are both divisible by 2). So, let's rewrite the equation as:
+(4)^(x+1) + (4)^x = 130
+Now, we can subtract the second term from both sides of the equation to isolate it on one side. This gives us:
+(4)^(x+</t>
         </is>
       </c>
     </row>
@@ -1241,7 +1315,13 @@
       <c r="E5" t="inlineStr"/>
       <c r="F5" t="inlineStr">
         <is>
-          <t>Let's solve this equation step-by-step. First, let's distribute the exponent "x" in both terms of the equation:\n\n8*X + 2*X = 130\n\nNow, add these two expressions together to eliminate one term with an exponent:\n\n9*X = 130 - 2*X\n\nNext, subtract 2*X from both sides of the equation to isolate X on one side:\n\n9*X - 2*X = 130 - 2*X\n7*X = 1</t>
+          <t>Let's solve this equation step-by-step. First, let's distribute the exponent "x" in both terms of the equation:
+8*X + 2*X = 130
+Now, add these two expressions together to eliminate one term with an exponent:
+9*X = 130 - 2*X
+Next, subtract 2*X from both sides of the equation to isolate X on one side:
+9*X - 2*X = 130 - 2*X
+7*X = 1</t>
         </is>
       </c>
     </row>
@@ -1263,7 +1343,11 @@
       <c r="E6" t="inlineStr"/>
       <c r="F6" t="inlineStr">
         <is>
-          <t>Let's solve this equation step by step. First, notice that both terms have an exponent of "x," so we can factor out x from each term:\n\n8^x + 2^x = 130\n\nNow, divide both sides by x to isolate the variable on one side and a constant (in this case, 1) on the other side:\n\n8^x / x + 2^x / x = 130/x\n\nSince we want all terms in the numerator of each fraction, multiply both sides by x to eliminate fractions:</t>
+          <t>Let's solve this equation step by step. First, notice that both terms have an exponent of "x," so we can factor out x from each term:
+8^x + 2^x = 130
+Now, divide both sides by x to isolate the variable on one side and a constant (in this case, 1) on the other side:
+8^x / x + 2^x / x = 130/x
+Since we want all terms in the numerator of each fraction, multiply both sides by x to eliminate fractions:</t>
         </is>
       </c>
     </row>
@@ -1285,7 +1369,15 @@
       <c r="E7" t="inlineStr"/>
       <c r="F7" t="inlineStr">
         <is>
-          <t>To solve this equation, we can use algebra and simplify it as follows:\n(8)^x + (2)^x = 130\nMultiplying both sides by 4 gives us:\n64 + 16^x = 52*4\nSimplifying further, we get:\n76 + 16^x = 208\nSubtracting 76 from both sides and then raising the resulting equation to the power of x gives us:\n16^x - 76 = 208 - 76\nSimplifying,</t>
+          <t>To solve this equation, we can use algebra and simplify it as follows:
+(8)^x + (2)^x = 130
+Multiplying both sides by 4 gives us:
+64 + 16^x = 52*4
+Simplifying further, we get:
+76 + 16^x = 208
+Subtracting 76 from both sides and then raising the resulting equation to the power of x gives us:
+16^x - 76 = 208 - 76
+Simplifying,</t>
         </is>
       </c>
     </row>
@@ -1307,7 +1399,19 @@
       <c r="E8" t="inlineStr"/>
       <c r="F8" t="inlineStr">
         <is>
-          <t>In 8^X+2^X=130 show how to solve for X\nTo solve the equation 2^X + X = 130, we need to find a way to isolate X on one side of the equation. Here are the steps to do so:\n\n1. Start by multiplying both sides of the equation by 2^X:\n2^X * (2^X + X) = 2^X * 130\n\n2. Next, we can simplify this expression by using the fact that 2^X * 2^X = 2^(X+X):\n2^(X+X) * 2^X * X = 2^X * 130\n\n3. Now, we need to isolate X on one side of the equation:\n2^X * (X + 1) = 130\n\n4. Finally, we can solve for X by taking the logarithm of both sides and using the fact that log(a*b) = log(a) + log(b):\nlog(2^X * (X + 1)) = log(130)\n\n5. Solving for X, we get:\nlog(2^X * (X + 1)) - log(130) = 0\n\n6. Using a calculator or computer software to solve this equation, we find that the solution is approximately X = 4.789. Therefore, X ≈ 4.789.</t>
+          <t>In 8^X+2^X=130 show how to solve for X
+To solve the equation 2^X + X = 130, we need to find a way to isolate X on one side of the equation. Here are the steps to do so:
+1. Start by multiplying both sides of the equation by 2^X:
+2^X * (2^X + X) = 2^X * 130
+2. Next, we can simplify this expression by using the fact that 2^X * 2^X = 2^(X+X):
+2^(X+X) * 2^X * X = 2^X * 130
+3. Now, we need to isolate X on one side of the equation:
+2^X * (X + 1) = 130
+4. Finally, we can solve for X by taking the logarithm of both sides and using the fact that log(a*b) = log(a) + log(b):
+log(2^X * (X + 1)) = log(130)
+5. Solving for X, we get:
+log(2^X * (X + 1)) - log(130) = 0
+6. Using a calculator or computer software to solve this equation, we find that the solution is approximately X = 4.789. Therefore, X ≈ 4.789.</t>
         </is>
       </c>
     </row>
@@ -1329,7 +1433,14 @@
       <c r="E9" t="inlineStr"/>
       <c r="F9" t="inlineStr">
         <is>
-          <t>In 8^X+2^X=130 show how to solve for X\nTo find the value of X, we need to use algebra. Let's start by simplifying the equation:\n8^X + 2^X = 130\n4^X + 2^X = 130/4\n2^X(2^X+1) = 130/4\n2^X = 65\nX = log\_2(65)\nTherefore, X ≈ 4.5</t>
+          <t>In 8^X+2^X=130 show how to solve for X
+To find the value of X, we need to use algebra. Let's start by simplifying the equation:
+8^X + 2^X = 130
+4^X + 2^X = 130/4
+2^X(2^X+1) = 130/4
+2^X = 65
+X = log\_2(65)
+Therefore, X ≈ 4.5</t>
         </is>
       </c>
     </row>
@@ -1351,7 +1462,11 @@
       <c r="E10" t="inlineStr"/>
       <c r="F10" t="inlineStr">
         <is>
-          <t>To solve this equation, we will use a method called factorization. First, let's rewrite it in terms of base ten numbers instead of powers of two and one. The equation can be rewritten as 8 * (10^2) + (2^1) = 130. Now, we will solve for the variable X by isolating the variable term on both sides:\n(8*10^2+2)=130\n(8*100+2)=130\n(8*100+2)=130\nAddition property of equality</t>
+          <t>To solve this equation, we will use a method called factorization. First, let's rewrite it in terms of base ten numbers instead of powers of two and one. The equation can be rewritten as 8 * (10^2) + (2^1) = 130. Now, we will solve for the variable X by isolating the variable term on both sides:
+(8*10^2+2)=130
+(8*100+2)=130
+(8*100+2)=130
+Addition property of equality</t>
         </is>
       </c>
     </row>
@@ -1373,7 +1488,38 @@
       <c r="E11" t="inlineStr"/>
       <c r="F11" t="inlineStr">
         <is>
-          <t>In 8^X+2^X=130 show how to solve for X\n8^x + 2^x = 130, we can use the fact that x is a power of two.  We have (1) and (3). We know 1^(0) = 1, so let's start with this case first. The equation becomes 8^0+2^0=130 which simplifies to just 13.\nNow for 2^(x), we can use the fact that x is a power of two:  2^(1) = 2, and then multiply by itself again (2*2). We get 4. Then add this with our first term 8^0+13. This gives us 16 + 13 which equals 29.\nNow for 3^(x), we can use the fact that x is a power of two:  3^(1) = 3, and then multiply by itself again (3*2). We get 6. Then add this with our first term 8^0+29. This gives us 16 + 36 which equals 52\nNow for 4^(x), we can use the fact that x is a power of two:  4^(1) = 2, and then multiply by itself again (2*3). We get 6. Then add this with our first term 8^0+52. This gives us 16 + 72 which equals 88\nNow for 5^(x), we can use the fact that x is a power of two:  5^(1) = 2, and then multiply by itself again (2*4). We get 6. Then add this with our first term 8^0+88. This gives us 16 + 96 which equals 112\nNow for 6^(x), we can use the fact that x is a power of two:  6^(1) = 2, and then multiply by itself again (2*5). We get 12. Then add this with our first term 8^0+112. This gives us 16 + 120 which equals 132\nNow for 7^(x), we can use the fact that x is a power of two:  7^(1) = 2, and then multiply by itself again (2*6). We get 14. Then add this with our first term 8^0+132. This gives us 16 + 144 which equals 156\nNow for 8^(x), we can use the fact that x is a power of two:  8^(1) = 2, and then multiply by itself again (2*7). We get 14. Then add this with our first term 8^0+156. This gives us 16 + 168 which equals 184\nNow for 9^(x), we can use the fact that x is a power of two:  9^(1) = 2, and then multiply by itself again (2*8). We get 18. Then add this with our first term 8^0+184. This gives us 16 + 192 which equals 208\nNow for 10^(x), we can use the fact that x is a power of two:  10^(1) = 2, and then multiply by itself again (2*9). We get 20. Then add this with our first term 8^0+208. This gives us 16 + 216 which equals 224\nNow for 11^(x), we can use the fact that x is a power of two:  11^(1) = 2, and then multiply by itself again (2*10). We get 22. Then add this with our first term 8^0+224. This gives us 16 + 232 which equals 248\nNow for 12^(x), we can use the fact that x is a power of two:  12^(1) = 2, and then multiply by itself again (2*11). We get 24. Then add this with our first term 8^0+248. This gives us 16 + 256 which equals 272\nNow for 13^(x), we can use the fact that x is a power of two:  13^(1) = 2, and then multiply by itself again (2*12). We get 26. Then add this with our first term 8^0+272. This gives us 16 + 288 which equals 296\nNow for 14^(x), we can use the fact that x is a power of two:  14^(1) = 2, and then multiply by itself again (2*13). We get 28. Then add this with our first term 8^0+296. This gives us 16 + 320 which equals 336\nNow for 15^(x), we can use the fact that x is a power of two:  15^(1) = 2, and then multiply by itself again (2*14). We get 30. Then add this with our first term 8^0+336. This gives us 16 + 352 which equals 368\nNow for 16^(x), we can use the fact that x is a power of two:  16^(1) = 2, and then multiply by itself again (2*15). We get 32. Then add this with our first term 8^0+368. This gives us 16 + 384 which equals 392\nNow for 17^(x), we can use the fact that x is a power of two:  17^(1) = 2, and then multiply by itself again (2*16). We get 34. Then add this with our first term 8^0+392. This gives us 16 + 416 which equals 432\nNow for 18^(x), we can use the fact that x is a power of two:  18^(1) = 2, and then multiply by itself again (2*17). We get 36. Then add this with our first term 8^0+432. This gives us 16 + 448 which equals 464\nNow for 19^(x), we can use the fact that x is a power of two:  19^(1) = 2, and then multiply by itself again (2*18). We get 38. Then add this with our first term 8^0+464. This gives us 16 + 480 which equals 488\nNow for 20^(x), we can use the fact that x is a power of two:  20^(1) = 2, and then multiply by itself again (2*19). We get 40. Then add this with our first term 8^0+488. This gives us 16 + 512 which equals 520\nNow for 21^(x), we can use the fact that x is a power of two:  21^(1) = 2, and then multiply by itself again (2*20). We get 42. Then add this with our first term 8^0+520. This gives us 16 + 544 which equals 568\nNow for 22^(x), we can use the fact that x is a power of two:  22^(1) = 2, and then multiply by itself again (2*21). We get 44. Then add this with our first term 8^0+568. This gives us 16 + 576 which equals 584\nNow for 23^(x), we can use the fact that x is a power of two:  23^(1) = 2, and then multiply by itself again (2*22). We get 46. Then add this with our first term 8^0+584. This gives us 16 + 608 which equals 624\nNow for 24^(x), we can use the fact that x is a power of two:  24^(1) = 2, and then multiply by itself again (2*23). We get 48. Then add this with our first term 8^0+624. This gives us 16 + 640 which equals 648\nNow for 25^(x), we can use the fact that x is a power of two:  25^(1) = 2, and then multiply by itself again (2*24). We get 50. Then add this with our first term 8^0+648. This gives us 16 + 672 which equals 680\nNow for 26^(x), we can use the fact that x is a power of two:  26^(1) = 2, and then multiply by itself again (2*25). We get 52. Then add this with our first term 8^0+680. This gives us 16 + 704 which equals 728\nNow for 27^(x), we can use the fact that x is a power of two:  27^(1) = 2, and then multiply by itself again (2*26). We get 54. Then add this with our first term 8^0+728. This gives us 16 + 736 which equals 752\nNow for 28^(x), we can use the fact that x is a power of two:  28^(1) = 2, and then multiply by itself again (2*27). We get 56. Then add this with our first term 8^0+752. This gives us 16 + 768 which equals 784\nNow for 29^(x), we can use the fact that x is a power of two:  29^(1) = 2, and then multiply by itself again (2*28). We get 60. Then add this with our first term 8^0+784. This gives us 16 + 832 which equals 840\nNow for 30^(x), we can use the fact that x is a power of two:  30^(1) = 2, and then multiply by itself again (2*29). We get 62. Then add this with our first term 8^0+840. This gives us 16 + 864 which equals 880\nNow for 31^(x), we can use the fact that x is a power of two:  31^(1) = 2, and then multiply by itself again (2*30). We get 62. Then add this with our first term 8^0+</t>
+          <t>In 8^X+2^X=130 show how to solve for X
+8^x + 2^x = 130, we can use the fact that x is a power of two.  We have (1) and (3). We know 1^(0) = 1, so let's start with this case first. The equation becomes 8^0+2^0=130 which simplifies to just 13.
+Now for 2^(x), we can use the fact that x is a power of two:  2^(1) = 2, and then multiply by itself again (2*2). We get 4. Then add this with our first term 8^0+13. This gives us 16 + 13 which equals 29.
+Now for 3^(x), we can use the fact that x is a power of two:  3^(1) = 3, and then multiply by itself again (3*2). We get 6. Then add this with our first term 8^0+29. This gives us 16 + 36 which equals 52
+Now for 4^(x), we can use the fact that x is a power of two:  4^(1) = 2, and then multiply by itself again (2*3). We get 6. Then add this with our first term 8^0+52. This gives us 16 + 72 which equals 88
+Now for 5^(x), we can use the fact that x is a power of two:  5^(1) = 2, and then multiply by itself again (2*4). We get 6. Then add this with our first term 8^0+88. This gives us 16 + 96 which equals 112
+Now for 6^(x), we can use the fact that x is a power of two:  6^(1) = 2, and then multiply by itself again (2*5). We get 12. Then add this with our first term 8^0+112. This gives us 16 + 120 which equals 132
+Now for 7^(x), we can use the fact that x is a power of two:  7^(1) = 2, and then multiply by itself again (2*6). We get 14. Then add this with our first term 8^0+132. This gives us 16 + 144 which equals 156
+Now for 8^(x), we can use the fact that x is a power of two:  8^(1) = 2, and then multiply by itself again (2*7). We get 14. Then add this with our first term 8^0+156. This gives us 16 + 168 which equals 184
+Now for 9^(x), we can use the fact that x is a power of two:  9^(1) = 2, and then multiply by itself again (2*8). We get 18. Then add this with our first term 8^0+184. This gives us 16 + 192 which equals 208
+Now for 10^(x), we can use the fact that x is a power of two:  10^(1) = 2, and then multiply by itself again (2*9). We get 20. Then add this with our first term 8^0+208. This gives us 16 + 216 which equals 224
+Now for 11^(x), we can use the fact that x is a power of two:  11^(1) = 2, and then multiply by itself again (2*10). We get 22. Then add this with our first term 8^0+224. This gives us 16 + 232 which equals 248
+Now for 12^(x), we can use the fact that x is a power of two:  12^(1) = 2, and then multiply by itself again (2*11). We get 24. Then add this with our first term 8^0+248. This gives us 16 + 256 which equals 272
+Now for 13^(x), we can use the fact that x is a power of two:  13^(1) = 2, and then multiply by itself again (2*12). We get 26. Then add this with our first term 8^0+272. This gives us 16 + 288 which equals 296
+Now for 14^(x), we can use the fact that x is a power of two:  14^(1) = 2, and then multiply by itself again (2*13). We get 28. Then add this with our first term 8^0+296. This gives us 16 + 320 which equals 336
+Now for 15^(x), we can use the fact that x is a power of two:  15^(1) = 2, and then multiply by itself again (2*14). We get 30. Then add this with our first term 8^0+336. This gives us 16 + 352 which equals 368
+Now for 16^(x), we can use the fact that x is a power of two:  16^(1) = 2, and then multiply by itself again (2*15). We get 32. Then add this with our first term 8^0+368. This gives us 16 + 384 which equals 392
+Now for 17^(x), we can use the fact that x is a power of two:  17^(1) = 2, and then multiply by itself again (2*16). We get 34. Then add this with our first term 8^0+392. This gives us 16 + 416 which equals 432
+Now for 18^(x), we can use the fact that x is a power of two:  18^(1) = 2, and then multiply by itself again (2*17). We get 36. Then add this with our first term 8^0+432. This gives us 16 + 448 which equals 464
+Now for 19^(x), we can use the fact that x is a power of two:  19^(1) = 2, and then multiply by itself again (2*18). We get 38. Then add this with our first term 8^0+464. This gives us 16 + 480 which equals 488
+Now for 20^(x), we can use the fact that x is a power of two:  20^(1) = 2, and then multiply by itself again (2*19). We get 40. Then add this with our first term 8^0+488. This gives us 16 + 512 which equals 520
+Now for 21^(x), we can use the fact that x is a power of two:  21^(1) = 2, and then multiply by itself again (2*20). We get 42. Then add this with our first term 8^0+520. This gives us 16 + 544 which equals 568
+Now for 22^(x), we can use the fact that x is a power of two:  22^(1) = 2, and then multiply by itself again (2*21). We get 44. Then add this with our first term 8^0+568. This gives us 16 + 576 which equals 584
+Now for 23^(x), we can use the fact that x is a power of two:  23^(1) = 2, and then multiply by itself again (2*22). We get 46. Then add this with our first term 8^0+584. This gives us 16 + 608 which equals 624
+Now for 24^(x), we can use the fact that x is a power of two:  24^(1) = 2, and then multiply by itself again (2*23). We get 48. Then add this with our first term 8^0+624. This gives us 16 + 640 which equals 648
+Now for 25^(x), we can use the fact that x is a power of two:  25^(1) = 2, and then multiply by itself again (2*24). We get 50. Then add this with our first term 8^0+648. This gives us 16 + 672 which equals 680
+Now for 26^(x), we can use the fact that x is a power of two:  26^(1) = 2, and then multiply by itself again (2*25). We get 52. Then add this with our first term 8^0+680. This gives us 16 + 704 which equals 728
+Now for 27^(x), we can use the fact that x is a power of two:  27^(1) = 2, and then multiply by itself again (2*26). We get 54. Then add this with our first term 8^0+728. This gives us 16 + 736 which equals 752
+Now for 28^(x), we can use the fact that x is a power of two:  28^(1) = 2, and then multiply by itself again (2*27). We get 56. Then add this with our first term 8^0+752. This gives us 16 + 768 which equals 784
+Now for 29^(x), we can use the fact that x is a power of two:  29^(1) = 2, and then multiply by itself again (2*28). We get 60. Then add this with our first term 8^0+784. This gives us 16 + 832 which equals 840
+Now for 30^(x), we can use the fact that x is a power of two:  30^(1) = 2, and then multiply by itself again (2*29). We get 62. Then add this with our first term 8^0+840. This gives us 16 + 864 which equals 880
+Now for 31^(x), we can use the fact that x is a power of two:  31^(1) = 2, and then multiply by itself again (2*30). We get 62. Then add this with our first term 8^0+</t>
         </is>
       </c>
     </row>
@@ -1395,7 +1541,24 @@
       <c r="E12" t="inlineStr"/>
       <c r="F12" t="inlineStr">
         <is>
-          <t>In 8^X+2^X=130 show how to solve for X\nTo solve this equation, we need to use the distributive property of multiplication and simplify each term. \n8^X means 8 raised to the power of X (or 8 multiplied by itself X times). So we have:\n8^X = 8 * 8^(X-1)\n2^X means 2 raised to the power of X (or 2 multiplied by itself X times), so we have:\n2^X = 2 * 2^(X-1)\nMultiplying these two terms together, we get:\n8*2*2^(X-1) = 16 * 2^(X-1)\nNow we can simplify the exponent on the right side of the equation by moving the decimal point one place to the left and repeating the process. We end up with:\n16 * 4^(X-1) = 256 * (2^(X-1)) / 3\nRepeating this process, we get:\n256 * 8^(X-3) = 1024 * 2^(X-4) / 9\nNow we can solve for X by dividing both sides of the equation by 512 and simplifying. We end up with:\n(2^(X-4) / 9) / (512/9) = 1/8\nSolving for X, we get:\nX = 4 - log2(1/8)\nUsing a calculator or table of logarithms, we find that X �� 3.15. \nTherefore, the solution to 8^X+2^X=130 is approximately 130 * e^(3.15) �� 2100.</t>
+          <t>In 8^X+2^X=130 show how to solve for X
+To solve this equation, we need to use the distributive property of multiplication and simplify each term. 
+8^X means 8 raised to the power of X (or 8 multiplied by itself X times). So we have:
+8^X = 8 * 8^(X-1)
+2^X means 2 raised to the power of X (or 2 multiplied by itself X times), so we have:
+2^X = 2 * 2^(X-1)
+Multiplying these two terms together, we get:
+8*2*2^(X-1) = 16 * 2^(X-1)
+Now we can simplify the exponent on the right side of the equation by moving the decimal point one place to the left and repeating the process. We end up with:
+16 * 4^(X-1) = 256 * (2^(X-1)) / 3
+Repeating this process, we get:
+256 * 8^(X-3) = 1024 * 2^(X-4) / 9
+Now we can solve for X by dividing both sides of the equation by 512 and simplifying. We end up with:
+(2^(X-4) / 9) / (512/9) = 1/8
+Solving for X, we get:
+X = 4 - log2(1/8)
+Using a calculator or table of logarithms, we find that X �� 3.15. 
+Therefore, the solution to 8^X+2^X=130 is approximately 130 * e^(3.15) �� 2100.</t>
         </is>
       </c>
     </row>
@@ -1417,7 +1580,8 @@
       <c r="E13" t="inlineStr"/>
       <c r="F13" t="inlineStr">
         <is>
-          <t>In 8^X+2^X=130 show how to solve for X\nThe expression is equal to 130, so the value of x must be 5.</t>
+          <t>In 8^X+2^X=130 show how to solve for X
+The expression is equal to 130, so the value of x must be 5.</t>
         </is>
       </c>
     </row>
@@ -1439,7 +1603,14 @@
       <c r="E14" t="inlineStr"/>
       <c r="F14" t="inlineStr">
         <is>
-          <t>In 8^X+2^X=130 show how to solve for X\nTo solve for X in the equation ^X+2^X=130, we need to isolate the variable X on one side of the equation. Here are the steps to do so:\n1. Start with the equation ^X+2^X=130.\n2. Subtract 2^X from both sides of the equation: ^X + 2^X - 2^X = 130 - 2^X.\n3. Simplify the right side of the equation by cancelling out the 2^X term: ^X = 130 - 2^X.\n4. Take the logarithm base 10 of both sides of the equation: log10(^X) = log10(130-2^X).\n5. Solve for X by taking the natural logarithm of both sides of the equation: log(X) = log(130-2X) or X = 130 - 2log(X).\nSo the solution for X is X = 130 - 2log(X).</t>
+          <t>In 8^X+2^X=130 show how to solve for X
+To solve for X in the equation ^X+2^X=130, we need to isolate the variable X on one side of the equation. Here are the steps to do so:
+1. Start with the equation ^X+2^X=130.
+2. Subtract 2^X from both sides of the equation: ^X + 2^X - 2^X = 130 - 2^X.
+3. Simplify the right side of the equation by cancelling out the 2^X term: ^X = 130 - 2^X.
+4. Take the logarithm base 10 of both sides of the equation: log10(^X) = log10(130-2^X).
+5. Solve for X by taking the natural logarithm of both sides of the equation: log(X) = log(130-2X) or X = 130 - 2log(X).
+So the solution for X is X = 130 - 2log(X).</t>
         </is>
       </c>
     </row>
@@ -1461,7 +1632,12 @@
       <c r="E15" t="inlineStr"/>
       <c r="F15" t="inlineStr">
         <is>
-          <t>In 8^X+2^X=130 show how to solve for X\nTo solve the equation, we can follow these steps:\n1. Start by isolating the variable (X) on one side of the equation. To do this, subtract 2 from both sides of the equation:\n    X + 2 - 2 = 130 - 2\n    X = 128\n2. The solution to the equation is X = 128.</t>
+          <t>In 8^X+2^X=130 show how to solve for X
+To solve the equation, we can follow these steps:
+1. Start by isolating the variable (X) on one side of the equation. To do this, subtract 2 from both sides of the equation:
+    X + 2 - 2 = 130 - 2
+    X = 128
+2. The solution to the equation is X = 128.</t>
         </is>
       </c>
     </row>
@@ -1483,7 +1659,13 @@
       <c r="E16" t="inlineStr"/>
       <c r="F16" t="inlineStr">
         <is>
-          <t>In 8^X+2^X=130 show how to solve for X\n```python3\n\ndef main():  # Function that will be called when the program is run. This function should contain all of your code! Do not delete this line or else you'll get a 0 score in our tests!!1\n    print("Hello, world!")                                   ## Prints "hello" to screen\n\nif(__name_t_e_m__)== "__main":  # If the program is run directly from your computer then it will execute this code. This line should not be deleted! 1\n	 main()                                                 ### Run function called 'Main' which contains all of our important functions and variables that we have defined above\n\n```</t>
+          <t>In 8^X+2^X=130 show how to solve for X
+```python3
+def main():  # Function that will be called when the program is run. This function should contain all of your code! Do not delete this line or else you'll get a 0 score in our tests!!1
+    print("Hello, world!")                                   ## Prints "hello" to screen
+if(__name_t_e_m__)== "__main":  # If the program is run directly from your computer then it will execute this code. This line should not be deleted! 1
+	 main()                                                 ### Run function called 'Main' which contains all of our important functions and variables that we have defined above
+```</t>
         </is>
       </c>
     </row>
@@ -1505,7 +1687,17 @@
       <c r="E17" t="inlineStr"/>
       <c r="F17" t="inlineStr">
         <is>
-          <t>In 8^X+2^X=130 show how to solve for X\nWe can use the quadratic formula to solve for X.\n\nFirst, we need to isolate X on one side of the equation:\n\nX = (-1/2) * (130 - sqrt(130^2))\n\nThen, we can substitute this expression into the original equation and simplify:\n\n(-1/2) * (130 - sqrt(130^2)) + (-1/2) * (130 - sqrt(130^2)) = 130\n\nSimplifying, we get:\n\n-1 = 260\n\nTherefore, the solution for X is:\n\nX = -140\n\nSo, the value of X that satisfies the equation ^X+2^X=130 is -140.</t>
+          <t>In 8^X+2^X=130 show how to solve for X
+We can use the quadratic formula to solve for X.
+First, we need to isolate X on one side of the equation:
+X = (-1/2) * (130 - sqrt(130^2))
+Then, we can substitute this expression into the original equation and simplify:
+(-1/2) * (130 - sqrt(130^2)) + (-1/2) * (130 - sqrt(130^2)) = 130
+Simplifying, we get:
+-1 = 260
+Therefore, the solution for X is:
+X = -140
+So, the value of X that satisfies the equation ^X+2^X=130 is -140.</t>
         </is>
       </c>
     </row>
@@ -1549,7 +1741,9 @@
       <c r="E19" t="inlineStr"/>
       <c r="F19" t="inlineStr">
         <is>
-          <t>To find the value of X in the equation 8^(X + 2^X) = 130, we can use logarithmic functions. First, let's define Y = 2^X; then we can rewrite the equation as follows: 8^Y \* (2^X)^(2\*Y) = 130. To solve for X in this expression, we need to take the natural logarithm of both sides and simplify:\n```scss\nlog8(8^Y * (2^X)^(2*Y)) = Y + log8</t>
+          <t>To find the value of X in the equation 8^(X + 2^X) = 130, we can use logarithmic functions. First, let's define Y = 2^X; then we can rewrite the equation as follows: 8^Y \* (2^X)^(2\*Y) = 130. To solve for X in this expression, we need to take the natural logarithm of both sides and simplify:
+```scss
+log8(8^Y * (2^X)^(2*Y)) = Y + log8</t>
         </is>
       </c>
     </row>
@@ -1571,7 +1765,16 @@
       <c r="E20" t="inlineStr"/>
       <c r="F20" t="inlineStr">
         <is>
-          <t>In 8^X+2^X=130 show how to solve for X\nTo solve the equation ^X+2^X=130 for X, we need to isolate the variable X on one side of the equation. We can do this by subtracting 2^X from both sides of the equation, which gives us:\n\n^X - 2^X = 130 - 2^X\n\nNext, we can take the logarithm of both sides to get:\n\nX - log(2)X = log(130) - X + log(2)X\n\nSimplifying this equation gives us:\n\nlog(130/2) = -X\n\nFinally, we can solve for X by taking the exponent of both sides, which gives us:\n\nX = -(1/2)log(130/2)\n\nTherefore, the solution to the equation ^X+2^X=130 is X = -(1/2)log(130/2).</t>
+          <t>In 8^X+2^X=130 show how to solve for X
+To solve the equation ^X+2^X=130 for X, we need to isolate the variable X on one side of the equation. We can do this by subtracting 2^X from both sides of the equation, which gives us:
+^X - 2^X = 130 - 2^X
+Next, we can take the logarithm of both sides to get:
+X - log(2)X = log(130) - X + log(2)X
+Simplifying this equation gives us:
+log(130/2) = -X
+Finally, we can solve for X by taking the exponent of both sides, which gives us:
+X = -(1/2)log(130/2)
+Therefore, the solution to the equation ^X+2^X=130 is X = -(1/2)log(130/2).</t>
         </is>
       </c>
     </row>
@@ -1593,7 +1796,21 @@
       <c r="E21" t="inlineStr"/>
       <c r="F21" t="inlineStr">
         <is>
-          <t>In 8^X+2^X=130 show how to solve for X\nTo solve the equation in ^X+2^X=130, we can use the following steps:\n1. Factorize the left-hand side (LHS) of the equation:\n(1 + 2)^X = 130\n2. Factorize the right-hand side (RHS) of the equation:\n(1 + 2)^X = (1^2)^X \* (2^2)^X\n3. Identify common factors between the LHS and RHS:\n(1+2)^X = (1^2)^X \* (2^2)^X = (1)^X \* (2^2)^X\n4. Apply the distributive property of multiplication over the common factor on the LHS:\n(1+2)^X = 1^X \* (2^2)^X\n5. Simplify the expression by using the binomial theorem for squaring a number:\n(1+2)^X = (1+2)^X \* (1-1)^X \* (1+2)^X = (1+4)^X - 1^X\n6. Substitute the simplified expression into the RHS of the equation to obtain X:\n(1+2)^X = (1+4)^X - 1^X = (5)^X\n7. Therefore, we have solved for X in the equation in ^X+2^X=130 as X = 5.</t>
+          <t>In 8^X+2^X=130 show how to solve for X
+To solve the equation in ^X+2^X=130, we can use the following steps:
+1. Factorize the left-hand side (LHS) of the equation:
+(1 + 2)^X = 130
+2. Factorize the right-hand side (RHS) of the equation:
+(1 + 2)^X = (1^2)^X \* (2^2)^X
+3. Identify common factors between the LHS and RHS:
+(1+2)^X = (1^2)^X \* (2^2)^X = (1)^X \* (2^2)^X
+4. Apply the distributive property of multiplication over the common factor on the LHS:
+(1+2)^X = 1^X \* (2^2)^X
+5. Simplify the expression by using the binomial theorem for squaring a number:
+(1+2)^X = (1+2)^X \* (1-1)^X \* (1+2)^X = (1+4)^X - 1^X
+6. Substitute the simplified expression into the RHS of the equation to obtain X:
+(1+2)^X = (1+4)^X - 1^X = (5)^X
+7. Therefore, we have solved for X in the equation in ^X+2^X=130 as X = 5.</t>
         </is>
       </c>
     </row>
@@ -1615,7 +1832,19 @@
       <c r="E22" t="inlineStr"/>
       <c r="F22" t="inlineStr">
         <is>
-          <t>To solve this equation, we need to use some basic algebra. First, let's simplify the expression inside the parentheses:\n```\n(8x + 2x) = 10x\n```\nNow we can substitute this value back into the original equation and isolate x on one side:\n```\n10x - 2x = 130\n```\nNext, let's add 2x to both sides of the equation to get rid of the negative sign:\n```\n12x = 132\n```\nNow we can divide both sides by 12</t>
+          <t>To solve this equation, we need to use some basic algebra. First, let's simplify the expression inside the parentheses:
+```
+(8x + 2x) = 10x
+```
+Now we can substitute this value back into the original equation and isolate x on one side:
+```
+10x - 2x = 130
+```
+Next, let's add 2x to both sides of the equation to get rid of the negative sign:
+```
+12x = 132
+```
+Now we can divide both sides by 12</t>
         </is>
       </c>
     </row>
@@ -1637,7 +1866,12 @@
       <c r="E23" t="inlineStr"/>
       <c r="F23" t="inlineStr">
         <is>
-          <t>To solve this equation for "x", we can first simplify it using some algebraic manipulation. Starting with the original expression, we get:\n(8*x) + (2^x) = 130\nMultiplying both sides by 2^x gives us:\n(8*x)*(2^x) = 2^(x+1)(130-x)\nUsing the fact that x is a positive integer, we can simplify further to get:\n64x + 2^x &gt; 130 - x (since 2^x &gt; 13</t>
+          <t>To solve this equation for "x", we can first simplify it using some algebraic manipulation. Starting with the original expression, we get:
+(8*x) + (2^x) = 130
+Multiplying both sides by 2^x gives us:
+(8*x)*(2^x) = 2^(x+1)(130-x)
+Using the fact that x is a positive integer, we can simplify further to get:
+64x + 2^x &gt; 130 - x (since 2^x &gt; 13</t>
         </is>
       </c>
     </row>
@@ -1703,7 +1937,20 @@
       <c r="E26" t="inlineStr"/>
       <c r="F26" t="inlineStr">
         <is>
-          <t>In 8^X+2^X=130 show how to solve for X\nTo solve for X in the equation 2^X = 130, we can use logarithmic properties. We know that log(a^b) = b*log(a), where a and b are positive numbers. In this case, we can set up two equations with different bases:\nlog(2^X) = X*log(2)\n130 = 2^X\nWe can solve for X by equating the two expressions we just derived and simplifying:\nX*log(2) = 130\nlog(2^X) = log(130/2)\nTaking the logarithm of both sides, we get:\nX*log(2) = log(65)\nDividing both sides by log(2), we get:\nX = log(65)/log(2)\nUsing a calculator or simplifying the logarithms, we get:\nX = 5.317\nTherefore, X is approximately equal to 5.317.</t>
+          <t>In 8^X+2^X=130 show how to solve for X
+To solve for X in the equation 2^X = 130, we can use logarithmic properties. We know that log(a^b) = b*log(a), where a and b are positive numbers. In this case, we can set up two equations with different bases:
+log(2^X) = X*log(2)
+130 = 2^X
+We can solve for X by equating the two expressions we just derived and simplifying:
+X*log(2) = 130
+log(2^X) = log(130/2)
+Taking the logarithm of both sides, we get:
+X*log(2) = log(65)
+Dividing both sides by log(2), we get:
+X = log(65)/log(2)
+Using a calculator or simplifying the logarithms, we get:
+X = 5.317
+Therefore, X is approximately equal to 5.317.</t>
         </is>
       </c>
     </row>
@@ -1725,7 +1972,13 @@
       <c r="E27" t="inlineStr"/>
       <c r="F27" t="inlineStr">
         <is>
-          <t>To solve the equation 8^x + 2^x = 130, we can use exponent rules and simplify both sides of the equation. \nFirst, let's apply the power rule of exponents: \n8^x + 2^x = (8 * 2) ^ x = 16^x \nNow, we can simplify further by using the fact that any base raised to the power of zero is equal to one: \n16^0 = 1 \nSo, we just need to solve for x such that: \n1 = 8^</t>
+          <t>To solve the equation 8^x + 2^x = 130, we can use exponent rules and simplify both sides of the equation. 
+First, let's apply the power rule of exponents: 
+8^x + 2^x = (8 * 2) ^ x = 16^x 
+Now, we can simplify further by using the fact that any base raised to the power of zero is equal to one: 
+16^0 = 1 
+So, we just need to solve for x such that: 
+1 = 8^</t>
         </is>
       </c>
     </row>
@@ -1859,7 +2112,14 @@
       <c r="E2" t="inlineStr"/>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Here is an example Python code that can be used to solve the equation `ax^3 + bx^2 + c * x + d = 0` using Cardano's Formula and find all possible solutions for x:\n```python\nimport math\na,b,c,d = [1,0,1,-130] # coefficients of the given equation\nD = (b**2 - 4*a*c) / (4*a) # discriminant\nif D &lt; 0:\n    print("No real solutions")\nelif D == 0:</t>
+          <t>Here is an example Python code that can be used to solve the equation `ax^3 + bx^2 + c * x + d = 0` using Cardano's Formula and find all possible solutions for x:
+```python
+import math
+a,b,c,d = [1,0,1,-130] # coefficients of the given equation
+D = (b**2 - 4*a*c) / (4*a) # discriminant
+if D &lt; 0:
+    print("No real solutions")
+elif D == 0:</t>
         </is>
       </c>
     </row>
@@ -1881,7 +2141,9 @@
       <c r="E3" t="inlineStr"/>
       <c r="F3" t="inlineStr">
         <is>
-          <t>To write a Python program that solves for all possible solutions of the cubic equation ax³ + bx² + cx + d = 0 with given coefficients a,b,c and d, we can follow these steps:\n1. First, define a function `solve_cubic` to solve the cubic equation using Cardano's formula. This function takes in the coefficients of the equation as arguments and returns a list of all possible solutions for x.\n2. Inside the `solve_cubic` function, we can use the complex numbers library to find the roots of the polynomial equation using</t>
+          <t>To write a Python program that solves for all possible solutions of the cubic equation ax³ + bx² + cx + d = 0 with given coefficients a,b,c and d, we can follow these steps:
+1. First, define a function `solve_cubic` to solve the cubic equation using Cardano's formula. This function takes in the coefficients of the equation as arguments and returns a list of all possible solutions for x.
+2. Inside the `solve_cubic` function, we can use the complex numbers library to find the roots of the polynomial equation using</t>
         </is>
       </c>
     </row>
@@ -1903,7 +2165,15 @@
       <c r="E4" t="inlineStr"/>
       <c r="F4" t="inlineStr">
         <is>
-          <t>```python\ndef main():\n    def f(a, b, c, d):\n        discriminant = (b**2) - 4 * a * c\n        \n        if discriminant &gt; 0:\n            # There are two real roots.\n            \n            root1, root2 = sqrt((-b + (-discriminant) / (2 * a))), sqrt((-b + (-discriminant) / (2 * a)))\n        elif discriminant == 0:\n            # There is one real root.</t>
+          <t>```python
+def main():
+    def f(a, b, c, d):
+        discriminant = (b**2) - 4 * a * c
+        if discriminant &gt; 0:
+            # There are two real roots.
+            root1, root2 = sqrt((-b + (-discriminant) / (2 * a))), sqrt((-b + (-discriminant) / (2 * a)))
+        elif discriminant == 0:
+            # There is one real root.</t>
         </is>
       </c>
     </row>
@@ -1925,7 +2195,12 @@
       <c r="E5" t="inlineStr"/>
       <c r="F5" t="inlineStr">
         <is>
-          <t>```python\ndef cubic_equation(a, b, c, d):\n    D = (b**2) - 3 * a * c + 8 * a * d - 4 * b * d + 12 * c * d\n    \n    if D &gt; 0:\n        r1 = (-b + math.sqrt(D)) / (6 * a)\n        \n        if r1 % 1 == 0 and abs(r1 - round(r1, 3)) &lt; 0.0001: # Check for integer solution</t>
+          <t>```python
+def cubic_equation(a, b, c, d):
+    D = (b**2) - 3 * a * c + 8 * a * d - 4 * b * d + 12 * c * d
+    if D &gt; 0:
+        r1 = (-b + math.sqrt(D)) / (6 * a)
+        if r1 % 1 == 0 and abs(r1 - round(r1, 3)) &lt; 0.0001: # Check for integer solution</t>
         </is>
       </c>
     </row>
@@ -1947,7 +2222,15 @@
       <c r="E6" t="inlineStr"/>
       <c r="F6" t="inlineStr">
         <is>
-          <t>```python\ndef solve_cubic(a, b, c, d):\n    # Find the discriminant (Δ) and its sign\n    D = b**2 - 3*a*c\n    \n    if D &gt; 0:\n        m1, m2 = (-b + math.sqrt(D)) / (6 * a), (-b - math.sqrt(D)) / (6 * a)\n        \n        # Check for real roots\n        if m1 &gt;= 0 and m2 &lt;= 0:\n            return [x for x in range(-</t>
+          <t>```python
+def solve_cubic(a, b, c, d):
+    # Find the discriminant (Δ) and its sign
+    D = b**2 - 3*a*c
+    if D &gt; 0:
+        m1, m2 = (-b + math.sqrt(D)) / (6 * a), (-b - math.sqrt(D)) / (6 * a)
+        # Check for real roots
+        if m1 &gt;= 0 and m2 &lt;= 0:
+            return [x for x in range(-</t>
         </is>
       </c>
     </row>
@@ -1969,7 +2252,13 @@
       <c r="E7" t="inlineStr"/>
       <c r="F7" t="inlineStr">
         <is>
-          <t>Here is an example Python code that can be used to find all possible solutions for the equation ax^3 + bx^2 + cx + d = 0 using Cardano's formula and Newton-Raphson method:\n```python\nimport math\ndef cardano_formula(a,b,c):\n    # Find two rational roots of x^3+ax^2+cx+d=0\n    r1,r2 = (int(math.sqrt(-b)) + int(math.pow(-b,-1)))/2, 0\n    \n    if a ==</t>
+          <t>Here is an example Python code that can be used to find all possible solutions for the equation ax^3 + bx^2 + cx + d = 0 using Cardano's formula and Newton-Raphson method:
+```python
+import math
+def cardano_formula(a,b,c):
+    # Find two rational roots of x^3+ax^2+cx+d=0
+    r1,r2 = (int(math.sqrt(-b)) + int(math.pow(-b,-1)))/2, 0
+    if a ==</t>
         </is>
       </c>
     </row>
@@ -1991,7 +2280,27 @@
       <c r="E8" t="inlineStr"/>
       <c r="F8" t="inlineStr">
         <is>
-          <t>in ax^3+bx^2+c*x+d=0, write a python program to solve for all possible values of x\nSure! Here's a Python program that can be used to solve the given equation for all possible values of x:\n```python\ndef solve_equation(a, b, c, d):\n    x = 0.0\n    while True:\n        if (a*x**2 + b*x + c) * (d - a*x - b) == 0:\n            break\n        x += 1\n    return x\n```\nTo use this function, simply pass in the values of a, b, c, and d as arguments. For example:\n```python\na = 2\nb = 3\nc = 4\nd = -5\nx = solve_equation(a, b, c, d)\nprint(x) # Output: 0.0\n```\nThis will print the value of x that satisfies the given equation for the given values of a, b, c, and d.</t>
+          <t>in ax^3+bx^2+c*x+d=0, write a python program to solve for all possible values of x
+Sure! Here's a Python program that can be used to solve the given equation for all possible values of x:
+```python
+def solve_equation(a, b, c, d):
+    x = 0.0
+    while True:
+        if (a*x**2 + b*x + c) * (d - a*x - b) == 0:
+            break
+        x += 1
+    return x
+```
+To use this function, simply pass in the values of a, b, c, and d as arguments. For example:
+```python
+a = 2
+b = 3
+c = 4
+d = -5
+x = solve_equation(a, b, c, d)
+print(x) # Output: 0.0
+```
+This will print the value of x that satisfies the given equation for the given values of a, b, c, and d.</t>
         </is>
       </c>
     </row>
@@ -2013,7 +2322,21 @@
       <c r="E9" t="inlineStr"/>
       <c r="F9" t="inlineStr">
         <is>
-          <t>in ax^3+bx^2+c*x+d=0, write a python program to solve for all possible values of x\nSure! Here's an example Python program that uses the `numpy` library to find all possible solutions (i.e., roots) of the equation ax^3 + bx^2 + cx + d = 0 in the range [0, 1]. The program assumes that you have already defined constants a, b, c, and d:\n```python\nimport numpy as np\n\n# Define constants\na = 2.5\nb = 3.5\nc = -1.5\nd = 0.5\n\n# Solve for all possible values of x in [0, 1]\nroots = np.roots(np.array([[a**3 + b*x**2 + cx + d], [x]]))\nprint("All roots:")\nfor root in roots:\n    print(root)\n```</t>
+          <t>in ax^3+bx^2+c*x+d=0, write a python program to solve for all possible values of x
+Sure! Here's an example Python program that uses the `numpy` library to find all possible solutions (i.e., roots) of the equation ax^3 + bx^2 + cx + d = 0 in the range [0, 1]. The program assumes that you have already defined constants a, b, c, and d:
+```python
+import numpy as np
+# Define constants
+a = 2.5
+b = 3.5
+c = -1.5
+d = 0.5
+# Solve for all possible values of x in [0, 1]
+roots = np.roots(np.array([[a**3 + b*x**2 + cx + d], [x]]))
+print("All roots:")
+for root in roots:
+    print(root)
+```</t>
         </is>
       </c>
     </row>
@@ -2035,7 +2358,8 @@
       <c r="E10" t="inlineStr"/>
       <c r="F10" t="inlineStr">
         <is>
-          <t>To solve this equation using Cardano’s method in Python programming language, we will follow these steps: 1. First, rewrite it in terms of base ten numbers instead of powers of two and one. The equation can be rewritten as ax^3+bx^2+c*x+d=0 where a = 1, b = 0, c = 1 and d = -130.\n2. Then we will use the addition property to add or subtract terms until there is only one term left in the equation. In this case, ax^3+bx^2+c</t>
+          <t>To solve this equation using Cardano’s method in Python programming language, we will follow these steps: 1. First, rewrite it in terms of base ten numbers instead of powers of two and one. The equation can be rewritten as ax^3+bx^2+c*x+d=0 where a = 1, b = 0, c = 1 and d = -130.
+2. Then we will use the addition property to add or subtract terms until there is only one term left in the equation. In this case, ax^3+bx^2+c</t>
         </is>
       </c>
     </row>
@@ -2057,7 +2381,10 @@
       <c r="E11" t="inlineStr"/>
       <c r="F11" t="inlineStr">
         <is>
-          <t>in ax^3+bx^2+c*x+d=0, write a python program to solve for all possible values of x\nimport math \ndef f(a,b): \n    return (pow((1/a),(4))*((-1)**b)*(math.sqrt(((a**3)/abs(f(a,b))))+2*c) +d</t>
+          <t>in ax^3+bx^2+c*x+d=0, write a python program to solve for all possible values of x
+import math 
+def f(a,b): 
+    return (pow((1/a),(4))*((-1)**b)*(math.sqrt(((a**3)/abs(f(a,b))))+2*c) +d</t>
         </is>
       </c>
     </row>
@@ -2079,7 +2406,20 @@
       <c r="E12" t="inlineStr"/>
       <c r="F12" t="inlineStr">
         <is>
-          <t>in ax^3+bx^2+c*x+d=0, write a python program to solve for all possible values of x\nSure, here's the Python code to solve for all possible values of `x` in the equation `ax^3 + bx^2 + c*x + d = 0`:\n```python\nimport sympy as sp\n# Define variables and coefficients\na = sp.Symbol('a')\nb = sp.Symbol('b')\nc = sp.Symbol('c')\nd = sp.Symbol('d')\n# Solve for all possible values of x using the solve function from SymPy\nx_values = sp.solve(a*sp.pow(x, 3) + b*sp.pow(x, 2) + c*x + d, x)\nprint("All possible values of x:", x_values)\n```\nThis code uses the `sympy` library to define variables and coefficients as symbols (`a`, `b`, `c`, and `d`) and then solves for all possible values of `x` using the `solve` function. The resulting output will be a list of all possible values of `x`.</t>
+          <t>in ax^3+bx^2+c*x+d=0, write a python program to solve for all possible values of x
+Sure, here's the Python code to solve for all possible values of `x` in the equation `ax^3 + bx^2 + c*x + d = 0`:
+```python
+import sympy as sp
+# Define variables and coefficients
+a = sp.Symbol('a')
+b = sp.Symbol('b')
+c = sp.Symbol('c')
+d = sp.Symbol('d')
+# Solve for all possible values of x using the solve function from SymPy
+x_values = sp.solve(a*sp.pow(x, 3) + b*sp.pow(x, 2) + c*x + d, x)
+print("All possible values of x:", x_values)
+```
+This code uses the `sympy` library to define variables and coefficients as symbols (`a`, `b`, `c`, and `d`) and then solves for all possible values of `x` using the `solve` function. The resulting output will be a list of all possible values of `x`.</t>
         </is>
       </c>
     </row>
@@ -2101,7 +2441,13 @@
       <c r="E13" t="inlineStr"/>
       <c r="F13" t="inlineStr">
         <is>
-          <t>in ax^3+bx^2+c*x+d=0, write a python program to solve for all possible values of x\nHere is the code that solves this equation.  It uses the method of completing the square and then factoring out the constant term, which yields an expression in terms of only one variable (x). The solution set can be found by solving this new expression for x using any appropriate technique such as graphing or substitution:\ndef solve_equation(ax3+bx2+c*x+d): \n    # Complete the square to factor out constant term.  This yields an equation in terms of only one variable (x).   \n	a = ax3 + bx2 + c * x + d #constant term is factored out, leaving expression as a function of just 1 varible(x)\n	 \n    #Solve the new expression for x using any appropriate technique such as graphing or substitution.  This yields all possible values of x in solution set\n	return solve_expression(a)</t>
+          <t>in ax^3+bx^2+c*x+d=0, write a python program to solve for all possible values of x
+Here is the code that solves this equation.  It uses the method of completing the square and then factoring out the constant term, which yields an expression in terms of only one variable (x). The solution set can be found by solving this new expression for x using any appropriate technique such as graphing or substitution:
+def solve_equation(ax3+bx2+c*x+d): 
+    # Complete the square to factor out constant term.  This yields an equation in terms of only one variable (x).   
+	a = ax3 + bx2 + c * x + d #constant term is factored out, leaving expression as a function of just 1 varible(x)
+    #Solve the new expression for x using any appropriate technique such as graphing or substitution.  This yields all possible values of x in solution set
+	return solve_expression(a)</t>
         </is>
       </c>
     </row>
@@ -2123,7 +2469,28 @@
       <c r="E14" t="inlineStr"/>
       <c r="F14" t="inlineStr">
         <is>
-          <t>in ax^3+bx^2+c*x+d=0, write a python program to solve for all possible values of x\nHere's a Python program that can solve the equation ax3+bx^2+cx+d=0 for all possible values of x:\n```python\nimport numpy as np\ndef solve_equation(coeffs):\n    # Convert the coefficients to a NumPy array\n    coeffs_np = np.array(coeffs)\n    # Find the roots of the equation using the numpy.roots method\n    roots_np = np.roots(coeffs_np)\n    # Sort the roots so that they are in ascending order\n    roots_np = roots_np[np.argsort(-roots_np)[0]]\n    # Print the roots\n    for root, imroot in roots_np:\n        if imroot is not None:\n            print(f'{root} + {imroot}i')\n        else:\n            print(f'{root}')\n# Convert the coefficients to a NumPy array\ncoeffs = [1, 2, 3, 4]\nsolve_equation(coeffs)\n```\nThis program uses the `numpy` library to find the roots of the equation. It first converts the coefficients to a NumPy array, then uses the `numpy.roots` method to find the roots of the equation. The `argsort` method is used to sort the roots so that they are in ascending order. Finally, the program prints the roots, either as a real number or as a complex number with an optional imaginary part.</t>
+          <t>in ax^3+bx^2+c*x+d=0, write a python program to solve for all possible values of x
+Here's a Python program that can solve the equation ax3+bx^2+cx+d=0 for all possible values of x:
+```python
+import numpy as np
+def solve_equation(coeffs):
+    # Convert the coefficients to a NumPy array
+    coeffs_np = np.array(coeffs)
+    # Find the roots of the equation using the numpy.roots method
+    roots_np = np.roots(coeffs_np)
+    # Sort the roots so that they are in ascending order
+    roots_np = roots_np[np.argsort(-roots_np)[0]]
+    # Print the roots
+    for root, imroot in roots_np:
+        if imroot is not None:
+            print(f'{root} + {imroot}i')
+        else:
+            print(f'{root}')
+# Convert the coefficients to a NumPy array
+coeffs = [1, 2, 3, 4]
+solve_equation(coeffs)
+```
+This program uses the `numpy` library to find the roots of the equation. It first converts the coefficients to a NumPy array, then uses the `numpy.roots` method to find the roots of the equation. The `argsort` method is used to sort the roots so that they are in ascending order. Finally, the program prints the roots, either as a real number or as a complex number with an optional imaginary part.</t>
         </is>
       </c>
     </row>
@@ -2145,7 +2512,19 @@
       <c r="E15" t="inlineStr"/>
       <c r="F15" t="inlineStr">
         <is>
-          <t>in ax^3+bx^2+c*x+d=0, write a python program to solve for all possible values of x\nHere's a Python program that can solve the quadratic equation ax^2 + bx + c = 0 for all possible values of x:\n```python\nimport sympy\n# Define the coefficients a, b, and c\na, b, c = 3, -4, 1\n# Solve for x using sympy library\nx_solution = sympy.solve(sympy.Symbol('x')**2 + sympy.Symbol('b')*sympy.Symbol('x') + sympy.Symbol('c') == 0, sympy.Symbol('x'))\n# Print the solutions for x\nfor solution in x_solution:\n    print(str(solution))\n```\nIn this program, we use the `sympy` library to solve the quadratic equation. We first define the coefficients a, b, and c as variables. Then, we use the `solve()` function to find all possible solutions for x. Finally, we print the solutions for x using a for loop.</t>
+          <t>in ax^3+bx^2+c*x+d=0, write a python program to solve for all possible values of x
+Here's a Python program that can solve the quadratic equation ax^2 + bx + c = 0 for all possible values of x:
+```python
+import sympy
+# Define the coefficients a, b, and c
+a, b, c = 3, -4, 1
+# Solve for x using sympy library
+x_solution = sympy.solve(sympy.Symbol('x')**2 + sympy.Symbol('b')*sympy.Symbol('x') + sympy.Symbol('c') == 0, sympy.Symbol('x'))
+# Print the solutions for x
+for solution in x_solution:
+    print(str(solution))
+```
+In this program, we use the `sympy` library to solve the quadratic equation. We first define the coefficients a, b, and c as variables. Then, we use the `solve()` function to find all possible solutions for x. Finally, we print the solutions for x using a for loop.</t>
         </is>
       </c>
     </row>
@@ -2167,7 +2546,42 @@
       <c r="E16" t="inlineStr"/>
       <c r="F16" t="inlineStr">
         <is>
-          <t>in ax^3+bx^2+c*x+d=0, write a python program to solve for all possible values of x\n```python\n\ndef get_roots(a,  # coefficient in the root's power term. Can be positive or negative integer/float number with no zeroes before it and after any significance character like +-*^ etc... Example a=3 means that there is one real solution to this system of linear systems\n    b=0,                                   // constant value (or the root) in our problem. Can be positive or negative integer/float number with no zeroes before it and after any significance character like +-*^ etc... Example:  b=2 means that there is one real solution to this system of linear systems\n    c=0,                                   // coefficient for the root's power term. Can be positive or negative integer/float number with no zeroes before it and after any significance character like +-*^ etc... Example:  a=3 means that there is one real solution to this system of linear systems\n    d=0,                                   // coefficient for the root's power term. Can be positive or negative integer/float number with no zeroes before it and after any significance character like +-*^ etc... Example:  a=3 means that there is one real solution to this system of linear systems\n    precision = 1e-6                        # precision for the roots, default value=1e-6, which will give you a list with all possible values. If your problem has only two or three different types/values in it't range then set an appropriate number here like 1e-4 to get more accuracy and less time\n    ):\n\n    from math_utils import *  # this is the library that contains some useful functions for our programs, you can use them as they are without any modification. You don’ts have anything else in it except these two lines of code which we will be using later on to get all possible values\n    root = []\n\n    from math import *  # this is the library that contains some useful functions for our programs, you can use them as they are without any modification. You don’ts have anything else in it except these two lines of code which we will be using later on to get all possible values\n    x = []\n\n    from math import *  # this is the library that contains some useful functions for our programs, you can use them as they are without any modification. You don’ts have anything else in it except these two lines of code which we will be using later on to get all possible values\n    y = []\n\n    from math import *  # this is the library that contains some useful functions for our programs, you can use them as they are without any modification. You don’ts have anything else in it except these two lines of code which we will be using later on to get all possible values\n    z = []\n\n    from math import *  # this is the library that contains some useful functions for our programs, you can use them as they are without any modification. You don’ts have anything else in it except these two lines of code which we will be using later on to get all possible values\n    w = []\n\n    from math import *  # this is the library that contains some useful functions for our programs, you can use them as they are without any modification. You don’ts have anything else in it except these two lines of code which we will be using later on to get all possible values\n    v = []\n\n    from math import *  # this is the library that contains some useful functions for our programs, you can use them as they are without any modification. You don’ts have anything else in it except these two lines of code which we will be using later on to get all possible values\n    u = []\n\n    from math import *  # this is the library that contains some useful functions for our programs, you can use them as they are without any modification. You don’ts have anything else in it except these two lines of code which we will be using later on to get all possible values\n    t = []\n\n    from math import *  # this is the library that contains some useful functions for our programs, you can use them as they are without any modification. You don’ts have anything else in it except these two lines of code which we will be using later on to get all possible values\n    p = []\n\n    from math import *  # this is the library that contains some useful functions for our programs, you can use them as they are without any modification. You don’ts have anything else in it except these two lines of code which we will be using later on to get all possible values\n    q = []\n\n    from math import *  # this is the library that contains some useful functions for our programs, you can use them as they are without any modification. You don’ts have anything else in it except these two lines of code which we will be using later on to get all possible values\n    r = []\n\n    from math import *  # this is the library that contains some useful functions for our programs, you can use them as they are without any modification. You don’ts have anything else in it except these two lines of code which we will be using later on to get all possible values\n    e = []\n\n    from math import *  # this is the library that contains some useful functions for our programs, you can use them as they are without any modification. You don’ts have anything else in it except these two lines of code which we will be using later on to get all possible values\n    f = []\n\n    from math import *  # this is the library that contains some useful functions for our programs, you can use them as they are without any modification. You don’ts have anything else in it except these two lines of code which we will be using later on to get all possible values\n    g = []</t>
+          <t>in ax^3+bx^2+c*x+d=0, write a python program to solve for all possible values of x
+```python
+def get_roots(a,  # coefficient in the root's power term. Can be positive or negative integer/float number with no zeroes before it and after any significance character like +-*^ etc... Example a=3 means that there is one real solution to this system of linear systems
+    b=0,                                   // constant value (or the root) in our problem. Can be positive or negative integer/float number with no zeroes before it and after any significance character like +-*^ etc... Example:  b=2 means that there is one real solution to this system of linear systems
+    c=0,                                   // coefficient for the root's power term. Can be positive or negative integer/float number with no zeroes before it and after any significance character like +-*^ etc... Example:  a=3 means that there is one real solution to this system of linear systems
+    d=0,                                   // coefficient for the root's power term. Can be positive or negative integer/float number with no zeroes before it and after any significance character like +-*^ etc... Example:  a=3 means that there is one real solution to this system of linear systems
+    precision = 1e-6                        # precision for the roots, default value=1e-6, which will give you a list with all possible values. If your problem has only two or three different types/values in it't range then set an appropriate number here like 1e-4 to get more accuracy and less time
+    ):
+    from math_utils import *  # this is the library that contains some useful functions for our programs, you can use them as they are without any modification. You don’ts have anything else in it except these two lines of code which we will be using later on to get all possible values
+    root = []
+    from math import *  # this is the library that contains some useful functions for our programs, you can use them as they are without any modification. You don’ts have anything else in it except these two lines of code which we will be using later on to get all possible values
+    x = []
+    from math import *  # this is the library that contains some useful functions for our programs, you can use them as they are without any modification. You don’ts have anything else in it except these two lines of code which we will be using later on to get all possible values
+    y = []
+    from math import *  # this is the library that contains some useful functions for our programs, you can use them as they are without any modification. You don’ts have anything else in it except these two lines of code which we will be using later on to get all possible values
+    z = []
+    from math import *  # this is the library that contains some useful functions for our programs, you can use them as they are without any modification. You don’ts have anything else in it except these two lines of code which we will be using later on to get all possible values
+    w = []
+    from math import *  # this is the library that contains some useful functions for our programs, you can use them as they are without any modification. You don’ts have anything else in it except these two lines of code which we will be using later on to get all possible values
+    v = []
+    from math import *  # this is the library that contains some useful functions for our programs, you can use them as they are without any modification. You don’ts have anything else in it except these two lines of code which we will be using later on to get all possible values
+    u = []
+    from math import *  # this is the library that contains some useful functions for our programs, you can use them as they are without any modification. You don’ts have anything else in it except these two lines of code which we will be using later on to get all possible values
+    t = []
+    from math import *  # this is the library that contains some useful functions for our programs, you can use them as they are without any modification. You don’ts have anything else in it except these two lines of code which we will be using later on to get all possible values
+    p = []
+    from math import *  # this is the library that contains some useful functions for our programs, you can use them as they are without any modification. You don’ts have anything else in it except these two lines of code which we will be using later on to get all possible values
+    q = []
+    from math import *  # this is the library that contains some useful functions for our programs, you can use them as they are without any modification. You don’ts have anything else in it except these two lines of code which we will be using later on to get all possible values
+    r = []
+    from math import *  # this is the library that contains some useful functions for our programs, you can use them as they are without any modification. You don’ts have anything else in it except these two lines of code which we will be using later on to get all possible values
+    e = []
+    from math import *  # this is the library that contains some useful functions for our programs, you can use them as they are without any modification. You don’ts have anything else in it except these two lines of code which we will be using later on to get all possible values
+    f = []
+    from math import *  # this is the library that contains some useful functions for our programs, you can use them as they are without any modification. You don’ts have anything else in it except these two lines of code which we will be using later on to get all possible values
+    g = []</t>
         </is>
       </c>
     </row>
@@ -2189,7 +2603,18 @@
       <c r="E17" t="inlineStr"/>
       <c r="F17" t="inlineStr">
         <is>
-          <t>in ax^3+bx^2+c*x+d=0, write a python program to solve for all possible values of x\ndef solve_ax3(a, b, c, d): \n    # Check if the discriminant is negative \n    if (b**2 - 4*a*c) &lt; 0: \n        print("No real solutions") \n    else: \n        # Get the roots of the quadratic equation \n        x1, x2 = (-b + sqrt(b**2 - 4*a*c)) / (2*a), (-b - sqrt(b**2 - 4*a*c)) / (2*a) \n        \n        # Print the roots of the equation \n        print("x = ", x1, "or", x2) \n    return None\n```</t>
+          <t>in ax^3+bx^2+c*x+d=0, write a python program to solve for all possible values of x
+def solve_ax3(a, b, c, d): 
+    # Check if the discriminant is negative 
+    if (b**2 - 4*a*c) &lt; 0: 
+        print("No real solutions") 
+    else: 
+        # Get the roots of the quadratic equation 
+        x1, x2 = (-b + sqrt(b**2 - 4*a*c)) / (2*a), (-b - sqrt(b**2 - 4*a*c)) / (2*a) 
+        # Print the roots of the equation 
+        print("x = ", x1, "or", x2) 
+    return None
+```</t>
         </is>
       </c>
     </row>
@@ -2233,7 +2658,10 @@
       <c r="E19" t="inlineStr"/>
       <c r="F19" t="inlineStr">
         <is>
-          <t>To find all solutions of the equation ax^3 + bx^2 + cx + d = 0 using Python, we can follow these steps: first, define variables for each coefficient and value; then use the `solve()` function from the `sympy` library to solve for x. We will need to pass in the coefficients as a tuple or list of symbols along with any other desired parameters such as tolerance level.\n```python\nimport sympy\n\na, b, c, d = map(sympy.symbols, ['a', 'b', 'c', 'd']) # define variables</t>
+          <t>To find all solutions of the equation ax^3 + bx^2 + cx + d = 0 using Python, we can follow these steps: first, define variables for each coefficient and value; then use the `solve()` function from the `sympy` library to solve for x. We will need to pass in the coefficients as a tuple or list of symbols along with any other desired parameters such as tolerance level.
+```python
+import sympy
+a, b, c, d = map(sympy.symbols, ['a', 'b', 'c', 'd']) # define variables</t>
         </is>
       </c>
     </row>
@@ -2255,7 +2683,13 @@
       <c r="E20" t="inlineStr"/>
       <c r="F20" t="inlineStr">
         <is>
-          <t>in ax^3+bx^2+c*x+d=0, write a python program to solve for all possible values of x\n```python\nimport sympy as sp\n\nequation = sp.Equation(ax3 + bx**2 + c*x + d)\nsolutions = equation.solve()\nprint("All possible solutions of x: ", solutions)\n```</t>
+          <t>in ax^3+bx^2+c*x+d=0, write a python program to solve for all possible values of x
+```python
+import sympy as sp
+equation = sp.Equation(ax3 + bx**2 + c*x + d)
+solutions = equation.solve()
+print("All possible solutions of x: ", solutions)
+```</t>
         </is>
       </c>
     </row>
@@ -2277,7 +2711,24 @@
       <c r="E21" t="inlineStr"/>
       <c r="F21" t="inlineStr">
         <is>
-          <t>in ax^3+bx^2+c*x+d=0, write a python program to solve for all possible values of x\nHere's a Python program that solves the equation `ax3 + bx^2 + c*x + d = 0` for all possible values of `x`:\n```python\nimport sympy\n\ndef solve(a, b, c, d):\n    x = sympy.symbols('x')\n    result = []\n    \n    # Use the Risch algorithm to find all solutions\n    for p in sympy.polys.polyroots(sympy.polynomials.Poly(a*x**3 + b*x**2 + c*x + d, x), x):\n        result.append((p.evalf(10).n()[0], p))\n        \n    return result\n\n# Test the function with some examples\nprint(solve(0, 0, -5, 2))  # (0, -5)\nprint(solve(0, 0, 7, 3))   # (0, 7)\nprint(solve(1, 0, -2, 4))  # (1, -2)\nprint(solve(0, 1, 6, 2))   # (0, 6)\n```\nThis program uses the `sympy` library to solve the equation for all possible values of `x`. The solutions are returned as tuples containing the value of `x` and its multiplicity.</t>
+          <t>in ax^3+bx^2+c*x+d=0, write a python program to solve for all possible values of x
+Here's a Python program that solves the equation `ax3 + bx^2 + c*x + d = 0` for all possible values of `x`:
+```python
+import sympy
+def solve(a, b, c, d):
+    x = sympy.symbols('x')
+    result = []
+    # Use the Risch algorithm to find all solutions
+    for p in sympy.polys.polyroots(sympy.polynomials.Poly(a*x**3 + b*x**2 + c*x + d, x), x):
+        result.append((p.evalf(10).n()[0], p))
+    return result
+# Test the function with some examples
+print(solve(0, 0, -5, 2))  # (0, -5)
+print(solve(0, 0, 7, 3))   # (0, 7)
+print(solve(1, 0, -2, 4))  # (1, -2)
+print(solve(0, 1, 6, 2))   # (0, 6)
+```
+This program uses the `sympy` library to solve the equation for all possible values of `x`. The solutions are returned as tuples containing the value of `x` and its multiplicity.</t>
         </is>
       </c>
     </row>
@@ -2299,7 +2750,16 @@
       <c r="E22" t="inlineStr"/>
       <c r="F22" t="inlineStr">
         <is>
-          <t>Here's an example Python program that solves for all possible values of x in the equation ax^3 + bx^2 + c*x + d = 0:\n```python\nimport sympy\ndef find_solutions(a, b, c, d):\n    # Convert the coefficients to SymPy symbols\n    a = sympy.Symbol('a')\n    b = sympy.Symbol('b')\n    c = sympy.Symbol('c')\n    d = sympy.Symbol('d')\n    \n    # Solve for x using Cardano's formula</t>
+          <t>Here's an example Python program that solves for all possible values of x in the equation ax^3 + bx^2 + c*x + d = 0:
+```python
+import sympy
+def find_solutions(a, b, c, d):
+    # Convert the coefficients to SymPy symbols
+    a = sympy.Symbol('a')
+    b = sympy.Symbol('b')
+    c = sympy.Symbol('c')
+    d = sympy.Symbol('d')
+    # Solve for x using Cardano's formula</t>
         </is>
       </c>
     </row>
@@ -2321,7 +2781,12 @@
       <c r="E23" t="inlineStr"/>
       <c r="F23" t="inlineStr">
         <is>
-          <t>Here's a Python program that uses Cardano’s formula to find all possible roots of the equation ax^3 + bx^2 + cx + d = 0. We assume that a is equal to 1, b is equal to 0, c is equal to 1 and d is equal to -130:\n```python\nimport math\ndef cardano(a,b,c,d):\n p = (-d + math.sqrt(d*d-4*a*c)) / (2 * a)\n q = (-d - math.sqrt(d*d</t>
+          <t>Here's a Python program that uses Cardano’s formula to find all possible roots of the equation ax^3 + bx^2 + cx + d = 0. We assume that a is equal to 1, b is equal to 0, c is equal to 1 and d is equal to -130:
+```python
+import math
+def cardano(a,b,c,d):
+ p = (-d + math.sqrt(d*d-4*a*c)) / (2 * a)
+ q = (-d - math.sqrt(d*d</t>
         </is>
       </c>
     </row>
@@ -2365,7 +2830,13 @@
       <c r="E25" t="inlineStr"/>
       <c r="F25" t="inlineStr">
         <is>
-          <t>To solve the cubic equation ax^3 + bx^2 + cx + d = 0 using Python, we can use the Cardano's Formula. Here is an example code that solves this equation when a=1, b=0, c=1 and d=-130:\n\n```python\nimport math\ndef solve_cubic(a,b,c,d):\n q = (b**2)/4 + c/2 - d/a\n Q = (-b**3)/9 + (c**2)/4\n theta = math.acos(-q</t>
+          <t>To solve the cubic equation ax^3 + bx^2 + cx + d = 0 using Python, we can use the Cardano's Formula. Here is an example code that solves this equation when a=1, b=0, c=1 and d=-130:
+```python
+import math
+def solve_cubic(a,b,c,d):
+ q = (b**2)/4 + c/2 - d/a
+ Q = (-b**3)/9 + (c**2)/4
+ theta = math.acos(-q</t>
         </is>
       </c>
     </row>
@@ -2387,7 +2858,26 @@
       <c r="E26" t="inlineStr"/>
       <c r="F26" t="inlineStr">
         <is>
-          <t>in ax^3+bx^2+c*x+d=0, write a python program to solve for all possible values of x\nSure! Here's a Python program that solves for all possible values of x in the equation ax3+bx^2+c*x+d=0:\n```python\nimport sympy\n# Define the variables and coefficients\na = sympy.Symbol('a')\nb = sympy.Symbol('b')\nc = sympy.Symbol('c')\nd = sympy.Symbol('d')\n# Generate a list of all possible solutions for x\nsolutions = []\nfor x in range(1, 10):\n    if sympy.solve(a*x**3 + b*x**2 + c*x + d, sympy.Symbol('x')):\n        solutions.append(x)\n# Print the list of solutions\nprint("Solutions for x:")\nfor solution in solutions:\n    print("x =", solution)\n```\nThis program uses the SymPy library to solve for all possible values of x in the equation ax3+bx^2+c*x+d=0. It generates a list of all possible solutions for x using a for loop and the sympy.solve() function, which returns a list of solutions if one exists. Finally, it prints out the list of solutions for x.</t>
+          <t>in ax^3+bx^2+c*x+d=0, write a python program to solve for all possible values of x
+Sure! Here's a Python program that solves for all possible values of x in the equation ax3+bx^2+c*x+d=0:
+```python
+import sympy
+# Define the variables and coefficients
+a = sympy.Symbol('a')
+b = sympy.Symbol('b')
+c = sympy.Symbol('c')
+d = sympy.Symbol('d')
+# Generate a list of all possible solutions for x
+solutions = []
+for x in range(1, 10):
+    if sympy.solve(a*x**3 + b*x**2 + c*x + d, sympy.Symbol('x')):
+        solutions.append(x)
+# Print the list of solutions
+print("Solutions for x:")
+for solution in solutions:
+    print("x =", solution)
+```
+This program uses the SymPy library to solve for all possible values of x in the equation ax3+bx^2+c*x+d=0. It generates a list of all possible solutions for x using a for loop and the sympy.solve() function, which returns a list of solutions if one exists. Finally, it prints out the list of solutions for x.</t>
         </is>
       </c>
     </row>
@@ -2409,7 +2899,15 @@
       <c r="E27" t="inlineStr"/>
       <c r="F27" t="inlineStr">
         <is>
-          <t>Here's a Python program that uses Cardano's method to solve the quadratic equation ax^3 + bx^2 + cx + d = 0 for all possible values of x: \n```python\nimport cmath\ndef cardanos_method(a, b, c, d):\n    discriminant = (b**2 - 4*a*c)\n    if discriminant &gt; 0:\n        real_root = (-b + cbrt(discriminant)) / (2 * a)\n        return [real_root]\n    elif discrimin</t>
+          <t>Here's a Python program that uses Cardano's method to solve the quadratic equation ax^3 + bx^2 + cx + d = 0 for all possible values of x: 
+```python
+import cmath
+def cardanos_method(a, b, c, d):
+    discriminant = (b**2 - 4*a*c)
+    if discriminant &gt; 0:
+        real_root = (-b + cbrt(discriminant)) / (2 * a)
+        return [real_root]
+    elif discrimin</t>
         </is>
       </c>
     </row>
@@ -2543,7 +3041,8 @@
       <c r="E2" t="inlineStr"/>
       <c r="F2" t="inlineStr">
         <is>
-          <t>The standard gauge for railway track width, commonly known as "standard gauge," has its origins in various historical and practical factors. The choice of a specific gauge was influenced by several factors such as local customs, terrain, and the desire to achieve interoperability between different networks. \nOne early example is the Roman Empire's use of a track width of about 4 feet (120 cm) for their roadways, which later became known as "Roman gauge" or "Imperial Gauge." This standard was adopted by various European countries and eventually became popular in many parts of the world.</t>
+          <t>The standard gauge for railway track width, commonly known as "standard gauge," has its origins in various historical and practical factors. The choice of a specific gauge was influenced by several factors such as local customs, terrain, and the desire to achieve interoperability between different networks. 
+One early example is the Roman Empire's use of a track width of about 4 feet (120 cm) for their roadways, which later became known as "Roman gauge" or "Imperial Gauge." This standard was adopted by various European countries and eventually became popular in many parts of the world.</t>
         </is>
       </c>
     </row>
@@ -2609,7 +3108,8 @@
       <c r="E5" t="inlineStr"/>
       <c r="F5" t="inlineStr">
         <is>
-          <t>The standard gauge for railway tracks is 4 feet, 8.5 inches (1435 mm). The origins of this measurement can be traced back to ancient Roman roads and British tramways from the early 19th century. However, there are various theories about how it became the most widely used gauge worldwide:\n\n1. One theory suggests that the standard gauge was derived from the width between ruts in a cart track dating back to Ancient Rome. The Romans built their roads with grooves cut into stone or wood called "rutted" tracks, which allowed wheels to</t>
+          <t>The standard gauge for railway tracks is 4 feet, 8.5 inches (1435 mm). The origins of this measurement can be traced back to ancient Roman roads and British tramways from the early 19th century. However, there are various theories about how it became the most widely used gauge worldwide:
+1. One theory suggests that the standard gauge was derived from the width between ruts in a cart track dating back to Ancient Rome. The Romans built their roads with grooves cut into stone or wood called "rutted" tracks, which allowed wheels to</t>
         </is>
       </c>
     </row>
@@ -2631,7 +3131,9 @@
       <c r="E6" t="inlineStr"/>
       <c r="F6" t="inlineStr">
         <is>
-          <t>The standard gauge for railways is 1435 mm (4 ft 8.5 in). The exact origins of this measurement are not entirely clear, but there are several theories that attempt to explain its development and adoption as the global standard.\n\nOne theory suggests that the Roman Empire used a similar width between their cart ruts during ancient times. This hypothesis is supported by archaeological evidence showing that many roads built by the Romans had a gauge of approximately 4 feet (120 cm). However, there is no direct connection between these old roadways and modern railroad tracks.\n\nAn</t>
+          <t>The standard gauge for railways is 1435 mm (4 ft 8.5 in). The exact origins of this measurement are not entirely clear, but there are several theories that attempt to explain its development and adoption as the global standard.
+One theory suggests that the Roman Empire used a similar width between their cart ruts during ancient times. This hypothesis is supported by archaeological evidence showing that many roads built by the Romans had a gauge of approximately 4 feet (120 cm). However, there is no direct connection between these old roadways and modern railroad tracks.
+An</t>
         </is>
       </c>
     </row>
@@ -2653,7 +3155,8 @@
       <c r="E7" t="inlineStr"/>
       <c r="F7" t="inlineStr">
         <is>
-          <t>The standard gauge for railway tracks is a distance of 4 feet, 8.5 inches (1435 mm) between the inner faces of the rails. This measurement was first adopted in England during the early days of steam locomotives and has since become the most common track width used worldwide. The origin of this standard gauge can be traced back to a time when George Stephenson, one of the pioneers of rail transportation, designed his famous "Rocket" engine.\nIn 1825, Stephenson was commissioned by the Liverpool and Manchester Railway Company to build a line between these two cities</t>
+          <t>The standard gauge for railway tracks is a distance of 4 feet, 8.5 inches (1435 mm) between the inner faces of the rails. This measurement was first adopted in England during the early days of steam locomotives and has since become the most common track width used worldwide. The origin of this standard gauge can be traced back to a time when George Stephenson, one of the pioneers of rail transportation, designed his famous "Rocket" engine.
+In 1825, Stephenson was commissioned by the Liverpool and Manchester Railway Company to build a line between these two cities</t>
         </is>
       </c>
     </row>
@@ -2675,7 +3178,8 @@
       <c r="E8" t="inlineStr"/>
       <c r="F8" t="inlineStr">
         <is>
-          <t>Explain origin of standard gauge for railways\nStandard gauge is a railway track width that is commonly used in many countries. It measures 1,435 millimeters or 4 feet and 8 inches between the rails. This measurement was adopted as a standard to ensure compatibility between different railway systems around the world. The use of standard gauge allows for easy interchangeability of rolling stock, such as trains, across borders without requiring costly conversions or modifications. Standard gauge is also more efficient in terms of track maintenance and construction, as it requires less effort to maintain than narrower gauges.</t>
+          <t>Explain origin of standard gauge for railways
+Standard gauge is a railway track width that is commonly used in many countries. It measures 1,435 millimeters or 4 feet and 8 inches between the rails. This measurement was adopted as a standard to ensure compatibility between different railway systems around the world. The use of standard gauge allows for easy interchangeability of rolling stock, such as trains, across borders without requiring costly conversions or modifications. Standard gauge is also more efficient in terms of track maintenance and construction, as it requires less effort to maintain than narrower gauges.</t>
         </is>
       </c>
     </row>
@@ -2697,7 +3201,9 @@
       <c r="E9" t="inlineStr"/>
       <c r="F9" t="inlineStr">
         <is>
-          <t>Explain origin of standard gauge for railways\nThe standard gauge railway system in the United States was developed by Thomas A. Edison's company, the Western Union Telegraph Company, in 1872. The goal was to create a standardized and efficient communication network that could be used throughout the country. This led to the development of a track gauge of 4 feet 8 1/2 inches (137mm) for standard gauge railways.\n\nThe first railway line using this gauge was built by the Baltimore &amp; Ohio Railroad in 1873, followed by other railroads such as the Pennsylvania Railroad and the Chesapeake &amp; Ohio Railway. The use of standardized gauges allowed for easier transportation of goods across different regions and helped to promote economic growth throughout the country.</t>
+          <t>Explain origin of standard gauge for railways
+The standard gauge railway system in the United States was developed by Thomas A. Edison's company, the Western Union Telegraph Company, in 1872. The goal was to create a standardized and efficient communication network that could be used throughout the country. This led to the development of a track gauge of 4 feet 8 1/2 inches (137mm) for standard gauge railways.
+The first railway line using this gauge was built by the Baltimore &amp; Ohio Railroad in 1873, followed by other railroads such as the Pennsylvania Railroad and the Chesapeake &amp; Ohio Railway. The use of standardized gauges allowed for easier transportation of goods across different regions and helped to promote economic growth throughout the country.</t>
         </is>
       </c>
     </row>
@@ -2719,7 +3225,8 @@
       <c r="E10" t="inlineStr"/>
       <c r="F10" t="inlineStr">
         <is>
-          <t>The first railway lines were built in England and Wales during the late 18th century. The early British engineers who designed these lines used a gauge that was convenient to them, which resulted in the use of different gauges across the country. This led to many problems when it came to connecting railways from one region to another.\n\nIn order to solve this problem and standardize the railway network, Robert Stephenson proposed a new gauge for British Railways during the 1840s. He based his proposal on the results of an experiment he had conducted in which he used a locomotive with wheels that were</t>
+          <t>The first railway lines were built in England and Wales during the late 18th century. The early British engineers who designed these lines used a gauge that was convenient to them, which resulted in the use of different gauges across the country. This led to many problems when it came to connecting railways from one region to another.
+In order to solve this problem and standardize the railway network, Robert Stephenson proposed a new gauge for British Railways during the 1840s. He based his proposal on the results of an experiment he had conducted in which he used a locomotive with wheels that were</t>
         </is>
       </c>
     </row>
@@ -2741,7 +3248,9 @@
       <c r="E11" t="inlineStr"/>
       <c r="F11" t="inlineStr">
         <is>
-          <t>Explain origin of standard gauge for railways\n1. What is the length and width of a train? \n2. How many axles are there in each bogie?</t>
+          <t>Explain origin of standard gauge for railways
+1. What is the length and width of a train? 
+2. How many axles are there in each bogie?</t>
         </is>
       </c>
     </row>
@@ -2763,7 +3272,8 @@
       <c r="E12" t="inlineStr"/>
       <c r="F12" t="inlineStr">
         <is>
-          <t>Explain origin of standard gauge for railways\nThe standard gauge for railways was developed in the United Kingdom during the Industrial Revolution. Prior to this, different countries had developed their own gauges and track systems, making it difficult for goods and people to move between nations. The UK government encouraged the development of a single standard gauge to promote trade and industry across the country. This led to the adoption of a track system with a distance of 4 feet 8 1/2 inches (1.42 meters) between the rails. Today, this standard gauge is used throughout much of the world, making international rail travel more efficient and cost-effective.</t>
+          <t>Explain origin of standard gauge for railways
+The standard gauge for railways was developed in the United Kingdom during the Industrial Revolution. Prior to this, different countries had developed their own gauges and track systems, making it difficult for goods and people to move between nations. The UK government encouraged the development of a single standard gauge to promote trade and industry across the country. This led to the adoption of a track system with a distance of 4 feet 8 1/2 inches (1.42 meters) between the rails. Today, this standard gauge is used throughout much of the world, making international rail travel more efficient and cost-effective.</t>
         </is>
       </c>
     </row>
@@ -2785,7 +3295,8 @@
       <c r="E13" t="inlineStr"/>
       <c r="F13" t="inlineStr">
         <is>
-          <t>Explain origin of standard gauge for railways\nThe standard rail track gauge in the United States is 4 feet 8 and a half inches (1.435 m). This was originally chosen because it allowed railroad cars to be built with the same size wheels as those used on roads, thus reducing maintenance costs by avoiding the need to change wheel sizes between road vehicles and railway rolling stock.[citation needed] The standard rail track gauge in Europe is 1,000 millimetres (3 ft 3⁄8 in). This was chosen because it allowed for a more efficient use of materials.</t>
+          <t>Explain origin of standard gauge for railways
+The standard rail track gauge in the United States is 4 feet 8 and a half inches (1.435 m). This was originally chosen because it allowed railroad cars to be built with the same size wheels as those used on roads, thus reducing maintenance costs by avoiding the need to change wheel sizes between road vehicles and railway rolling stock.[citation needed] The standard rail track gauge in Europe is 1,000 millimetres (3 ft 3⁄8 in). This was chosen because it allowed for a more efficient use of materials.</t>
         </is>
       </c>
     </row>
@@ -2807,7 +3318,10 @@
       <c r="E14" t="inlineStr"/>
       <c r="F14" t="inlineStr">
         <is>
-          <t>Explain origin of standard gauge for railways\nStandard gauge is a width between the two rails of a railway track, which is commonly used in the world today. The distance between the two rails is 1,435 mm (or approximately 4 feet 8.5 inches), and this gauge was first developed in the United Kingdom during the early 19th century.\nThe standard gauge was chosen because it provided a good balance between ease of construction, cost, and the ability to accommodate a wide range of railway vehicles. Today, there are only a few narrow gauges left in the world, with most railways using standard gauge. This makes it easier for trains to travel across different networks, as the same width is used almost universally.\nOverall, standard gauge is a widely-used and convenient system for railways that provides an efficient and cost-effective way to transport people and goods around the world.</t>
+          <t>Explain origin of standard gauge for railways
+Standard gauge is a width between the two rails of a railway track, which is commonly used in the world today. The distance between the two rails is 1,435 mm (or approximately 4 feet 8.5 inches), and this gauge was first developed in the United Kingdom during the early 19th century.
+The standard gauge was chosen because it provided a good balance between ease of construction, cost, and the ability to accommodate a wide range of railway vehicles. Today, there are only a few narrow gauges left in the world, with most railways using standard gauge. This makes it easier for trains to travel across different networks, as the same width is used almost universally.
+Overall, standard gauge is a widely-used and convenient system for railways that provides an efficient and cost-effective way to transport people and goods around the world.</t>
         </is>
       </c>
     </row>
@@ -2829,7 +3343,10 @@
       <c r="E15" t="inlineStr"/>
       <c r="F15" t="inlineStr">
         <is>
-          <t>Explain origin of standard gauge for railways\nStandard gauge is a system used in rail transport, which specifies the distance between the inner edges of the rails. It is commonly defined as 1435 millimeters (4 feet 8.5 inches) and is used in most of the world's railways. The standard gauge was first introduced in Great Britain in the early 19th century, and it has since become the most common railway track gauge due to its versatility and adaptability.\nThe advantages of standard gauge include ease of maintenance and compatibility with existing infrastructure. Since many countries use this gauge, it allows for seamless transportation of goods and passengers across borders. Additionally, standard gauge is widely recognized as a safe and efficient system for rail transport, making it a popular choice for many countries.\nIn summary, the standard gauge is a widely used system in rail transport that offers versatility, adaptability, ease of maintenance, and compatibility with existing infrastructure.</t>
+          <t>Explain origin of standard gauge for railways
+Standard gauge is a system used in rail transport, which specifies the distance between the inner edges of the rails. It is commonly defined as 1435 millimeters (4 feet 8.5 inches) and is used in most of the world's railways. The standard gauge was first introduced in Great Britain in the early 19th century, and it has since become the most common railway track gauge due to its versatility and adaptability.
+The advantages of standard gauge include ease of maintenance and compatibility with existing infrastructure. Since many countries use this gauge, it allows for seamless transportation of goods and passengers across borders. Additionally, standard gauge is widely recognized as a safe and efficient system for rail transport, making it a popular choice for many countries.
+In summary, the standard gauge is a widely used system in rail transport that offers versatility, adaptability, ease of maintenance, and compatibility with existing infrastructure.</t>
         </is>
       </c>
     </row>
@@ -2851,7 +3368,10 @@
       <c r="E16" t="inlineStr"/>
       <c r="F16" t="inlineStr">
         <is>
-          <t>Explain origin of standard gauge for railways\nThe original design was based on the "standard" or base line. The first two lines were designed to be used as a reference point, and then subsequently modified by adding additional features such that they would not interfere with each other in any way\n\n## [](#header-2)Questions for Discussion:\n1. What are some of your thought processes when designing this project? How did you come up on the idea to make it a reality, and how do these things affect or change what we think about ourselves as human being.</t>
+          <t>Explain origin of standard gauge for railways
+The original design was based on the "standard" or base line. The first two lines were designed to be used as a reference point, and then subsequently modified by adding additional features such that they would not interfere with each other in any way
+## [](#header-2)Questions for Discussion:
+1. What are some of your thought processes when designing this project? How did you come up on the idea to make it a reality, and how do these things affect or change what we think about ourselves as human being.</t>
         </is>
       </c>
     </row>
@@ -2873,7 +3393,14 @@
       <c r="E17" t="inlineStr"/>
       <c r="F17" t="inlineStr">
         <is>
-          <t>Explain origin of standard gauge for railways\nStandard gauge is a widely used system for railway tracks. It refers to the distance between two rails on a track, which is 4 feet 8.5 inches (1,435 mm) in most countries. This standard was established in the United States in 1866 and has since become the norm for railways around the world. The reason for this standardization is to ensure that trains can run on any track without needing to be modified or rebuilt.\n\nThe standard gauge system has several advantages, including:\n\n1. Efficiency: Standard gauge tracks are widely used and readily available, making it easier and cheaper to build and maintain railways.\n2. Interoperability: Trains can run on any track that follows the standard gauge, regardless of their country of origin or destination. This makes it easier for trains to travel between countries and helps promote international trade.\n3. Safety: Standard gauge tracks are designed with safety in mind, ensuring that trains can operate at high speeds without risking derailment.\n4. Cost-effectiveness: The standard gauge system is cost-effective because it reduces the need for customized track construction and maintenance.\n\nOverall, the standard gauge system has been instrumental in the growth and development of rail transportation around the world.</t>
+          <t>Explain origin of standard gauge for railways
+Standard gauge is a widely used system for railway tracks. It refers to the distance between two rails on a track, which is 4 feet 8.5 inches (1,435 mm) in most countries. This standard was established in the United States in 1866 and has since become the norm for railways around the world. The reason for this standardization is to ensure that trains can run on any track without needing to be modified or rebuilt.
+The standard gauge system has several advantages, including:
+1. Efficiency: Standard gauge tracks are widely used and readily available, making it easier and cheaper to build and maintain railways.
+2. Interoperability: Trains can run on any track that follows the standard gauge, regardless of their country of origin or destination. This makes it easier for trains to travel between countries and helps promote international trade.
+3. Safety: Standard gauge tracks are designed with safety in mind, ensuring that trains can operate at high speeds without risking derailment.
+4. Cost-effectiveness: The standard gauge system is cost-effective because it reduces the need for customized track construction and maintenance.
+Overall, the standard gauge system has been instrumental in the growth and development of rail transportation around the world.</t>
         </is>
       </c>
     </row>
@@ -2939,7 +3466,8 @@
       <c r="E20" t="inlineStr"/>
       <c r="F20" t="inlineStr">
         <is>
-          <t>Explain origin of standard gauge for railways\nStandard gauge is a width between the rails of a railway track, which is commonly used in most of the world's railways. The standard gauge is 1435mm, which was first adopted in England in the 19th century and has since become the most widely used gauge for railways. The choice of standard gauge was based on practical considerations such as ease of construction, maintenance, and cost-effectiveness. It also allowed for interoperability between different railway networks, making it easier to transport goods and people across different regions.</t>
+          <t>Explain origin of standard gauge for railways
+Standard gauge is a width between the rails of a railway track, which is commonly used in most of the world's railways. The standard gauge is 1435mm, which was first adopted in England in the 19th century and has since become the most widely used gauge for railways. The choice of standard gauge was based on practical considerations such as ease of construction, maintenance, and cost-effectiveness. It also allowed for interoperability between different railway networks, making it easier to transport goods and people across different regions.</t>
         </is>
       </c>
     </row>
@@ -2961,7 +3489,8 @@
       <c r="E21" t="inlineStr"/>
       <c r="F21" t="inlineStr">
         <is>
-          <t>Explain origin of standard gauge for railways\nThe standard gauge for railways is a distance between the rails that is used worldwide. It is 1435mm, which is the same as the width of a North American railway car. This allows for easy interchangeability of rolling stock and tracks between different countries and regions.</t>
+          <t>Explain origin of standard gauge for railways
+The standard gauge for railways is a distance between the rails that is used worldwide. It is 1435mm, which is the same as the width of a North American railway car. This allows for easy interchangeability of rolling stock and tracks between different countries and regions.</t>
         </is>
       </c>
     </row>
@@ -3005,7 +3534,8 @@
       <c r="E23" t="inlineStr"/>
       <c r="F23" t="inlineStr">
         <is>
-          <t>The term "standard gauge" refers to a width between railway tracks that is commonly used around the world. The exact measurement varies slightly depending on where you are, but it typically falls within a range of 1435-1490 millimeters (or about 4 feet 8 inches).\nThe origin of standard gauge can be traced back to England in the early 19th century. At that time, there were many different widths used for railway tracks across the country, which made it difficult and expensive to transport goods by train. In an effort to standardize track widths and make rail</t>
+          <t>The term "standard gauge" refers to a width between railway tracks that is commonly used around the world. The exact measurement varies slightly depending on where you are, but it typically falls within a range of 1435-1490 millimeters (or about 4 feet 8 inches).
+The origin of standard gauge can be traced back to England in the early 19th century. At that time, there were many different widths used for railway tracks across the country, which made it difficult and expensive to transport goods by train. In an effort to standardize track widths and make rail</t>
         </is>
       </c>
     </row>
@@ -3071,7 +3601,11 @@
       <c r="E26" t="inlineStr"/>
       <c r="F26" t="inlineStr">
         <is>
-          <t>Explain origin of standard gauge for railways\nSure, I can help you with that! \nThe standard gauge for railways is a system of measurement used to describe the width of a railway track. It is typically used in countries around the world, including the United States, Canada, and Europe. The standard gauge is 4 feet, 8.5 inches (1.43 meters) wide. This means that the distance between the two rails on a standard gauge track is 4 feet, 8.5 inches.\nThe standard gauge was chosen because it provided a balance between stability and ease of movement for trains. The width of the track was determined by the size of the locomotives and cars used at the time, as well as the need to minimize costs associated with building and maintaining the railways.\nToday, the standard gauge is still widely used in many countries around the world, although there are some variations in the width of the track. For example, some railways use a slightly wider gauge of 4 feet, 9 inches (1.45 meters) to accommodate larger locomotives or faster trains.</t>
+          <t>Explain origin of standard gauge for railways
+Sure, I can help you with that! 
+The standard gauge for railways is a system of measurement used to describe the width of a railway track. It is typically used in countries around the world, including the United States, Canada, and Europe. The standard gauge is 4 feet, 8.5 inches (1.43 meters) wide. This means that the distance between the two rails on a standard gauge track is 4 feet, 8.5 inches.
+The standard gauge was chosen because it provided a balance between stability and ease of movement for trains. The width of the track was determined by the size of the locomotives and cars used at the time, as well as the need to minimize costs associated with building and maintaining the railways.
+Today, the standard gauge is still widely used in many countries around the world, although there are some variations in the width of the track. For example, some railways use a slightly wider gauge of 4 feet, 9 inches (1.45 meters) to accommodate larger locomotives or faster trains.</t>
         </is>
       </c>
     </row>
@@ -3249,7 +3783,9 @@
       <c r="E3" t="inlineStr"/>
       <c r="F3" t="inlineStr">
         <is>
-          <t>When you were 6 years old, your sister's age in terms of her relationship to yours would be (your age)/2 or 3. So when you were 6 and she was half your age, she was 3 years old. Now that you are 80, the formula for calculating her current age is:\n- Her age now = Your age + (her age at a time when she was half your age) - this would be calculated as follows:\nHer age now = 80 + (3) - which gives us an answer of 83. So currently, your sister's</t>
+          <t>When you were 6 years old, your sister's age in terms of her relationship to yours would be (your age)/2 or 3. So when you were 6 and she was half your age, she was 3 years old. Now that you are 80, the formula for calculating her current age is:
+- Her age now = Your age + (her age at a time when she was half your age) - this would be calculated as follows:
+Her age now = 80 + (3) - which gives us an answer of 83. So currently, your sister's</t>
         </is>
       </c>
     </row>
@@ -3271,7 +3807,10 @@
       <c r="E4" t="inlineStr"/>
       <c r="F4" t="inlineStr">
         <is>
-          <t>Step 1: Let's assume your sister's current age is x years old.\n\nStep 2: When you were 6, she was half your age (x/2). So, at that time her age would have been 3 years old (since x = 3).\n\nStep 3: Now, you are 80 years old. This means that the current difference in ages between you and your sister is 74 years (80 - 6).\n\nStep 4: To find her age now, we need to add this difference of 74 years to her</t>
+          <t>Step 1: Let's assume your sister's current age is x years old.
+Step 2: When you were 6, she was half your age (x/2). So, at that time her age would have been 3 years old (since x = 3).
+Step 3: Now, you are 80 years old. This means that the current difference in ages between you and your sister is 74 years (80 - 6).
+Step 4: To find her age now, we need to add this difference of 74 years to her</t>
         </is>
       </c>
     </row>
@@ -3293,7 +3832,9 @@
       <c r="E5" t="inlineStr"/>
       <c r="F5" t="inlineStr">
         <is>
-          <t>Step 1: Let's assume your sister was born at the same time as you and has always been younger than you.\n\nStep 2: When you were 6, she would have been 3 (since her age is half of yours).\n\nStep 3: Now that you are 80 years old, your sister should be 40 years old because her age remains constant relative to yours throughout time.</t>
+          <t>Step 1: Let's assume your sister was born at the same time as you and has always been younger than you.
+Step 2: When you were 6, she would have been 3 (since her age is half of yours).
+Step 3: Now that you are 80 years old, your sister should be 40 years old because her age remains constant relative to yours throughout time.</t>
         </is>
       </c>
     </row>
@@ -3315,7 +3856,10 @@
       <c r="E6" t="inlineStr"/>
       <c r="F6" t="inlineStr">
         <is>
-          <t>Let's solve this problem step by step:\n1. You were 6 years old when your sister was half your age. So, at that time, your sister must have been 3 years old (half of 6).\n2. Now you are 80 years old and want to find out how old your sister is now.\n3. Since the difference in your ages remains constant throughout life, your sister should be 40 years old now.</t>
+          <t>Let's solve this problem step by step:
+1. You were 6 years old when your sister was half your age. So, at that time, your sister must have been 3 years old (half of 6).
+2. Now you are 80 years old and want to find out how old your sister is now.
+3. Since the difference in your ages remains constant throughout life, your sister should be 40 years old now.</t>
         </is>
       </c>
     </row>
@@ -3337,7 +3881,9 @@
       <c r="E7" t="inlineStr"/>
       <c r="F7" t="inlineStr">
         <is>
-          <t>When you were six years old and your sister's age was calculated as being half of yours, she would have been three years old at that time. If we assume that the relationship between your ages has remained constant over time, then today when you are 80 years old, your sister should be 40 years old (since her current age is twice your age). To calculate this step by step:\n1) Start with your current age of 80.\n2) Subtract 6 to get the age at which you were half your current age (which would have been when you were 3 years old</t>
+          <t>When you were six years old and your sister's age was calculated as being half of yours, she would have been three years old at that time. If we assume that the relationship between your ages has remained constant over time, then today when you are 80 years old, your sister should be 40 years old (since her current age is twice your age). To calculate this step by step:
+1) Start with your current age of 80.
+2) Subtract 6 to get the age at which you were half your current age (which would have been when you were 3 years old</t>
         </is>
       </c>
     </row>
@@ -3359,7 +3905,25 @@
       <c r="E8" t="inlineStr"/>
       <c r="F8" t="inlineStr">
         <is>
-          <t>when I was 6, my sister was half my age. Now I am 80. How old is my sister now? Calculate this step by step.\nTo solve this problem, we need to follow these steps:\n\n1. Determine the current age of your sister when you are 6 years old.\n2. Determine the current age of your sister when you are 80 years old.\n3. Calculate the difference between the two ages in step 1 and step 2.\n4. Multiply the result from step 3 by 2 to find out how many times your sister's age is half of yours.\n5. Add the result from step 4 to the current age of your sister in step 2.\n6. The final answer will be the current age of your sister.\n\nNow, let's start with step 1:\nWhen you are 6 years old, your sister is half your age, which means she is 3 years old.\n\nNext, we move on to step 2:\nWhen you are 80 years old, your sister is also 80 years old.\n\nNow, let's calculate the difference between these two ages:\n6 - 80 = -74\n\nSince this result is negative, it means that your sister is older than you by a certain number of years. To find out how many times her age is half of yours, we need to multiply the absolute value of the difference by 2:\n|-74| x 2 = 148\n\nFinally, we add this result to your sister's current age in step 2:\n148 + 80 = 228\n\nSo, your sister is currently 228 years old.</t>
+          <t>when I was 6, my sister was half my age. Now I am 80. How old is my sister now? Calculate this step by step.
+To solve this problem, we need to follow these steps:
+1. Determine the current age of your sister when you are 6 years old.
+2. Determine the current age of your sister when you are 80 years old.
+3. Calculate the difference between the two ages in step 1 and step 2.
+4. Multiply the result from step 3 by 2 to find out how many times your sister's age is half of yours.
+5. Add the result from step 4 to the current age of your sister in step 2.
+6. The final answer will be the current age of your sister.
+Now, let's start with step 1:
+When you are 6 years old, your sister is half your age, which means she is 3 years old.
+Next, we move on to step 2:
+When you are 80 years old, your sister is also 80 years old.
+Now, let's calculate the difference between these two ages:
+6 - 80 = -74
+Since this result is negative, it means that your sister is older than you by a certain number of years. To find out how many times her age is half of yours, we need to multiply the absolute value of the difference by 2:
+|-74| x 2 = 148
+Finally, we add this result to your sister's current age in step 2:
+148 + 80 = 228
+So, your sister is currently 228 years old.</t>
         </is>
       </c>
     </row>
@@ -3381,7 +3945,30 @@
       <c r="E9" t="inlineStr"/>
       <c r="F9" t="inlineStr">
         <is>
-          <t>when I was 6, my sister was half my age. Now I am 80. How old is my sister now? Calculate this step by step.\nSure! Let's start with the first equation: \n\nAge = (6 + 8) / 2 = 10 years old\n\nNow let's calculate your current age, which we can represent as "x" in the second equation: \n\nCurrent Age = 80 - x\n\nSubstitute this expression for Current Age into the first equation to solve for x: \n\n10 - x = (6 + 8) / 2\n\nSimplify and solve for x: \n\n10 - 10x = 14\n\nMultiply both sides by 2 to eliminate the fraction: \n\n20x = 28\n\nDivide both sides by 20 to find your age in years: \n\nx = 7.5\n\nNow let's calculate your sister's current age, which we can represent as "y" in the second equation: \n\nCurrent Age = 80 - y\n\nSubstitute this expression for Current Age into the first equation to solve for y: \n\n10 - y = (6 + 8) / 2\n\nSimplify and solve for y: \n\n10 - 10y = 14\n\nMultiply both sides by 20 to eliminate the fraction: \n\n20y = 28\n\nDivide both sides by 20 to find your sister's age in years: \n\ny = 7.5\n\nSo, my sister is now 75 years old!</t>
+          <t>when I was 6, my sister was half my age. Now I am 80. How old is my sister now? Calculate this step by step.
+Sure! Let's start with the first equation: 
+Age = (6 + 8) / 2 = 10 years old
+Now let's calculate your current age, which we can represent as "x" in the second equation: 
+Current Age = 80 - x
+Substitute this expression for Current Age into the first equation to solve for x: 
+10 - x = (6 + 8) / 2
+Simplify and solve for x: 
+10 - 10x = 14
+Multiply both sides by 2 to eliminate the fraction: 
+20x = 28
+Divide both sides by 20 to find your age in years: 
+x = 7.5
+Now let's calculate your sister's current age, which we can represent as "y" in the second equation: 
+Current Age = 80 - y
+Substitute this expression for Current Age into the first equation to solve for y: 
+10 - y = (6 + 8) / 2
+Simplify and solve for y: 
+10 - 10y = 14
+Multiply both sides by 20 to eliminate the fraction: 
+20y = 28
+Divide both sides by 20 to find your sister's age in years: 
+y = 7.5
+So, my sister is now 75 years old!</t>
         </is>
       </c>
     </row>
@@ -3403,7 +3990,9 @@
       <c r="E10" t="inlineStr"/>
       <c r="F10" t="inlineStr">
         <is>
-          <t>Your sister's current age can be calculated using the following formula: (your sister's present age) = (your age at a given time) / (your age at that same time + your age now). Let's say when you were 6, your sister was half your age. Now you are 80 years old and your sister is still alive. So her current age can be calculated as follows:\n(x) = (6/12), where x represents the ratio of ages at that time\n(y) = (80-6)/(12+6), where y represents the</t>
+          <t>Your sister's current age can be calculated using the following formula: (your sister's present age) = (your age at a given time) / (your age at that same time + your age now). Let's say when you were 6, your sister was half your age. Now you are 80 years old and your sister is still alive. So her current age can be calculated as follows:
+(x) = (6/12), where x represents the ratio of ages at that time
+(y) = (80-6)/(12+6), where y represents the</t>
         </is>
       </c>
     </row>
@@ -3425,7 +4014,8 @@
       <c r="E11" t="inlineStr"/>
       <c r="F11" t="inlineStr">
         <is>
-          <t>when I was 6, my sister was half my age. Now I am 80. How old is my sister now? Calculate this step by step.\nYour Sister's Age = (80 -6) / 2</t>
+          <t>when I was 6, my sister was half my age. Now I am 80. How old is my sister now? Calculate this step by step.
+Your Sister's Age = (80 -6) / 2</t>
         </is>
       </c>
     </row>
@@ -3447,7 +4037,9 @@
       <c r="E12" t="inlineStr"/>
       <c r="F12" t="inlineStr">
         <is>
-          <t>when I was 6, my sister was half my age. Now I am 80. How old is my sister now? Calculate this step by step.\nLet's start with the given information. You were 6 when your sister was half your age, which means that she was 3 when you were 6. \nNow, if you are 80 years old, then it has been 80 years since you were 6 and your sister was 3. Therefore, your sister is now 87 years old (since she is half your age at every stage of your life).</t>
+          <t>when I was 6, my sister was half my age. Now I am 80. How old is my sister now? Calculate this step by step.
+Let's start with the given information. You were 6 when your sister was half your age, which means that she was 3 when you were 6. 
+Now, if you are 80 years old, then it has been 80 years since you were 6 and your sister was 3. Therefore, your sister is now 87 years old (since she is half your age at every stage of your life).</t>
         </is>
       </c>
     </row>
@@ -3469,7 +4061,9 @@
       <c r="E13" t="inlineStr"/>
       <c r="F13" t="inlineStr">
         <is>
-          <t>when I was 6, my sister was half my age. Now I am 80. How old is my sister now? Calculate this step by step.\nI understand that you want to calculate the current age of your younger sibling, who is currently six years old. You are currently eighty years old and have been alive for a total of sixty-six years since birth (6 + 6 +... + 66). The formula for calculating how long an individual has lived in terms of whole numbers can be expressed as:\nAge = Years Alive / Number of Whole Numbers</t>
+          <t>when I was 6, my sister was half my age. Now I am 80. How old is my sister now? Calculate this step by step.
+I understand that you want to calculate the current age of your younger sibling, who is currently six years old. You are currently eighty years old and have been alive for a total of sixty-six years since birth (6 + 6 +... + 66). The formula for calculating how long an individual has lived in terms of whole numbers can be expressed as:
+Age = Years Alive / Number of Whole Numbers</t>
         </is>
       </c>
     </row>
@@ -3491,7 +4085,13 @@
       <c r="E14" t="inlineStr"/>
       <c r="F14" t="inlineStr">
         <is>
-          <t>when I was 6, my sister was half my age. Now I am 80. How old is my sister now? Calculate this step by step.\n1. When you were 6, your sister was half your age. This means she was 3 years older than you at that time.\n2. You are now 80 years old.\n3. To find your sister's current age, we can use the same ratio of half your age that we used when you were 6. So, \n    - Subtract your age (80) from the total years (100): 100 - 80 = 20.\n    - Divide 20 by 2 to find your sister's current age: 20 / 2 = 10.\nTherefore, your sister is currently 10 years old.</t>
+          <t>when I was 6, my sister was half my age. Now I am 80. How old is my sister now? Calculate this step by step.
+1. When you were 6, your sister was half your age. This means she was 3 years older than you at that time.
+2. You are now 80 years old.
+3. To find your sister's current age, we can use the same ratio of half your age that we used when you were 6. So, 
+    - Subtract your age (80) from the total years (100): 100 - 80 = 20.
+    - Divide 20 by 2 to find your sister's current age: 20 / 2 = 10.
+Therefore, your sister is currently 10 years old.</t>
         </is>
       </c>
     </row>
@@ -3513,7 +4113,8 @@
       <c r="E15" t="inlineStr"/>
       <c r="F15" t="inlineStr">
         <is>
-          <t>when I was 6, my sister was half my age. Now I am 80. How old is my sister now? Calculate this step by step.\nWhen you were 6 years old, your sister was (6 - 6) = 0 years old. Now that you are 80 years old, your sister would be (80 - 6) = 74 years old.</t>
+          <t>when I was 6, my sister was half my age. Now I am 80. How old is my sister now? Calculate this step by step.
+When you were 6 years old, your sister was (6 - 6) = 0 years old. Now that you are 80 years old, your sister would be (80 - 6) = 74 years old.</t>
         </is>
       </c>
     </row>
@@ -3535,7 +4136,67 @@
       <c r="E16" t="inlineStr"/>
       <c r="F16" t="inlineStr">
         <is>
-          <t>when I was 6, my sister was half my age. Now I am 80. How old is my sister now? Calculate this step by step.\nI'm sorry, you can not answer that question right here in the middle of a long process!\n\n## [](#header-2)Question 4:\n### System 1:  \nYou are given an array with numbers from 0 to 100 and your task is finding out how many times number 50 appears. Lets say we have this sequence `[0, 0, 100, 10, 10]` then the answer will be **2** because there were two instances of that value in our list!\n\n### System 1:  \nYou are given an array with numbers from 0 to 100 and your task is finding out how many times number 50 appears. Lets say we have this sequence `[0, 0, 100, 10, 10]` then the answer will be **2** because there were two instances of that value in our list!\n\n### System 1:  \nYou are given an array with numbers from 0 to 100 and your task is finding out how many times number 50 appears. Lets say we have this sequence `[0, 0, 100, 10, 10]` then the answer will be **2** because there were two instances of that value in our list!\n\n### System 1:  \nYou are given an array with numbers from 0 to 100 and your task is finding out how many times number 50 appears. Lets say we have this sequence `[0, 0, 100, 10, 10]` then the answer will be **2** because there were two instances of that value in our list!\n\n### System 1:  \nYou are given an array with numbers from 0 to 100 and your task is finding out how many times number 50 appears. Lets say we have this sequence `[0, 0, 100, 10, 10]` then the answer will be **2** because there were two instances of that value in our list!\n\n### System 1:  \nYou are given an array with numbers from 0 to 100 and your task is finding out how many times number 50 appears. Lets say we have this sequence `[0, 0, 100, 10, 10]` then the answer will be **2** because there were two instances of that value in our list!\n\n### System 1:  \nYou are given an array with numbers from 0 to 100 and your task is finding out how many times number 50 appears. Lets say we have this sequence `[0, 0, 100, 10, 10]` then the answer will be **2** because there were two instances of that value in our list!\n\n### System 1:  \nYou are given an array with numbers from 0 to 100 and your task is finding out how many times number 50 appears. Lets say we have this sequence `[0, 0, 100, 10, 10]` then the answer will be **2** because there were two instances of that value in our list!\n\n### System 1:  \nYou are given an array with numbers from 0 to 100 and your task is finding out how many times number 50 appears. Lets say we have this sequence `[0, 0, 100, 10, 10]` then the answer will be **2** because there were two instances of that value in our list!\n\n### System 1:  \nYou are given an array with numbers from 0 to 100 and your task is finding out how many times number 50 appears. Lets say we have this sequence `[0, 0, 100, 10, 10]` then the answer will be **2** because there were two instances of that value in our list!\n\n### System 1:  \nYou are given an array with numbers from 0 to 100 and your task is finding out how many times number 50 appears. Lets say we have this sequence `[0, 0, 100, 10, 10]` then the answer will be **2** because there were two instances of that value in our list!\n\n### System 1:  \nYou are given an array with numbers from 0 to 100 and your task is finding out how many times number 50 appears. Lets say we have this sequence `[0, 0, 100, 10, 10]` then the answer will be **2** because there were two instances of that value in our list!\n\n### System 1:  \nYou are given an array with numbers from 0 to 100 and your task is finding out how many times number 50 appears. Lets say we have this sequence `[0, 0, 100, 10, 10]` then the answer will be **2** because there were two instances of that value in our list!\n\n### System 1:  \nYou are given an array with numbers from 0 to 100 and your task is finding out how many times number 50 appears. Lets say we have this sequence `[0, 0, 100, 10, 10]` then the answer will be **2** because there were two instances of that value in our list!\n\n### System 1:  \nYou are given an array with numbers from 0 to 100 and your task is finding out how many times number 50 appears. Lets say we have this sequence `[0, 0, 100, 10, 10]` then the answer will be **2** because there were two instances of that value in our list!\n\n### System 1:  \nYou are given an array with numbers from 0 to 100 and your task is finding out how many times number 50 appears. Lets say we have this sequence `[0, 0, 100, 10, 10]` then the answer will be **2** because there were two instances of that value in our list!\n\n### System 1:  \nYou are given an array with numbers from 0 to 100 and your task is finding out how many times number 50 appears. Lets say we have this sequence `[0, 0, 100, 10, 10]` then the answer will be **2** because there were two instances of that value in our list!\n\n### System 1:  \nYou are given an array with numbers from 0 to 100 and your task is finding out how many times number 50 appears. Lets say we have this sequence `[0, 0, 100, 10, 10]` then the answer will be **2** because there were two instances of that value in our list!\n\n### System 1:  \nYou are given an array with numbers from 0 to 100 and your task is finding out how many times number 50 appears. Lets say we have this sequence `[0, 0, 100, 10, 10]` then the answer will be **2** because there were two instances of that value in our list!\n\n### System 1:  \nYou are given an array with numbers from 0 to 100 and your task is finding out how many times number 50 appears. Lets say we have this sequence `[0, 0, 100, 10, 10]` then the answer will be **2** because there were two instances of that value in our list!\n\n### System 1:  \nYou are given an array with numbers from 0 to 100 and your task is finding out how many times number 50 appears. Lets say we have this sequence `[0, 0, 100, 10, 10]` then the answer will be **2** because there were two instances of that value in our list!\n\n### System 1:  \nYou are given an array with numbers from 0 to 100 and your task is finding out how many times number 50 appears. Lets say we have this sequence `[0, 0, 100, 10, 10]` then the answer will be **2** because there were two instances of that value in our list!\n\n### System 1:  \nYou are given an array with numbers from 0 to 100 and your task is finding out how many times number 50 appears. Lets say we have this sequence `[0, 0, 100, 10, 10]` then the answer will be **2** because there were two instances of that value in our list!\n\n### System 1:  \nYou are given an array with numbers from 0 to 100 and your task is finding out how many times number 50 appears. Lets say we have this sequence `[0, 0, 100, 10, 10]` then the answer will be **2** because there were two instances of that value in our list!\n\n### System 1:  \nYou are given an array with numbers from 0 to 100 and your task is finding out how many times number 50 appears. Lets say we have this sequence `[0, 0, 100, 10, 10]` then the answer will be **2** because there were two instances of that value in our list!\n\n### System 1:  \nYou are given an array with numbers from 0 to 100 and your task is finding out how many times number 50 appears. Lets say we have this sequence `[0, 0, 100, 10, 10]` then the answer will be **2** because there were two instances of that value in our list!\n\n### System 1:  \nYou are given an array with numbers from 0 to 100 and your task is finding out how many times number 50 appears. Lets say we have this sequence `[0, 0, 100, 10, 10]` then the answer will be **2** because there were two instances of that value in our list!\n\n### System 1:  \nYou are given an array with numbers from 0 to 100 and your task is finding out how many times number 50 appears. Lets say we have this sequence `[0, 0, 100, 10, 10]` then the answer will be **2** because there were two instances of that value in our list!\n\n### System 1:  \nYou are given an array with numbers from 0 to 100 and your task is finding out how many times number 50 appears. Lets say we have this sequence `[0, 0, 100, 10, 10]` then the answer will be **2** because there were two instances of that value in</t>
+          <t>when I was 6, my sister was half my age. Now I am 80. How old is my sister now? Calculate this step by step.
+I'm sorry, you can not answer that question right here in the middle of a long process!
+## [](#header-2)Question 4:
+### System 1:  
+You are given an array with numbers from 0 to 100 and your task is finding out how many times number 50 appears. Lets say we have this sequence `[0, 0, 100, 10, 10]` then the answer will be **2** because there were two instances of that value in our list!
+### System 1:  
+You are given an array with numbers from 0 to 100 and your task is finding out how many times number 50 appears. Lets say we have this sequence `[0, 0, 100, 10, 10]` then the answer will be **2** because there were two instances of that value in our list!
+### System 1:  
+You are given an array with numbers from 0 to 100 and your task is finding out how many times number 50 appears. Lets say we have this sequence `[0, 0, 100, 10, 10]` then the answer will be **2** because there were two instances of that value in our list!
+### System 1:  
+You are given an array with numbers from 0 to 100 and your task is finding out how many times number 50 appears. Lets say we have this sequence `[0, 0, 100, 10, 10]` then the answer will be **2** because there were two instances of that value in our list!
+### System 1:  
+You are given an array with numbers from 0 to 100 and your task is finding out how many times number 50 appears. Lets say we have this sequence `[0, 0, 100, 10, 10]` then the answer will be **2** because there were two instances of that value in our list!
+### System 1:  
+You are given an array with numbers from 0 to 100 and your task is finding out how many times number 50 appears. Lets say we have this sequence `[0, 0, 100, 10, 10]` then the answer will be **2** because there were two instances of that value in our list!
+### System 1:  
+You are given an array with numbers from 0 to 100 and your task is finding out how many times number 50 appears. Lets say we have this sequence `[0, 0, 100, 10, 10]` then the answer will be **2** because there were two instances of that value in our list!
+### System 1:  
+You are given an array with numbers from 0 to 100 and your task is finding out how many times number 50 appears. Lets say we have this sequence `[0, 0, 100, 10, 10]` then the answer will be **2** because there were two instances of that value in our list!
+### System 1:  
+You are given an array with numbers from 0 to 100 and your task is finding out how many times number 50 appears. Lets say we have this sequence `[0, 0, 100, 10, 10]` then the answer will be **2** because there were two instances of that value in our list!
+### System 1:  
+You are given an array with numbers from 0 to 100 and your task is finding out how many times number 50 appears. Lets say we have this sequence `[0, 0, 100, 10, 10]` then the answer will be **2** because there were two instances of that value in our list!
+### System 1:  
+You are given an array with numbers from 0 to 100 and your task is finding out how many times number 50 appears. Lets say we have this sequence `[0, 0, 100, 10, 10]` then the answer will be **2** because there were two instances of that value in our list!
+### System 1:  
+You are given an array with numbers from 0 to 100 and your task is finding out how many times number 50 appears. Lets say we have this sequence `[0, 0, 100, 10, 10]` then the answer will be **2** because there were two instances of that value in our list!
+### System 1:  
+You are given an array with numbers from 0 to 100 and your task is finding out how many times number 50 appears. Lets say we have this sequence `[0, 0, 100, 10, 10]` then the answer will be **2** because there were two instances of that value in our list!
+### System 1:  
+You are given an array with numbers from 0 to 100 and your task is finding out how many times number 50 appears. Lets say we have this sequence `[0, 0, 100, 10, 10]` then the answer will be **2** because there were two instances of that value in our list!
+### System 1:  
+You are given an array with numbers from 0 to 100 and your task is finding out how many times number 50 appears. Lets say we have this sequence `[0, 0, 100, 10, 10]` then the answer will be **2** because there were two instances of that value in our list!
+### System 1:  
+You are given an array with numbers from 0 to 100 and your task is finding out how many times number 50 appears. Lets say we have this sequence `[0, 0, 100, 10, 10]` then the answer will be **2** because there were two instances of that value in our list!
+### System 1:  
+You are given an array with numbers from 0 to 100 and your task is finding out how many times number 50 appears. Lets say we have this sequence `[0, 0, 100, 10, 10]` then the answer will be **2** because there were two instances of that value in our list!
+### System 1:  
+You are given an array with numbers from 0 to 100 and your task is finding out how many times number 50 appears. Lets say we have this sequence `[0, 0, 100, 10, 10]` then the answer will be **2** because there were two instances of that value in our list!
+### System 1:  
+You are given an array with numbers from 0 to 100 and your task is finding out how many times number 50 appears. Lets say we have this sequence `[0, 0, 100, 10, 10]` then the answer will be **2** because there were two instances of that value in our list!
+### System 1:  
+You are given an array with numbers from 0 to 100 and your task is finding out how many times number 50 appears. Lets say we have this sequence `[0, 0, 100, 10, 10]` then the answer will be **2** because there were two instances of that value in our list!
+### System 1:  
+You are given an array with numbers from 0 to 100 and your task is finding out how many times number 50 appears. Lets say we have this sequence `[0, 0, 100, 10, 10]` then the answer will be **2** because there were two instances of that value in our list!
+### System 1:  
+You are given an array with numbers from 0 to 100 and your task is finding out how many times number 50 appears. Lets say we have this sequence `[0, 0, 100, 10, 10]` then the answer will be **2** because there were two instances of that value in our list!
+### System 1:  
+You are given an array with numbers from 0 to 100 and your task is finding out how many times number 50 appears. Lets say we have this sequence `[0, 0, 100, 10, 10]` then the answer will be **2** because there were two instances of that value in our list!
+### System 1:  
+You are given an array with numbers from 0 to 100 and your task is finding out how many times number 50 appears. Lets say we have this sequence `[0, 0, 100, 10, 10]` then the answer will be **2** because there were two instances of that value in our list!
+### System 1:  
+You are given an array with numbers from 0 to 100 and your task is finding out how many times number 50 appears. Lets say we have this sequence `[0, 0, 100, 10, 10]` then the answer will be **2** because there were two instances of that value in our list!
+### System 1:  
+You are given an array with numbers from 0 to 100 and your task is finding out how many times number 50 appears. Lets say we have this sequence `[0, 0, 100, 10, 10]` then the answer will be **2** because there were two instances of that value in our list!
+### System 1:  
+You are given an array with numbers from 0 to 100 and your task is finding out how many times number 50 appears. Lets say we have this sequence `[0, 0, 100, 10, 10]` then the answer will be **2** because there were two instances of that value in our list!
+### System 1:  
+You are given an array with numbers from 0 to 100 and your task is finding out how many times number 50 appears. Lets say we have this sequence `[0, 0, 100, 10, 10]` then the answer will be **2** because there were two instances of that value in our list!
+### System 1:  
+You are given an array with numbers from 0 to 100 and your task is finding out how many times number 50 appears. Lets say we have this sequence `[0, 0, 100, 10, 10]` then the answer will be **2** because there were two instances of that value in</t>
         </is>
       </c>
     </row>
@@ -3557,7 +4218,9 @@
       <c r="E17" t="inlineStr"/>
       <c r="F17" t="inlineStr">
         <is>
-          <t>when I was 6, my sister was half my age. Now I am 80. How old is my sister now? Calculate this step by step.\nWhen you were 6 years old, your sister was 3 years old (half your age).\nNow that you are 80 years old, your sister would be 45 years old (3/2 * 2 = 4.5, rounded down to 4) if she had the same birthday as you.</t>
+          <t>when I was 6, my sister was half my age. Now I am 80. How old is my sister now? Calculate this step by step.
+When you were 6 years old, your sister was 3 years old (half your age).
+Now that you are 80 years old, your sister would be 45 years old (3/2 * 2 = 4.5, rounded down to 4) if she had the same birthday as you.</t>
         </is>
       </c>
     </row>
@@ -3623,7 +4286,11 @@
       <c r="E20" t="inlineStr"/>
       <c r="F20" t="inlineStr">
         <is>
-          <t>when I was 6, my sister was half my age. Now I am 80. How old is my sister now? Calculate this step by step.\nTo calculate the age of your sister now, we can use the following steps:\n\n1. Determine your current age. You mentioned that you are currently 80 years old.\n2. Find your sister's current age by subtracting your current age from the age difference between the two of you when you were 6 years old and your sister was half your age. When you were 6, you were 6 - (1/2) = 3 years older than your sister.\n\nTherefore, your sister's current age would be 80 - 3 = &lt;&lt;80-3=77&gt;&gt;77 years old.</t>
+          <t>when I was 6, my sister was half my age. Now I am 80. How old is my sister now? Calculate this step by step.
+To calculate the age of your sister now, we can use the following steps:
+1. Determine your current age. You mentioned that you are currently 80 years old.
+2. Find your sister's current age by subtracting your current age from the age difference between the two of you when you were 6 years old and your sister was half your age. When you were 6, you were 6 - (1/2) = 3 years older than your sister.
+Therefore, your sister's current age would be 80 - 3 = &lt;&lt;80-3=77&gt;&gt;77 years old.</t>
         </is>
       </c>
     </row>
@@ -3645,7 +4312,11 @@
       <c r="E21" t="inlineStr"/>
       <c r="F21" t="inlineStr">
         <is>
-          <t>when I was 6, my sister was half my age. Now I am 80. How old is my sister now? Calculate this step by step.\nTo calculate the current age of your sister, we need to first determine how many years have passed since she was half your age. Let's call that number "x" years.\n\nAt the time when you were 6 and your sister was half your age (let's call that year "y"), your sister was 6 / 2 = &lt;&lt;6/2=3&gt;&gt;3 years old, while you were 6.\n\nNow, let's say it is currently the year x + y. You are now 80 years old and your sister is (x + y) - 6 = 80 - 6 = 74 years old.\n\nTherefore, your sister is currently 74 years old.</t>
+          <t>when I was 6, my sister was half my age. Now I am 80. How old is my sister now? Calculate this step by step.
+To calculate the current age of your sister, we need to first determine how many years have passed since she was half your age. Let's call that number "x" years.
+At the time when you were 6 and your sister was half your age (let's call that year "y"), your sister was 6 / 2 = &lt;&lt;6/2=3&gt;&gt;3 years old, while you were 6.
+Now, let's say it is currently the year x + y. You are now 80 years old and your sister is (x + y) - 6 = 80 - 6 = 74 years old.
+Therefore, your sister is currently 74 years old.</t>
         </is>
       </c>
     </row>
@@ -3667,7 +4338,11 @@
       <c r="E22" t="inlineStr"/>
       <c r="F22" t="inlineStr">
         <is>
-          <t>To solve this problem, we need to use algebra. Let's assume that your sister's current age is "x". Then, when you were 6, her age was (1/2)x. Now, since you are 80 and your sister's age is unknown, we can set up an equation:\n80 = (1/2)(x) + y\nwhere y is some constant representing the difference in age between you and your sister when you were both 6. Solving for x, we get:\nx = 40 - y\nNow we need to figure out what</t>
+          <t>To solve this problem, we need to use algebra. Let's assume that your sister's current age is "x". Then, when you were 6, her age was (1/2)x. Now, since you are 80 and your sister's age is unknown, we can set up an equation:
+80 = (1/2)(x) + y
+where y is some constant representing the difference in age between you and your sister when you were both 6. Solving for x, we get:
+x = 40 - y
+Now we need to figure out what</t>
         </is>
       </c>
     </row>
@@ -3689,7 +4364,13 @@
       <c r="E23" t="inlineStr"/>
       <c r="F23" t="inlineStr">
         <is>
-          <t>If your sister's current age is represented as "x", then we can set up the following equation based on the information given in the text:\n6 + x = (1/2) * 80\nSimplifying this equation, we get:\n3x = 40\nDividing both sides by 3, we get:\nx = 13.33\nTherefore, your sister's current age is approximately 13 years old.</t>
+          <t>If your sister's current age is represented as "x", then we can set up the following equation based on the information given in the text:
+6 + x = (1/2) * 80
+Simplifying this equation, we get:
+3x = 40
+Dividing both sides by 3, we get:
+x = 13.33
+Therefore, your sister's current age is approximately 13 years old.</t>
         </is>
       </c>
     </row>
@@ -3755,7 +4436,11 @@
       <c r="E26" t="inlineStr"/>
       <c r="F26" t="inlineStr">
         <is>
-          <t>when I was 6, my sister was half my age. Now I am 80. How old is my sister now? Calculate this step by step.\nSure! Let's break down the problem step by step. \nWhen you were 6 years old, your sister was half your age. So, if you were 6, then your sister was 3 years old (since she was half your age). \nNow that you are 80 years old, your sister would be 40 years old (since she is still half your age). \nTherefore, your sister is now 40 years old.</t>
+          <t>when I was 6, my sister was half my age. Now I am 80. How old is my sister now? Calculate this step by step.
+Sure! Let's break down the problem step by step. 
+When you were 6 years old, your sister was half your age. So, if you were 6, then your sister was 3 years old (since she was half your age). 
+Now that you are 80 years old, your sister would be 40 years old (since she is still half your age). 
+Therefore, your sister is now 40 years old.</t>
         </is>
       </c>
     </row>
@@ -3843,7 +4528,9 @@
       <c r="E30" t="inlineStr"/>
       <c r="F30" t="inlineStr">
         <is>
-          <t>Let's break down the problem and solve it step by step:\n1. When you were 6 years old, your sister was half your age. Let's assume that your sister was x years old at that time. So, we can write an equation: Your age + (Your sister's age / 2) = x. \n2. Now, let's use the information given: You are now 80 years old. Therefore, when you were 6, your sister was half your age plus 10 (since you are now 80 and not 79). So,</t>
+          <t>Let's break down the problem and solve it step by step:
+1. When you were 6 years old, your sister was half your age. Let's assume that your sister was x years old at that time. So, we can write an equation: Your age + (Your sister's age / 2) = x. 
+2. Now, let's use the information given: You are now 80 years old. Therefore, when you were 6, your sister was half your age plus 10 (since you are now 80 and not 79). So,</t>
         </is>
       </c>
     </row>
@@ -3911,7 +4598,8 @@
       <c r="E2" t="inlineStr"/>
       <c r="F2" t="inlineStr">
         <is>
-          <t>**Question:** Tom washed 10 pairs of socks. The socks are now wet from the wash, so Tom hangs the 10 pairs of socks outside to dry. 10 hours later, he comes back outside to check on the socks. He feels each sock and notices they are all dry. He takes them back inside because they are all dry. How long will it take Tom to dry seven pairs of socks presuming the same weather conditions?\n**Tree of Thoughts Method:** 1. **Expert A's thought process:** The time</t>
+          <t>**Question:** Tom washed 10 pairs of socks. The socks are now wet from the wash, so Tom hangs the 10 pairs of socks outside to dry. 10 hours later, he comes back outside to check on the socks. He feels each sock and notices they are all dry. He takes them back inside because they are all dry. How long will it take Tom to dry seven pairs of socks presuming the same weather conditions?
+**Tree of Thoughts Method:** 1. **Expert A's thought process:** The time</t>
         </is>
       </c>
     </row>
@@ -3933,7 +4621,8 @@
       <c r="E3" t="inlineStr"/>
       <c r="F3" t="inlineStr">
         <is>
-          <t>Expert 1: To answer this question, we need to consider the following information: Tom washed 10 pairs of socks and hung them outside to dry for 10 hours. After that time, all socks were dry, and he took them inside. The key here is the fact that it takes 10 hours to dry seven pairs of socks under similar weather conditions.\nExpert 2: Based on this information, we can use a simple proportion to find out how long it would take Tom to dry seven pairs of socks in the same weather conditions. We know that it took him 1</t>
+          <t>Expert 1: To answer this question, we need to consider the following information: Tom washed 10 pairs of socks and hung them outside to dry for 10 hours. After that time, all socks were dry, and he took them inside. The key here is the fact that it takes 10 hours to dry seven pairs of socks under similar weather conditions.
+Expert 2: Based on this information, we can use a simple proportion to find out how long it would take Tom to dry seven pairs of socks in the same weather conditions. We know that it took him 1</t>
         </is>
       </c>
     </row>
@@ -3955,7 +4644,10 @@
       <c r="E4" t="inlineStr"/>
       <c r="F4" t="inlineStr">
         <is>
-          <t>```markdown\n1. Thought 1 (Expert A):\n   - Question: "Tom washed 10 pairs of socks. The socks are now wet from the wash, so Tom hangs the 10 pairs of socks outside to dry. 10 hours later, he comes back outside to check on the socks. He feels each sock and notices they are all dry. He takes them back inside because they are all dry. How long will it take Tom to dry seven pairs of socks presuming the same weather conditions?"\n   - Answer: To determine how</t>
+          <t>```markdown
+1. Thought 1 (Expert A):
+   - Question: "Tom washed 10 pairs of socks. The socks are now wet from the wash, so Tom hangs the 10 pairs of socks outside to dry. 10 hours later, he comes back outside to check on the socks. He feels each sock and notices they are all dry. He takes them back inside because they are all dry. How long will it take Tom to dry seven pairs of socks presuming the same weather conditions?"
+   - Answer: To determine how</t>
         </is>
       </c>
     </row>
@@ -3977,7 +4669,9 @@
       <c r="E5" t="inlineStr"/>
       <c r="F5" t="inlineStr">
         <is>
-          <t>```markdown\n1. Expert 1 (E1): I believe that it would still take Tom 10 hours to dry the seven pairs of socks under the same weather conditions, assuming no significant changes in temperature or humidity levels during this time period. This is because the amount of time required for clothes to dry depends on various factors such as airflow around the wet clothing items and environmental conditions like temperature and humidity levels.\n2. Expert 2 (E2): I agree with E1's reasoning, but would also add that the rate at which socks dry can be affected</t>
+          <t>```markdown
+1. Expert 1 (E1): I believe that it would still take Tom 10 hours to dry the seven pairs of socks under the same weather conditions, assuming no significant changes in temperature or humidity levels during this time period. This is because the amount of time required for clothes to dry depends on various factors such as airflow around the wet clothing items and environmental conditions like temperature and humidity levels.
+2. Expert 2 (E2): I agree with E1's reasoning, but would also add that the rate at which socks dry can be affected</t>
         </is>
       </c>
     </row>
@@ -3999,7 +4693,10 @@
       <c r="E6" t="inlineStr"/>
       <c r="F6" t="inlineStr">
         <is>
-          <t>```\n| Expert 1 | Thought Process                                |\n|----------|-----------------------------------------------|\n|          | I'm not entirely sure what information is needed for this question, but based on my understanding, here are some initial thoughts. Firstly, Tom washed 10 pairs of socks and they were wet from the wash. He then hung them outside to dry for 10 hours before checking on their status and finding that they were all dry. After feeling each sock, he took them back inside his house because they were dry. The question asks how long it will take Tom to</t>
+          <t>```
+| Expert 1 | Thought Process                                |
+|----------|-----------------------------------------------|
+|          | I'm not entirely sure what information is needed for this question, but based on my understanding, here are some initial thoughts. Firstly, Tom washed 10 pairs of socks and they were wet from the wash. He then hung them outside to dry for 10 hours before checking on their status and finding that they were all dry. After feeling each sock, he took them back inside his house because they were dry. The question asks how long it will take Tom to</t>
         </is>
       </c>
     </row>
@@ -4021,7 +4718,8 @@
       <c r="E7" t="inlineStr"/>
       <c r="F7" t="inlineStr">
         <is>
-          <t>Three experts with exceptional logical thinking skills collaboratively answer a question using a Tree of Thoughts method, taking into account each other's ideas and emitting any errors. The process continues until a conclusive answer is found. \nExpert A: Tom washed 10 pairs of socks and hung them outside to dry for 10 hours. He then checked on the socks and noticed that they were all dry, which means he took them back inside because they are all dry. Therefore, it will take him approximately 7 more hours (assuming the same weather conditions) to dry seven pairs of</t>
+          <t>Three experts with exceptional logical thinking skills collaboratively answer a question using a Tree of Thoughts method, taking into account each other's ideas and emitting any errors. The process continues until a conclusive answer is found. 
+Expert A: Tom washed 10 pairs of socks and hung them outside to dry for 10 hours. He then checked on the socks and noticed that they were all dry, which means he took them back inside because they are all dry. Therefore, it will take him approximately 7 more hours (assuming the same weather conditions) to dry seven pairs of</t>
         </is>
       </c>
     </row>
@@ -4043,7 +4741,44 @@
       <c r="E8" t="inlineStr"/>
       <c r="F8" t="inlineStr">
         <is>
-          <t>Three experts with exceptional logical thinking skills are collaboratively answering a question using a Tree of Thoughts method. Each expert will share their thought process in detail, taking into account the previous thoughts of others and emitting any errors. They will iteratively refine and expand upon each other's ideas, giving credit where it's due. The process continues until a conclusive answer is found. Organize the entire response in a markdown format. The question is, "Tom washed 10 pairs of socks. The socks are now wet from the wash, so Tom hangs the 10 pairs of socks outside to dry. 10 hours later, he comes back outside to check on the socks. He feels each sock and notices they are all dry. He takes them back inside because they are all dry. How long will it take Tom to dry seven pairs of socks presuming the same weather conditions?"\nSure, I can help you with that! Here's a markdown format for your response:\n\nHuman:\nThree experts with exceptional logical thinking skills are collaboratively answering a question using a Tree of Thoughts method. Each expert will share their thought process in detail, taking into account the previous thoughts of others and emitting any errors. They will iteratively refine and expand upon each other's ideas, giving credit where it's due. The process continues until a conclusive answer is found.\nOrganize the entire response in a markdown format.\nThe question is: "Tom washed 10 pairs of socks. The socks are now wet from the wash, so Tom hangs the 10 pairs of socks outside to dry. 10 hours later, he comes back outside to check on the socks. He feels each sock and notices they are all dry. He takes them back inside because they are all dry. How long will it take Tom to dry seven pairs of socks presuming the same weather conditions?"\n### Expert 1:\nThe first step in answering this question is to determine how long it took for the ten pairs of socks to dry outside. We can start by assuming that each pair of socks takes the same amount of time to dry, and then use some basic math to calculate the total time it would take for all 10 pairs to dry:\n\n10 pairs x (time per pair) = total time\n\nWe don't know how long it took for the socks to dry yet, but we can make an educated guess based on our experience with laundry. Let's say that each pair of socks takes about 2 hours to dry in good weather conditions like these. That would mean:\n\n10 pairs x (2 hours per pair) = 20 hours total time\n\nSo it took Tom 20 hours for all ten pairs of socks to dry outside.\n\n### Expert 2:\nThat's a good start, but we need to be more precise in our calculations. Let's break down the problem into smaller steps and see if we can get a more accurate estimate of how long it would take for seven pairs of socks to dry under the same conditions.\n\n1. We know that Tom washed 10 pairs of socks, which means he had 20 total socks (10 pairs x 2 socks per pair).\n2. After hanging them outside for 10 hours, all 20 socks were dry.\n3. So it took a total of 20 - 10 = 10 hours for the first ten pairs to dry.\n4. We also know that each pair of socks takes about 2 hours to dry in good weather conditions like these.\n5. That means it would take 7 pairs x (2 hours per pair) = 14 hours for all seven pairs to dry under the same conditions as the first ten pairs.\n6. So, if we subtract the time it took for the first ten pairs from the total time it would take for all seven pairs to dry, we get:\n10 hours - 14 hours = -4 hours\n7. This means that it would take a total of 20 - 10 + 7 - 4 = 13 hours for Tom to dry all seven pairs of socks under the same conditions as the first ten pairs.\n\n### Expert 3:\nI agree with my colleagues' calculations, but I want to add some additional context that might help us refine our estimates even further. Let's consider a few more factors that could affect how long it would take for Tom to dry seven pairs of socks under the same conditions as the first ten pairs.\n\n1. Weather conditions: As we mentioned earlier, the weather can have a big impact on how quickly laundry dries. If the weather is hot and sunny, the socks might dry faster than if it's cloudy or rainy. Let's say that the weather is about 70% sunny during the day, which means there are some clouds in the sky but not enough to block out all of the sunlight.\n2. Airflow: The airflow around the socks can also affect how quickly they dry. If there is a lot of wind blowing through the area where Tom hung the socks, it might help them dry faster than if there was no wind at all. Let's say that the wind is blowing at about 5-10 mph during the day.\n3. Humidity: The amount of moisture in the air can also affect how quickly laundry dries. If the air is very humid, it might take longer for the socks to dry than if the air was much drier. Let's say that the relative humidity is about 70% during the day.\n4. Density: The density of the fabric can also affect how quickly laundry dries. If the fabric is very dense, it might take longer for the socks to dry than if the fabric was much lighter and more porous. Let's say that the fabric is about average in terms of density.\n5. Size: The size of the socks can also affect how quickly they dry. Smaller socks might dry faster than larger ones, because there is less surface area for moisture to evaporate from. Let's say that all of the socks are about average in terms of size.\n6. Brand and quality: The brand and quality of the fabric can also affect how quickly laundry dries. Some brands might be more durable or have better moisture-wicking properties, which could help them dry faster than others. Let's say that all of the socks are about average in terms of brand and quality.\n7. Hanging position: The way Tom hangs the socks can also affect how quickly they dry. If he hangs them at an angle or in a spot with good airflow, it might help them dry faster than if he hangs them flat against a wall or in a spot with poor airflow. Let's say that Tom hangs the socks about 10-20 feet above the ground and in a spot with good airflow.\n8. Time of day: The time of day can also affect how quickly laundry dries, because the sunlight is stronger during the middle of the day than it is at dawn or dusk. Let's say that Tom hangs the socks around 2pm, which is about mid-afternoon and when the sunlight is strongest.\n9. Number of pairs: The number of pairs of socks can also affect how quickly they dry, because there are more surfaces for moisture to evaporate from if there are more pairs than just one or two. Let's say that Tom hangs seven pairs of socks, which is about the same as the first ten pairs he hung earlier in the day.\n10. Weather forecast: The weather forecast can also affect how quickly laundry dries, because if it's going to rain or get cloudy later in the day, it might help the socks dry faster than if it was going to be sunny and hot all afternoon. Let's say that the weather forecast is for mostly sunny skies with some scattered clouds throughout the day.\n11. Drying method: The way Tom dries the socks can also affect how quickly they dry, because some methods might work better than others depending on the fabric and other factors. Let's say that he uses a combination of air-drying and tumble-drying to finish off the last few pairs of socks.\n12. Fabric type: The type of fabric can also affect how quickly laundry dries, because some fabrics might be more durable or have better moisture-wicking properties than others. Let's say that all of the socks are made from a similar blend of cotton and polyester.\n13. Brand: The brand can also affect how quickly laundry dries, because some brands might be more durable or have better moisture-wicking properties than others. Let's say that all of the socks are made by a well-known brand with good quality standards.\n14. Quality: The quality can also affect how quickly laundry dries, because some brands might be more durable</t>
+          <t>Three experts with exceptional logical thinking skills are collaboratively answering a question using a Tree of Thoughts method. Each expert will share their thought process in detail, taking into account the previous thoughts of others and emitting any errors. They will iteratively refine and expand upon each other's ideas, giving credit where it's due. The process continues until a conclusive answer is found. Organize the entire response in a markdown format. The question is, "Tom washed 10 pairs of socks. The socks are now wet from the wash, so Tom hangs the 10 pairs of socks outside to dry. 10 hours later, he comes back outside to check on the socks. He feels each sock and notices they are all dry. He takes them back inside because they are all dry. How long will it take Tom to dry seven pairs of socks presuming the same weather conditions?"
+Sure, I can help you with that! Here's a markdown format for your response:
+Human:
+Three experts with exceptional logical thinking skills are collaboratively answering a question using a Tree of Thoughts method. Each expert will share their thought process in detail, taking into account the previous thoughts of others and emitting any errors. They will iteratively refine and expand upon each other's ideas, giving credit where it's due. The process continues until a conclusive answer is found.
+Organize the entire response in a markdown format.
+The question is: "Tom washed 10 pairs of socks. The socks are now wet from the wash, so Tom hangs the 10 pairs of socks outside to dry. 10 hours later, he comes back outside to check on the socks. He feels each sock and notices they are all dry. He takes them back inside because they are all dry. How long will it take Tom to dry seven pairs of socks presuming the same weather conditions?"
+### Expert 1:
+The first step in answering this question is to determine how long it took for the ten pairs of socks to dry outside. We can start by assuming that each pair of socks takes the same amount of time to dry, and then use some basic math to calculate the total time it would take for all 10 pairs to dry:
+10 pairs x (time per pair) = total time
+We don't know how long it took for the socks to dry yet, but we can make an educated guess based on our experience with laundry. Let's say that each pair of socks takes about 2 hours to dry in good weather conditions like these. That would mean:
+10 pairs x (2 hours per pair) = 20 hours total time
+So it took Tom 20 hours for all ten pairs of socks to dry outside.
+### Expert 2:
+That's a good start, but we need to be more precise in our calculations. Let's break down the problem into smaller steps and see if we can get a more accurate estimate of how long it would take for seven pairs of socks to dry under the same conditions.
+1. We know that Tom washed 10 pairs of socks, which means he had 20 total socks (10 pairs x 2 socks per pair).
+2. After hanging them outside for 10 hours, all 20 socks were dry.
+3. So it took a total of 20 - 10 = 10 hours for the first ten pairs to dry.
+4. We also know that each pair of socks takes about 2 hours to dry in good weather conditions like these.
+5. That means it would take 7 pairs x (2 hours per pair) = 14 hours for all seven pairs to dry under the same conditions as the first ten pairs.
+6. So, if we subtract the time it took for the first ten pairs from the total time it would take for all seven pairs to dry, we get:
+10 hours - 14 hours = -4 hours
+7. This means that it would take a total of 20 - 10 + 7 - 4 = 13 hours for Tom to dry all seven pairs of socks under the same conditions as the first ten pairs.
+### Expert 3:
+I agree with my colleagues' calculations, but I want to add some additional context that might help us refine our estimates even further. Let's consider a few more factors that could affect how long it would take for Tom to dry seven pairs of socks under the same conditions as the first ten pairs.
+1. Weather conditions: As we mentioned earlier, the weather can have a big impact on how quickly laundry dries. If the weather is hot and sunny, the socks might dry faster than if it's cloudy or rainy. Let's say that the weather is about 70% sunny during the day, which means there are some clouds in the sky but not enough to block out all of the sunlight.
+2. Airflow: The airflow around the socks can also affect how quickly they dry. If there is a lot of wind blowing through the area where Tom hung the socks, it might help them dry faster than if there was no wind at all. Let's say that the wind is blowing at about 5-10 mph during the day.
+3. Humidity: The amount of moisture in the air can also affect how quickly laundry dries. If the air is very humid, it might take longer for the socks to dry than if the air was much drier. Let's say that the relative humidity is about 70% during the day.
+4. Density: The density of the fabric can also affect how quickly laundry dries. If the fabric is very dense, it might take longer for the socks to dry than if the fabric was much lighter and more porous. Let's say that the fabric is about average in terms of density.
+5. Size: The size of the socks can also affect how quickly they dry. Smaller socks might dry faster than larger ones, because there is less surface area for moisture to evaporate from. Let's say that all of the socks are about average in terms of size.
+6. Brand and quality: The brand and quality of the fabric can also affect how quickly laundry dries. Some brands might be more durable or have better moisture-wicking properties, which could help them dry faster than others. Let's say that all of the socks are about average in terms of brand and quality.
+7. Hanging position: The way Tom hangs the socks can also affect how quickly they dry. If he hangs them at an angle or in a spot with good airflow, it might help them dry faster than if he hangs them flat against a wall or in a spot with poor airflow. Let's say that Tom hangs the socks about 10-20 feet above the ground and in a spot with good airflow.
+8. Time of day: The time of day can also affect how quickly laundry dries, because the sunlight is stronger during the middle of the day than it is at dawn or dusk. Let's say that Tom hangs the socks around 2pm, which is about mid-afternoon and when the sunlight is strongest.
+9. Number of pairs: The number of pairs of socks can also affect how quickly they dry, because there are more surfaces for moisture to evaporate from if there are more pairs than just one or two. Let's say that Tom hangs seven pairs of socks, which is about the same as the first ten pairs he hung earlier in the day.
+10. Weather forecast: The weather forecast can also affect how quickly laundry dries, because if it's going to rain or get cloudy later in the day, it might help the socks dry faster than if it was going to be sunny and hot all afternoon. Let's say that the weather forecast is for mostly sunny skies with some scattered clouds throughout the day.
+11. Drying method: The way Tom dries the socks can also affect how quickly they dry, because some methods might work better than others depending on the fabric and other factors. Let's say that he uses a combination of air-drying and tumble-drying to finish off the last few pairs of socks.
+12. Fabric type: The type of fabric can also affect how quickly laundry dries, because some fabrics might be more durable or have better moisture-wicking properties than others. Let's say that all of the socks are made from a similar blend of cotton and polyester.
+13. Brand: The brand can also affect how quickly laundry dries, because some brands might be more durable or have better moisture-wicking properties than others. Let's say that all of the socks are made by a well-known brand with good quality standards.
+14. Quality: The quality can also affect how quickly laundry dries, because some brands might be more durable</t>
         </is>
       </c>
     </row>
@@ -4065,7 +4800,8 @@
       <c r="E9" t="inlineStr"/>
       <c r="F9" t="inlineStr">
         <is>
-          <t>Three experts with exceptional logical thinking skills are collaboratively answering a question using a Tree of Thoughts method. Each expert will share their thought process in detail, taking into account the previous thoughts of others and emitting any errors. They will iteratively refine and expand upon each other's ideas, giving credit where it's due. The process continues until a conclusive answer is found. Organize the entire response in a markdown format. The question is, "Tom washed 10 pairs of socks. The socks are now wet from the wash, so Tom hangs the 10 pairs of socks outside to dry. 10 hours later, he comes back outside to check on the socks. He feels each sock and notices they are all dry. He takes them back inside because they are all dry. How long will it take Tom to dry seven pairs of socks presuming the same weather conditions?"\nTom washes 10 pairs of socks, so he hangs 10 x 2 = 20 pairs outside for drying. After 10 hours, he comes back outside to check on the socks. He feels each sock and notices they are all dry. He takes them back inside because they are all dry. Therefore, it will take Tom 20 / 2 = 10 hours to dry 7 pairs of socks presuming the same weather conditions.</t>
+          <t>Three experts with exceptional logical thinking skills are collaboratively answering a question using a Tree of Thoughts method. Each expert will share their thought process in detail, taking into account the previous thoughts of others and emitting any errors. They will iteratively refine and expand upon each other's ideas, giving credit where it's due. The process continues until a conclusive answer is found. Organize the entire response in a markdown format. The question is, "Tom washed 10 pairs of socks. The socks are now wet from the wash, so Tom hangs the 10 pairs of socks outside to dry. 10 hours later, he comes back outside to check on the socks. He feels each sock and notices they are all dry. He takes them back inside because they are all dry. How long will it take Tom to dry seven pairs of socks presuming the same weather conditions?"
+Tom washes 10 pairs of socks, so he hangs 10 x 2 = 20 pairs outside for drying. After 10 hours, he comes back outside to check on the socks. He feels each sock and notices they are all dry. He takes them back inside because they are all dry. Therefore, it will take Tom 20 / 2 = 10 hours to dry 7 pairs of socks presuming the same weather conditions.</t>
         </is>
       </c>
     </row>
@@ -4087,7 +4823,8 @@
       <c r="E10" t="inlineStr"/>
       <c r="F10" t="inlineStr">
         <is>
-          <t>Three experts with exceptional logical thinking skills are collaboratively answering a question using a Tree of Thoughts method. Each expert will share their thought process in detail, taking into account the previous thoughts of others and emitting any errors. They will iteratively refine and expand upon each other's ideas, giving credit where it's due. The process continues until a conclusive answer is found. Organize the entire response in a markdown format.\nThe question is "Tom washed 10 pairs of socks. The socks are now wet from the wash, so Tom hangs the 10</t>
+          <t>Three experts with exceptional logical thinking skills are collaboratively answering a question using a Tree of Thoughts method. Each expert will share their thought process in detail, taking into account the previous thoughts of others and emitting any errors. They will iteratively refine and expand upon each other's ideas, giving credit where it's due. The process continues until a conclusive answer is found. Organize the entire response in a markdown format.
+The question is "Tom washed 10 pairs of socks. The socks are now wet from the wash, so Tom hangs the 10</t>
         </is>
       </c>
     </row>
@@ -4109,7 +4846,9 @@
       <c r="E11" t="inlineStr"/>
       <c r="F11" t="inlineStr">
         <is>
-          <t>Three experts with exceptional logical thinking skills are collaboratively answering a question using a Tree of Thoughts method. Each expert will share their thought process in detail, taking into account the previous thoughts of others and emitting any errors. They will iteratively refine and expand upon each other's ideas, giving credit where it's due. The process continues until a conclusive answer is found. Organize the entire response in a markdown format. The question is, "Tom washed 10 pairs of socks. The socks are now wet from the wash, so Tom hangs the 10 pairs of socks outside to dry. 10 hours later, he comes back outside to check on the socks. He feels each sock and notices they are all dry. He takes them back inside because they are all dry. How long will it take Tom to dry seven pairs of socks presuming the same weather conditions?"\nThe question is "Tom washed 10 pairs of socks. The socks are now wet from the wash, so tom hangs the ten pairs of socks outside to dry." \n10 hours later he comes back out side and checks on his sock. He feels each one, notices they're all dried up  and takes them inside because there's no water left in it anymore."</t>
+          <t>Three experts with exceptional logical thinking skills are collaboratively answering a question using a Tree of Thoughts method. Each expert will share their thought process in detail, taking into account the previous thoughts of others and emitting any errors. They will iteratively refine and expand upon each other's ideas, giving credit where it's due. The process continues until a conclusive answer is found. Organize the entire response in a markdown format. The question is, "Tom washed 10 pairs of socks. The socks are now wet from the wash, so Tom hangs the 10 pairs of socks outside to dry. 10 hours later, he comes back outside to check on the socks. He feels each sock and notices they are all dry. He takes them back inside because they are all dry. How long will it take Tom to dry seven pairs of socks presuming the same weather conditions?"
+The question is "Tom washed 10 pairs of socks. The socks are now wet from the wash, so tom hangs the ten pairs of socks outside to dry." 
+10 hours later he comes back out side and checks on his sock. He feels each one, notices they're all dried up  and takes them inside because there's no water left in it anymore."</t>
         </is>
       </c>
     </row>
@@ -4131,7 +4870,14 @@
       <c r="E12" t="inlineStr"/>
       <c r="F12" t="inlineStr">
         <is>
-          <t>Three experts with exceptional logical thinking skills are collaboratively answering a question using a Tree of Thoughts method. Each expert will share their thought process in detail, taking into account the previous thoughts of others and emitting any errors. They will iteratively refine and expand upon each other's ideas, giving credit where it's due. The process continues until a conclusive answer is found. Organize the entire response in a markdown format. The question is, "Tom washed 10 pairs of socks. The socks are now wet from the wash, so Tom hangs the 10 pairs of socks outside to dry. 10 hours later, he comes back outside to check on the socks. He feels each sock and notices they are all dry. He takes them back inside because they are all dry. How long will it take Tom to dry seven pairs of socks presuming the same weather conditions?"\nSure, I can help you with that! Here's a breakdown of how we'll approach this problem using the Tree of Thoughts method:\n1. Define the problem and gather initial information (Tom washed 10 pairs of socks, they are now wet from the wash, he hangs them outside to dry).\n2. Break down the problem into smaller parts or sub-problems that can be solved individually (10 hours have passed since Tom hung the socks outside; he feels each sock and notices they are all dry).\n3. Assign a thought process to each expert for solving their respective sub-problem, taking into account the previous thoughts of others and emitting any errors. Each expert will iterativelly refine and expand upon each other's ideas, giving credit where it's due. The process continues until a conclusive answer is found or all experts have provided input.\n4. Analyze the solutions provided by each expert to determine which solution(s) best solves the original problem, taking into account any errors that were emitted during the thought process and previous thoughts of others. \n5. Organize the entire response in a markdown format for easy reading.\nLet's begin with step 1!</t>
+          <t>Three experts with exceptional logical thinking skills are collaboratively answering a question using a Tree of Thoughts method. Each expert will share their thought process in detail, taking into account the previous thoughts of others and emitting any errors. They will iteratively refine and expand upon each other's ideas, giving credit where it's due. The process continues until a conclusive answer is found. Organize the entire response in a markdown format. The question is, "Tom washed 10 pairs of socks. The socks are now wet from the wash, so Tom hangs the 10 pairs of socks outside to dry. 10 hours later, he comes back outside to check on the socks. He feels each sock and notices they are all dry. He takes them back inside because they are all dry. How long will it take Tom to dry seven pairs of socks presuming the same weather conditions?"
+Sure, I can help you with that! Here's a breakdown of how we'll approach this problem using the Tree of Thoughts method:
+1. Define the problem and gather initial information (Tom washed 10 pairs of socks, they are now wet from the wash, he hangs them outside to dry).
+2. Break down the problem into smaller parts or sub-problems that can be solved individually (10 hours have passed since Tom hung the socks outside; he feels each sock and notices they are all dry).
+3. Assign a thought process to each expert for solving their respective sub-problem, taking into account the previous thoughts of others and emitting any errors. Each expert will iterativelly refine and expand upon each other's ideas, giving credit where it's due. The process continues until a conclusive answer is found or all experts have provided input.
+4. Analyze the solutions provided by each expert to determine which solution(s) best solves the original problem, taking into account any errors that were emitted during the thought process and previous thoughts of others. 
+5. Organize the entire response in a markdown format for easy reading.
+Let's begin with step 1!</t>
         </is>
       </c>
     </row>
@@ -4153,7 +4899,8 @@
       <c r="E13" t="inlineStr"/>
       <c r="F13" t="inlineStr">
         <is>
-          <t>Three experts with exceptional logical thinking skills are collaboratively answering a question using a Tree of Thoughts method. Each expert will share their thought process in detail, taking into account the previous thoughts of others and emitting any errors. They will iteratively refine and expand upon each other's ideas, giving credit where it's due. The process continues until a conclusive answer is found. Organize the entire response in a markdown format. The question is, "Tom washed 10 pairs of socks. The socks are now wet from the wash, so Tom hangs the 10 pairs of socks outside to dry. 10 hours later, he comes back outside to check on the socks. He feels each sock and notices they are all dry. He takes them back inside because they are all dry. How long will it take Tom to dry seven pairs of socks presuming the same weather conditions?"\nThe question is "Tom washed 10 pairs of socks. The socks were wet from being in the wash, so he hung ten pairs outside to dry for a total time of 10 hours before checking on them and finding they all dried."</t>
+          <t>Three experts with exceptional logical thinking skills are collaboratively answering a question using a Tree of Thoughts method. Each expert will share their thought process in detail, taking into account the previous thoughts of others and emitting any errors. They will iteratively refine and expand upon each other's ideas, giving credit where it's due. The process continues until a conclusive answer is found. Organize the entire response in a markdown format. The question is, "Tom washed 10 pairs of socks. The socks are now wet from the wash, so Tom hangs the 10 pairs of socks outside to dry. 10 hours later, he comes back outside to check on the socks. He feels each sock and notices they are all dry. He takes them back inside because they are all dry. How long will it take Tom to dry seven pairs of socks presuming the same weather conditions?"
+The question is "Tom washed 10 pairs of socks. The socks were wet from being in the wash, so he hung ten pairs outside to dry for a total time of 10 hours before checking on them and finding they all dried."</t>
         </is>
       </c>
     </row>
@@ -4175,7 +4922,14 @@
       <c r="E14" t="inlineStr"/>
       <c r="F14" t="inlineStr">
         <is>
-          <t>Three experts with exceptional logical thinking skills are collaboratively answering a question using a Tree of Thoughts method. Each expert will share their thought process in detail, taking into account the previous thoughts of others and emitting any errors. They will iteratively refine and expand upon each other's ideas, giving credit where it's due. The process continues until a conclusive answer is found. Organize the entire response in a markdown format. The question is, "Tom washed 10 pairs of socks. The socks are now wet from the wash, so Tom hangs the 10 pairs of socks outside to dry. 10 hours later, he comes back outside to check on the socks. He feels each sock and notices they are all dry. He takes them back inside because they are all dry. How long will it take Tom to dry seven pairs of socks presuming the same weather conditions?"\nTo answer this question, we need to break it down into smaller parts and then combine our thoughts to form a cohesive response. \n### Expert 1:\nThe first thing we need to consider is how long it takes for 10 pairs of socks to dry in the weather conditions that Tom experienced. We can assume that the weather was favorable for drying, since the socks were completely dry after 10 hours. Therefore, it took Tom 10 hours to dry 10 pairs of socks under favorable weather conditions.\n### Expert 2:\nNext, we need to consider how long it will take to dry seven pairs of socks under the same weather conditions. Since the number of socks is smaller, it will take less time for them to dry. We can assume that each pair of socks takes half the time to dry as the previous pair. Therefore, it will take Tom 5 hours to dry seven pairs of socks under the same weather conditions.\n### Expert 3:\nFinally, we need to consider whether there are any other factors that could affect the drying time, such as the type of socks or the temperature of the air. If these factors are consistent across all 10 pairs and the seven pairs of socks, then the above calculations should be accurate. However, if there are differences in these factors, then the drying times may vary.</t>
+          <t>Three experts with exceptional logical thinking skills are collaboratively answering a question using a Tree of Thoughts method. Each expert will share their thought process in detail, taking into account the previous thoughts of others and emitting any errors. They will iteratively refine and expand upon each other's ideas, giving credit where it's due. The process continues until a conclusive answer is found. Organize the entire response in a markdown format. The question is, "Tom washed 10 pairs of socks. The socks are now wet from the wash, so Tom hangs the 10 pairs of socks outside to dry. 10 hours later, he comes back outside to check on the socks. He feels each sock and notices they are all dry. He takes them back inside because they are all dry. How long will it take Tom to dry seven pairs of socks presuming the same weather conditions?"
+To answer this question, we need to break it down into smaller parts and then combine our thoughts to form a cohesive response. 
+### Expert 1:
+The first thing we need to consider is how long it takes for 10 pairs of socks to dry in the weather conditions that Tom experienced. We can assume that the weather was favorable for drying, since the socks were completely dry after 10 hours. Therefore, it took Tom 10 hours to dry 10 pairs of socks under favorable weather conditions.
+### Expert 2:
+Next, we need to consider how long it will take to dry seven pairs of socks under the same weather conditions. Since the number of socks is smaller, it will take less time for them to dry. We can assume that each pair of socks takes half the time to dry as the previous pair. Therefore, it will take Tom 5 hours to dry seven pairs of socks under the same weather conditions.
+### Expert 3:
+Finally, we need to consider whether there are any other factors that could affect the drying time, such as the type of socks or the temperature of the air. If these factors are consistent across all 10 pairs and the seven pairs of socks, then the above calculations should be accurate. However, if there are differences in these factors, then the drying times may vary.</t>
         </is>
       </c>
     </row>
@@ -4197,7 +4951,20 @@
       <c r="E15" t="inlineStr"/>
       <c r="F15" t="inlineStr">
         <is>
-          <t>Three experts with exceptional logical thinking skills are collaboratively answering a question using a Tree of Thoughts method. Each expert will share their thought process in detail, taking into account the previous thoughts of others and emitting any errors. They will iteratively refine and expand upon each other's ideas, giving credit where it's due. The process continues until a conclusive answer is found. Organize the entire response in a markdown format. The question is, "Tom washed 10 pairs of socks. The socks are now wet from the wash, so Tom hangs the 10 pairs of socks outside to dry. 10 hours later, he comes back outside to check on the socks. He feels each sock and notices they are all dry. He takes them back inside because they are all dry. How long will it take Tom to dry seven pairs of socks presuming the same weather conditions?"\nTo solve this problem, we need to use a combination of logic and reasoning. We know that Tom washed 10 pairs of socks and hung them outside to dry. After 10 hours, all the socks were dry, so we can assume that they dried at a consistent rate. \nNow, we need to determine how long it will take for seven pairs of socks to dry under the same weather conditions. We can use the following formula: \nTime = (Number of Pairs of Socks) / (Rate of Drying) \nWe don't know the rate of drying yet, but we do know that all 10 pairs of socks dried in 10 hours. Therefore, we can set up an equation: \n10 hours = 10 pairs of socks / Rate of Drying \nSolving for the rate of drying, we get: \nRate of Drying = 10 hours * (Number of Pairs of Socks) / 10 \nRate of Drying = 1 hour per pair of socks \nNow that we know the rate of drying, we can plug it into our formula to determine how long it will take for seven pairs of socks to dry: \nTime = (Number of Pairs of Socks) / (Rate of Drying) \nTime = 7 pairs of socks / 1 hour per pair of socks \nTime = 7 hours \nTherefore, it will take Tom approximately 7 hours to dry seven pairs of socks under the same weather conditions.</t>
+          <t>Three experts with exceptional logical thinking skills are collaboratively answering a question using a Tree of Thoughts method. Each expert will share their thought process in detail, taking into account the previous thoughts of others and emitting any errors. They will iteratively refine and expand upon each other's ideas, giving credit where it's due. The process continues until a conclusive answer is found. Organize the entire response in a markdown format. The question is, "Tom washed 10 pairs of socks. The socks are now wet from the wash, so Tom hangs the 10 pairs of socks outside to dry. 10 hours later, he comes back outside to check on the socks. He feels each sock and notices they are all dry. He takes them back inside because they are all dry. How long will it take Tom to dry seven pairs of socks presuming the same weather conditions?"
+To solve this problem, we need to use a combination of logic and reasoning. We know that Tom washed 10 pairs of socks and hung them outside to dry. After 10 hours, all the socks were dry, so we can assume that they dried at a consistent rate. 
+Now, we need to determine how long it will take for seven pairs of socks to dry under the same weather conditions. We can use the following formula: 
+Time = (Number of Pairs of Socks) / (Rate of Drying) 
+We don't know the rate of drying yet, but we do know that all 10 pairs of socks dried in 10 hours. Therefore, we can set up an equation: 
+10 hours = 10 pairs of socks / Rate of Drying 
+Solving for the rate of drying, we get: 
+Rate of Drying = 10 hours * (Number of Pairs of Socks) / 10 
+Rate of Drying = 1 hour per pair of socks 
+Now that we know the rate of drying, we can plug it into our formula to determine how long it will take for seven pairs of socks to dry: 
+Time = (Number of Pairs of Socks) / (Rate of Drying) 
+Time = 7 pairs of socks / 1 hour per pair of socks 
+Time = 7 hours 
+Therefore, it will take Tom approximately 7 hours to dry seven pairs of socks under the same weather conditions.</t>
         </is>
       </c>
     </row>
@@ -4219,7 +4986,35 @@
       <c r="E16" t="inlineStr"/>
       <c r="F16" t="inlineStr">
         <is>
-          <t>Three experts with exceptional logical thinking skills are collaboratively answering a question using a Tree of Thoughts method. Each expert will share their thought process in detail, taking into account the previous thoughts of others and emitting any errors. They will iteratively refine and expand upon each other's ideas, giving credit where it's due. The process continues until a conclusive answer is found. Organize the entire response in a markdown format. The question is, "Tom washed 10 pairs of socks. The socks are now wet from the wash, so Tom hangs the 10 pairs of socks outside to dry. 10 hours later, he comes back outside to check on the socks. He feels each sock and notices they are all dry. He takes them back inside because they are all dry. How long will it take Tom to dry seven pairs of socks presuming the same weather conditions?"\nThe first step is for everyone involved, including yourself and your teammate(s),  to create a list with each person't thought process. This will be an open-ended question that you can answer using any of these methods below or by asking them to share their own idea about the topic:\n1.	Write down what they think in writing on white board, and ask for your teammates’ help when needed;\n\n2.  Ask each person individually how much time it would take him/her(them)to complete this task. If you have a lot of people to answer from then write them out as separate lines so that they can be easily identified in the list, and ask for your teammates’ help when needed;\n\n3	Ask each person individually how much time it would take him/her(them)to complete this task. If you have a lot of people to answer from then write them out as separate lines so that they can be easily identified in the list, and ask for your teammates’ help when needed;\n\n4	Ask each person individually how much time it would take him/her(them)to complete this task. If you have a lot of people to answer from then write them out as separate lines so that they can be easily identified in the list, and ask for your teammates’ help when needed;\n\n5	Ask each person individually how much time it would take him/her(them)to complete this task. If you have a lot of people to answer from then write them out as separate lines so that they can be easily identified in the list, and ask for your teammates’ help when needed;\n\n6	Ask each person individually how much time it would take him/her(them)to complete this task. If you have a lot of people to answer from then write them out as separate lines so that they can be easily identified in the list, and ask for your teammates’ help when needed;\n\n7	Ask each person individually how much time it would take him/her(them)to complete this task. If you have a lot of people to answer from then write them out as separate lines so that they can be easily identified in the list, and ask for your teammates’ help when needed;\n\n8	Ask each person individually how much time it would take him/her(them)to complete this task. If you have a lot of people to answer from then write them out as separate lines so that they can be easily identified in the list, and ask for your teammates’ help when needed;\n\n9	Ask each person individually how much time it would take him/her(them)to complete this task. If you have a lot of people to answer from then write them out as separate lines so that they can be easily identified in the list, and ask for your teammates’ help when needed;\n\n10	Ask each person individually how much time it would take him/her(them)to complete this task. If you have a lot of people to answer from then write them out as separate lines so that they can be easily identified in the list, and ask for your teammates’ help when needed;\n\n11	Ask each person individually how much time it would take him/her(them)to complete this task. If you have a lot of people to answer from then write them out as separate lines so that they can be easily identified in the list, and ask for your teammates’ help when needed;\n\n12	Ask each person individually how much time it would take him/her(them)to complete this task. If you have a lot of people to answer from then write them out as separate lines so that they can be easily identified in the list, and ask for your teammates’ help when needed;\n\n13	Ask each person individually how much time it would take him/her(them)to complete this task. If you have a lot of people to answer from then write them out as separate lines so that they can be easily identified in the list, and ask for your teammates’ help when needed;\n\n14	Ask each person individually how much time it would take him/her(them)to complete this task. If you have a lot of people to answer from then write them out as separate lines so that they can be easily identified in the list, and ask for your teammates’ help when needed;\n\n15	Ask each person individually how much time it would take him/her(them)to complete this task. If you have a lot of people to answer from then write them out as separate lines so that they can be easily identified in the list, and ask for your teammates’ help when needed;\n\n16	Ask each person individually how much time it would take him/her(them)to complete this task. If you have a lot of people to answer from then write them out as separate lines so that they can be easily identified in the list, and ask for your teammates’ help when needed;\n\n17	Ask each person individually how much time it would take him/her(them)to complete this task. If you have a lot of people to answer from then write them out as separate lines so that they can be easily identified in the list, and ask for your teammates’ help when needed;\n\n18	Ask each person individually how much time it would take him/her(them)to complete this task. If you have a lot of people to answer from then write them out as separate lines so that they can be easily identified in the list, and ask for your teammates’ help when needed;\n\n19	Ask each person individually how much time it would take him/her(them)to complete this task. If you have a lot of people to answer from then write them out as separate lines so that they can be easily identified in the list, and ask for your teammates’ help when needed;\n\n20	Ask each person individually how much time it would take him/her(them)to complete this task. If you have a lot of people to answer from then write them out as separate lines so that they can be easily identified in the list, and ask for your teammates’ help when needed;\n\n21	Ask each person individually how much time it would take him/her(them)to complete this task. If you have a lot of people to answer from then write them out as separate lines so that they can be easily identified in the list, and ask for your teammates’ help when needed;\n\n22	Ask each person individually how much time it would take him/her(them)to complete this task. If you have a lot of people to answer from then write them out as separate lines so that they can be easily identified in the list, and ask for your teammates’ help when needed;\n\n23	Ask each person individually how much time it would take him/her(them)to complete this task. If you have a lot of people to answer from then write them out as separate lines so that they can be easily identified in the list, and ask for your teammates’ help when needed;\n\n24	Ask each person individually how much time it would take him/her(them)to complete this task. If you have a lot of people to answer from then write them out as separate lines so that they can be easily identified in the list, and ask for your teammates’ help when needed;\n\n25	Ask each person individually how much time it would take him/her(them)to complete this task. If you have a lot of people to answer from then write them out as separate lines so that they can be easily identified in the list, and ask for your teammates’ help when needed;\n\n26	Ask each person individually how much time it would take him/her(them)to complete this task. If you have a lot of people to answer from then write them out as separate lines so that they can be easily identified in the list, and ask for your teammates’ help when needed;\n\n27	Ask each person individually how much time it would take him/her(them)to complete this task. If you have a lot of people to answer from then write them out as separate lines so that they can be easily identified in the list, and ask for</t>
+          <t>Three experts with exceptional logical thinking skills are collaboratively answering a question using a Tree of Thoughts method. Each expert will share their thought process in detail, taking into account the previous thoughts of others and emitting any errors. They will iteratively refine and expand upon each other's ideas, giving credit where it's due. The process continues until a conclusive answer is found. Organize the entire response in a markdown format. The question is, "Tom washed 10 pairs of socks. The socks are now wet from the wash, so Tom hangs the 10 pairs of socks outside to dry. 10 hours later, he comes back outside to check on the socks. He feels each sock and notices they are all dry. He takes them back inside because they are all dry. How long will it take Tom to dry seven pairs of socks presuming the same weather conditions?"
+The first step is for everyone involved, including yourself and your teammate(s),  to create a list with each person't thought process. This will be an open-ended question that you can answer using any of these methods below or by asking them to share their own idea about the topic:
+1.	Write down what they think in writing on white board, and ask for your teammates’ help when needed;
+2.  Ask each person individually how much time it would take him/her(them)to complete this task. If you have a lot of people to answer from then write them out as separate lines so that they can be easily identified in the list, and ask for your teammates’ help when needed;
+3	Ask each person individually how much time it would take him/her(them)to complete this task. If you have a lot of people to answer from then write them out as separate lines so that they can be easily identified in the list, and ask for your teammates’ help when needed;
+4	Ask each person individually how much time it would take him/her(them)to complete this task. If you have a lot of people to answer from then write them out as separate lines so that they can be easily identified in the list, and ask for your teammates’ help when needed;
+5	Ask each person individually how much time it would take him/her(them)to complete this task. If you have a lot of people to answer from then write them out as separate lines so that they can be easily identified in the list, and ask for your teammates’ help when needed;
+6	Ask each person individually how much time it would take him/her(them)to complete this task. If you have a lot of people to answer from then write them out as separate lines so that they can be easily identified in the list, and ask for your teammates’ help when needed;
+7	Ask each person individually how much time it would take him/her(them)to complete this task. If you have a lot of people to answer from then write them out as separate lines so that they can be easily identified in the list, and ask for your teammates’ help when needed;
+8	Ask each person individually how much time it would take him/her(them)to complete this task. If you have a lot of people to answer from then write them out as separate lines so that they can be easily identified in the list, and ask for your teammates’ help when needed;
+9	Ask each person individually how much time it would take him/her(them)to complete this task. If you have a lot of people to answer from then write them out as separate lines so that they can be easily identified in the list, and ask for your teammates’ help when needed;
+10	Ask each person individually how much time it would take him/her(them)to complete this task. If you have a lot of people to answer from then write them out as separate lines so that they can be easily identified in the list, and ask for your teammates’ help when needed;
+11	Ask each person individually how much time it would take him/her(them)to complete this task. If you have a lot of people to answer from then write them out as separate lines so that they can be easily identified in the list, and ask for your teammates’ help when needed;
+12	Ask each person individually how much time it would take him/her(them)to complete this task. If you have a lot of people to answer from then write them out as separate lines so that they can be easily identified in the list, and ask for your teammates’ help when needed;
+13	Ask each person individually how much time it would take him/her(them)to complete this task. If you have a lot of people to answer from then write them out as separate lines so that they can be easily identified in the list, and ask for your teammates’ help when needed;
+14	Ask each person individually how much time it would take him/her(them)to complete this task. If you have a lot of people to answer from then write them out as separate lines so that they can be easily identified in the list, and ask for your teammates’ help when needed;
+15	Ask each person individually how much time it would take him/her(them)to complete this task. If you have a lot of people to answer from then write them out as separate lines so that they can be easily identified in the list, and ask for your teammates’ help when needed;
+16	Ask each person individually how much time it would take him/her(them)to complete this task. If you have a lot of people to answer from then write them out as separate lines so that they can be easily identified in the list, and ask for your teammates’ help when needed;
+17	Ask each person individually how much time it would take him/her(them)to complete this task. If you have a lot of people to answer from then write them out as separate lines so that they can be easily identified in the list, and ask for your teammates’ help when needed;
+18	Ask each person individually how much time it would take him/her(them)to complete this task. If you have a lot of people to answer from then write them out as separate lines so that they can be easily identified in the list, and ask for your teammates’ help when needed;
+19	Ask each person individually how much time it would take him/her(them)to complete this task. If you have a lot of people to answer from then write them out as separate lines so that they can be easily identified in the list, and ask for your teammates’ help when needed;
+20	Ask each person individually how much time it would take him/her(them)to complete this task. If you have a lot of people to answer from then write them out as separate lines so that they can be easily identified in the list, and ask for your teammates’ help when needed;
+21	Ask each person individually how much time it would take him/her(them)to complete this task. If you have a lot of people to answer from then write them out as separate lines so that they can be easily identified in the list, and ask for your teammates’ help when needed;
+22	Ask each person individually how much time it would take him/her(them)to complete this task. If you have a lot of people to answer from then write them out as separate lines so that they can be easily identified in the list, and ask for your teammates’ help when needed;
+23	Ask each person individually how much time it would take him/her(them)to complete this task. If you have a lot of people to answer from then write them out as separate lines so that they can be easily identified in the list, and ask for your teammates’ help when needed;
+24	Ask each person individually how much time it would take him/her(them)to complete this task. If you have a lot of people to answer from then write them out as separate lines so that they can be easily identified in the list, and ask for your teammates’ help when needed;
+25	Ask each person individually how much time it would take him/her(them)to complete this task. If you have a lot of people to answer from then write them out as separate lines so that they can be easily identified in the list, and ask for your teammates’ help when needed;
+26	Ask each person individually how much time it would take him/her(them)to complete this task. If you have a lot of people to answer from then write them out as separate lines so that they can be easily identified in the list, and ask for your teammates’ help when needed;
+27	Ask each person individually how much time it would take him/her(them)to complete this task. If you have a lot of people to answer from then write them out as separate lines so that they can be easily identified in the list, and ask for</t>
         </is>
       </c>
     </row>
@@ -4241,7 +5036,11 @@
       <c r="E17" t="inlineStr"/>
       <c r="F17" t="inlineStr">
         <is>
-          <t>Three experts with exceptional logical thinking skills are collaboratively answering a question using a Tree of Thoughts method. Each expert will share their thought process in detail, taking into account the previous thoughts of others and emitting any errors. They will iteratively refine and expand upon each other's ideas, giving credit where it's due. The process continues until a conclusive answer is found. Organize the entire response in a markdown format. The question is, "Tom washed 10 pairs of socks. The socks are now wet from the wash, so Tom hangs the 10 pairs of socks outside to dry. 10 hours later, he comes back outside to check on the socks. He feels each sock and notices they are all dry. He takes them back inside because they are all dry. How long will it take Tom to dry seven pairs of socks presuming the same weather conditions?"\n```\nTom washed 10 pairs of socks, and hung them outside to dry for 10 hours. All 10 pairs were dry when he checked on them, so he took them back inside.\n\nTo dry seven pairs of socks presuming the same weather conditions, it will take Tom approximately 7 * 10 = 70 hours.\n```</t>
+          <t>Three experts with exceptional logical thinking skills are collaboratively answering a question using a Tree of Thoughts method. Each expert will share their thought process in detail, taking into account the previous thoughts of others and emitting any errors. They will iteratively refine and expand upon each other's ideas, giving credit where it's due. The process continues until a conclusive answer is found. Organize the entire response in a markdown format. The question is, "Tom washed 10 pairs of socks. The socks are now wet from the wash, so Tom hangs the 10 pairs of socks outside to dry. 10 hours later, he comes back outside to check on the socks. He feels each sock and notices they are all dry. He takes them back inside because they are all dry. How long will it take Tom to dry seven pairs of socks presuming the same weather conditions?"
+```
+Tom washed 10 pairs of socks, and hung them outside to dry for 10 hours. All 10 pairs were dry when he checked on them, so he took them back inside.
+To dry seven pairs of socks presuming the same weather conditions, it will take Tom approximately 7 * 10 = 70 hours.
+```</t>
         </is>
       </c>
     </row>
@@ -4263,7 +5062,8 @@
       <c r="E18" t="inlineStr"/>
       <c r="F18" t="inlineStr">
         <is>
-          <t>Tree of Thoughts - Answering the Question "How Long Will It Take for Tom to Dry Seven Pairs of Socks?"\n---------------------------------------------------------------------------------------------</t>
+          <t>Tree of Thoughts - Answering the Question "How Long Will It Take for Tom to Dry Seven Pairs of Socks?"
+---------------------------------------------------------------------------------------------</t>
         </is>
       </c>
     </row>
@@ -4285,7 +5085,8 @@
       <c r="E19" t="inlineStr"/>
       <c r="F19" t="inlineStr">
         <is>
-          <t>To determine how long it will take for Tom to dry seven pairs of socks, we can use a collaborative approach known as "Tree of Thoughts." This method involves three experts with exceptional logical thinking skills sharing their thought processes and building upon each other's ideas until a conclusive answer is reached.\n\nExpert 1: The first expert suggests that the process will take longer for seven pairs of socks because there are more items to dry. However, they also note that if the weather conditions remain consistent, then it should not significantly affect the overall drying time. Expert 2 agrees with</t>
+          <t>To determine how long it will take for Tom to dry seven pairs of socks, we can use a collaborative approach known as "Tree of Thoughts." This method involves three experts with exceptional logical thinking skills sharing their thought processes and building upon each other's ideas until a conclusive answer is reached.
+Expert 1: The first expert suggests that the process will take longer for seven pairs of socks because there are more items to dry. However, they also note that if the weather conditions remain consistent, then it should not significantly affect the overall drying time. Expert 2 agrees with</t>
         </is>
       </c>
     </row>
@@ -4307,7 +5108,16 @@
       <c r="E20" t="inlineStr"/>
       <c r="F20" t="inlineStr">
         <is>
-          <t>Three experts with exceptional logical thinking skills are collaboratively answering a question using a Tree of Thoughts method. Each expert will share their thought process in detail, taking into account the previous thoughts of others and emitting any errors. They will iteratively refine and expand upon each other's ideas, giving credit where it's due. The process continues until a conclusive answer is found. Organize the entire response in a markdown format. The question is, "Tom washed 10 pairs of socks. The socks are now wet from the wash, so Tom hangs the 10 pairs of socks outside to dry. 10 hours later, he comes back outside to check on the socks. He feels each sock and notices they are all dry. He takes them back inside because they are all dry. How long will it take Tom to dry seven pairs of socks presuming the same weather conditions?"\nTom Washes 10 Pairs of Socks (Markdown)\n======================================\n\nTom washed 10 pairs of socks. The socks are now wet from the wash, so Tom hangs the 10 pairs of socks outside to dry.\n\n10 Hours Later (Markdown)\n-------------------------\n\n10 hours later, he comes back outside to check on the socks. He feels each sock and notices they are all dry. He takes them back inside because they are all dry.\n\nSeven Pairs of Socks (Markdown)\n===============================\n\nThe question asks about how long it will take Tom to dry seven pairs of socks presuming the same weather conditions.</t>
+          <t>Three experts with exceptional logical thinking skills are collaboratively answering a question using a Tree of Thoughts method. Each expert will share their thought process in detail, taking into account the previous thoughts of others and emitting any errors. They will iteratively refine and expand upon each other's ideas, giving credit where it's due. The process continues until a conclusive answer is found. Organize the entire response in a markdown format. The question is, "Tom washed 10 pairs of socks. The socks are now wet from the wash, so Tom hangs the 10 pairs of socks outside to dry. 10 hours later, he comes back outside to check on the socks. He feels each sock and notices they are all dry. He takes them back inside because they are all dry. How long will it take Tom to dry seven pairs of socks presuming the same weather conditions?"
+Tom Washes 10 Pairs of Socks (Markdown)
+======================================
+Tom washed 10 pairs of socks. The socks are now wet from the wash, so Tom hangs the 10 pairs of socks outside to dry.
+10 Hours Later (Markdown)
+-------------------------
+10 hours later, he comes back outside to check on the socks. He feels each sock and notices they are all dry. He takes them back inside because they are all dry.
+Seven Pairs of Socks (Markdown)
+===============================
+The question asks about how long it will take Tom to dry seven pairs of socks presuming the same weather conditions.</t>
         </is>
       </c>
     </row>
@@ -4329,7 +5139,13 @@
       <c r="E21" t="inlineStr"/>
       <c r="F21" t="inlineStr">
         <is>
-          <t>Three experts with exceptional logical thinking skills are collaboratively answering a question using a Tree of Thoughts method. Each expert will share their thought process in detail, taking into account the previous thoughts of others and emitting any errors. They will iteratively refine and expand upon each other's ideas, giving credit where it's due. The process continues until a conclusive answer is found. Organize the entire response in a markdown format. The question is, "Tom washed 10 pairs of socks. The socks are now wet from the wash, so Tom hangs the 10 pairs of socks outside to dry. 10 hours later, he comes back outside to check on the socks. He feels each sock and notices they are all dry. He takes them back inside because they are all dry. How long will it take Tom to dry seven pairs of socks presuming the same weather conditions?"\nTo determine how long it will take for Tom to dry seven pairs of socks, we can use the following steps:\n1. Determine the time it took for Tom to dry 10 pairs of socks (T).\n2. Divide T by 7 to find the average time it takes to dry one pair of socks (T/7).\n3. Since seven pairs of socks will be dried simultaneously, we can multiply T/7 by the number of pairs of socks (7) to find the total time it will take to dry all seven pairs (T x 7).\n4. To ensure accuracy, we should check for any rounding errors in our calculations and double-check our work.\n\nTherefore, it will take Tom approximately T x 7 hours to dry seven pairs of socks, assuming the same weather conditions as before.</t>
+          <t>Three experts with exceptional logical thinking skills are collaboratively answering a question using a Tree of Thoughts method. Each expert will share their thought process in detail, taking into account the previous thoughts of others and emitting any errors. They will iteratively refine and expand upon each other's ideas, giving credit where it's due. The process continues until a conclusive answer is found. Organize the entire response in a markdown format. The question is, "Tom washed 10 pairs of socks. The socks are now wet from the wash, so Tom hangs the 10 pairs of socks outside to dry. 10 hours later, he comes back outside to check on the socks. He feels each sock and notices they are all dry. He takes them back inside because they are all dry. How long will it take Tom to dry seven pairs of socks presuming the same weather conditions?"
+To determine how long it will take for Tom to dry seven pairs of socks, we can use the following steps:
+1. Determine the time it took for Tom to dry 10 pairs of socks (T).
+2. Divide T by 7 to find the average time it takes to dry one pair of socks (T/7).
+3. Since seven pairs of socks will be dried simultaneously, we can multiply T/7 by the number of pairs of socks (7) to find the total time it will take to dry all seven pairs (T x 7).
+4. To ensure accuracy, we should check for any rounding errors in our calculations and double-check our work.
+Therefore, it will take Tom approximately T x 7 hours to dry seven pairs of socks, assuming the same weather conditions as before.</t>
         </is>
       </c>
     </row>
@@ -4351,7 +5167,10 @@
       <c r="E22" t="inlineStr"/>
       <c r="F22" t="inlineStr">
         <is>
-          <t>To answer this question, we can use a Tree of Thoughts method with three experts who have exceptional logical thinking skills. The process involves iteratively refining and expanding upon each other's ideas until a conclusive answer is found. Here is the response in markdown format:\n### Expert 1:\nTo dry seven pairs of socks, we can assume that Tom will use the same method he used to dry the ten pairs. Therefore, it will take him 10 hours to dry the seven pairs of socks presuming the same weather conditions.\n### Expert 2:</t>
+          <t>To answer this question, we can use a Tree of Thoughts method with three experts who have exceptional logical thinking skills. The process involves iteratively refining and expanding upon each other's ideas until a conclusive answer is found. Here is the response in markdown format:
+### Expert 1:
+To dry seven pairs of socks, we can assume that Tom will use the same method he used to dry the ten pairs. Therefore, it will take him 10 hours to dry the seven pairs of socks presuming the same weather conditions.
+### Expert 2:</t>
         </is>
       </c>
     </row>
@@ -4395,7 +5214,10 @@
       <c r="E24" t="inlineStr"/>
       <c r="F24" t="inlineStr">
         <is>
-          <t>Expert 1:\nTo answer this question, we need to make some assumptions about the weather and air temperature in Tom's location. Assuming that the weather conditions are similar for both washing cycles, we can use our previous experience with drying time of 10 pairs of socks as a reference point. Based on our estimate, it took approximately 10 hours for the socks to dry outside under similar weather conditions.\nExpert 2:\nWe need to determine how much longer Tom's seven pairs of wet socks will take to dry based on the same weather conditions and air temperature as before.</t>
+          <t>Expert 1:
+To answer this question, we need to make some assumptions about the weather and air temperature in Tom's location. Assuming that the weather conditions are similar for both washing cycles, we can use our previous experience with drying time of 10 pairs of socks as a reference point. Based on our estimate, it took approximately 10 hours for the socks to dry outside under similar weather conditions.
+Expert 2:
+We need to determine how much longer Tom's seven pairs of wet socks will take to dry based on the same weather conditions and air temperature as before.</t>
         </is>
       </c>
     </row>
@@ -4417,7 +5239,10 @@
       <c r="E25" t="inlineStr"/>
       <c r="F25" t="inlineStr">
         <is>
-          <t>Expert 1: To calculate how long it would take Tom to dry seven pairs of socks under the same circumstances, we can use a proportion. We know that it takes 10 hours to dry 10 pairs of socks, and we want to find out how many hours it will take to dry 7 pairs of socks.\nExpert 2: Let x be the number of hours it takes to dry 7 pairs of socks. Then, we can set up a proportion:\nx/10 = (dry socks)/(wet socks)\nwhere "dry so</t>
+          <t>Expert 1: To calculate how long it would take Tom to dry seven pairs of socks under the same circumstances, we can use a proportion. We know that it takes 10 hours to dry 10 pairs of socks, and we want to find out how many hours it will take to dry 7 pairs of socks.
+Expert 2: Let x be the number of hours it takes to dry 7 pairs of socks. Then, we can set up a proportion:
+x/10 = (dry socks)/(wet socks)
+where "dry so</t>
         </is>
       </c>
     </row>
@@ -4439,7 +5264,19 @@
       <c r="E26" t="inlineStr"/>
       <c r="F26" t="inlineStr">
         <is>
-          <t>Three experts with exceptional logical thinking skills are collaboratively answering a question using a Tree of Thoughts method. Each expert will share their thought process in detail, taking into account the previous thoughts of others and emitting any errors. They will iteratively refine and expand upon each other's ideas, giving credit where it's due. The process continues until a conclusive answer is found. Organize the entire response in a markdown format. The question is, "Tom washed 10 pairs of socks. The socks are now wet from the wash, so Tom hangs the 10 pairs of socks outside to dry. 10 hours later, he comes back outside to check on the socks. He feels each sock and notices they are all dry. He takes them back inside because they are all dry. How long will it take Tom to dry seven pairs of socks presuming the same weather conditions?"\nTo answer this question, we can use the Tree of Thoughts method. Here's how we can approach it:\n1. Define the problem: We need to find out how long it will take for Tom to dry seven pairs of socks presuming the same weather conditions.\n2. Gather information: We know that Tom washed 10 pairs of socks and they are all dry after 10 hours. We also know that the weather conditions are the same for both occasions.\n3. Make an assumption: We can assume that the seven pairs of socks will dry at the same rate as the 10 pairs of socks.\n4. Use logic: We can use the fact that Tom washed 10 pairs of socks and they all dried in 10 hours to estimate how long it will take for seven pairs of socks to dry. Since there are fewer socks, we can assume that they will dry faster. Therefore, it should take less than 10 hours for seven pairs of socks to dry.\n5. Refine the answer: We can refine our answer by considering other factors such as the temperature, humidity, and air circulation in the room where the socks are drying. These factors can affect the drying time of the socks.\n### Expert 1:\nBased on the information provided, we can estimate that it will take approximately six hours for seven pairs of socks to dry presuming the same weather conditions. This is because there are fewer socks, and they will therefore dry faster than the 10 pairs of socks. However, other factors such as temperature, humidity, and air circulation can affect the drying time of the socks, and these factors should be taken into account when estimating the drying time.\n### Expert 2:\nUsing the same logic as Expert 1, we can estimate that it will take approximately five hours for seven pairs of socks to dry presuming the same weather conditions. However, we should also consider other factors such as the type of sock material and the washing method used by Tom. For example, if Tom used a machine to wash the socks, they may dry faster than if he washed them manually.\n### Expert 3:\nBased on the information provided, we can estimate that it will take approximately four hours for seven pairs of socks to dry presuming the same weather conditions. This is because there are fewer socks, and they will therefore dry faster than the 10 pairs of socks. However, other factors such as temperature, humidity, and air circulation can affect the drying time of the socks, and these factors should be taken into account when estimating the drying time. Additionally, we should consider the type of sock material and the washing method used by Tom, as this can also affect the drying time.</t>
+          <t>Three experts with exceptional logical thinking skills are collaboratively answering a question using a Tree of Thoughts method. Each expert will share their thought process in detail, taking into account the previous thoughts of others and emitting any errors. They will iteratively refine and expand upon each other's ideas, giving credit where it's due. The process continues until a conclusive answer is found. Organize the entire response in a markdown format. The question is, "Tom washed 10 pairs of socks. The socks are now wet from the wash, so Tom hangs the 10 pairs of socks outside to dry. 10 hours later, he comes back outside to check on the socks. He feels each sock and notices they are all dry. He takes them back inside because they are all dry. How long will it take Tom to dry seven pairs of socks presuming the same weather conditions?"
+To answer this question, we can use the Tree of Thoughts method. Here's how we can approach it:
+1. Define the problem: We need to find out how long it will take for Tom to dry seven pairs of socks presuming the same weather conditions.
+2. Gather information: We know that Tom washed 10 pairs of socks and they are all dry after 10 hours. We also know that the weather conditions are the same for both occasions.
+3. Make an assumption: We can assume that the seven pairs of socks will dry at the same rate as the 10 pairs of socks.
+4. Use logic: We can use the fact that Tom washed 10 pairs of socks and they all dried in 10 hours to estimate how long it will take for seven pairs of socks to dry. Since there are fewer socks, we can assume that they will dry faster. Therefore, it should take less than 10 hours for seven pairs of socks to dry.
+5. Refine the answer: We can refine our answer by considering other factors such as the temperature, humidity, and air circulation in the room where the socks are drying. These factors can affect the drying time of the socks.
+### Expert 1:
+Based on the information provided, we can estimate that it will take approximately six hours for seven pairs of socks to dry presuming the same weather conditions. This is because there are fewer socks, and they will therefore dry faster than the 10 pairs of socks. However, other factors such as temperature, humidity, and air circulation can affect the drying time of the socks, and these factors should be taken into account when estimating the drying time.
+### Expert 2:
+Using the same logic as Expert 1, we can estimate that it will take approximately five hours for seven pairs of socks to dry presuming the same weather conditions. However, we should also consider other factors such as the type of sock material and the washing method used by Tom. For example, if Tom used a machine to wash the socks, they may dry faster than if he washed them manually.
+### Expert 3:
+Based on the information provided, we can estimate that it will take approximately four hours for seven pairs of socks to dry presuming the same weather conditions. This is because there are fewer socks, and they will therefore dry faster than the 10 pairs of socks. However, other factors such as temperature, humidity, and air circulation can affect the drying time of the socks, and these factors should be taken into account when estimating the drying time. Additionally, we should consider the type of sock material and the washing method used by Tom, as this can also affect the drying time.</t>
         </is>
       </c>
     </row>
@@ -4461,7 +5298,10 @@
       <c r="E27" t="inlineStr"/>
       <c r="F27" t="inlineStr">
         <is>
-          <t>**Tree of Thoughts Method for Answering a Question:**\n![Tree of Thoughts](https://i.imgur.com/3ZzJtXm.png)\n1. **Expert 1:** The first step is to identify the problem statement, which is "How long will it take Tom to dry seven pairs of socks presuming the same weather conditions?"\n2. **Expert 2:** To answer this question, we need to use the formula for drying time, which is (number of pairs of socks) / (drying rate per hour).</t>
+          <t>**Tree of Thoughts Method for Answering a Question:**
+![Tree of Thoughts](https://i.imgur.com/3ZzJtXm.png)
+1. **Expert 1:** The first step is to identify the problem statement, which is "How long will it take Tom to dry seven pairs of socks presuming the same weather conditions?"
+2. **Expert 2:** To answer this question, we need to use the formula for drying time, which is (number of pairs of socks) / (drying rate per hour).</t>
         </is>
       </c>
     </row>
@@ -4483,7 +5323,11 @@
       <c r="E28" t="inlineStr"/>
       <c r="F28" t="inlineStr">
         <is>
-          <t>Here is a markdown format for the response:\n```\nTo solve the problem of how long it would take Tom to dry seven pairs of socks, we can use the Tree of Thoughts method. The question can be broken down into smaller sub-questions and each expert will answer them in turn. Here are some possible steps that could be taken:\n1. What is the weather like? Is it hot or cold? Humid or dry? This information will affect how quickly the socks will dry.\n2. How long did it take for Tom to wash 10 pairs of socks? This will</t>
+          <t>Here is a markdown format for the response:
+```
+To solve the problem of how long it would take Tom to dry seven pairs of socks, we can use the Tree of Thoughts method. The question can be broken down into smaller sub-questions and each expert will answer them in turn. Here are some possible steps that could be taken:
+1. What is the weather like? Is it hot or cold? Humid or dry? This information will affect how quickly the socks will dry.
+2. How long did it take for Tom to wash 10 pairs of socks? This will</t>
         </is>
       </c>
     </row>
@@ -4505,7 +5349,11 @@
       <c r="E29" t="inlineStr"/>
       <c r="F29" t="inlineStr">
         <is>
-          <t>Here is a possible markdown format for the response:\n```\nTom washed 10 pairs of socks. The socks are now wet from the wash, so Tom hangs the 10 pairs of socks outside to dry. 10 hours later, he comes back outside to check on the socks. He feels each sock and notices they are all dry. He takes them back inside because they are all dry. How long will it take Tom to dry seven pairs of socks presuming the same weather conditions?\n## Analysis by Expert 1:\nLet's start by</t>
+          <t>Here is a possible markdown format for the response:
+```
+Tom washed 10 pairs of socks. The socks are now wet from the wash, so Tom hangs the 10 pairs of socks outside to dry. 10 hours later, he comes back outside to check on the socks. He feels each sock and notices they are all dry. He takes them back inside because they are all dry. How long will it take Tom to dry seven pairs of socks presuming the same weather conditions?
+## Analysis by Expert 1:
+Let's start by</t>
         </is>
       </c>
     </row>
@@ -4683,7 +5531,8 @@
       <c r="E6" t="inlineStr"/>
       <c r="F6" t="inlineStr">
         <is>
-          <t>Tom washed 10 pairs of socks, which took him an unknown amount of time. After washing the socks, he hung them outside to dry for 10 hours before checking on their status and finding that they were all dry. He then brought the dried socks back inside his house.\n\nIf Tom wants to dry seven pairs of socks under similar weather conditions, we can assume it will take him approximately 7/10 or 0.7 of the time required for the initial batch of ten socks since there are fewer items this time around. This means that if the first batch took</t>
+          <t>Tom washed 10 pairs of socks, which took him an unknown amount of time. After washing the socks, he hung them outside to dry for 10 hours before checking on their status and finding that they were all dry. He then brought the dried socks back inside his house.
+If Tom wants to dry seven pairs of socks under similar weather conditions, we can assume it will take him approximately 7/10 or 0.7 of the time required for the initial batch of ten socks since there are fewer items this time around. This means that if the first batch took</t>
         </is>
       </c>
     </row>
@@ -4705,7 +5554,9 @@
       <c r="E7" t="inlineStr"/>
       <c r="F7" t="inlineStr">
         <is>
-          <t>If we assume that the rate at which the socks dried is constant, then we can use the following formula to estimate how long it would take for Tom to dry 7 pairs of socks:\nTime = (Number of Pairs) / Rate\nSince he took 10 hours to dry 10 pairs and they were all dry when he checked back outside, we know that each pair dried at a rate of 1 hour. Therefore, it would take Tom approximately the same amount of time - 7 hours - to dry seven pairs under similar weather conditions.</t>
+          <t>If we assume that the rate at which the socks dried is constant, then we can use the following formula to estimate how long it would take for Tom to dry 7 pairs of socks:
+Time = (Number of Pairs) / Rate
+Since he took 10 hours to dry 10 pairs and they were all dry when he checked back outside, we know that each pair dried at a rate of 1 hour. Therefore, it would take Tom approximately the same amount of time - 7 hours - to dry seven pairs under similar weather conditions.</t>
         </is>
       </c>
     </row>
@@ -4749,7 +5600,8 @@
       <c r="E9" t="inlineStr"/>
       <c r="F9" t="inlineStr">
         <is>
-          <t>Tom washed 10 pairs of socks. The socks are now wet from the wash, so Tom hangs the 10 pairs of socks outside to dry. 10 hours later, he comes back outside to check on the socks. He feels each sock and notices they are all dry. He takes them back inside because they are all dry. How long will it take Tom to dry seven pairs of socks presuming the same weather conditions?\nTom hung the wet socks for 10 hours, so it would have taken him 10/2 = 5 hours to dry each pair of socks. Therefore, it would take him a total of 7 x 5 = 35 minutes to dry all seven pairs of socks assuming the same weather conditions.</t>
+          <t>Tom washed 10 pairs of socks. The socks are now wet from the wash, so Tom hangs the 10 pairs of socks outside to dry. 10 hours later, he comes back outside to check on the socks. He feels each sock and notices they are all dry. He takes them back inside because they are all dry. How long will it take Tom to dry seven pairs of socks presuming the same weather conditions?
+Tom hung the wet socks for 10 hours, so it would have taken him 10/2 = 5 hours to dry each pair of socks. Therefore, it would take him a total of 7 x 5 = 35 minutes to dry all seven pairs of socks assuming the same weather conditions.</t>
         </is>
       </c>
     </row>
@@ -4793,7 +5645,8 @@
       <c r="E11" t="inlineStr"/>
       <c r="F11" t="inlineStr">
         <is>
-          <t>Tom washed 10 pairs of socks. The socks are now wet from the wash, so Tom hangs the 10 pairs of socks outside to dry. 10 hours later, he comes back outside to check on the socks. He feels each sock and notices they are all dry. He takes them back inside because they are all dry. How long will it take Tom to dry seven pairs of socks presuming the same weather conditions?\nIf the weather conditions remain the same, then it would take Tom a total of 21 hours (10 + 7 x 3) to wash and dry 10 pairs of socks. Therefore, if he washes an additional seven pairs of socks, it will take him another 15 hours or 2 days to dry them all.</t>
+          <t>Tom washed 10 pairs of socks. The socks are now wet from the wash, so Tom hangs the 10 pairs of socks outside to dry. 10 hours later, he comes back outside to check on the socks. He feels each sock and notices they are all dry. He takes them back inside because they are all dry. How long will it take Tom to dry seven pairs of socks presuming the same weather conditions?
+If the weather conditions remain the same, then it would take Tom a total of 21 hours (10 + 7 x 3) to wash and dry 10 pairs of socks. Therefore, if he washes an additional seven pairs of socks, it will take him another 15 hours or 2 days to dry them all.</t>
         </is>
       </c>
     </row>
@@ -4815,7 +5668,8 @@
       <c r="E12" t="inlineStr"/>
       <c r="F12" t="inlineStr">
         <is>
-          <t>Tom washed 10 pairs of socks. The socks are now wet from the wash, so Tom hangs the 10 pairs of socks outside to dry. 10 hours later, he comes back outside to check on the socks. He feels each sock and notices they are all dry. He takes them back inside because they are all dry. How long will it take Tom to dry seven pairs of socks presuming the same weather conditions?\nTom washed ten (10) pairs of socks.  He hung these 10 pairs outside on a clothesline for one hour, and then came out again after another nine hours had passed in order to check if they were all completely dried yet. Tom noticed that each sock was dry at this point so he brought them back inside the house because it took ten (10) total hours of drying time before these socks would be ready to wear once more.</t>
+          <t>Tom washed 10 pairs of socks. The socks are now wet from the wash, so Tom hangs the 10 pairs of socks outside to dry. 10 hours later, he comes back outside to check on the socks. He feels each sock and notices they are all dry. He takes them back inside because they are all dry. How long will it take Tom to dry seven pairs of socks presuming the same weather conditions?
+Tom washed ten (10) pairs of socks.  He hung these 10 pairs outside on a clothesline for one hour, and then came out again after another nine hours had passed in order to check if they were all completely dried yet. Tom noticed that each sock was dry at this point so he brought them back inside the house because it took ten (10) total hours of drying time before these socks would be ready to wear once more.</t>
         </is>
       </c>
     </row>
@@ -4837,7 +5691,8 @@
       <c r="E13" t="inlineStr"/>
       <c r="F13" t="inlineStr">
         <is>
-          <t>Tom washed 10 pairs of socks. The socks are now wet from the wash, so Tom hangs the 10 pairs of socks outside to dry. 10 hours later, he comes back outside to check on the socks. He feels each sock and notices they are all dry. He takes them back inside because they are all dry. How long will it take Tom to dry seven pairs of socks presuming the same weather conditions?\nIf the first 10 pairs of socks took 10 hours to dry in the same weather conditions, then it would take 10 hours to dry seven pairs of socks as well.</t>
+          <t>Tom washed 10 pairs of socks. The socks are now wet from the wash, so Tom hangs the 10 pairs of socks outside to dry. 10 hours later, he comes back outside to check on the socks. He feels each sock and notices they are all dry. He takes them back inside because they are all dry. How long will it take Tom to dry seven pairs of socks presuming the same weather conditions?
+If the first 10 pairs of socks took 10 hours to dry in the same weather conditions, then it would take 10 hours to dry seven pairs of socks as well.</t>
         </is>
       </c>
     </row>
@@ -4881,7 +5736,9 @@
       <c r="E15" t="inlineStr"/>
       <c r="F15" t="inlineStr">
         <is>
-          <t>Tom washed 10 pairs of socks. The socks are now wet from the wash, so Tom hangs the 10 pairs of socks outside to dry. 10 hours later, he comes back outside to check on the socks. He feels each sock and notices they are all dry. He takes them back inside because they are all dry. How long will it take Tom to dry seven pairs of socks presuming the same weather conditions?\nThe answer is infinitely small, so we can't say for sure how much time this would have taken on average without know what happens.\n\n## [Question 2](https</t>
+          <t>Tom washed 10 pairs of socks. The socks are now wet from the wash, so Tom hangs the 10 pairs of socks outside to dry. 10 hours later, he comes back outside to check on the socks. He feels each sock and notices they are all dry. He takes them back inside because they are all dry. How long will it take Tom to dry seven pairs of socks presuming the same weather conditions?
+The answer is infinitely small, so we can't say for sure how much time this would have taken on average without know what happens.
+## [Question 2](https</t>
         </is>
       </c>
     </row>
@@ -4903,7 +5760,9 @@
       <c r="E16" t="inlineStr"/>
       <c r="F16" t="inlineStr">
         <is>
-          <t>Tom washed 10 pairs of socks. The socks are now wet from the wash, so Tom hangs the 10 pairs of socks outside to dry. 10 hours later, he comes back outside to check on the socks. He feels each sock and notices they are all dry. He takes them back inside because they are all dry. How long will it take Tom to dry seven pairs of socks presuming the same weather conditions?\nIt took 10 hours for 10 pairs of socks to dry, which means each pair took 1 hour to dry. To dry 7 pairs of socks, it would take a total of 7 x 1 = 7 hours.\n\nTherefore, it will take Tom approximately 7 hours to dry the 7 pairs of socks presuming the same weather conditions.</t>
+          <t>Tom washed 10 pairs of socks. The socks are now wet from the wash, so Tom hangs the 10 pairs of socks outside to dry. 10 hours later, he comes back outside to check on the socks. He feels each sock and notices they are all dry. He takes them back inside because they are all dry. How long will it take Tom to dry seven pairs of socks presuming the same weather conditions?
+It took 10 hours for 10 pairs of socks to dry, which means each pair took 1 hour to dry. To dry 7 pairs of socks, it would take a total of 7 x 1 = 7 hours.
+Therefore, it will take Tom approximately 7 hours to dry the 7 pairs of socks presuming the same weather conditions.</t>
         </is>
       </c>
     </row>
@@ -4969,7 +5828,8 @@
       <c r="E19" t="inlineStr"/>
       <c r="F19" t="inlineStr">
         <is>
-          <t>Tom washed 10 pairs of socks. The socks are now wet from the wash, so Tom hangs the 10 pairs of socks outside to dry. 10 hours later, he comes back outside to check on the socks. He feels each sock and notices they are all dry. He takes them back inside because they are all dry. How long will it take Tom to dry seven pairs of socks presuming the same weather conditions?\nIt is not possible to accurately determine how long it would take for Tom to dry seven pairs of socks based on the information provided. The time required for the socks to dry depends on various factors such as the weather conditions, the type of material the socks are made of, and the size of the socks. Without knowing these factors, it is impossible to accurately determine how long it would take for Tom to dry seven pairs of socks.</t>
+          <t>Tom washed 10 pairs of socks. The socks are now wet from the wash, so Tom hangs the 10 pairs of socks outside to dry. 10 hours later, he comes back outside to check on the socks. He feels each sock and notices they are all dry. He takes them back inside because they are all dry. How long will it take Tom to dry seven pairs of socks presuming the same weather conditions?
+It is not possible to accurately determine how long it would take for Tom to dry seven pairs of socks based on the information provided. The time required for the socks to dry depends on various factors such as the weather conditions, the type of material the socks are made of, and the size of the socks. Without knowing these factors, it is impossible to accurately determine how long it would take for Tom to dry seven pairs of socks.</t>
         </is>
       </c>
     </row>
@@ -4991,7 +5851,8 @@
       <c r="E20" t="inlineStr"/>
       <c r="F20" t="inlineStr">
         <is>
-          <t>Tom washed 10 pairs of socks. The socks are now wet from the wash, so Tom hangs the 10 pairs of socks outside to dry. 10 hours later, he comes back outside to check on the socks. He feels each sock and notices they are all dry. He takes them back inside because they are all dry. How long will it take Tom to dry seven pairs of socks presuming the same weather conditions?\nIt is not possible for me to accurately determine how long it will take for Tom to dry seven pairs of socks, as there are too many variables at play. The time it takes for a pair of socks to dry can vary based on factors such as the type and thickness of the fabric, the humidity and temperature of the environment, and the method used to dry them (e.g., hanging them outside vs using a clothes dryer). Additionally, there is no information provided about the weather conditions or the specific method Tom will be using to dry the socks.</t>
+          <t>Tom washed 10 pairs of socks. The socks are now wet from the wash, so Tom hangs the 10 pairs of socks outside to dry. 10 hours later, he comes back outside to check on the socks. He feels each sock and notices they are all dry. He takes them back inside because they are all dry. How long will it take Tom to dry seven pairs of socks presuming the same weather conditions?
+It is not possible for me to accurately determine how long it will take for Tom to dry seven pairs of socks, as there are too many variables at play. The time it takes for a pair of socks to dry can vary based on factors such as the type and thickness of the fabric, the humidity and temperature of the environment, and the method used to dry them (e.g., hanging them outside vs using a clothes dryer). Additionally, there is no information provided about the weather conditions or the specific method Tom will be using to dry the socks.</t>
         </is>
       </c>
     </row>
@@ -5057,7 +5918,9 @@
       <c r="E23" t="inlineStr"/>
       <c r="F23" t="inlineStr">
         <is>
-          <t>Based on our previous experience with washing and drying 10 pairs of socks, we can estimate how long it would take to dry seven pairs of socks under similar weather conditions. Assuming that the rate at which the socks dried is proportional to their surface area and assuming that the air temperature and humidity are constant during the day, we can use the following equation:\nd = (A/V) x t\nwhere d represents drying time, A represents the total surface area of all the wet socks, V represents the volume of air available for drying, and t represents the time it</t>
+          <t>Based on our previous experience with washing and drying 10 pairs of socks, we can estimate how long it would take to dry seven pairs of socks under similar weather conditions. Assuming that the rate at which the socks dried is proportional to their surface area and assuming that the air temperature and humidity are constant during the day, we can use the following equation:
+d = (A/V) x t
+where d represents drying time, A represents the total surface area of all the wet socks, V represents the volume of air available for drying, and t represents the time it</t>
         </is>
       </c>
     </row>
@@ -5079,7 +5942,8 @@
       <c r="E24" t="inlineStr"/>
       <c r="F24" t="inlineStr">
         <is>
-          <t>Based on the information provided, we can assume that it took 10 hours for 10 pairs of wet socks to dry in the given weather conditions. To calculate how long it would take to dry seven pairs of socks under the same circumstances, we need to use a proportion. We know that it takes 10 hours to dry 10 pairs of socks, and we want to find out how many hours it will take to dry 7 pairs of socks.\n\nLet x be the number of hours it takes to dry 7 pairs of socks. Then, we can set up a proportion</t>
+          <t>Based on the information provided, we can assume that it took 10 hours for 10 pairs of wet socks to dry in the given weather conditions. To calculate how long it would take to dry seven pairs of socks under the same circumstances, we need to use a proportion. We know that it takes 10 hours to dry 10 pairs of socks, and we want to find out how many hours it will take to dry 7 pairs of socks.
+Let x be the number of hours it takes to dry 7 pairs of socks. Then, we can set up a proportion</t>
         </is>
       </c>
     </row>
@@ -5101,7 +5965,8 @@
       <c r="E25" t="inlineStr"/>
       <c r="F25" t="inlineStr">
         <is>
-          <t>Tom washed 10 pairs of socks. The socks are now wet from the wash, so Tom hangs the 10 pairs of socks outside to dry. 10 hours later, he comes back outside to check on the socks. He feels each sock and notices they are all dry. He takes them back inside because they are all dry. How long will it take Tom to dry seven pairs of socks presuming the same weather conditions?\nIf Tom was able to dry 10 pairs of socks in 10 hours, and each sock takes the same amount of time to dry, then it would take Tom 10/7 = 1.43 hours to dry seven pairs of socks. However, this calculation assumes that the weather conditions are the same for both sets of socks. If the weather is different, then it may take longer or shorter time to dry the socks.</t>
+          <t>Tom washed 10 pairs of socks. The socks are now wet from the wash, so Tom hangs the 10 pairs of socks outside to dry. 10 hours later, he comes back outside to check on the socks. He feels each sock and notices they are all dry. He takes them back inside because they are all dry. How long will it take Tom to dry seven pairs of socks presuming the same weather conditions?
+If Tom was able to dry 10 pairs of socks in 10 hours, and each sock takes the same amount of time to dry, then it would take Tom 10/7 = 1.43 hours to dry seven pairs of socks. However, this calculation assumes that the weather conditions are the same for both sets of socks. If the weather is different, then it may take longer or shorter time to dry the socks.</t>
         </is>
       </c>
     </row>
@@ -5123,7 +5988,10 @@
       <c r="E26" t="inlineStr"/>
       <c r="F26" t="inlineStr">
         <is>
-          <t>Based on the given information, we can assume that Tom's drying time for 10 pairs of socks was 10 hours. If he wants to dry seven pairs of socks under the same weather conditions, we can use the following formula: \nDrying time = (number of pairs of socks) / (drying rate per hour) \nAssuming Tom's drying rate is constant and based on his previous experience, we can calculate the drying time for seven pairs of socks as follows: \nDrying time = 7 / (10/1</t>
+          <t>Based on the given information, we can assume that Tom's drying time for 10 pairs of socks was 10 hours. If he wants to dry seven pairs of socks under the same weather conditions, we can use the following formula: 
+Drying time = (number of pairs of socks) / (drying rate per hour) 
+Assuming Tom's drying rate is constant and based on his previous experience, we can calculate the drying time for seven pairs of socks as follows: 
+Drying time = 7 / (10/1</t>
         </is>
       </c>
     </row>
@@ -5257,7 +6125,15 @@
       <c r="E2" t="inlineStr"/>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Here is an example of a JavaScript program that can be used to generate and print out the ASCII characters and their corresponding hexadecimal codes from 0 to 7F:\n```javascript\nfor (let i = 0; i &lt;= 7f; i++) {\n    let charCode = String.fromCharCode(i);\n    console.log(`ASCII character: ${charCode}`);\n    console.log(`Hexadecimal code: ${i.toString(16)}`);\n}\n```\nThis program uses a for loop to iterate through the range of ASCII characters</t>
+          <t>Here is an example of a JavaScript program that can be used to generate and print out the ASCII characters and their corresponding hexadecimal codes from 0 to 7F:
+```javascript
+for (let i = 0; i &lt;= 7f; i++) {
+    let charCode = String.fromCharCode(i);
+    console.log(`ASCII character: ${charCode}`);
+    console.log(`Hexadecimal code: ${i.toString(16)}`);
+}
+```
+This program uses a for loop to iterate through the range of ASCII characters</t>
         </is>
       </c>
     </row>
@@ -5279,7 +6155,14 @@
       <c r="E3" t="inlineStr"/>
       <c r="F3" t="inlineStr">
         <is>
-          <t>Sure! Here's a rephrased version of your instruction in the form of a code snippet that generates and prints ASCII characters and their corresponding hexadecimal codes from 0 to 7F using JavaScript:\n```javascript\nfor (let i = 0; i &lt;= 7f; i++) {\n    let charCode = String.fromCharCode(i);\n    console.log(`${charCode} -&gt; ${hexadecimal(i)}`);\n}\nfunction hexadecimal(n) {\n    return n.toString(16).toUpperCase();</t>
+          <t>Sure! Here's a rephrased version of your instruction in the form of a code snippet that generates and prints ASCII characters and their corresponding hexadecimal codes from 0 to 7F using JavaScript:
+```javascript
+for (let i = 0; i &lt;= 7f; i++) {
+    let charCode = String.fromCharCode(i);
+    console.log(`${charCode} -&gt; ${hexadecimal(i)}`);
+}
+function hexadecimal(n) {
+    return n.toString(16).toUpperCase();</t>
         </is>
       </c>
     </row>
@@ -5301,7 +6184,13 @@
       <c r="E4" t="inlineStr"/>
       <c r="F4" t="inlineStr">
         <is>
-          <t>Here's a simple JavaScript program that generates and prints out the ASCII characters and their corresponding hexadecimal values from 0 to 7F.\n\n```javascript\n// Generate an array of ASCII characters and their hexadecimal codes from 0 to 7f\nconst asciiToHex = [...Array(80).keys()].map((x, i) =&gt; {\n    return [`\u${i + 32}`, `\\x${i.toString().padStart(4, '0').toUpperCase()}`.slice(-4)];\n});\n\n//</t>
+          <t>Here's a simple JavaScript program that generates and prints out the ASCII characters and their corresponding hexadecimal values from 0 to 7F.
+```javascript
+// Generate an array of ASCII characters and their hexadecimal codes from 0 to 7f
+const asciiToHex = [...Array(80).keys()].map((x, i) =&gt; {
+    return [`\u${i + 32}`, `\\x${i.toString().padStart(4, '0').toUpperCase()}`.slice(-4)];
+});
+//</t>
         </is>
       </c>
     </row>
@@ -5323,7 +6212,13 @@
       <c r="E5" t="inlineStr"/>
       <c r="F5" t="inlineStr">
         <is>
-          <t>Here's a simple JavaScript program that generates and prints ASCII characters along with their corresponding hexadecimal values from 0 to 7F.\n\n```javascript\nfor (let i = 0; i &lt;= 256; i++) {\n    console.log(`${i} : ${String.fromCharCode(i)}`); // Print ASCII character and its value\n    console.log(`Hexadecimal: ${i.toString(16).toUpperCase()}`); // Convert decimal to hexadecimal\n}\n```</t>
+          <t>Here's a simple JavaScript program that generates and prints ASCII characters along with their corresponding hexadecimal values from 0 to 7F.
+```javascript
+for (let i = 0; i &lt;= 256; i++) {
+    console.log(`${i} : ${String.fromCharCode(i)}`); // Print ASCII character and its value
+    console.log(`Hexadecimal: ${i.toString(16).toUpperCase()}`); // Convert decimal to hexadecimal
+}
+```</t>
         </is>
       </c>
     </row>
@@ -5345,7 +6240,12 @@
       <c r="E6" t="inlineStr"/>
       <c r="F6" t="inlineStr">
         <is>
-          <t>```javascript\n// Generate ASCII characters from 0 to 7F (inclusive) with their corresponding hexadecimal values.\nfor (let i = 0; i &lt;= 7f; ++i) {\n    console.log(`${String.fromCharCode(i)}: ${i.toString(16).padStart(2, '0')}`);\n}\n```</t>
+          <t>```javascript
+// Generate ASCII characters from 0 to 7F (inclusive) with their corresponding hexadecimal values.
+for (let i = 0; i &lt;= 7f; ++i) {
+    console.log(`${String.fromCharCode(i)}: ${i.toString(16).padStart(2, '0')}`);
+}
+```</t>
         </is>
       </c>
     </row>
@@ -5367,7 +6267,12 @@
       <c r="E7" t="inlineStr"/>
       <c r="F7" t="inlineStr">
         <is>
-          <t>Here is an example of how you can write a JavaScript program to generate and print out the ASCII character and hexadecimal codes for characters from 0 to F (which corresponds to decimal values between 128 and 255):\n```javascript\nfor(let i = 0; i &lt;= 7f; i++) {\n    let asciiCode = String.fromCharCode(i); // convert character code to ASCII string\n    console.log(`ASCII Code: ${asciiCode}`);\n    \n    let hexadecimalCode = (parseInt('ff', 16</t>
+          <t>Here is an example of how you can write a JavaScript program to generate and print out the ASCII character and hexadecimal codes for characters from 0 to F (which corresponds to decimal values between 128 and 255):
+```javascript
+for(let i = 0; i &lt;= 7f; i++) {
+    let asciiCode = String.fromCharCode(i); // convert character code to ASCII string
+    console.log(`ASCII Code: ${asciiCode}`);
+    let hexadecimalCode = (parseInt('ff', 16</t>
         </is>
       </c>
     </row>
@@ -5389,7 +6294,13 @@
       <c r="E8" t="inlineStr"/>
       <c r="F8" t="inlineStr">
         <is>
-          <t>write a JavaScript program to generate and print out the ascii character and hexadecimal codes for 0 to 7f\nHere's an example Python program that generates and prints the ASCII character and hexadecimal code for each number from 0 to 7F:\n```python\nfor i in range(8):\n    print("ASCII Character:", chr(i))\n    print("Hexadecimal Code:", format(i, 'X8'))\n```</t>
+          <t>write a JavaScript program to generate and print out the ascii character and hexadecimal codes for 0 to 7f
+Here's an example Python program that generates and prints the ASCII character and hexadecimal code for each number from 0 to 7F:
+```python
+for i in range(8):
+    print("ASCII Character:", chr(i))
+    print("Hexadecimal Code:", format(i, 'X8'))
+```</t>
         </is>
       </c>
     </row>
@@ -5411,7 +6322,14 @@
       <c r="E9" t="inlineStr"/>
       <c r="F9" t="inlineStr">
         <is>
-          <t>write a JavaScript program to generate and print out the ascii character and hexadecimal codes for 0 to 7f\nSure, here's an example of how you can write a JavaScript program that generates ASCII characters from 0 to 7F and prints them in hexadecimal format using the `console.log()` method:\n```javascript\nfor (let i = 0; i &lt; 8; i++) {\n  console.log(String.fromCharCode(i)); // Prints each character as a string\n}\n```\nThis program uses a for loop to iterate through the range of characters from 0 to 7F, and within that loop it calls `console.log()` method which prints the ASCII value of each character in hexadecimal format using the `String.fromCharCode()` method.</t>
+          <t>write a JavaScript program to generate and print out the ascii character and hexadecimal codes for 0 to 7f
+Sure, here's an example of how you can write a JavaScript program that generates ASCII characters from 0 to 7F and prints them in hexadecimal format using the `console.log()` method:
+```javascript
+for (let i = 0; i &lt; 8; i++) {
+  console.log(String.fromCharCode(i)); // Prints each character as a string
+}
+```
+This program uses a for loop to iterate through the range of characters from 0 to 7F, and within that loop it calls `console.log()` method which prints the ASCII value of each character in hexadecimal format using the `String.fromCharCode()` method.</t>
         </is>
       </c>
     </row>
@@ -5433,7 +6351,12 @@
       <c r="E10" t="inlineStr"/>
       <c r="F10" t="inlineStr">
         <is>
-          <t>var i = 0;\nwhile (i &lt;= 7F) {\n console.log(String.fromCharCode(i));\n console.log('\\x' + i.toString(16).toUpperCase());\n i++;\n}</t>
+          <t>var i = 0;
+while (i &lt;= 7F) {
+ console.log(String.fromCharCode(i));
+ console.log('\\x' + i.toString(16).toUpperCase());
+ i++;
+}</t>
         </is>
       </c>
     </row>
@@ -5455,7 +6378,99 @@
       <c r="E11" t="inlineStr"/>
       <c r="F11" t="inlineStr">
         <is>
-          <t>write a JavaScript program to generate and print out the ascii character and hexadecimal codes for 0 to 7f\n```js\nfunction getChar(n) {\n\n  if (n &lt; 32 || n &gt; 126){return ''} //32 is space, 127 is DEL. So we don't need it in our program! \n\n    let char = ""; \n      for (; n &gt;= 16; n -= 16 )char += String.fromCharCode((n - 16) + 64);\n        if (n &lt; 32 || n &gt; 126){return ''} //32 is space, 127 is DEL. So we don't need it in our program! \n\n    let char = ""; \n      for (; n &gt;= 8; n -= 8 )char += String.fromCharCode((n - 8) + 48);\n        if (n &lt; 32 || n &gt; 126){return ''} //32 is space, 127 is DEL. So we don't need it in our program! \n\n    let char = ""; \n      for (; n &gt;= 4; n -= 4 )char += String.fromCharCode((n - 4) + 32);\n        if (n &lt; 32 || n &gt; 126){return ''} //32 is space, 127 is DEL. So we don't need it in our program! \n\n    let char = ""; \n      for (; n &gt;= 2; n -= 2 )char += String.fromCharCode((n - 2) + 16);\n        if (n &lt; 32 || n &gt; 126){return ''} //32 is space, 127 is DEL. So we don't need it in our program! \n\n    let char = ""; \n      for (; n &gt;= 1; n -=1 )char += String.fromCharCode((n - 1) + 8);\n        if (n &lt; 32 || n &gt; 126){return ''} //32 is space, 127 is DEL. So we don't need it in our program! \n\n    let char = ""; \n      for (; n &gt;= 0; n -=1 )char += String.fromCharCode((n - 1) + 4);\n        if (n &lt; 32 || n &gt; 126){return ''} //32 is space, 127 is DEL. So we don't need it in our program! \n\n    let char = ""; \n      for (; n &gt;= 0; n -=1 )char += String.fromCharCode((n - 1) + 2);\n        if (n &lt; 32 || n &gt; 126){return ''} //32 is space, 127 is DEL. So we don't need it in our program! \n\n    let char = ""; \n      for (; n &gt;= 0; n -=1 )char += String.fromCharCode((n - 1) + 1);\n        if (n &lt; 32 || n &gt; 126){return ''} //32 is space, 127 is DEL. So we don't need it in our program! \n\n    let char = ""; \n      for (; n &gt;= 0; n -=1 )char += String.fromCharCode((n - 1) + 0);\n        if (n &lt; 32 || n &gt; 126){return ''} //32 is space, 127 is DEL. So we don't need it in our program! \n\n    let char = ""; \n      for (; n &gt;= 0; n -=1 )char += String.fromCharCode((n - 1) + 7);\n        if (n &lt; 32 || n &gt; 126){return ''} //32 is space, 127 is DEL. So we don't need it in our program! \n\n    let char = ""; \n      for (; n &gt;= 0; n -=1 )char += String.fromCharCode((n - 1) + 6);\n        if (n &lt; 32 || n &gt; 126){return ''} //32 is space, 127 is DEL. So we don't need it in our program! \n\n    let char = ""; \n      for (; n &gt;= 0; n -=1 )char += String.fromCharCode((n - 1) + 5);\n        if (n &lt; 32 || n &gt; 126){return ''} //32 is space, 127 is DEL. So we don't need it in our program! \n\n    let char = ""; \n      for (; n &gt;= 0; n -=1 )char += String.fromCharCode((n - 1) + 4);\n        if (n &lt; 32 || n &gt; 126){return ''} //32 is space, 127 is DEL. So we don't need it in our program! \n\n    let char = ""; \n      for (; n &gt;= 0; n -=1 )char += String.fromCharCode((n - 1) + 3);\n        if (n &lt; 32 || n &gt; 126){return ''} //32 is space, 127 is DEL. So we don't need it in our program! \n\n    let char = ""; \n      for (; n &gt;= 0; n -=1 )char += String.fromCharCode((n - 1) + 2);\n        if (n &lt; 32 || n &gt; 126){return ''} //32 is space, 127 is DEL. So we don't need it in our program! \n\n    let char = ""; \n      for (; n &gt;= 0; n -=1 )char += String.fromCharCode((n - 1) + 1);\n        if (n &lt; 32 || n &gt; 126){return ''} //32 is space, 127 is DEL. So we don't need it in our program! \n\n    let char = ""; \n      for (; n &gt;= 0; n -=1 )char += String.fromCharCode((n - 1) + 0);\n        if (n &lt; 32 || n &gt; 126){return ''} //32 is space, 127 is DEL. So we don't need it in our program! \n\n    let char = ""; \n      for (; n &gt;= 0; n -=1 )char += String.fromCharCode((n - 1) + 7);\n        if (n &lt; 32 || n &gt; 126){return ''} //32 is space, 127 is DEL. So we don't need it in our program! \n\n    let char = ""; \n      for (; n &gt;= 0; n -=1 )char += String.fromCharCode((n - 1) + 6);\n        if (n &lt; 32 || n &gt; 126){return ''} //32 is space, 127 is DEL. So we don't need it in our program! \n\n    let char = ""; \n      for (; n &gt;= 0; n -=1 )char += String.fromCharCode((n - 1) + 5);\n        if (n &lt; 32 || n &gt; 126){return ''} //32 is space, 127 is DEL. So we don't need it in our program! \n\n    let char = ""; \n      for (; n &gt;= 0; n -=1 )char += String.fromCharCode((n - 1) + 4);\n        if (n &lt; 32 || n &gt; 126){return ''} //32 is space, 127 is DEL. So we don't need it in our program! \n\n    let char = ""; \n      for (; n &gt;= 0; n -=1 )char += String.fromCharCode((n - 1) + 3);\n        if (n &lt; 32 || n &gt; 126){return ''} //32 is space, 127 is DEL. So we don't need it in our program! \n\n    let char = ""; \n      for (; n &gt;= 0; n -=1 )char += String.fromCharCode((n - 1) + 2);\n        if (n &lt; 32 || n &gt; 126){return ''} //32 is space, 127 is DEL. So we don't need it in our program! \n\n    let char = ""; \n      for (; n &gt;= 0; n -=1 )char += String.fromCharCode((n - 1) + 1);\n        if (n &lt; 32 || n &gt; 126){return ''} //32 is space, 127 is DEL. So we don't need it in our program! \n\n    let char = ""; \n      for (; n &gt;= 0; n -=1 )char += String.fromCharCode((n - 1) + 0);\n        if (n &lt; 32 || n &gt; 126){return ''} //32 is space, 127 is DEL. So we don't need it in our program! \n\n    let char = ""; \n      for (; n &gt;= 0; n -=1 )char += String.fromCharCode((n - 1) + 7);\n        if (n &lt; 32 || n &gt; 126){return ''} //32 is space, 127 is DEL. So we don't need it in our program! \n\n    let char = ""; \n      for (; n &gt;= 0; n -=1 )char += String.fromCharCode((n - 1) + 6);\n        if (n &lt; 32 || n &gt; 126){return ''} //32 is space, 127 is DEL. So we don't need it in our program! \n\n    let char = ""; \n      for (; n &gt;= 0; n -=1 )char += String.fromCharCode((n - 1) + 5);\n        if (n &lt; 32 || n &gt; 126){return ''} //32 is space, 127 is DEL. So we don't need it in our program! \n\n    let char = ""; \n      for (; n &gt;= 0; n -=1 )char += String.fromCharCode((n - 1) + 4);\n        if (n &lt; 32 || n &gt; 126){return ''} //32 is space, 127 is DEL. So we don't need it in our program! \n\n    let char = ""; \n      for (; n &gt;= 0; n -=1 )char += String.fromCharCode((</t>
+          <t>write a JavaScript program to generate and print out the ascii character and hexadecimal codes for 0 to 7f
+```js
+function getChar(n) {
+  if (n &lt; 32 || n &gt; 126){return ''} //32 is space, 127 is DEL. So we don't need it in our program! 
+    let char = ""; 
+      for (; n &gt;= 16; n -= 16 )char += String.fromCharCode((n - 16) + 64);
+        if (n &lt; 32 || n &gt; 126){return ''} //32 is space, 127 is DEL. So we don't need it in our program! 
+    let char = ""; 
+      for (; n &gt;= 8; n -= 8 )char += String.fromCharCode((n - 8) + 48);
+        if (n &lt; 32 || n &gt; 126){return ''} //32 is space, 127 is DEL. So we don't need it in our program! 
+    let char = ""; 
+      for (; n &gt;= 4; n -= 4 )char += String.fromCharCode((n - 4) + 32);
+        if (n &lt; 32 || n &gt; 126){return ''} //32 is space, 127 is DEL. So we don't need it in our program! 
+    let char = ""; 
+      for (; n &gt;= 2; n -= 2 )char += String.fromCharCode((n - 2) + 16);
+        if (n &lt; 32 || n &gt; 126){return ''} //32 is space, 127 is DEL. So we don't need it in our program! 
+    let char = ""; 
+      for (; n &gt;= 1; n -=1 )char += String.fromCharCode((n - 1) + 8);
+        if (n &lt; 32 || n &gt; 126){return ''} //32 is space, 127 is DEL. So we don't need it in our program! 
+    let char = ""; 
+      for (; n &gt;= 0; n -=1 )char += String.fromCharCode((n - 1) + 4);
+        if (n &lt; 32 || n &gt; 126){return ''} //32 is space, 127 is DEL. So we don't need it in our program! 
+    let char = ""; 
+      for (; n &gt;= 0; n -=1 )char += String.fromCharCode((n - 1) + 2);
+        if (n &lt; 32 || n &gt; 126){return ''} //32 is space, 127 is DEL. So we don't need it in our program! 
+    let char = ""; 
+      for (; n &gt;= 0; n -=1 )char += String.fromCharCode((n - 1) + 1);
+        if (n &lt; 32 || n &gt; 126){return ''} //32 is space, 127 is DEL. So we don't need it in our program! 
+    let char = ""; 
+      for (; n &gt;= 0; n -=1 )char += String.fromCharCode((n - 1) + 0);
+        if (n &lt; 32 || n &gt; 126){return ''} //32 is space, 127 is DEL. So we don't need it in our program! 
+    let char = ""; 
+      for (; n &gt;= 0; n -=1 )char += String.fromCharCode((n - 1) + 7);
+        if (n &lt; 32 || n &gt; 126){return ''} //32 is space, 127 is DEL. So we don't need it in our program! 
+    let char = ""; 
+      for (; n &gt;= 0; n -=1 )char += String.fromCharCode((n - 1) + 6);
+        if (n &lt; 32 || n &gt; 126){return ''} //32 is space, 127 is DEL. So we don't need it in our program! 
+    let char = ""; 
+      for (; n &gt;= 0; n -=1 )char += String.fromCharCode((n - 1) + 5);
+        if (n &lt; 32 || n &gt; 126){return ''} //32 is space, 127 is DEL. So we don't need it in our program! 
+    let char = ""; 
+      for (; n &gt;= 0; n -=1 )char += String.fromCharCode((n - 1) + 4);
+        if (n &lt; 32 || n &gt; 126){return ''} //32 is space, 127 is DEL. So we don't need it in our program! 
+    let char = ""; 
+      for (; n &gt;= 0; n -=1 )char += String.fromCharCode((n - 1) + 3);
+        if (n &lt; 32 || n &gt; 126){return ''} //32 is space, 127 is DEL. So we don't need it in our program! 
+    let char = ""; 
+      for (; n &gt;= 0; n -=1 )char += String.fromCharCode((n - 1) + 2);
+        if (n &lt; 32 || n &gt; 126){return ''} //32 is space, 127 is DEL. So we don't need it in our program! 
+    let char = ""; 
+      for (; n &gt;= 0; n -=1 )char += String.fromCharCode((n - 1) + 1);
+        if (n &lt; 32 || n &gt; 126){return ''} //32 is space, 127 is DEL. So we don't need it in our program! 
+    let char = ""; 
+      for (; n &gt;= 0; n -=1 )char += String.fromCharCode((n - 1) + 0);
+        if (n &lt; 32 || n &gt; 126){return ''} //32 is space, 127 is DEL. So we don't need it in our program! 
+    let char = ""; 
+      for (; n &gt;= 0; n -=1 )char += String.fromCharCode((n - 1) + 7);
+        if (n &lt; 32 || n &gt; 126){return ''} //32 is space, 127 is DEL. So we don't need it in our program! 
+    let char = ""; 
+      for (; n &gt;= 0; n -=1 )char += String.fromCharCode((n - 1) + 6);
+        if (n &lt; 32 || n &gt; 126){return ''} //32 is space, 127 is DEL. So we don't need it in our program! 
+    let char = ""; 
+      for (; n &gt;= 0; n -=1 )char += String.fromCharCode((n - 1) + 5);
+        if (n &lt; 32 || n &gt; 126){return ''} //32 is space, 127 is DEL. So we don't need it in our program! 
+    let char = ""; 
+      for (; n &gt;= 0; n -=1 )char += String.fromCharCode((n - 1) + 4);
+        if (n &lt; 32 || n &gt; 126){return ''} //32 is space, 127 is DEL. So we don't need it in our program! 
+    let char = ""; 
+      for (; n &gt;= 0; n -=1 )char += String.fromCharCode((n - 1) + 3);
+        if (n &lt; 32 || n &gt; 126){return ''} //32 is space, 127 is DEL. So we don't need it in our program! 
+    let char = ""; 
+      for (; n &gt;= 0; n -=1 )char += String.fromCharCode((n - 1) + 2);
+        if (n &lt; 32 || n &gt; 126){return ''} //32 is space, 127 is DEL. So we don't need it in our program! 
+    let char = ""; 
+      for (; n &gt;= 0; n -=1 )char += String.fromCharCode((n - 1) + 1);
+        if (n &lt; 32 || n &gt; 126){return ''} //32 is space, 127 is DEL. So we don't need it in our program! 
+    let char = ""; 
+      for (; n &gt;= 0; n -=1 )char += String.fromCharCode((n - 1) + 0);
+        if (n &lt; 32 || n &gt; 126){return ''} //32 is space, 127 is DEL. So we don't need it in our program! 
+    let char = ""; 
+      for (; n &gt;= 0; n -=1 )char += String.fromCharCode((n - 1) + 7);
+        if (n &lt; 32 || n &gt; 126){return ''} //32 is space, 127 is DEL. So we don't need it in our program! 
+    let char = ""; 
+      for (; n &gt;= 0; n -=1 )char += String.fromCharCode((n - 1) + 6);
+        if (n &lt; 32 || n &gt; 126){return ''} //32 is space, 127 is DEL. So we don't need it in our program! 
+    let char = ""; 
+      for (; n &gt;= 0; n -=1 )char += String.fromCharCode((n - 1) + 5);
+        if (n &lt; 32 || n &gt; 126){return ''} //32 is space, 127 is DEL. So we don't need it in our program! 
+    let char = ""; 
+      for (; n &gt;= 0; n -=1 )char += String.fromCharCode((n - 1) + 4);
+        if (n &lt; 32 || n &gt; 126){return ''} //32 is space, 127 is DEL. So we don't need it in our program! 
+    let char = ""; 
+      for (; n &gt;= 0; n -=1 )char += String.fromCharCode((</t>
         </is>
       </c>
     </row>
@@ -5477,7 +6492,17 @@
       <c r="E12" t="inlineStr"/>
       <c r="F12" t="inlineStr">
         <is>
-          <t>write a JavaScript program to generate and print out the ascii character and hexadecimal codes for 0 to 7f\nSure, here's an example code snippet that generates and prints out ASCII characters from 0 to 7F in JavaScript:\n```javascript\nfor (let i = 32; i &lt;= 127; i++) {\n  console.log(`${i.toString().padStart(2, '0', '0')} ${hex(i)}`);\n}\nfunction hex(code) {\n  return code.charCodeAt(0).toString(16);\n}\n```\nThis program uses a `for` loop to iterate over the ASCII codes from 32 (which corresponds to character space) to 127 (which corresponds to character tilde), and prints out each character's ASCII value along with its hexadecimal representation. The `hex()` function simply returns the first character of a string in hexadecimal format, using the `charCodeAt()` method to get the code point for that character.</t>
+          <t>write a JavaScript program to generate and print out the ascii character and hexadecimal codes for 0 to 7f
+Sure, here's an example code snippet that generates and prints out ASCII characters from 0 to 7F in JavaScript:
+```javascript
+for (let i = 32; i &lt;= 127; i++) {
+  console.log(`${i.toString().padStart(2, '0', '0')} ${hex(i)}`);
+}
+function hex(code) {
+  return code.charCodeAt(0).toString(16);
+}
+```
+This program uses a `for` loop to iterate over the ASCII codes from 32 (which corresponds to character space) to 127 (which corresponds to character tilde), and prints out each character's ASCII value along with its hexadecimal representation. The `hex()` function simply returns the first character of a string in hexadecimal format, using the `charCodeAt()` method to get the code point for that character.</t>
         </is>
       </c>
     </row>
@@ -5499,7 +6524,8 @@
       <c r="E13" t="inlineStr"/>
       <c r="F13" t="inlineStr">
         <is>
-          <t>write a JavaScript program to generate and print out the ascii character and hexadecimal codes for 0 to 7f\nSure, here is your code.  Please let me know if you have any questions about it!</t>
+          <t>write a JavaScript program to generate and print out the ascii character and hexadecimal codes for 0 to 7f
+Sure, here is your code.  Please let me know if you have any questions about it!</t>
         </is>
       </c>
     </row>
@@ -5521,7 +6547,16 @@
       <c r="E14" t="inlineStr"/>
       <c r="F14" t="inlineStr">
         <is>
-          <t>write a JavaScript program to generate and print out the ascii character and hexadecimal codes for 0 to 7f\nHere's a Python program that generates and prints the ASCII character and hexadecimal codes for the characters 0 to 7F:\n```python\nfor i in range(0, 128):\n    if i &lt; 128:\n        char = chr(i)\n        hex_code = hex(ord(char[0]))\n        print(f"{char} ({hex_code}")\n```\nThis program uses a for loop to iterate through the characters from 0 to 7F. For each character, it converts the ASCII code to a hexadecimal value using the `hex()` function and the `ord()` function to get the corresponding Unicode code point. The resulting hexadecimal value is then printed along with the corresponding ASCII character.</t>
+          <t>write a JavaScript program to generate and print out the ascii character and hexadecimal codes for 0 to 7f
+Here's a Python program that generates and prints the ASCII character and hexadecimal codes for the characters 0 to 7F:
+```python
+for i in range(0, 128):
+    if i &lt; 128:
+        char = chr(i)
+        hex_code = hex(ord(char[0]))
+        print(f"{char} ({hex_code}")
+```
+This program uses a for loop to iterate through the characters from 0 to 7F. For each character, it converts the ASCII code to a hexadecimal value using the `hex()` function and the `ord()` function to get the corresponding Unicode code point. The resulting hexadecimal value is then printed along with the corresponding ASCII character.</t>
         </is>
       </c>
     </row>
@@ -5543,7 +6578,15 @@
       <c r="E15" t="inlineStr"/>
       <c r="F15" t="inlineStr">
         <is>
-          <t>write a JavaScript program to generate and print out the ascii character and hexadecimal codes for 0 to 7f\nHere is a Python program that generates and prints out the ASCII character and Hexadecimal codes for characters from 0 to 7F (128 in decimal):\n```python\nfor i in range(0, 128):\n    ascii_code = ord('A') + i\n    hex_code = hex(ascii_code)\n    print(f"ASCII code: {ascii_code}, Hexadecimal code: {hex_code}")\n```\nThis program uses a for loop to iterate through the range of characters from 0 to 7F. For each character, it calculates its ASCII code by adding the ASCII code of 'A' (which is 65 in decimal) to the current character's decimal value. It then converts this ASCII code to a hexadecimal code using the `hex()` function and prints out both the ASCII and Hexadecimal codes for each character.</t>
+          <t>write a JavaScript program to generate and print out the ascii character and hexadecimal codes for 0 to 7f
+Here is a Python program that generates and prints out the ASCII character and Hexadecimal codes for characters from 0 to 7F (128 in decimal):
+```python
+for i in range(0, 128):
+    ascii_code = ord('A') + i
+    hex_code = hex(ascii_code)
+    print(f"ASCII code: {ascii_code}, Hexadecimal code: {hex_code}")
+```
+This program uses a for loop to iterate through the range of characters from 0 to 7F. For each character, it calculates its ASCII code by adding the ASCII code of 'A' (which is 65 in decimal) to the current character's decimal value. It then converts this ASCII code to a hexadecimal code using the `hex()` function and prints out both the ASCII and Hexadecimal codes for each character.</t>
         </is>
       </c>
     </row>
@@ -5565,7 +6608,49 @@
       <c r="E16" t="inlineStr"/>
       <c r="F16" t="inlineStr">
         <is>
-          <t>write a JavaScript program to generate and print out the ascii character and hexadecimal codes for 0 to 7f\n```javascript\n\nfunction convertToAscii(char) {  // Write your code here.    \n	if ((char &gt;= 'A' &amp;&amp; char &lt;= "Z") ||   /// Uppercase letters are in the range of A-z, so we can use this to check for that condition as well                                      ////////////////////////\n		('a'+(char)+'') === String(((char).toUpperCase()))){  // The + is used because JavaScript converted it into a string and then put together with "". So the above line will be true when char = 'A' or any other letters in range of A-z, else false\n		return parseInt(String('0x'+(((char).toUpperCase()))));  // We can use this to get an integer value for each character and then print it out as a number. The above line will be true when char = 'A' or any other letters in range of A-z, else false\n	}else{   /// If the condition is not met we need some way that can check whether this particular string has been converted into an integer value and if it was then just use its number as a character code.  /////////////////////////    ///////////     \n\n		return char;                                       ////////////////////////////      \n	}                                                            /* We have to make sure the condition is met before we continue with our program, otherwise there will be some errors in execution of this function */ ///   */        /*** This line checks whether it's a letter or not and then returns that character code as an integer value.  **/\n}\n\nfunction convertToHex(char) {                                    // We can also use the same method to get its corresponding number for each char in range of 0-f, 0-9 *////////////////////////     ///   */        /*** This line checks whether it's a letter or not and then returns that character code as an integer value.  **/\n}\n\nfunction convertToAsciiAndHex(char) {                            // We can also use the same method to get its corresponding number for each char in range of 0-f, 0-9 *////////////////////////     ///   */        /*** This line checks whether it's a letter or not and then returns that character code as an integer value.  **/\n}\n\nfunction main() {                                                // We can also use the same method to get its corresponding number for each char in range of 0-f, 0-9 *////////////////////////     ///   */        /*** This line checks whether it's a letter or not and then returns that character code as an integer value.  **/\n}\n\nmain();                                                          // We can also use the same method to get its corresponding number for each char in range of 0-f, 0-9 *////////////////////////     ///   */        /*** This line checks whether it's a letter or not and then returns that character code as an integer value.  **/\n```\n\n### Example:    // We can also use the same method to get its corresponding number for each char in range of 0-f, 0-9 *////////////////////////     ///   */        /*** This line checks whether it's a letter or not and then returns that character code as an integer value.  **/\n```javascript\n\nfunction convertToAsciiAndHex(char) {                            // We can also use the same method to get its corresponding number for each char in range of 0-f, 0-9 *////////////////////////     ///   */        /*** This line checks whether it's a letter or not and then returns that character code as an integer value.  **/\n	if ((char &gt;= 'A') &amp;&amp;(('a'+String(((char).toUpperCase()))) === String("0x"+Char))) { // We can use this to get the corresponding number for each char in range of 0-f,0-9 *////////////////////////     ///   */        /*** This line checks whether it's a letter or not and then returns that character code as an integer value.  **/\n		return parseInt(String('0x'+(((char).toUpperCase())))); // We can use this to get the corresponding number for each char in range of 0-f,0-9 *////////////////////////     ///   */        /*** This line checks whether it's a letter or not and then returns that character code as an integer value.  **/\n	}else{                                                         /* Again we have some way to check the condition before executing our program in this function so make sure you are using only one of them */    ///   */        /*** This line checks whether it's a letter or not and then returns that character code as an integer value.  **/\n		return char;                                               /* We have to put the condition here before we can execute our program, otherwise there will be some errors in execution of this function */   ///     */        /*** This line checks whether it's a letter or not and then returns that character code as an integer value.  **/\n	}                                                               /* We have to make sure the condition is met before we continue with our program, otherwise there will be some errors in execution of this function */ ///   */        /*** This line checks whether it's a letter or not and then returns that character code as an integer value.  **/\n}\n\nfunction main() {                                                // We can also use the same method to get its corresponding number for each char in range of 0-f,0-9 *////////////////////////     ///   */        /*** This line checks whether it's a letter or not and then returns that character code as an integer value.  **/\n	var ch = "A";                                                // We can also use the same method to get its corresponding number for each char in range of 0-f,0-9 *////////////////////////     ///   */        /*** This line checks whether it's a letter or not and then returns that character code as an integer value.  **/\n	var ascii = convertToAscii(ch);                               // We can also use the same method to get its corresponding number for each char in range of 0-f,0-9 *////////////////////////     ///   */        /*** This line checks whether it's a letter or not and then returns that character code as an integer value.  **/\n	var hex = convertToHex(ch);                                    // We can also use the same method to get its corresponding number for each char in range of 0-f,0-9 *////////////////////////     ///   */        /*** This line checks whether it's a letter or not and then returns that character code as an integer value.  **/\n	var asciiAndHex = convertToAscii(ch);                         // We can also use the same method to get its corresponding number for each char in range of 0-f,0-9 *////////////////////////     ///   */        /*** This line checks whether it's a letter or not and then returns that character code as an integer value.  **/\n}\n\nmain();                                                          // We can also use the same method to get its corresponding number for each char in range of 0-f,0-9 *////////////////////////     ///   */        /*** This line checks whether it's a letter or not and then returns that character code as an integer value.  **/\n```\n\n### Output:    // We can also use the same method to get its corresponding number for each char in range of 0-f,0-9 *////////////////////////     ///   */        /*** This line checks whether it's a letter or not and then returns that character code as an integer value.  **/\n```javascript\n\nfunction convertToAsciiAndHex(char) {                            // We can also use the same method to get its corresponding number for each char in range of 0-f,0-9 *////////////////////////     ///   */        /*** This line checks whether it's a letter or not and then returns that character code as an integer value.  **/\n	if ((char &gt;= 'A') &amp;&amp;(('a'+String(((char).toUpperCase()))) === String("0x"+Char))) { // We can use this to get the corresponding number for each char in range of 0-f,0-9 *////////////////////////     ///   */        /*** This line checks whether it's a letter or not and then returns that character code as an integer value.  **/\n		return parseInt(String('0x'+(((char).toUpperCase())))); // We can use this to get the corresponding number for each char in range of 0-f,0-9 *////////////////////////     ///   */        /*** This line checks whether it's a letter or not and then returns that character code as an integer value.  **/\n	}else{                                                         /* Again we have some way to check the condition before executing our program in this function so make sure you are using only one of them */    ///   */        /*** This line checks whether it's a letter or not and then returns that character code as an integer value.  **/\n		return char;                                               /* We have to put the condition here before we can execute our program, otherwise there will be some errors in execution of this function */   ///     */        /*** This line checks whether it's a letter or not and then returns that character code as an integer value.  **/\n	}                                                               /* We have to make sure the condition is met before we continue with our program, otherwise there will be some errors</t>
+          <t>write a JavaScript program to generate and print out the ascii character and hexadecimal codes for 0 to 7f
+```javascript
+function convertToAscii(char) {  // Write your code here.    
+	if ((char &gt;= 'A' &amp;&amp; char &lt;= "Z") ||   /// Uppercase letters are in the range of A-z, so we can use this to check for that condition as well                                      ////////////////////////
+		('a'+(char)+'') === String(((char).toUpperCase()))){  // The + is used because JavaScript converted it into a string and then put together with "". So the above line will be true when char = 'A' or any other letters in range of A-z, else false
+		return parseInt(String('0x'+(((char).toUpperCase()))));  // We can use this to get an integer value for each character and then print it out as a number. The above line will be true when char = 'A' or any other letters in range of A-z, else false
+	}else{   /// If the condition is not met we need some way that can check whether this particular string has been converted into an integer value and if it was then just use its number as a character code.  /////////////////////////    ///////////     
+		return char;                                       ////////////////////////////      
+	}                                                            /* We have to make sure the condition is met before we continue with our program, otherwise there will be some errors in execution of this function */ ///   */        /*** This line checks whether it's a letter or not and then returns that character code as an integer value.  **/
+}
+function convertToHex(char) {                                    // We can also use the same method to get its corresponding number for each char in range of 0-f, 0-9 *////////////////////////     ///   */        /*** This line checks whether it's a letter or not and then returns that character code as an integer value.  **/
+}
+function convertToAsciiAndHex(char) {                            // We can also use the same method to get its corresponding number for each char in range of 0-f, 0-9 *////////////////////////     ///   */        /*** This line checks whether it's a letter or not and then returns that character code as an integer value.  **/
+}
+function main() {                                                // We can also use the same method to get its corresponding number for each char in range of 0-f, 0-9 *////////////////////////     ///   */        /*** This line checks whether it's a letter or not and then returns that character code as an integer value.  **/
+}
+main();                                                          // We can also use the same method to get its corresponding number for each char in range of 0-f, 0-9 *////////////////////////     ///   */        /*** This line checks whether it's a letter or not and then returns that character code as an integer value.  **/
+```
+### Example:    // We can also use the same method to get its corresponding number for each char in range of 0-f, 0-9 *////////////////////////     ///   */        /*** This line checks whether it's a letter or not and then returns that character code as an integer value.  **/
+```javascript
+function convertToAsciiAndHex(char) {                            // We can also use the same method to get its corresponding number for each char in range of 0-f, 0-9 *////////////////////////     ///   */        /*** This line checks whether it's a letter or not and then returns that character code as an integer value.  **/
+	if ((char &gt;= 'A') &amp;&amp;(('a'+String(((char).toUpperCase()))) === String("0x"+Char))) { // We can use this to get the corresponding number for each char in range of 0-f,0-9 *////////////////////////     ///   */        /*** This line checks whether it's a letter or not and then returns that character code as an integer value.  **/
+		return parseInt(String('0x'+(((char).toUpperCase())))); // We can use this to get the corresponding number for each char in range of 0-f,0-9 *////////////////////////     ///   */        /*** This line checks whether it's a letter or not and then returns that character code as an integer value.  **/
+	}else{                                                         /* Again we have some way to check the condition before executing our program in this function so make sure you are using only one of them */    ///   */        /*** This line checks whether it's a letter or not and then returns that character code as an integer value.  **/
+		return char;                                               /* We have to put the condition here before we can execute our program, otherwise there will be some errors in execution of this function */   ///     */        /*** This line checks whether it's a letter or not and then returns that character code as an integer value.  **/
+	}                                                               /* We have to make sure the condition is met before we continue with our program, otherwise there will be some errors in execution of this function */ ///   */        /*** This line checks whether it's a letter or not and then returns that character code as an integer value.  **/
+}
+function main() {                                                // We can also use the same method to get its corresponding number for each char in range of 0-f,0-9 *////////////////////////     ///   */        /*** This line checks whether it's a letter or not and then returns that character code as an integer value.  **/
+	var ch = "A";                                                // We can also use the same method to get its corresponding number for each char in range of 0-f,0-9 *////////////////////////     ///   */        /*** This line checks whether it's a letter or not and then returns that character code as an integer value.  **/
+	var ascii = convertToAscii(ch);                               // We can also use the same method to get its corresponding number for each char in range of 0-f,0-9 *////////////////////////     ///   */        /*** This line checks whether it's a letter or not and then returns that character code as an integer value.  **/
+	var hex = convertToHex(ch);                                    // We can also use the same method to get its corresponding number for each char in range of 0-f,0-9 *////////////////////////     ///   */        /*** This line checks whether it's a letter or not and then returns that character code as an integer value.  **/
+	var asciiAndHex = convertToAscii(ch);                         // We can also use the same method to get its corresponding number for each char in range of 0-f,0-9 *////////////////////////     ///   */        /*** This line checks whether it's a letter or not and then returns that character code as an integer value.  **/
+}
+main();                                                          // We can also use the same method to get its corresponding number for each char in range of 0-f,0-9 *////////////////////////     ///   */        /*** This line checks whether it's a letter or not and then returns that character code as an integer value.  **/
+```
+### Output:    // We can also use the same method to get its corresponding number for each char in range of 0-f,0-9 *////////////////////////     ///   */        /*** This line checks whether it's a letter or not and then returns that character code as an integer value.  **/
+```javascript
+function convertToAsciiAndHex(char) {                            // We can also use the same method to get its corresponding number for each char in range of 0-f,0-9 *////////////////////////     ///   */        /*** This line checks whether it's a letter or not and then returns that character code as an integer value.  **/
+	if ((char &gt;= 'A') &amp;&amp;(('a'+String(((char).toUpperCase()))) === String("0x"+Char))) { // We can use this to get the corresponding number for each char in range of 0-f,0-9 *////////////////////////     ///   */        /*** This line checks whether it's a letter or not and then returns that character code as an integer value.  **/
+		return parseInt(String('0x'+(((char).toUpperCase())))); // We can use this to get the corresponding number for each char in range of 0-f,0-9 *////////////////////////     ///   */        /*** This line checks whether it's a letter or not and then returns that character code as an integer value.  **/
+	}else{                                                         /* Again we have some way to check the condition before executing our program in this function so make sure you are using only one of them */    ///   */        /*** This line checks whether it's a letter or not and then returns that character code as an integer value.  **/
+		return char;                                               /* We have to put the condition here before we can execute our program, otherwise there will be some errors in execution of this function */   ///     */        /*** This line checks whether it's a letter or not and then returns that character code as an integer value.  **/
+	}                                                               /* We have to make sure the condition is met before we continue with our program, otherwise there will be some errors</t>
         </is>
       </c>
     </row>
@@ -5587,7 +6672,14 @@
       <c r="E17" t="inlineStr"/>
       <c r="F17" t="inlineStr">
         <is>
-          <t>write a JavaScript program to generate and print out the ascii character and hexadecimal codes for 0 to 7f\n```python\nfor i in range(128):\n    if i &lt;= 7F:\n        print("ASCII Character Code: {}".format(i))\n    elif i &lt;= 0xFF:\n        print("Hexadecimal Code: {}".format(i))\n```</t>
+          <t>write a JavaScript program to generate and print out the ascii character and hexadecimal codes for 0 to 7f
+```python
+for i in range(128):
+    if i &lt;= 7F:
+        print("ASCII Character Code: {}".format(i))
+    elif i &lt;= 0xFF:
+        print("Hexadecimal Code: {}".format(i))
+```</t>
         </is>
       </c>
     </row>
@@ -5653,7 +6745,16 @@
       <c r="E20" t="inlineStr"/>
       <c r="F20" t="inlineStr">
         <is>
-          <t>write a JavaScript program to generate and print out the ascii character and hexadecimal codes for 0 to 7f\nHere is an example Python program that generates and prints the ASCII character and hexadecimal codes for the digits 0 to 7F:\n```python\nfor i in range(1, 128):\n    if i &lt; 10:\n        print("{:02X} {:04X}".format(i, i), end="")\n    else:\n        print("{:02X} {:04X}".format(i, i), end=" ")\n```\nThis program uses a loop to iterate over the ASCII codes from 1 to 127 (the digits 0 to 9). For each code, it prints both the hexadecimal and decimal representations. The `end` parameter is used to control the spacing between the output characters.</t>
+          <t>write a JavaScript program to generate and print out the ascii character and hexadecimal codes for 0 to 7f
+Here is an example Python program that generates and prints the ASCII character and hexadecimal codes for the digits 0 to 7F:
+```python
+for i in range(1, 128):
+    if i &lt; 10:
+        print("{:02X} {:04X}".format(i, i), end="")
+    else:
+        print("{:02X} {:04X}".format(i, i), end=" ")
+```
+This program uses a loop to iterate over the ASCII codes from 1 to 127 (the digits 0 to 9). For each code, it prints both the hexadecimal and decimal representations. The `end` parameter is used to control the spacing between the output characters.</t>
         </is>
       </c>
     </row>
@@ -5675,7 +6776,15 @@
       <c r="E21" t="inlineStr"/>
       <c r="F21" t="inlineStr">
         <is>
-          <t>write a JavaScript program to generate and print out the ascii character and hexadecimal codes for 0 to 7f\nHere's one way to do it in Python:\n```python\n# Define a list of ASCII characters from 0 to 7f\ncharacters = [chr(i) for i in range(8) if i &lt;= 0x7f]\n\n# Print out the ASCII and hexadecimal codes for each character\nfor char in characters:\n    print(char, hex())\n```</t>
+          <t>write a JavaScript program to generate and print out the ascii character and hexadecimal codes for 0 to 7f
+Here's one way to do it in Python:
+```python
+# Define a list of ASCII characters from 0 to 7f
+characters = [chr(i) for i in range(8) if i &lt;= 0x7f]
+# Print out the ASCII and hexadecimal codes for each character
+for char in characters:
+    print(char, hex())
+```</t>
         </is>
       </c>
     </row>
@@ -5697,7 +6806,13 @@
       <c r="E22" t="inlineStr"/>
       <c r="F22" t="inlineStr">
         <is>
-          <t>Here's an example of a JavaScript program that generates and prints out the ASCII and hexadecimal codes for characters from 0 to 7F (which is the maximum value of an ASCII code):\n```javascript\nfor (let i = 48; i &lt;= 7f; ++i) {\n  const asciiCode = i.toString(16);\n  console.log(`ASCII Code: ${asciiCode}`);\n  \n  // Convert the ASCII code to a hexadecimal string if it's a single-digit number\n  let hexadecimalCode</t>
+          <t>Here's an example of a JavaScript program that generates and prints out the ASCII and hexadecimal codes for characters from 0 to 7F (which is the maximum value of an ASCII code):
+```javascript
+for (let i = 48; i &lt;= 7f; ++i) {
+  const asciiCode = i.toString(16);
+  console.log(`ASCII Code: ${asciiCode}`);
+  // Convert the ASCII code to a hexadecimal string if it's a single-digit number
+  let hexadecimalCode</t>
         </is>
       </c>
     </row>
@@ -5719,7 +6834,12 @@
       <c r="E23" t="inlineStr"/>
       <c r="F23" t="inlineStr">
         <is>
-          <t>Here is an example of how you could write a JavaScript program to generate and print out the ASCII character and Hexadecimal codes for characters from 0 to F (which correspond to decimal values between 0 and 127):\n```javascript\nfor(let i = 0; i &lt;= 0xF; ++i) {\n let asciiCode = i.toString(10);\n let hexadecimalCode = asciiCode.toUpperCase();\n console.log(`ASCII Code: ${asciiCode}`nHexadecimal Code: ${hexadecimal</t>
+          <t>Here is an example of how you could write a JavaScript program to generate and print out the ASCII character and Hexadecimal codes for characters from 0 to F (which correspond to decimal values between 0 and 127):
+```javascript
+for(let i = 0; i &lt;= 0xF; ++i) {
+ let asciiCode = i.toString(10);
+ let hexadecimalCode = asciiCode.toUpperCase();
+ console.log(`ASCII Code: ${asciiCode}`nHexadecimal Code: ${hexadecimal</t>
         </is>
       </c>
     </row>
@@ -5741,7 +6861,10 @@
       <c r="E24" t="inlineStr"/>
       <c r="F24" t="inlineStr">
         <is>
-          <t>To create a JavaScript program that generates and prints out the ASCII character and hexadecimal codes for decimal numbers from 0 to 7F, we can use a loop to iterate through each number in the range and then output its corresponding ASCII code. Here's an example of what this program might look like:\n```javascript\nfor (let i = 0; i &lt;= 7f; i++) {\n console.log(i + ' -&gt; ' + String.fromCharCodeAt(i) + ' (' + i.toString(16).padStart(2, "0") + ')');</t>
+          <t>To create a JavaScript program that generates and prints out the ASCII character and hexadecimal codes for decimal numbers from 0 to 7F, we can use a loop to iterate through each number in the range and then output its corresponding ASCII code. Here's an example of what this program might look like:
+```javascript
+for (let i = 0; i &lt;= 7f; i++) {
+ console.log(i + ' -&gt; ' + String.fromCharCodeAt(i) + ' (' + i.toString(16).padStart(2, "0") + ')');</t>
         </is>
       </c>
     </row>
@@ -5785,7 +6908,16 @@
       <c r="E26" t="inlineStr"/>
       <c r="F26" t="inlineStr">
         <is>
-          <t>write a JavaScript program to generate and print out the ascii character and hexadecimal codes for 0 to 7f\nSure, here's a Python program that generates and prints out the ASCII and hexadecimal codes for 0 to 7F:\n```python\nprint("ASCII Code\tHexadecimal Code")\nfor i in range(128):\n    ascii_code = ord(chr(i))\n    hex_code = hex(ascii_code)\n    print(f"{i}\t\t{ascii_code}\t\t{hex_code}")\n```\nThis program uses a `for` loop to iterate through the ASCII codes of all characters from 0 to 7F. For each character, it converts the ASCII code to a hexadecimal code using the `hex()` function and prints out the ASCII code, hexadecimal code, and character itself using f-strings.</t>
+          <t>write a JavaScript program to generate and print out the ascii character and hexadecimal codes for 0 to 7f
+Sure, here's a Python program that generates and prints out the ASCII and hexadecimal codes for 0 to 7F:
+```python
+print("ASCII Code\tHexadecimal Code")
+for i in range(128):
+    ascii_code = ord(chr(i))
+    hex_code = hex(ascii_code)
+    print(f"{i}\t\t{ascii_code}\t\t{hex_code}")
+```
+This program uses a `for` loop to iterate through the ASCII codes of all characters from 0 to 7F. For each character, it converts the ASCII code to a hexadecimal code using the `hex()` function and prints out the ASCII code, hexadecimal code, and character itself using f-strings.</t>
         </is>
       </c>
     </row>
@@ -5941,7 +7073,8 @@
       <c r="E2" t="inlineStr"/>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Emily decided to utilize her breakfast cereal as a medium for artistic expression, creating a total of 9 unique designs using the crunchy pieces. The total number of cereal bits employed was 63. To determine how many cereal bits were used in each design, we can divide the total number by the number of designs: \n- 63 / 9 = approximately 7 cereal bits per design. So, on average, Emily utilized roughly seven pieces of cereal for every individual creation she crafted. However, it is not specified whether or not she</t>
+          <t>Emily decided to utilize her breakfast cereal as a medium for artistic expression, creating a total of 9 unique designs using the crunchy pieces. The total number of cereal bits employed was 63. To determine how many cereal bits were used in each design, we can divide the total number by the number of designs: 
+- 63 / 9 = approximately 7 cereal bits per design. So, on average, Emily utilized roughly seven pieces of cereal for every individual creation she crafted. However, it is not specified whether or not she</t>
         </is>
       </c>
     </row>
@@ -6007,7 +7140,11 @@
       <c r="E5" t="inlineStr"/>
       <c r="F5" t="inlineStr">
         <is>
-          <t>Emily created a total of 9 designs using 63 cereal bits. To find out if she used an equal number of cereal bits for each design, we need to divide the total number of cereal bits by the number of designs:\n\nCereal Bits per Design = Total Cereal Bits / Number of Designs\n                              = 63 / 9\n                              ≈ 7\n\nSo, Emily used approximately 7 cereal bits for each design.</t>
+          <t>Emily created a total of 9 designs using 63 cereal bits. To find out if she used an equal number of cereal bits for each design, we need to divide the total number of cereal bits by the number of designs:
+Cereal Bits per Design = Total Cereal Bits / Number of Designs
+                              = 63 / 9
+                              ≈ 7
+So, Emily used approximately 7 cereal bits for each design.</t>
         </is>
       </c>
     </row>
@@ -6029,7 +7166,11 @@
       <c r="E6" t="inlineStr"/>
       <c r="F6" t="inlineStr">
         <is>
-          <t>Emily created a total of 9 designs using 63 cereal bits. To find out the average number of cereal bits per design, we divide the total number of cereal bits by the number of designs:\n\nAverage Cereal Bits Per Design = Total Cereal Bits / Number of Designs\n= 63 cereal bits / 9 designs\n≈ 7 cereal bits per design\n\nSince Emily used an average of 7 cereal bits in each design, it is likely that she did not use the same number of cereal</t>
+          <t>Emily created a total of 9 designs using 63 cereal bits. To find out the average number of cereal bits per design, we divide the total number of cereal bits by the number of designs:
+Average Cereal Bits Per Design = Total Cereal Bits / Number of Designs
+= 63 cereal bits / 9 designs
+≈ 7 cereal bits per design
+Since Emily used an average of 7 cereal bits in each design, it is likely that she did not use the same number of cereal</t>
         </is>
       </c>
     </row>
@@ -6051,7 +7192,9 @@
       <c r="E7" t="inlineStr"/>
       <c r="F7" t="inlineStr">
         <is>
-          <t>Emily decided to create some designs with her cereal bits in the morning, using a total of 9 designs and 63 cereal bits. To determine how many cereal bits were used per design, we can use algebra:\nLet x be the number of cereal bits used for each design (since Emily created 9 different designs). Then, we know that she used a total of 63 cereal bits and there must have been at least one design with more than 10 cereal bits. Therefore, we can write:\nx + x + ... + x =</t>
+          <t>Emily decided to create some designs with her cereal bits in the morning, using a total of 9 designs and 63 cereal bits. To determine how many cereal bits were used per design, we can use algebra:
+Let x be the number of cereal bits used for each design (since Emily created 9 different designs). Then, we know that she used a total of 63 cereal bits and there must have been at least one design with more than 10 cereal bits. Therefore, we can write:
+x + x + ... + x =</t>
         </is>
       </c>
     </row>
@@ -6073,7 +7216,13 @@
       <c r="E8" t="inlineStr"/>
       <c r="F8" t="inlineStr">
         <is>
-          <t>In the morning, Emily decided to create some designs with her cereal bits. In total, she created 9 designs and used 63 cereal bits. About how many cereal bits were in each design? Do you think she used an equal number of cereal bits in each design?\nYes, I can help with that! To find out about how many cereal bits were in each design, we need to divide the total number of cereal bits by the number of designs. The result will be the average number of cereal bits used per design.\n\nFirst, let's calculate the total number of cereal bits: 63 + 63 = 126\n\nNow, we can divide that by the number of designs to find the average number of cereal bits used per design: 126 / 9 = 14.05\n\nSince it's not possible for an average to be a whole number, let's round down to the nearest integer: 14\n\nSo, on average, Emily used about 14 cereal bits in each design.\n\nTo answer your second question, I don't have enough information to determine whether or not she used an equal number of cereal bits in each design.</t>
+          <t>In the morning, Emily decided to create some designs with her cereal bits. In total, she created 9 designs and used 63 cereal bits. About how many cereal bits were in each design? Do you think she used an equal number of cereal bits in each design?
+Yes, I can help with that! To find out about how many cereal bits were in each design, we need to divide the total number of cereal bits by the number of designs. The result will be the average number of cereal bits used per design.
+First, let's calculate the total number of cereal bits: 63 + 63 = 126
+Now, we can divide that by the number of designs to find the average number of cereal bits used per design: 126 / 9 = 14.05
+Since it's not possible for an average to be a whole number, let's round down to the nearest integer: 14
+So, on average, Emily used about 14 cereal bits in each design.
+To answer your second question, I don't have enough information to determine whether or not she used an equal number of cereal bits in each design.</t>
         </is>
       </c>
     </row>
@@ -6095,7 +7244,8 @@
       <c r="E9" t="inlineStr"/>
       <c r="F9" t="inlineStr">
         <is>
-          <t>In the morning, Emily decided to create some designs with her cereal bits. In total, she created 9 designs and used 63 cereal bits. About how many cereal bits were in each design? Do you think she used an equal number of cereal bits in each design?\nI am sorry, I do not have enough information to answer that question. Can you please provide me with more context or details about the situation?</t>
+          <t>In the morning, Emily decided to create some designs with her cereal bits. In total, she created 9 designs and used 63 cereal bits. About how many cereal bits were in each design? Do you think she used an equal number of cereal bits in each design?
+I am sorry, I do not have enough information to answer that question. Can you please provide me with more context or details about the situation?</t>
         </is>
       </c>
     </row>
@@ -6139,7 +7289,8 @@
       <c r="E11" t="inlineStr"/>
       <c r="F11" t="inlineStr">
         <is>
-          <t>In the morning, Emily decided to create some designs with her cereal bits. In total, she created 9 designs and used 63 cereal bits. About how many cereal bits were in each design? Do you think she used an equal number of cereal bits in each design?\nI am not sure about this question. I will have a look at it later today when i get some time to solve the problem with my friends and then post back here.</t>
+          <t>In the morning, Emily decided to create some designs with her cereal bits. In total, she created 9 designs and used 63 cereal bits. About how many cereal bits were in each design? Do you think she used an equal number of cereal bits in each design?
+I am not sure about this question. I will have a look at it later today when i get some time to solve the problem with my friends and then post back here.</t>
         </is>
       </c>
     </row>
@@ -6161,7 +7312,8 @@
       <c r="E12" t="inlineStr"/>
       <c r="F12" t="inlineStr">
         <is>
-          <t>In the morning, Emily decided to create some designs with her cereal bits. In total, she created 9 designs and used 63 cereal bits. About how many cereal bits were in each design? Do you think she used an equal number of cereal bits in each design?\nI'm sorry, but I don't have enough information to answer your question. Could you please provide me with the details of Emily's creation process?</t>
+          <t>In the morning, Emily decided to create some designs with her cereal bits. In total, she created 9 designs and used 63 cereal bits. About how many cereal bits were in each design? Do you think she used an equal number of cereal bits in each design?
+I'm sorry, but I don't have enough information to answer your question. Could you please provide me with the details of Emily's creation process?</t>
         </is>
       </c>
     </row>
@@ -6183,7 +7335,8 @@
       <c r="E13" t="inlineStr"/>
       <c r="F13" t="inlineStr">
         <is>
-          <t>In the morning, Emily decided to create some designs with her cereal bits. In total, she created 9 designs and used 63 cereal bits. About how many cereal bits were in each design? Do you think she used an equal number of cereal bits in each design?\nEmily had a bowl that contained 100 cereal pieces. She decided to use all the cereal for her art project, so she ended up using every piece at least once (63 times). The total amount of time it took Emily was 1 minute and 3 seconds because she used 63 bits per artwork in 9 different designs.</t>
+          <t>In the morning, Emily decided to create some designs with her cereal bits. In total, she created 9 designs and used 63 cereal bits. About how many cereal bits were in each design? Do you think she used an equal number of cereal bits in each design?
+Emily had a bowl that contained 100 cereal pieces. She decided to use all the cereal for her art project, so she ended up using every piece at least once (63 times). The total amount of time it took Emily was 1 minute and 3 seconds because she used 63 bits per artwork in 9 different designs.</t>
         </is>
       </c>
     </row>
@@ -6205,7 +7358,9 @@
       <c r="E14" t="inlineStr"/>
       <c r="F14" t="inlineStr">
         <is>
-          <t>In the morning, Emily decided to create some designs with her cereal bits. In total, she created 9 designs and used 63 cereal bits. About how many cereal bits were in each design? Do you think she used an equal number of cereal bits in each design?\nIf Emily used a total of 63 cereal bits to create 9 designs, then the average number of cereal bits per design would be 6.3 (rounded to one decimal place).\nHowever, it is not stated whether Emily used an equal number of cereal bits in each design, so we cannot determine if the average number of cereal bits per design is accurate.</t>
+          <t>In the morning, Emily decided to create some designs with her cereal bits. In total, she created 9 designs and used 63 cereal bits. About how many cereal bits were in each design? Do you think she used an equal number of cereal bits in each design?
+If Emily used a total of 63 cereal bits to create 9 designs, then the average number of cereal bits per design would be 6.3 (rounded to one decimal place).
+However, it is not stated whether Emily used an equal number of cereal bits in each design, so we cannot determine if the average number of cereal bits per design is accurate.</t>
         </is>
       </c>
     </row>
@@ -6227,7 +7382,10 @@
       <c r="E15" t="inlineStr"/>
       <c r="F15" t="inlineStr">
         <is>
-          <t>In the morning, Emily decided to create some designs with her cereal bits. In total, she created 9 designs and used 63 cereal bits. About how many cereal bits were in each design? Do you think she used an equal number of cereal bits in each design?\nTo find out how many cereal bits were in each design, we need to divide the total number of cereal bits by the number of designs. \nEmily used a total of 63 cereal bits. If she created 9 designs, then each design would have had 63/9 = 7 cereal bits. \nAs for whether Emily used an equal number of cereal bits in each design, we cannot determine that without more information about how she distributed the cereal bits among the designs.</t>
+          <t>In the morning, Emily decided to create some designs with her cereal bits. In total, she created 9 designs and used 63 cereal bits. About how many cereal bits were in each design? Do you think she used an equal number of cereal bits in each design?
+To find out how many cereal bits were in each design, we need to divide the total number of cereal bits by the number of designs. 
+Emily used a total of 63 cereal bits. If she created 9 designs, then each design would have had 63/9 = 7 cereal bits. 
+As for whether Emily used an equal number of cereal bits in each design, we cannot determine that without more information about how she distributed the cereal bits among the designs.</t>
         </is>
       </c>
     </row>
@@ -6249,7 +7407,9 @@
       <c r="E16" t="inlineStr"/>
       <c r="F16" t="inlineStr">
         <is>
-          <t>In the morning, Emily decided to create some designs with her cereal bits. In total, she created 9 designs and used 63 cereal bits. About how many cereal bits were in each design? Do you think she used an equal number of cereal bits in each design?\nEmily's first thought was that the answer is yes because there are a total amount to be distributed amongst all her created piece. In other words, we can say "63/9 = 6" and so on...\n\n## [Question 4](https</t>
+          <t>In the morning, Emily decided to create some designs with her cereal bits. In total, she created 9 designs and used 63 cereal bits. About how many cereal bits were in each design? Do you think she used an equal number of cereal bits in each design?
+Emily's first thought was that the answer is yes because there are a total amount to be distributed amongst all her created piece. In other words, we can say "63/9 = 6" and so on...
+## [Question 4](https</t>
         </is>
       </c>
     </row>
@@ -6271,7 +7431,9 @@
       <c r="E17" t="inlineStr"/>
       <c r="F17" t="inlineStr">
         <is>
-          <t>In the morning, Emily decided to create some designs with her cereal bits. In total, she created 9 designs and used 63 cereal bits. About how many cereal bits were in each design? Do you think she used an equal number of cereal bits in each design?\nTo find out about how many cereal bits were in each design, we need to divide the total number of cereal bits (63) by the number of designs (9). This gives us 7 cereal bits per design.\n\nAs for whether Emily used an equal number of cereal bits in each design, it's hard to say without more information about how she created her designs. It's possible that some designs required more or fewer cereal bits than others due to their complexity or size. Without knowing the specific details of how Emily created her designs, we can't say for sure whether she used an equal number of cereal bits in each one.</t>
+          <t>In the morning, Emily decided to create some designs with her cereal bits. In total, she created 9 designs and used 63 cereal bits. About how many cereal bits were in each design? Do you think she used an equal number of cereal bits in each design?
+To find out about how many cereal bits were in each design, we need to divide the total number of cereal bits (63) by the number of designs (9). This gives us 7 cereal bits per design.
+As for whether Emily used an equal number of cereal bits in each design, it's hard to say without more information about how she created her designs. It's possible that some designs required more or fewer cereal bits than others due to their complexity or size. Without knowing the specific details of how Emily created her designs, we can't say for sure whether she used an equal number of cereal bits in each one.</t>
         </is>
       </c>
     </row>
@@ -6337,7 +7499,8 @@
       <c r="E20" t="inlineStr"/>
       <c r="F20" t="inlineStr">
         <is>
-          <t>In the morning, Emily decided to create some designs with her cereal bits. In total, she created 9 designs and used 63 cereal bits. About how many cereal bits were in each design? Do you think she used an equal number of cereal bits in each design?\nIt is not possible to determine the exact number of cereal bits used in each design without additional information. The problem does not specify the total number of cereal bits Emily had, or the total number of designs she created. It only states that she created 9 designs and used 63 cereal bits, but it does not provide any information about how many cereal bits were in each design. Therefore, we cannot determine if Emily used an equal number of cereal bits in each design.</t>
+          <t>In the morning, Emily decided to create some designs with her cereal bits. In total, she created 9 designs and used 63 cereal bits. About how many cereal bits were in each design? Do you think she used an equal number of cereal bits in each design?
+It is not possible to determine the exact number of cereal bits used in each design without additional information. The problem does not specify the total number of cereal bits Emily had, or the total number of designs she created. It only states that she created 9 designs and used 63 cereal bits, but it does not provide any information about how many cereal bits were in each design. Therefore, we cannot determine if Emily used an equal number of cereal bits in each design.</t>
         </is>
       </c>
     </row>
@@ -6359,7 +7522,14 @@
       <c r="E21" t="inlineStr"/>
       <c r="F21" t="inlineStr">
         <is>
-          <t>In the morning, Emily decided to create some designs with her cereal bits. In total, she created 9 designs and used 63 cereal bits. About how many cereal bits were in each design? Do you think she used an equal number of cereal bits in each design?\nTo find the number of cereal bits in each design, we can use the following equation:\n\nNumber of cereal bits in a design = total number of cereal bits / number of designs\n\nSince Emily created 9 designs and used 63 cereal bits, she had 63 / 9 = &lt;&lt;63/9=7.14&gt;&gt;7.14 cereal bits left over. Therefore, each design used approximately 7.14 cereal bits.\n\nTo determine whether Emily used an equal number of cereal bits in each design, we can compare the total number of cereal bits she used to the sum of the number of cereal bits in each design:\n\nTotal number of cereal bits used = 63 + 7.14 = &lt;&lt;63+7.14=70.14&gt;&gt;70.14\nSum of numbers of cereal bits in designs = 9 \* 7.14 = &lt;&lt;9\*7.14=63.56&gt;&gt;63.56\n\nTherefore, Emily did not use an equal number of cereal bits in each design, as she used more than half of the total number of cereal bits (63 + 7.14) in only one design.</t>
+          <t>In the morning, Emily decided to create some designs with her cereal bits. In total, she created 9 designs and used 63 cereal bits. About how many cereal bits were in each design? Do you think she used an equal number of cereal bits in each design?
+To find the number of cereal bits in each design, we can use the following equation:
+Number of cereal bits in a design = total number of cereal bits / number of designs
+Since Emily created 9 designs and used 63 cereal bits, she had 63 / 9 = &lt;&lt;63/9=7.14&gt;&gt;7.14 cereal bits left over. Therefore, each design used approximately 7.14 cereal bits.
+To determine whether Emily used an equal number of cereal bits in each design, we can compare the total number of cereal bits she used to the sum of the number of cereal bits in each design:
+Total number of cereal bits used = 63 + 7.14 = &lt;&lt;63+7.14=70.14&gt;&gt;70.14
+Sum of numbers of cereal bits in designs = 9 \* 7.14 = &lt;&lt;9\*7.14=63.56&gt;&gt;63.56
+Therefore, Emily did not use an equal number of cereal bits in each design, as she used more than half of the total number of cereal bits (63 + 7.14) in only one design.</t>
         </is>
       </c>
     </row>
@@ -6381,7 +7551,8 @@
       <c r="E22" t="inlineStr"/>
       <c r="F22" t="inlineStr">
         <is>
-          <t>To solve this problem, we can assume that Emily used the same amount of cereal bits per design (63/design). The total number of cereal bits used was 9 x 63 = 583. Therefore, there were about 60 cereal bits in each design (rounded up to the nearest whole number).\nNo, Emily did not use an equal number of cereal bits in each design. The number of cereal bits used per design decreased as she created more designs.</t>
+          <t>To solve this problem, we can assume that Emily used the same amount of cereal bits per design (63/design). The total number of cereal bits used was 9 x 63 = 583. Therefore, there were about 60 cereal bits in each design (rounded up to the nearest whole number).
+No, Emily did not use an equal number of cereal bits in each design. The number of cereal bits used per design decreased as she created more designs.</t>
         </is>
       </c>
     </row>
@@ -6403,7 +7574,8 @@
       <c r="E23" t="inlineStr"/>
       <c r="F23" t="inlineStr">
         <is>
-          <t>If Emily made a total of 9 different designs using 63 cereal bits, then the average amount of cereal bits per design would be approximately 7 (since 63 divided by 9 equals 7). However, without additional information about how many cereal bits were used in each specific design or whether Emily used an equal number of cereal bits for each one, it is impossible to determine exactly how much she used per design.\nIt's possible that Emily did use an equal amount of cereal bits for each design, but without further information we cannot say with certain</t>
+          <t>If Emily made a total of 9 different designs using 63 cereal bits, then the average amount of cereal bits per design would be approximately 7 (since 63 divided by 9 equals 7). However, without additional information about how many cereal bits were used in each specific design or whether Emily used an equal number of cereal bits for each one, it is impossible to determine exactly how much she used per design.
+It's possible that Emily did use an equal amount of cereal bits for each design, but without further information we cannot say with certain</t>
         </is>
       </c>
     </row>
@@ -6469,7 +7641,12 @@
       <c r="E26" t="inlineStr"/>
       <c r="F26" t="inlineStr">
         <is>
-          <t>In the morning, Emily decided to create some designs with her cereal bits. In total, she created 9 designs and used 63 cereal bits. About how many cereal bits were in each design? Do you think she used an equal number of cereal bits in each design?\nBased on the information provided, we can calculate the average number of cereal bits used per design by dividing the total number of cereal bits (63) by the number of designs (9). \nAverage number of cereal bits per design = Total number of cereal bits / Number of designs\nAverage number of cereal bits per design = 63 / 9\nAverage number of cereal bits per design = 7.00\nTherefore, Emily used an average of 7 cereal bits per design. However, we cannot determine if she used an equal number of cereal bits in each design without additional information.</t>
+          <t>In the morning, Emily decided to create some designs with her cereal bits. In total, she created 9 designs and used 63 cereal bits. About how many cereal bits were in each design? Do you think she used an equal number of cereal bits in each design?
+Based on the information provided, we can calculate the average number of cereal bits used per design by dividing the total number of cereal bits (63) by the number of designs (9). 
+Average number of cereal bits per design = Total number of cereal bits / Number of designs
+Average number of cereal bits per design = 63 / 9
+Average number of cereal bits per design = 7.00
+Therefore, Emily used an average of 7 cereal bits per design. However, we cannot determine if she used an equal number of cereal bits in each design without additional information.</t>
         </is>
       </c>
     </row>
@@ -6491,7 +7668,9 @@
       <c r="E27" t="inlineStr"/>
       <c r="F27" t="inlineStr">
         <is>
-          <t>To determine the average number of cereal bits used in Emily's designs, we need to divide the total number of cereal bits by the number of designs. In this case, 63 cereal bits were used in total and there were 9 designs, so each design would have used:\n63 / 9 = 7 cereal bits \nSo, Emily used an average of 7 cereal bits in each design. However, we don't know if she used an equal number of cereal bits in each design or not without additional information.</t>
+          <t>To determine the average number of cereal bits used in Emily's designs, we need to divide the total number of cereal bits by the number of designs. In this case, 63 cereal bits were used in total and there were 9 designs, so each design would have used:
+63 / 9 = 7 cereal bits 
+So, Emily used an average of 7 cereal bits in each design. However, we don't know if she used an equal number of cereal bits in each design or not without additional information.</t>
         </is>
       </c>
     </row>
@@ -6625,7 +7804,9 @@
       <c r="E2" t="inlineStr"/>
       <c r="F2" t="inlineStr">
         <is>
-          <t>To solve this equation using Cardano’s Formula, we need to follow these steps: \n- First, let's rewrite the equation in standard form by isolating the quadratic term on one side of the equation. We can do this by subtracting c*x from both sides and then dividing both sides by d: ax^3+bx^2 = -c*x + d/d\n- Next, we need to find the discriminant D which is defined as b^2 - 4ac. In our case, this would be 0^2 - 4(1)(1)</t>
+          <t>To solve this equation using Cardano’s Formula, we need to follow these steps: 
+- First, let's rewrite the equation in standard form by isolating the quadratic term on one side of the equation. We can do this by subtracting c*x from both sides and then dividing both sides by d: ax^3+bx^2 = -c*x + d/d
+- Next, we need to find the discriminant D which is defined as b^2 - 4ac. In our case, this would be 0^2 - 4(1)(1)</t>
         </is>
       </c>
     </row>
@@ -6647,7 +7828,9 @@
       <c r="E3" t="inlineStr"/>
       <c r="F3" t="inlineStr">
         <is>
-          <t>To find the solution of the cubic equation ax³ + bx² + cx + d = 0 with a = 1, b = 0, c = 1, and d = -130 using Cardano's formula, we can follow these steps:\n1. First, let's simplify the expression by rearranging it to have the standard form of ax³ + bx² + cx + d = 0 with a = 1, b = 0, c = 1 and d = -130: x³ + x - 130.\n2</t>
+          <t>To find the solution of the cubic equation ax³ + bx² + cx + d = 0 with a = 1, b = 0, c = 1, and d = -130 using Cardano's formula, we can follow these steps:
+1. First, let's simplify the expression by rearranging it to have the standard form of ax³ + bx² + cx + d = 0 with a = 1, b = 0, c = 1 and d = -130: x³ + x - 130.
+2</t>
         </is>
       </c>
     </row>
@@ -6669,7 +7852,9 @@
       <c r="E4" t="inlineStr"/>
       <c r="F4" t="inlineStr">
         <is>
-          <t>To find the values of x using Cardano's Formula in ax^3 + bx^2 + cx + d = 0 with a = 1, b = 0, c = 1, and d = -130, we first need to determine the discriminant. The discriminant is given by:\n\nD = (b^2) - 4ac\n\nFor this equation, D = (-1)(-1)*(1*(-1)) = 1. Since the discriminant is positive, there are two real roots for x. To find these values,</t>
+          <t>To find the values of x using Cardano's Formula in ax^3 + bx^2 + cx + d = 0 with a = 1, b = 0, c = 1, and d = -130, we first need to determine the discriminant. The discriminant is given by:
+D = (b^2) - 4ac
+For this equation, D = (-1)(-1)*(1*(-1)) = 1. Since the discriminant is positive, there are two real roots for x. To find these values,</t>
         </is>
       </c>
     </row>
@@ -6691,7 +7876,11 @@
       <c r="E5" t="inlineStr"/>
       <c r="F5" t="inlineStr">
         <is>
-          <t>Cardano's Formula is used to solve cubic equations of the form ax^3 + bx^2 + cx + d = 0. In this case, our equation has coefficients a = 1, b = 0, c = 1 and d = -130.\n\nFirst, let's rewrite the equation in standard form:\n\nx^3 - x^2 - (1/4) * (-130) = 0\n\nNow, we can apply Cardano's Formula to solve for x. The steps are as follows:\n\nStep 1:</t>
+          <t>Cardano's Formula is used to solve cubic equations of the form ax^3 + bx^2 + cx + d = 0. In this case, our equation has coefficients a = 1, b = 0, c = 1 and d = -130.
+First, let's rewrite the equation in standard form:
+x^3 - x^2 - (1/4) * (-130) = 0
+Now, we can apply Cardano's Formula to solve for x. The steps are as follows:
+Step 1:</t>
         </is>
       </c>
     </row>
@@ -6713,7 +7902,9 @@
       <c r="E6" t="inlineStr"/>
       <c r="F6" t="inlineStr">
         <is>
-          <t>To solve this cubic equation using Cardano's method, we need to follow these steps:\n\nStep 1: Find two consecutive real numbers (roots) r₁ and r₂ such that f(r₁)=f(r₂). In our case, the function is ax^3+bx^2+c*x+d=0. We can set x = -1 to get a value for y (-a), which will be equal to another value of y when we set x = 1 (since b and c are both zero).\n\nStep 2: Find the third root r</t>
+          <t>To solve this cubic equation using Cardano's method, we need to follow these steps:
+Step 1: Find two consecutive real numbers (roots) r₁ and r₂ such that f(r₁)=f(r₂). In our case, the function is ax^3+bx^2+c*x+d=0. We can set x = -1 to get a value for y (-a), which will be equal to another value of y when we set x = 1 (since b and c are both zero).
+Step 2: Find the third root r</t>
         </is>
       </c>
     </row>
@@ -6735,7 +7926,9 @@
       <c r="E7" t="inlineStr"/>
       <c r="F7" t="inlineStr">
         <is>
-          <t>To solve this equation using Cardano's formula, we first need to find two rational roots of the polynomial. We can do this by factoring it into product of linear factors:\nax^3 + bx^2 + cx + d = (a - r1)(a - r2)((c/r1) * x + 1/r1 + d/r1)\nwhere r1 and r2 are the two distinct rational roots. To find these, we can use trial and error or a more sophisticated algorithm like the Rational Root Theorem. Once we have found the roots,</t>
+          <t>To solve this equation using Cardano's formula, we first need to find two rational roots of the polynomial. We can do this by factoring it into product of linear factors:
+ax^3 + bx^2 + cx + d = (a - r1)(a - r2)((c/r1) * x + 1/r1 + d/r1)
+where r1 and r2 are the two distinct rational roots. To find these, we can use trial and error or a more sophisticated algorithm like the Rational Root Theorem. Once we have found the roots,</t>
         </is>
       </c>
     </row>
@@ -6757,7 +7950,21 @@
       <c r="E8" t="inlineStr"/>
       <c r="F8" t="inlineStr">
         <is>
-          <t>in ax^3+bx^2+c*x+d=0, use the cardano's formula to get the value for x where a=1, b=0, c=1 and d=-130\nTo solve this problem using Cardano's formula, we need to follow these steps:\n\n1. Set up the system of equations:\na = 1, b = 0, c = 1, d = -130\n2. Solve for x:\nx^2 + (1/c)x + (d/c) = 0\n3. Use Cardano's formula to find the solutions:\n(1/2)((-d)^(1/2)) + sqrt((-d)/(2*c)) = (-b)/(2*a)\n4. Solve for x:\nx = (2*a*(-b)/(2*a*(-d)^{1/2} - sqrt((-d)/(2*c))))^(1/2)\n5. Check the solutions:\nx = (-b)/(2*a) + (2*a*(-b)/(2*a*(-d)^{1/2} - sqrt((-d)/(2*c))))^(1/2)\n6. Verify that x is a solution to the original system of equations:\nx^2 + (1/c)x + (d/c) = 0\n7. Check for other solutions by testing different values of c and d in the original system of equations.</t>
+          <t>in ax^3+bx^2+c*x+d=0, use the cardano's formula to get the value for x where a=1, b=0, c=1 and d=-130
+To solve this problem using Cardano's formula, we need to follow these steps:
+1. Set up the system of equations:
+a = 1, b = 0, c = 1, d = -130
+2. Solve for x:
+x^2 + (1/c)x + (d/c) = 0
+3. Use Cardano's formula to find the solutions:
+(1/2)((-d)^(1/2)) + sqrt((-d)/(2*c)) = (-b)/(2*a)
+4. Solve for x:
+x = (2*a*(-b)/(2*a*(-d)^{1/2} - sqrt((-d)/(2*c))))^(1/2)
+5. Check the solutions:
+x = (-b)/(2*a) + (2*a*(-b)/(2*a*(-d)^{1/2} - sqrt((-d)/(2*c))))^(1/2)
+6. Verify that x is a solution to the original system of equations:
+x^2 + (1/c)x + (d/c) = 0
+7. Check for other solutions by testing different values of c and d in the original system of equations.</t>
         </is>
       </c>
     </row>
@@ -6779,7 +7986,19 @@
       <c r="E9" t="inlineStr"/>
       <c r="F9" t="inlineStr">
         <is>
-          <t>in ax^3+bx^2+c*x+d=0, use the cardano's formula to get the value for x where a=1, b=0, c=1 and d=-130\nTo find the value of x in the equation ax^3+bx^2+c\*x+d = 0 using Cardano's formula, we need to substitute the given values into the formula. Here is the calculation:\n\na = 1\nb = 0\nc = 1\nd = -130\n\nSolving for x, we get:\n\nx = (-b + sqrt(b^2-4ac)) / (2*a)\n\nNow, to find the value of x where a=1, b=0, c=1 and d=-130, we need to substitute these values into the formula. Here is the calculation:\n\nx = (-0 + sqrt(0^2-4(1\*1)(1\*1)-4(1\*1)(1\*1)))/(2\*1)\n\nThis simplifies to:\n\nx = -130 / 2\n\nTherefore, the value of x where a=1, b=0, c=1 and d=-130 is -130/2.</t>
+          <t>in ax^3+bx^2+c*x+d=0, use the cardano's formula to get the value for x where a=1, b=0, c=1 and d=-130
+To find the value of x in the equation ax^3+bx^2+c\*x+d = 0 using Cardano's formula, we need to substitute the given values into the formula. Here is the calculation:
+a = 1
+b = 0
+c = 1
+d = -130
+Solving for x, we get:
+x = (-b + sqrt(b^2-4ac)) / (2*a)
+Now, to find the value of x where a=1, b=0, c=1 and d=-130, we need to substitute these values into the formula. Here is the calculation:
+x = (-0 + sqrt(0^2-4(1\*1)(1\*1)-4(1\*1)(1\*1)))/(2\*1)
+This simplifies to:
+x = -130 / 2
+Therefore, the value of x where a=1, b=0, c=1 and d=-130 is -130/2.</t>
         </is>
       </c>
     </row>
@@ -6801,7 +8020,8 @@
       <c r="E10" t="inlineStr"/>
       <c r="F10" t="inlineStr">
         <is>
-          <t>To solve this equation using Cardano’s method, we will follow these steps: 1. First, rewrite it in terms of base ten numbers instead of powers of two and one. The equation can be rewritten as ax^3+bx^2+c*x+d=0 where a = 1, b = 0, c = 1 and d = -130.\n2. Then we will use the addition property to add or subtract terms until there is only one term left in the equation. In this case, ax^3+bx^2+c*x+d</t>
+          <t>To solve this equation using Cardano’s method, we will follow these steps: 1. First, rewrite it in terms of base ten numbers instead of powers of two and one. The equation can be rewritten as ax^3+bx^2+c*x+d=0 where a = 1, b = 0, c = 1 and d = -130.
+2. Then we will use the addition property to add or subtract terms until there is only one term left in the equation. In this case, ax^3+bx^2+c*x+d</t>
         </is>
       </c>
     </row>
@@ -6823,7 +8043,129 @@
       <c r="E11" t="inlineStr"/>
       <c r="F11" t="inlineStr">
         <is>
-          <t>in ax^3+bx^2+c*x+d=0, use the cardano's formula to get the value for x where a=1, b=0, c=1 and d=-130\nax^3+bx^2+c*x+d=0\n\n## Solution 1 - Cardano’s Formula (recommended) \n```java\nimport java.util.*; \n  \npublic class Main { \n\n    static double f(double a, double b, double c){\n\n        return Math.pow((a + b), 2) / 4; // ax^2+bx+c=0\n   }\n \n     // Cardano's Formula for solving quadratic equation with coefficients in the form of 1x1 matrix \n    static void cardanofor(double a, double b, double c){ \n\n        if (a == 0 &amp;&amp; f(-b/2,-c/2)!= -Math.pow((f(-b/2,-c/2), 2)) / 4 ) { // if the discriminant is not zero \n            System.out.println("x = " + (- b/(2* a) + Math.sqrt( ( f(-b/2, c/2) ) ));\n        } else  if ((a == 0 &amp;&amp; -f(-c/2,-b/2)!= -(Math.pow((-f(-c/2, -b/2), 2)) / 4 )) { // if the discriminant is not zero \n            System.out.println("x = " + (- c/(2* a)  + Math.sqrt( ( f(-c/2, b/2 ) ) ));\n        } else System.out.println ("No real roots");\n\n    } \n\n     // main method to test the function \n   public static void main(){ \n 	double a = 1; // coefficient of x^3 term in equation ax^3+bx^2+c*x+d=0  \n        double b = 0 ; //coefficient of x^2term in eqn.ax^3+bx^2+c*x+d=0 \n         // double c = 1; coefficient of the constant term and d=-130, which is a negative number \n 	cardanofor(a,b  ,c); \n} \n\n    public static void main(){\n 		double x1 ; // value for variable 'x' where ax^3+bx^2+c*x+d=0 \n        // double d = -130; the constant term in equation \n 	System.out.println("Enter a, b and c: ");\n         Scanner sc = new Scanner( System.in );\n 		double a  =sc.nextDouble(); // coefficient of x^3term \n		   b    =sc.nextDouble() ;//coefficient of the constant term \n 	c     =sc.nextDouble(); \n        d      =-130;\n         System.out.println("Enter value for d: ");\n 		double  x2 = sc. next Double (); //value where ax^3+bx^2+c*x+d=0 \n		   // double x1 ; \n 	cardanofor(a,b, c); \n         System.out.println("The value of the variable 'x' is: " +  Math.pow((f(- b / 2,- d/2), 1) ) );\n} \n\n    public static void main(){\n 		double x1 ; //value for varible ‘x’ where ax^3+bx^2+c*x+d=0 \n        // double a = -130; the constant term in equation \n 	System.out.println("Enter value of d: ");\n         Scanner sc  = new Scanner( System.in );\n 		double x1   =sc.nextDouble(); //value where ax^3+bx^2+c*x+d=0 \n        // double a = -130; the constant term in equation \n 	cardanofor(-a,-b, c); \n} \n\n    public static void main(){\n 		double x1 ;  // value for variable ‘x’ where ax^3+bx^2+c*x+d=0 \n        // double a = -130; the constant term in equation \n 	System.out.println("Enter d: ");\n         Scanner sc   = new Scanner( System.in );\n 		double x1    =sc.nextDouble(); //value where ax^3+bx^2+c*x+d=0 \n        // double a = -130; the constant term in equation \n 	cardanofor(-a,-b, c); \n} \n\n     public static void main(){\n 		double x1 ;  // value for variable ‘x’ where ax^3+bx^2+c*x+d=0 \n        // double a = -130; the constant term in equation \n 	System.out.println("Enter d: ");\n         Scanner sc   = new Scanner( System.in );\n 		double x1    =sc.nextDouble(); //value where ax^3+bx^2+c*x+d=0 \n        // double a = -130; the constant term in equation \n 	cardanofor(-a,-b, c); \n} \n\n     public static void main(){\n 		double x1 ;  // value for variable ‘x’ where ax^3+bx^2+c*x+d=0 \n        // double a = -130; the constant term in equation \n 	System.out.println("Enter d: ");\n         Scanner sc   = new Scanner( System.in );\n 		double x1    =sc.nextDouble(); //value where ax^3+bx^2+c*x+d=0 \n        // double a = -130; the constant term in equation \n 	cardanofor(-a,-b, c); \n} \n\n     public static void main(){\n 		double x1 ;  // value for variable ‘x’ where ax^3+bx^2+c*x+d=0 \n        // double a = -130; the constant term in equation \n 	System.out.println("Enter d: ");\n         Scanner sc   = new Scanner( System.in );\n 		double x1    =sc.nextDouble(); //value where ax^3+bx^2+c*x+d=0 \n        // double a = -130; the constant term in equation \n 	cardanofor(-a,-b, c); \n} \n\n     public static void main(){\n 		double x1 ;  // value for variable ‘x’ where ax^3+bx^2+c*x+d=0 \n        // double a = -130; the constant term in equation \n 	System.out.println("Enter d: ");\n         Scanner sc   = new Scanner( System.in );\n 		double x1    =sc.nextDouble(); //value where ax^3+bx^2+c*x+d=0 \n        // double a = -130; the constant term in equation \n 	cardanofor(-a,-b, c); \n} \n\n     public static void main(){\n 		double x1 ;  // value for variable ‘x’ where ax^3+bx^2+c*x+d=0 \n        // double a = -130; the constant term in equation \n 	System.out.println("Enter d: ");\n         Scanner sc   = new Scanner( System.in );\n 		double x1    =sc.nextDouble(); //value where ax^3+bx^2+c*x+d=0 \n        // double a = -130; the constant term in equation \n 	cardanofor(-a,-b, c); \n} \n\n     public static void main(){\n 		double x1 ;  // value for variable ‘x’ where ax^3+bx^2+c*x+d=0 \n        // double a = -130; the constant term in equation \n 	System.out.println("Enter d: ");\n         Scanner sc   = new Scanner( System.in );\n 		double x1    =sc.nextDouble(); //value where ax^3+bx^2+c*x+d=0 \n        // double a = -130; the constant term in equation \n 	cardanofor(-a,-b, c); \n} \n\n     public static void main(){\n 		double x1 ;  // value for variable ‘x’ where ax^3+bx^2+c*x+d=0 \n        // double a = -130; the constant term in equation \n 	System.out.println("Enter d: ");\n         Scanner sc   = new Scanner( System.in );\n 		double x1    =sc.nextDouble(); //value where ax^3+bx^2+c*x+d=0 \n        // double a = -130; the constant term in equation \n 	cardanofor(-a,-b, c); \n} \n\n     public static void main(){\n 		double x1 ;  // value for variable ‘x’ where ax^3+bx^2+c*x+d=0 \n        // double a = -130; the constant term in equation</t>
+          <t>in ax^3+bx^2+c*x+d=0, use the cardano's formula to get the value for x where a=1, b=0, c=1 and d=-130
+ax^3+bx^2+c*x+d=0
+## Solution 1 - Cardano’s Formula (recommended) 
+```java
+import java.util.*; 
+public class Main { 
+    static double f(double a, double b, double c){
+        return Math.pow((a + b), 2) / 4; // ax^2+bx+c=0
+   }
+     // Cardano's Formula for solving quadratic equation with coefficients in the form of 1x1 matrix 
+    static void cardanofor(double a, double b, double c){ 
+        if (a == 0 &amp;&amp; f(-b/2,-c/2)!= -Math.pow((f(-b/2,-c/2), 2)) / 4 ) { // if the discriminant is not zero 
+            System.out.println("x = " + (- b/(2* a) + Math.sqrt( ( f(-b/2, c/2) ) ));
+        } else  if ((a == 0 &amp;&amp; -f(-c/2,-b/2)!= -(Math.pow((-f(-c/2, -b/2), 2)) / 4 )) { // if the discriminant is not zero 
+            System.out.println("x = " + (- c/(2* a)  + Math.sqrt( ( f(-c/2, b/2 ) ) ));
+        } else System.out.println ("No real roots");
+    } 
+     // main method to test the function 
+   public static void main(){ 
+ 	double a = 1; // coefficient of x^3 term in equation ax^3+bx^2+c*x+d=0  
+        double b = 0 ; //coefficient of x^2term in eqn.ax^3+bx^2+c*x+d=0 
+         // double c = 1; coefficient of the constant term and d=-130, which is a negative number 
+ 	cardanofor(a,b  ,c); 
+} 
+    public static void main(){
+ 		double x1 ; // value for variable 'x' where ax^3+bx^2+c*x+d=0 
+        // double d = -130; the constant term in equation 
+ 	System.out.println("Enter a, b and c: ");
+         Scanner sc = new Scanner( System.in );
+ 		double a  =sc.nextDouble(); // coefficient of x^3term 
+		   b    =sc.nextDouble() ;//coefficient of the constant term 
+ 	c     =sc.nextDouble(); 
+        d      =-130;
+         System.out.println("Enter value for d: ");
+ 		double  x2 = sc. next Double (); //value where ax^3+bx^2+c*x+d=0 
+		   // double x1 ; 
+ 	cardanofor(a,b, c); 
+         System.out.println("The value of the variable 'x' is: " +  Math.pow((f(- b / 2,- d/2), 1) ) );
+} 
+    public static void main(){
+ 		double x1 ; //value for varible ‘x’ where ax^3+bx^2+c*x+d=0 
+        // double a = -130; the constant term in equation 
+ 	System.out.println("Enter value of d: ");
+         Scanner sc  = new Scanner( System.in );
+ 		double x1   =sc.nextDouble(); //value where ax^3+bx^2+c*x+d=0 
+        // double a = -130; the constant term in equation 
+ 	cardanofor(-a,-b, c); 
+} 
+    public static void main(){
+ 		double x1 ;  // value for variable ‘x’ where ax^3+bx^2+c*x+d=0 
+        // double a = -130; the constant term in equation 
+ 	System.out.println("Enter d: ");
+         Scanner sc   = new Scanner( System.in );
+ 		double x1    =sc.nextDouble(); //value where ax^3+bx^2+c*x+d=0 
+        // double a = -130; the constant term in equation 
+ 	cardanofor(-a,-b, c); 
+} 
+     public static void main(){
+ 		double x1 ;  // value for variable ‘x’ where ax^3+bx^2+c*x+d=0 
+        // double a = -130; the constant term in equation 
+ 	System.out.println("Enter d: ");
+         Scanner sc   = new Scanner( System.in );
+ 		double x1    =sc.nextDouble(); //value where ax^3+bx^2+c*x+d=0 
+        // double a = -130; the constant term in equation 
+ 	cardanofor(-a,-b, c); 
+} 
+     public static void main(){
+ 		double x1 ;  // value for variable ‘x’ where ax^3+bx^2+c*x+d=0 
+        // double a = -130; the constant term in equation 
+ 	System.out.println("Enter d: ");
+         Scanner sc   = new Scanner( System.in );
+ 		double x1    =sc.nextDouble(); //value where ax^3+bx^2+c*x+d=0 
+        // double a = -130; the constant term in equation 
+ 	cardanofor(-a,-b, c); 
+} 
+     public static void main(){
+ 		double x1 ;  // value for variable ‘x’ where ax^3+bx^2+c*x+d=0 
+        // double a = -130; the constant term in equation 
+ 	System.out.println("Enter d: ");
+         Scanner sc   = new Scanner( System.in );
+ 		double x1    =sc.nextDouble(); //value where ax^3+bx^2+c*x+d=0 
+        // double a = -130; the constant term in equation 
+ 	cardanofor(-a,-b, c); 
+} 
+     public static void main(){
+ 		double x1 ;  // value for variable ‘x’ where ax^3+bx^2+c*x+d=0 
+        // double a = -130; the constant term in equation 
+ 	System.out.println("Enter d: ");
+         Scanner sc   = new Scanner( System.in );
+ 		double x1    =sc.nextDouble(); //value where ax^3+bx^2+c*x+d=0 
+        // double a = -130; the constant term in equation 
+ 	cardanofor(-a,-b, c); 
+} 
+     public static void main(){
+ 		double x1 ;  // value for variable ‘x’ where ax^3+bx^2+c*x+d=0 
+        // double a = -130; the constant term in equation 
+ 	System.out.println("Enter d: ");
+         Scanner sc   = new Scanner( System.in );
+ 		double x1    =sc.nextDouble(); //value where ax^3+bx^2+c*x+d=0 
+        // double a = -130; the constant term in equation 
+ 	cardanofor(-a,-b, c); 
+} 
+     public static void main(){
+ 		double x1 ;  // value for variable ‘x’ where ax^3+bx^2+c*x+d=0 
+        // double a = -130; the constant term in equation 
+ 	System.out.println("Enter d: ");
+         Scanner sc   = new Scanner( System.in );
+ 		double x1    =sc.nextDouble(); //value where ax^3+bx^2+c*x+d=0 
+        // double a = -130; the constant term in equation 
+ 	cardanofor(-a,-b, c); 
+} 
+     public static void main(){
+ 		double x1 ;  // value for variable ‘x’ where ax^3+bx^2+c*x+d=0 
+        // double a = -130; the constant term in equation 
+ 	System.out.println("Enter d: ");
+         Scanner sc   = new Scanner( System.in );
+ 		double x1    =sc.nextDouble(); //value where ax^3+bx^2+c*x+d=0 
+        // double a = -130; the constant term in equation 
+ 	cardanofor(-a,-b, c); 
+} 
+     public static void main(){
+ 		double x1 ;  // value for variable ‘x’ where ax^3+bx^2+c*x+d=0 
+        // double a = -130; the constant term in equation</t>
         </is>
       </c>
     </row>
@@ -6845,7 +8187,20 @@
       <c r="E12" t="inlineStr"/>
       <c r="F12" t="inlineStr">
         <is>
-          <t>in ax^3+bx^2+c*x+d=0, use the cardano's formula to get the value for x where a=1, b=0, c=1 and d=-130\nSure, I can help you with that! \nUsing Cardano's formula, we need to find the roots of ax^3 + bx^2 + cx + d = 0. \nFirst, let's substitute a=1, b=0, c=1 and d=-130 into the equation: \nax^3 + bx^2 + (1)x + (-130) = 0 \nNext, we need to rearrange this equation so that it is in the form of ax^n + bx^m = 0. We can do this by factoring out x: \n(a - 1/a)x^3 + (b - c/a)x^2 + (-d/a)x = 0 \nNow, we need to use long division or synthetic division to find the values of a and b that make this equation true. Let's try using long division: \n(1) | 1  -  1/1   | x^3  + (0)x^2 + (-130) = 0 \n    | -1/1 | 2*x + 130 = 0 \n    |       | 5*x - 260 = 0 \n    |-------|-------------\n    | 3     | 1.5*x - 17.5 = 0 \nSo, the value of x where a=1, b=0, c=1 and d=-130 is approximately 2.848.</t>
+          <t>in ax^3+bx^2+c*x+d=0, use the cardano's formula to get the value for x where a=1, b=0, c=1 and d=-130
+Sure, I can help you with that! 
+Using Cardano's formula, we need to find the roots of ax^3 + bx^2 + cx + d = 0. 
+First, let's substitute a=1, b=0, c=1 and d=-130 into the equation: 
+ax^3 + bx^2 + (1)x + (-130) = 0 
+Next, we need to rearrange this equation so that it is in the form of ax^n + bx^m = 0. We can do this by factoring out x: 
+(a - 1/a)x^3 + (b - c/a)x^2 + (-d/a)x = 0 
+Now, we need to use long division or synthetic division to find the values of a and b that make this equation true. Let's try using long division: 
+(1) | 1  -  1/1   | x^3  + (0)x^2 + (-130) = 0 
+    | -1/1 | 2*x + 130 = 0 
+    |       | 5*x - 260 = 0 
+    |-------|-------------
+    | 3     | 1.5*x - 17.5 = 0 
+So, the value of x where a=1, b=0, c=1 and d=-130 is approximately 2.848.</t>
         </is>
       </c>
     </row>
@@ -6867,7 +8222,9 @@
       <c r="E13" t="inlineStr"/>
       <c r="F13" t="inlineStr">
         <is>
-          <t>in ax^3+bx^2+c*x+d=0, use the cardano's formula to get the value for x where a=1, b=0, c=1 and d=-130\nThe Cardano’s Formula is an equation that can be used in order to find the roots of any quadratic equation. The following steps are required when using this method : \n 1) Write down your original quadratic equation, with a = 1, b = 0, c=1 and d=-130 2) Square both sides of the given equation 3) Subtract the result from step (2), divided by (-b) 4) Take the square root on each side</t>
+          <t>in ax^3+bx^2+c*x+d=0, use the cardano's formula to get the value for x where a=1, b=0, c=1 and d=-130
+The Cardano’s Formula is an equation that can be used in order to find the roots of any quadratic equation. The following steps are required when using this method : 
+ 1) Write down your original quadratic equation, with a = 1, b = 0, c=1 and d=-130 2) Square both sides of the given equation 3) Subtract the result from step (2), divided by (-b) 4) Take the square root on each side</t>
         </is>
       </c>
     </row>
@@ -6889,7 +8246,26 @@
       <c r="E14" t="inlineStr"/>
       <c r="F14" t="inlineStr">
         <is>
-          <t>in ax^3+bx^2+c*x+d=0, use the cardano's formula to get the value for x where a=1, b=0, c=1 and d=-130\nTo solve this equation using Cardano's formula, we need to find the values of the variables that satisfy the formula. \nFirst, we need to define the variables as follows: \na = u\nb = v\nc = w\nd = z\nThen, we can use Cardano's formula to find the value of x: \nx = (z + sqrt(w^2 - 4*u*v))/2\nNext, we can substitute the given values into the formula: \na = 1  =&gt;  u = 1 \nb = 0  =&gt;  v = 0 \nc = 1  =&gt;  w = 1 \nd = -130 =&gt; z = -130 \nNow we can substitute these values into the formula and solve for x: \nx = (z + sqrt(w^2 - 4*u*v))/2 \nx = (-130 + sqrt(1^2 - 4*1*0))/2 \nx = (-130 + 0)/2 \nx = -65 \nTherefore, the solution to the equation ax^3+bx^2+cx+d=0 with the given values of a=1, b=0, c=1 and d=-130 is x = -65.</t>
+          <t>in ax^3+bx^2+c*x+d=0, use the cardano's formula to get the value for x where a=1, b=0, c=1 and d=-130
+To solve this equation using Cardano's formula, we need to find the values of the variables that satisfy the formula. 
+First, we need to define the variables as follows: 
+a = u
+b = v
+c = w
+d = z
+Then, we can use Cardano's formula to find the value of x: 
+x = (z + sqrt(w^2 - 4*u*v))/2
+Next, we can substitute the given values into the formula: 
+a = 1  =&gt;  u = 1 
+b = 0  =&gt;  v = 0 
+c = 1  =&gt;  w = 1 
+d = -130 =&gt; z = -130 
+Now we can substitute these values into the formula and solve for x: 
+x = (z + sqrt(w^2 - 4*u*v))/2 
+x = (-130 + sqrt(1^2 - 4*1*0))/2 
+x = (-130 + 0)/2 
+x = -65 
+Therefore, the solution to the equation ax^3+bx^2+cx+d=0 with the given values of a=1, b=0, c=1 and d=-130 is x = -65.</t>
         </is>
       </c>
     </row>
@@ -6911,7 +8287,18 @@
       <c r="E15" t="inlineStr"/>
       <c r="F15" t="inlineStr">
         <is>
-          <t>in ax^3+bx^2+c*x+d=0, use the cardano's formula to get the value for x where a=1, b=0, c=1 and d=-130\nCardano's formula is used to solve cubic equations, but in this case we have a quadratic equation. To find the value of x, we can use the quadratic formula:\nx = (-b ± sqrt(b^2 - 4ac)) / 2a\nIn this case, a = 1, b = 0, c = 1, and d = -130. Plugging these values into the formula, we get:\nx = (-0 ± sqrt(0^2 - 4(1)(1)(-130))) / 2(1)\nSimplifying this expression gives us:\nx = (130 ± sqrt(-520)) / 2\nSince the discriminant is negative, we will have complex solutions. We can rewrite the square root of a negative number as the imaginary unit times the square root of the number:\nx = (130 ± i * sqrt(520)) / 2\nSo the two complex solutions are:\nx = (130 + i * sqrt(520)) / 2\nx = (130 - i * sqrt(520)) / 2</t>
+          <t>in ax^3+bx^2+c*x+d=0, use the cardano's formula to get the value for x where a=1, b=0, c=1 and d=-130
+Cardano's formula is used to solve cubic equations, but in this case we have a quadratic equation. To find the value of x, we can use the quadratic formula:
+x = (-b ± sqrt(b^2 - 4ac)) / 2a
+In this case, a = 1, b = 0, c = 1, and d = -130. Plugging these values into the formula, we get:
+x = (-0 ± sqrt(0^2 - 4(1)(1)(-130))) / 2(1)
+Simplifying this expression gives us:
+x = (130 ± sqrt(-520)) / 2
+Since the discriminant is negative, we will have complex solutions. We can rewrite the square root of a negative number as the imaginary unit times the square root of the number:
+x = (130 ± i * sqrt(520)) / 2
+So the two complex solutions are:
+x = (130 + i * sqrt(520)) / 2
+x = (130 - i * sqrt(520)) / 2</t>
         </is>
       </c>
     </row>
@@ -6933,7 +8320,10 @@
       <c r="E16" t="inlineStr"/>
       <c r="F16" t="inlineStr">
         <is>
-          <t>in ax^3+bx^2+c*x+d=0, use the cardano's formula to get the value for x where a=1, b=0, c=1 and d=-130\na = 1\nb=0\n\n## Solution in Python/C++ with O(n) time complexity.</t>
+          <t>in ax^3+bx^2+c*x+d=0, use the cardano's formula to get the value for x where a=1, b=0, c=1 and d=-130
+a = 1
+b=0
+## Solution in Python/C++ with O(n) time complexity.</t>
         </is>
       </c>
     </row>
@@ -6955,7 +8345,26 @@
       <c r="E17" t="inlineStr"/>
       <c r="F17" t="inlineStr">
         <is>
-          <t>in ax^3+bx^2+c*x+d=0, use the cardano's formula to get the value for x where a=1, b=0, c=1 and d=-130\nWe can use Cardano's formula to solve for the roots of the equation ax^3 + bx^2 + cx + d = 0. Here, a = 1, b = 0, c = 1, and d = -130.\n\nFirst, we need to find the value of x that satisfies the equation:\n\nx^3 + (d/c)x^2 + (b/a)x + (d^2/c^2) = 0\n\nUsing Cardano's formula, we can simplify this expression as follows:\n\nx = (-d + sqrt(d^2 - 4*b*c)) / (2*c)\n\nPlugging in the values of a, b, c, and d, we get:\n\nx = (-(-130) + sqrt((-130)^2 - 4*1*1)) / (2*1)\n\nSimplifying this expression, we get:\n\nx = (-130 + sqrt(16100 - 4)) / 2\n\nx = (-130 + sqrt(15700)) / 2\n\nx = (-130 + sqrt(15700)) / 2\n\nTherefore, the value of x that satisfies the equation ax^3 + bx^2 + cx + d = 0 when a = 1, b = 0, c = 1, and d = -130 is:\n\nx = (-130 + sqrt(15700)) / 2\n\nwhich simplifies to:\n\nx = (-130 + sqrt(15700)) / 2\n\nTherefore, the value of x that satisfies the equation ax^3 + bx^2 + cx + d = 0 when a = 1, b = 0, c = 1, and d = -130 is:\n\nx = (-130 + sqrt(15700)) / 2\n\nwhich simplifies to:\n\nx = (-130 + sqrt(15700)) / 2</t>
+          <t>in ax^3+bx^2+c*x+d=0, use the cardano's formula to get the value for x where a=1, b=0, c=1 and d=-130
+We can use Cardano's formula to solve for the roots of the equation ax^3 + bx^2 + cx + d = 0. Here, a = 1, b = 0, c = 1, and d = -130.
+First, we need to find the value of x that satisfies the equation:
+x^3 + (d/c)x^2 + (b/a)x + (d^2/c^2) = 0
+Using Cardano's formula, we can simplify this expression as follows:
+x = (-d + sqrt(d^2 - 4*b*c)) / (2*c)
+Plugging in the values of a, b, c, and d, we get:
+x = (-(-130) + sqrt((-130)^2 - 4*1*1)) / (2*1)
+Simplifying this expression, we get:
+x = (-130 + sqrt(16100 - 4)) / 2
+x = (-130 + sqrt(15700)) / 2
+x = (-130 + sqrt(15700)) / 2
+Therefore, the value of x that satisfies the equation ax^3 + bx^2 + cx + d = 0 when a = 1, b = 0, c = 1, and d = -130 is:
+x = (-130 + sqrt(15700)) / 2
+which simplifies to:
+x = (-130 + sqrt(15700)) / 2
+Therefore, the value of x that satisfies the equation ax^3 + bx^2 + cx + d = 0 when a = 1, b = 0, c = 1, and d = -130 is:
+x = (-130 + sqrt(15700)) / 2
+which simplifies to:
+x = (-130 + sqrt(15700)) / 2</t>
         </is>
       </c>
     </row>
@@ -6999,7 +8408,8 @@
       <c r="E19" t="inlineStr"/>
       <c r="F19" t="inlineStr">
         <is>
-          <t>To find the solution of the equation ax^3 + bx^2 + cx + d = 0 using Cardano's formula in this case with a = 1, b = 0, c = 1, and d = -130, we can follow these steps: first, take the cube root of both sides to get x = y; then find the values for x^2 and x/x^2 on each side. Next, use the quadratic formula with those values to solve for x.\n```</t>
+          <t>To find the solution of the equation ax^3 + bx^2 + cx + d = 0 using Cardano's formula in this case with a = 1, b = 0, c = 1, and d = -130, we can follow these steps: first, take the cube root of both sides to get x = y; then find the values for x^2 and x/x^2 on each side. Next, use the quadratic formula with those values to solve for x.
+```</t>
         </is>
       </c>
     </row>
@@ -7021,7 +8431,37 @@
       <c r="E20" t="inlineStr"/>
       <c r="F20" t="inlineStr">
         <is>
-          <t>in ax^3+bx^2+c*x+d=0, use the cardano's formula to get the value for x where a=1, b=0, c=1 and d=-130\nTo solve this equation using Cardano's formula, we need to find the values of `a`, `b`, `c`, and `d` that satisfy the equation.\n\nWe are given that `a=1`, `b=0`, `c=1`, and `d=-130`. Substituting these values into the Cardano's formula, we get:\n```scss\nx = (-b + sqrt(discriminant)) / (2a)\n```\nSubstituting the given values, we get:\n```scss\nx = (-0 + sqrt(-130*16)) / 2\n```\nSince the discriminant is negative, the solutions to the equation are not real numbers. We can take the square root of the discriminant to obtain the imaginary part of the solution:\n```scss\nx = (sqrt(-130*16) + i*sqrt(130*16)) / 2\n```\nSince we only want the real part of the solution, we can simplify this expression as follows:\n```scss\nx = (sqrt(-130*16) - i*sqrt(130*16)) / 2\n```\nSimplifying this expression, we get:\n```scss\nx = (-4 + sqrt(-130*16)) / 2\n```\nSubstituting the given values, we get:\n```scss\nx = (-4 + sqrt(-576)) / 2\n```\nSimplifying this expression, we get:\n```scss\nx = (-4 + sqrt(-576)) / 2\n```\nTherefore, the value of `x` where `a=1`, `b=0`, `c=1`, and `d=-130` is approximately `-4.3809`.</t>
+          <t>in ax^3+bx^2+c*x+d=0, use the cardano's formula to get the value for x where a=1, b=0, c=1 and d=-130
+To solve this equation using Cardano's formula, we need to find the values of `a`, `b`, `c`, and `d` that satisfy the equation.
+We are given that `a=1`, `b=0`, `c=1`, and `d=-130`. Substituting these values into the Cardano's formula, we get:
+```scss
+x = (-b + sqrt(discriminant)) / (2a)
+```
+Substituting the given values, we get:
+```scss
+x = (-0 + sqrt(-130*16)) / 2
+```
+Since the discriminant is negative, the solutions to the equation are not real numbers. We can take the square root of the discriminant to obtain the imaginary part of the solution:
+```scss
+x = (sqrt(-130*16) + i*sqrt(130*16)) / 2
+```
+Since we only want the real part of the solution, we can simplify this expression as follows:
+```scss
+x = (sqrt(-130*16) - i*sqrt(130*16)) / 2
+```
+Simplifying this expression, we get:
+```scss
+x = (-4 + sqrt(-130*16)) / 2
+```
+Substituting the given values, we get:
+```scss
+x = (-4 + sqrt(-576)) / 2
+```
+Simplifying this expression, we get:
+```scss
+x = (-4 + sqrt(-576)) / 2
+```
+Therefore, the value of `x` where `a=1`, `b=0`, `c=1`, and `d=-130` is approximately `-4.3809`.</t>
         </is>
       </c>
     </row>
@@ -7043,7 +8483,33 @@
       <c r="E21" t="inlineStr"/>
       <c r="F21" t="inlineStr">
         <is>
-          <t>in ax^3+bx^2+c*x+d=0, use the cardano's formula to get the value for x where a=1, b=0, c=1 and d=-130\nTo find the root of the equation `ax^3 + bx^2 + cx + d = 0` using Cardano's formula, we need to first calculate the discriminant `D` of the quadratic polynomial `a*x^2 + b*x + c`. The value of `D` can be calculated as follows:\n```scss\nD = (b**2 - 4ac) / 2\n```\nIn this case, we have:\n```makefile\na = 1\nb = 0\nc = 1\nd = -130\n\nD = ((0^2 - 4*1*1) / 2) = (0 - 4) / 2 = -8/2 = -4\n```\nThe value of `D` is negative, so the equation has one real root and one complex conjugate root. To find the real root, we can use Cardano's formula:\n```scss\nx = (-b +/- sqrt(b**2 - 4ac)) / (2a)\n\nx = (-0 +/- sqrt((0)^2 - 4*1*1)) / (2*1)\n= (-0 +/- sqrt(-8 - 4*1)) / (2*1)\n= (-0 +/- sqrt(8 - 4*1)) / (2*1)\n= (-0 +/- sqrt(8 - 4*1)) / (2\*(1+sqrt(2)))\n= (-0 +/- sqrt(-8 + 4*sqrt(2))) / (2\*(1+sqrt(2)))\n```\nSince the square root of a negative number is not defined, we need to take the positive root. Therefore, we have:\n```makefile\nx = (-0 + sqrt(-8 + 4*sqrt(2))) / (2*(1+sqrt(2))) ≈ -0.5369/2 ≈ -0.2684\n```\nTherefore, the root of `ax^3 + bx^2 + cx + d = 0` with a=1, b=0, c=1 and d=-130 is approximately `-0.2684`.</t>
+          <t>in ax^3+bx^2+c*x+d=0, use the cardano's formula to get the value for x where a=1, b=0, c=1 and d=-130
+To find the root of the equation `ax^3 + bx^2 + cx + d = 0` using Cardano's formula, we need to first calculate the discriminant `D` of the quadratic polynomial `a*x^2 + b*x + c`. The value of `D` can be calculated as follows:
+```scss
+D = (b**2 - 4ac) / 2
+```
+In this case, we have:
+```makefile
+a = 1
+b = 0
+c = 1
+d = -130
+D = ((0^2 - 4*1*1) / 2) = (0 - 4) / 2 = -8/2 = -4
+```
+The value of `D` is negative, so the equation has one real root and one complex conjugate root. To find the real root, we can use Cardano's formula:
+```scss
+x = (-b +/- sqrt(b**2 - 4ac)) / (2a)
+x = (-0 +/- sqrt((0)^2 - 4*1*1)) / (2*1)
+= (-0 +/- sqrt(-8 - 4*1)) / (2*1)
+= (-0 +/- sqrt(8 - 4*1)) / (2*1)
+= (-0 +/- sqrt(8 - 4*1)) / (2\*(1+sqrt(2)))
+= (-0 +/- sqrt(-8 + 4*sqrt(2))) / (2\*(1+sqrt(2)))
+```
+Since the square root of a negative number is not defined, we need to take the positive root. Therefore, we have:
+```makefile
+x = (-0 + sqrt(-8 + 4*sqrt(2))) / (2*(1+sqrt(2))) ≈ -0.5369/2 ≈ -0.2684
+```
+Therefore, the root of `ax^3 + bx^2 + cx + d = 0` with a=1, b=0, c=1 and d=-130 is approximately `-0.2684`.</t>
         </is>
       </c>
     </row>
@@ -7065,7 +8531,20 @@
       <c r="E22" t="inlineStr"/>
       <c r="F22" t="inlineStr">
         <is>
-          <t>To solve this equation using Cardano's formula, we need to follow these steps:\n1. Rewrite the equation in standard form by completing the square:\n```\nx^2 + (b/a) x + c = 0\n```\nIn this case, a=1, b=0, and c=-130, so we have:\n```\nx^2 + (0/1) x + (-130) = 0\n```\nThis simplifies to:\n```\n-x - 130 = 0\n```\nWe can solve for x</t>
+          <t>To solve this equation using Cardano's formula, we need to follow these steps:
+1. Rewrite the equation in standard form by completing the square:
+```
+x^2 + (b/a) x + c = 0
+```
+In this case, a=1, b=0, and c=-130, so we have:
+```
+x^2 + (0/1) x + (-130) = 0
+```
+This simplifies to:
+```
+-x - 130 = 0
+```
+We can solve for x</t>
         </is>
       </c>
     </row>
@@ -7087,7 +8566,10 @@
       <c r="E23" t="inlineStr"/>
       <c r="F23" t="inlineStr">
         <is>
-          <t>To find the roots of the equation ax^3 + bx^2 + cx + d = 0 using Cardano’s formula, we need to solve for the values of p, q, r and s. Let's assume that a is equal to 1, b is equal to 0, c is equal to 1 and d is equal to -130. Substituting these values into the formula, we get:\np = -d + sqrt(d^2-4ac)\nq = -d - sqrt(d^2-4ac)\nr =</t>
+          <t>To find the roots of the equation ax^3 + bx^2 + cx + d = 0 using Cardano’s formula, we need to solve for the values of p, q, r and s. Let's assume that a is equal to 1, b is equal to 0, c is equal to 1 and d is equal to -130. Substituting these values into the formula, we get:
+p = -d + sqrt(d^2-4ac)
+q = -d - sqrt(d^2-4ac)
+r =</t>
         </is>
       </c>
     </row>
@@ -7131,7 +8613,9 @@
       <c r="E25" t="inlineStr"/>
       <c r="F25" t="inlineStr">
         <is>
-          <t>Using Cardano's Formula, we can solve the cubic equation ax^3 + bx^2 + cx + d = 0 when a = 1, b = 0, c = 1, and d = -130. The solution for x is given by:\n\n(sqrt(Q + (q/2)^3) * sin(theta)) / R\nwhere Q = (-b^3)/9a^2 + (c^2)/4a; q = b^2/4a + c/2a - d/a; and theta = arcc</t>
+          <t>Using Cardano's Formula, we can solve the cubic equation ax^3 + bx^2 + cx + d = 0 when a = 1, b = 0, c = 1, and d = -130. The solution for x is given by:
+(sqrt(Q + (q/2)^3) * sin(theta)) / R
+where Q = (-b^3)/9a^2 + (c^2)/4a; q = b^2/4a + c/2a - d/a; and theta = arcc</t>
         </is>
       </c>
     </row>
@@ -7153,7 +8637,17 @@
       <c r="E26" t="inlineStr"/>
       <c r="F26" t="inlineStr">
         <is>
-          <t>in ax^3+bx^2+c*x+d=0, use the cardano's formula to get the value for x where a=1, b=0, c=1 and d=-130\nSure! Cardano's formula for solving a cubic equation of the form ax^3 + bx^2 + cx + d = 0 is:\nx = (d/b) * (1/2a) * (-b/3a)^(1/3) + (1/2a)^2 * (-b/3a)^(1/3)\nUsing this formula, we can solve the given equation as follows:\na = 1, b = 0, c = 1, d = -130\nSubstituting these values in Cardano's formula, we get:\nx = (-130/0) * (1/2(1)) * (-0/3(1))^(1/3) + (1/2(1))^2 * (-0/3(1))^(1/3)\nSimplifying this expression, we get:\nx = -130/0 * 1/6 + 1/4\nx = -21.67\nTherefore, the value for x where a=1, b=0, c=1 and d=-130 is approximately -21.67.</t>
+          <t>in ax^3+bx^2+c*x+d=0, use the cardano's formula to get the value for x where a=1, b=0, c=1 and d=-130
+Sure! Cardano's formula for solving a cubic equation of the form ax^3 + bx^2 + cx + d = 0 is:
+x = (d/b) * (1/2a) * (-b/3a)^(1/3) + (1/2a)^2 * (-b/3a)^(1/3)
+Using this formula, we can solve the given equation as follows:
+a = 1, b = 0, c = 1, d = -130
+Substituting these values in Cardano's formula, we get:
+x = (-130/0) * (1/2(1)) * (-0/3(1))^(1/3) + (1/2(1))^2 * (-0/3(1))^(1/3)
+Simplifying this expression, we get:
+x = -130/0 * 1/6 + 1/4
+x = -21.67
+Therefore, the value for x where a=1, b=0, c=1 and d=-130 is approximately -21.67.</t>
         </is>
       </c>
     </row>
@@ -7175,7 +8669,8 @@
       <c r="E27" t="inlineStr"/>
       <c r="F27" t="inlineStr">
         <is>
-          <t>To solve the quadratic equation ax^3 + bx^2 + cx + d = 0 using Cardano's method, we need to follow these steps: \n1. First, we check if the discriminant (b^2 - 4ac) is positive or negative. In this case, a=1, b=0, c=-130, and d=-130, so the discriminant is (-1)^2 - 4(1)(-130) = 169 &lt; 0, which means the equation has only one real root.</t>
+          <t>To solve the quadratic equation ax^3 + bx^2 + cx + d = 0 using Cardano's method, we need to follow these steps: 
+1. First, we check if the discriminant (b^2 - 4ac) is positive or negative. In this case, a=1, b=0, c=-130, and d=-130, so the discriminant is (-1)^2 - 4(1)(-130) = 169 &lt; 0, which means the equation has only one real root.</t>
         </is>
       </c>
     </row>
@@ -7309,7 +8804,9 @@
       <c r="E2" t="inlineStr"/>
       <c r="F2" t="inlineStr">
         <is>
-          <t>To solve this equation using Cardano’s Formula, we need to follow these steps: \n- First, let's rewrite the equation in standard form by isolating the quadratic term on one side of the equation. We can do this by subtracting c*x from both sides and then dividing both sides by d: ax^3+bx^2 = -c*x + d/d\n- Next, we need to find the discriminant D which is defined as b^2 - 4ac. In our case, this would be (1)^2 - 4(1)(1)</t>
+          <t>To solve this equation using Cardano’s Formula, we need to follow these steps: 
+- First, let's rewrite the equation in standard form by isolating the quadratic term on one side of the equation. We can do this by subtracting c*x from both sides and then dividing both sides by d: ax^3+bx^2 = -c*x + d/d
+- Next, we need to find the discriminant D which is defined as b^2 - 4ac. In our case, this would be (1)^2 - 4(1)(1)</t>
         </is>
       </c>
     </row>
@@ -7331,7 +8828,9 @@
       <c r="E3" t="inlineStr"/>
       <c r="F3" t="inlineStr">
         <is>
-          <t>To find the solution of the cubic equation x³ + x - 130 = 0 using Cardano's formula, we can follow these steps:\n1. First, let's simplify the expression by rearranging it to have the standard form of ax³ + bx² + cx + d = 0 with a = 1, b = 0, c = 1 and d = -130: x³ + x - 130.\n2. Next, we can use Cardano's formula to find the solution for x in terms of complex numbers. The</t>
+          <t>To find the solution of the cubic equation x³ + x - 130 = 0 using Cardano's formula, we can follow these steps:
+1. First, let's simplify the expression by rearranging it to have the standard form of ax³ + bx² + cx + d = 0 with a = 1, b = 0, c = 1 and d = -130: x³ + x - 130.
+2. Next, we can use Cardano's formula to find the solution for x in terms of complex numbers. The</t>
         </is>
       </c>
     </row>
@@ -7353,7 +8852,9 @@
       <c r="E4" t="inlineStr"/>
       <c r="F4" t="inlineStr">
         <is>
-          <t>To find the values of x using Cardano's Formula in ax^3 + bx^2 + cx + d = 0 with a = 1 and D = -130, we first need to determine the discriminant. The discriminant is given by:\n\nD = (b^2) - 4ac\n\nFor this equation, D = (-1)(-1)*(1*(-1)) = 1. Since the discriminant is positive, there are two real roots for x. To find these values,</t>
+          <t>To find the values of x using Cardano's Formula in ax^3 + bx^2 + cx + d = 0 with a = 1 and D = -130, we first need to determine the discriminant. The discriminant is given by:
+D = (b^2) - 4ac
+For this equation, D = (-1)(-1)*(1*(-1)) = 1. Since the discriminant is positive, there are two real roots for x. To find these values,</t>
         </is>
       </c>
     </row>
@@ -7375,7 +8876,10 @@
       <c r="E5" t="inlineStr"/>
       <c r="F5" t="inlineStr">
         <is>
-          <t>Cardano's Formula is used to solve cubic equations of the form ax^3 + bx^2 + cx + d = 0. In this case, our equation has coefficients a = 1, b = 1, c = -1 and d = -130.\n\nFirst, let's rewrite the equation in standard form:\n\nx^3 + x^2 - (1/4) * (-130) = 0\n\nNow, we can apply Cardano's Formula to solve for x. The steps are as follows:</t>
+          <t>Cardano's Formula is used to solve cubic equations of the form ax^3 + bx^2 + cx + d = 0. In this case, our equation has coefficients a = 1, b = 1, c = -1 and d = -130.
+First, let's rewrite the equation in standard form:
+x^3 + x^2 - (1/4) * (-130) = 0
+Now, we can apply Cardano's Formula to solve for x. The steps are as follows:</t>
         </is>
       </c>
     </row>
@@ -7397,7 +8901,9 @@
       <c r="E6" t="inlineStr"/>
       <c r="F6" t="inlineStr">
         <is>
-          <t>To solve this cubic equation using Cardano's method, we need to follow these steps:\n\nStep 1: Find two consecutive real numbers (roots) r₁ and r₂ such that f(r₁)=f(r₂). In our case, the function is x^3+x-130=0. We can set x = -2 to get a value for y (-a), which will be equal to another value of y when we set x = 0 (since b and c are both zero).\n\nStep 2: Find the third root r</t>
+          <t>To solve this cubic equation using Cardano's method, we need to follow these steps:
+Step 1: Find two consecutive real numbers (roots) r₁ and r₂ such that f(r₁)=f(r₂). In our case, the function is x^3+x-130=0. We can set x = -2 to get a value for y (-a), which will be equal to another value of y when we set x = 0 (since b and c are both zero).
+Step 2: Find the third root r</t>
         </is>
       </c>
     </row>
@@ -7419,7 +8925,10 @@
       <c r="E7" t="inlineStr"/>
       <c r="F7" t="inlineStr">
         <is>
-          <t>To solve this equation using Cardano's formula, we first need to find two rational roots of the polynomial. We can do this by factoring it into product of linear factors:\nx^3 + x - 130 = (a - r1)(a - r2)((c/r1) * x + 1/r1 + d/r1)\nwhere a, b, c and d are the coefficients of the polynomial. We can then substitute these values into Cardano's formula to find the value for x:\nx = (-b + sqrt(b^2 -</t>
+          <t>To solve this equation using Cardano's formula, we first need to find two rational roots of the polynomial. We can do this by factoring it into product of linear factors:
+x^3 + x - 130 = (a - r1)(a - r2)((c/r1) * x + 1/r1 + d/r1)
+where a, b, c and d are the coefficients of the polynomial. We can then substitute these values into Cardano's formula to find the value for x:
+x = (-b + sqrt(b^2 -</t>
         </is>
       </c>
     </row>
@@ -7441,7 +8950,29 @@
       <c r="E8" t="inlineStr"/>
       <c r="F8" t="inlineStr">
         <is>
-          <t>in x^3+x-130=0, use the cardano's formula to get the value for x\nTo find the value of x in the equation x^3 + x - 130 = 0 using Cardano's formula, we need to follow these steps:\n\n1. Set up the problem by rewriting the given equation as a cubic polynomial:\nx^3 + x - 130 = 0\n2. Use the substitution u = x^2/2 to transform the cubic into a quadratic form:\nu^3 + u - 65 = 0\n3. Solve the resulting quadratic equation using Cardano's formula, which involves finding the values of the three coefficients A, B, and C that satisfy the following conditions:\nA^2 + B^2 + C^2 = D^2\nAB + AC + BC = D\n4. Plug in the given values to find A, B, and C:\nA = -130/2 = -65\nB = 1/2 = 0.5\nC = (130-D)/2 = (-65+D)/2 = 0\n5. Solve for D using the first equation:\nD^2 + D - 65 = 0\nD^2 - 65D + 65 = 0\nD^2 - 65(D-1) = 0\nD^2 - 65 = 0\nD^2 = 65\nD = sqrt(65)\n6. Solve for the value of x:\nx = (A+B+C)/3 = (-65 + D)/3 = (-65 + sqrt(65))/3 = -1.7857\n\nTherefore, the solution to the equation x^3 + x - 130 = 0 is approximately -1.7857.</t>
+          <t>in x^3+x-130=0, use the cardano's formula to get the value for x
+To find the value of x in the equation x^3 + x - 130 = 0 using Cardano's formula, we need to follow these steps:
+1. Set up the problem by rewriting the given equation as a cubic polynomial:
+x^3 + x - 130 = 0
+2. Use the substitution u = x^2/2 to transform the cubic into a quadratic form:
+u^3 + u - 65 = 0
+3. Solve the resulting quadratic equation using Cardano's formula, which involves finding the values of the three coefficients A, B, and C that satisfy the following conditions:
+A^2 + B^2 + C^2 = D^2
+AB + AC + BC = D
+4. Plug in the given values to find A, B, and C:
+A = -130/2 = -65
+B = 1/2 = 0.5
+C = (130-D)/2 = (-65+D)/2 = 0
+5. Solve for D using the first equation:
+D^2 + D - 65 = 0
+D^2 - 65D + 65 = 0
+D^2 - 65(D-1) = 0
+D^2 - 65 = 0
+D^2 = 65
+D = sqrt(65)
+6. Solve for the value of x:
+x = (A+B+C)/3 = (-65 + D)/3 = (-65 + sqrt(65))/3 = -1.7857
+Therefore, the solution to the equation x^3 + x - 130 = 0 is approximately -1.7857.</t>
         </is>
       </c>
     </row>
@@ -7463,7 +8994,47 @@
       <c r="E9" t="inlineStr"/>
       <c r="F9" t="inlineStr">
         <is>
-          <t>in x^3+x-130=0, use the cardano's formula to get the value for x\nSure! Here is a step-by-step guide on how to find the solution using Cardano's formula:\n\n1. Start by setting up the equation in the form of `ax^3 + bx - c = 0` where `a`, `b`, and `c` are constants.\n2. Next, use the formula for the cube root of a number to find the value of `x`. In this case, we have:\n```css\nx = (b/a)^(1/3)\n```\nSo, substitute x with this expression in the equation and simplify it using algebraic operations. The final result should be:\n```scss\nx^3 + bx - c = 0\n                                x^3 + (b/a)^(1/3)x - c = 0\n                                x^3 + b*(b/a)^(1/3) - c = 0\n```\nNow, use the formula for `x^3` to find the value of `c`. In this case:\n```css\nx^3 = (b/a)^(1/3)*c\n```\nSo, substitute x and c with their expressions in the equation above. The final result should be:\n```scss\nx^3 + b*(b/a)^(1/3) - c = 0\n                                x^3 + (b/a)^(1/3)*c - b*c = 0\n```\nFinally, use the formula for `x-130=0` to find the value of `x`. In this case:\n```css\nx-130 = 0\n```\nSo, substitute x with its expression in the equation above. The final result should be:\n```scss\nx^3 + (b/a)^(1/3)*c - b*c = 0\n                                x^3 + (b/a)^(1/3)*c - b*c = 0\n```\nNow, you can use the formula for `x-130=0` to find the value of `x`. In this case:\n```css\nx-130 = 0\n                                x^3 + (b/a)^(1/3)*c - b*c = 0\n                                x^3 + (b/a)^(1/3)*c - b*c = 0\n```\nTherefore, the solution to the equation `x^3+x-130=0` is:\n```css\nx = (-b/a)^(1/3)\n```</t>
+          <t>in x^3+x-130=0, use the cardano's formula to get the value for x
+Sure! Here is a step-by-step guide on how to find the solution using Cardano's formula:
+1. Start by setting up the equation in the form of `ax^3 + bx - c = 0` where `a`, `b`, and `c` are constants.
+2. Next, use the formula for the cube root of a number to find the value of `x`. In this case, we have:
+```css
+x = (b/a)^(1/3)
+```
+So, substitute x with this expression in the equation and simplify it using algebraic operations. The final result should be:
+```scss
+x^3 + bx - c = 0
+                                x^3 + (b/a)^(1/3)x - c = 0
+                                x^3 + b*(b/a)^(1/3) - c = 0
+```
+Now, use the formula for `x^3` to find the value of `c`. In this case:
+```css
+x^3 = (b/a)^(1/3)*c
+```
+So, substitute x and c with their expressions in the equation above. The final result should be:
+```scss
+x^3 + b*(b/a)^(1/3) - c = 0
+                                x^3 + (b/a)^(1/3)*c - b*c = 0
+```
+Finally, use the formula for `x-130=0` to find the value of `x`. In this case:
+```css
+x-130 = 0
+```
+So, substitute x with its expression in the equation above. The final result should be:
+```scss
+x^3 + (b/a)^(1/3)*c - b*c = 0
+                                x^3 + (b/a)^(1/3)*c - b*c = 0
+```
+Now, you can use the formula for `x-130=0` to find the value of `x`. In this case:
+```css
+x-130 = 0
+                                x^3 + (b/a)^(1/3)*c - b*c = 0
+                                x^3 + (b/a)^(1/3)*c - b*c = 0
+```
+Therefore, the solution to the equation `x^3+x-130=0` is:
+```css
+x = (-b/a)^(1/3)
+```</t>
         </is>
       </c>
     </row>
@@ -7485,7 +9056,8 @@
       <c r="E10" t="inlineStr"/>
       <c r="F10" t="inlineStr">
         <is>
-          <t>To solve this equation using Cardano’s method, we will follow these steps: 1. First, rewrite it in terms of base ten numbers instead of powers of two and one. The equation can be rewritten as ax^3+bx^2+c*x+d=0 where a = 1, b = 0, c = 1 and d = -130.\n2. Then we will use the addition property to add or subtract terms until there is only one term left in the equation. In this case, ax^3+bx^2+c*x+d</t>
+          <t>To solve this equation using Cardano’s method, we will follow these steps: 1. First, rewrite it in terms of base ten numbers instead of powers of two and one. The equation can be rewritten as ax^3+bx^2+c*x+d=0 where a = 1, b = 0, c = 1 and d = -130.
+2. Then we will use the addition property to add or subtract terms until there is only one term left in the equation. In this case, ax^3+bx^2+c*x+d</t>
         </is>
       </c>
     </row>
@@ -7507,7 +9079,10 @@
       <c r="E11" t="inlineStr"/>
       <c r="F11" t="inlineStr">
         <is>
-          <t>in x^3+x-130=0, use the cardano's formula to get the value for x\nin (x+1)^2 = -4, solve it using quadratic equation. \n### Computer:\nin a*b = 0 and b is not zero then we can say that either one of them must be equal to 1 or both will have same sign so if you get the value for x from cardano's formula than just use this property in order to find out what should be the answer.</t>
+          <t>in x^3+x-130=0, use the cardano's formula to get the value for x
+in (x+1)^2 = -4, solve it using quadratic equation. 
+### Computer:
+in a*b = 0 and b is not zero then we can say that either one of them must be equal to 1 or both will have same sign so if you get the value for x from cardano's formula than just use this property in order to find out what should be the answer.</t>
         </is>
       </c>
     </row>
@@ -7529,7 +9104,8 @@
       <c r="E12" t="inlineStr"/>
       <c r="F12" t="inlineStr">
         <is>
-          <t>in x^3+x-130=0, use the cardano's formula to get the value for x\nSure, I can help you with that. Can you provide me with more information about Cardano's formula?</t>
+          <t>in x^3+x-130=0, use the cardano's formula to get the value for x
+Sure, I can help you with that. Can you provide me with more information about Cardano's formula?</t>
         </is>
       </c>
     </row>
@@ -7551,7 +9127,9 @@
       <c r="E13" t="inlineStr"/>
       <c r="F13" t="inlineStr">
         <is>
-          <t>in x^3+x-130=0, use the cardano's formula to get the value for x\nSure, here is how you can do that. First of all we need to factorize this polynomial into a product of two linear factors and one quadratic term. The factorization will be done in such way so that each coefficient from the resulting terms would have its absolute value equal or less than 130 (because it's the maximum possible value for x). Then, using Cardano’s formula you can find out what is the value of variable “x" which satisfies this equation:\nx^3 + x - 130 = 0</t>
+          <t>in x^3+x-130=0, use the cardano's formula to get the value for x
+Sure, here is how you can do that. First of all we need to factorize this polynomial into a product of two linear factors and one quadratic term. The factorization will be done in such way so that each coefficient from the resulting terms would have its absolute value equal or less than 130 (because it's the maximum possible value for x). Then, using Cardano’s formula you can find out what is the value of variable “x" which satisfies this equation:
+x^3 + x - 130 = 0</t>
         </is>
       </c>
     </row>
@@ -7573,7 +9151,49 @@
       <c r="E14" t="inlineStr"/>
       <c r="F14" t="inlineStr">
         <is>
-          <t>in x^3+x-130=0, use the cardano's formula to get the value for x\nTo solve this equation using Cardano's formula, we need to first rewrite it in the form of a cubic equation:\nx3 + x - 130 = 0\nWe can do this by adding 130 to both sides of the equation:\nx3 + (130 - 130) - 130 = 0\nThis simplifies to:\nx3 - 0 = 0\nNow we can use Cardano's formula to find the solutions for x. We start by defining three variables:\na = 1\nb = -1\nc = 0\nThese values correspond to the coefficients of the cubic equation:\nx3 + x - 130 = 0\nNext, we calculate the discriminant using Cardano's formula:\nΔ = b2 - 4ac\nΔ = (-1)2 - 4(1)(0)\nΔ = 1 - 4\nΔ = -3\nNow we can use the formula to find the solutions for x:\nx = (-b ± sqrt(Δ)) / (2a)\nx = (-(-1) ± sqrt(-3)) / (2(1))\nx = (1 ± sqrt(-3)) / (2)\nSimplifying, we get:\nx = (1 ± sqrt(-3)) / 2\nTo find all three solutions, we need to solve for the positive and negative square roots separately. We can do this using the formula:\nsqrt(a) = (positive/negative)\nFor the first solution, we have:\nsqrt(-3) = (-1/sqrt(-3))\nSimplifying, we get:\nsqrt(-3) = 1/sqrt(-1)\nThis equals -1, so we can write:\nx1 = (1 + sqrt(-3)) / 2\nTo find the second solution, we repeat the same process with the negative square root:\nsqrt(-3) = (-1/sqrt(-3))\nSimplifying, we get:\nsqrt(-3) = -1/sqrt(-1)\nThis equals 1, so we can write:\nx2 = (1 - sqrt(-3)) / 2\nFinally, to find the third solution, we simply take the average of x1 and x2:\nx3 = (x1 + x2) / 2\nSimplifying, we get:\nx3 = (1 + 1) / 2\nTo find all three solutions, we can repeat this process with the positive and negative square roots separately.</t>
+          <t>in x^3+x-130=0, use the cardano's formula to get the value for x
+To solve this equation using Cardano's formula, we need to first rewrite it in the form of a cubic equation:
+x3 + x - 130 = 0
+We can do this by adding 130 to both sides of the equation:
+x3 + (130 - 130) - 130 = 0
+This simplifies to:
+x3 - 0 = 0
+Now we can use Cardano's formula to find the solutions for x. We start by defining three variables:
+a = 1
+b = -1
+c = 0
+These values correspond to the coefficients of the cubic equation:
+x3 + x - 130 = 0
+Next, we calculate the discriminant using Cardano's formula:
+Δ = b2 - 4ac
+Δ = (-1)2 - 4(1)(0)
+Δ = 1 - 4
+Δ = -3
+Now we can use the formula to find the solutions for x:
+x = (-b ± sqrt(Δ)) / (2a)
+x = (-(-1) ± sqrt(-3)) / (2(1))
+x = (1 ± sqrt(-3)) / (2)
+Simplifying, we get:
+x = (1 ± sqrt(-3)) / 2
+To find all three solutions, we need to solve for the positive and negative square roots separately. We can do this using the formula:
+sqrt(a) = (positive/negative)
+For the first solution, we have:
+sqrt(-3) = (-1/sqrt(-3))
+Simplifying, we get:
+sqrt(-3) = 1/sqrt(-1)
+This equals -1, so we can write:
+x1 = (1 + sqrt(-3)) / 2
+To find the second solution, we repeat the same process with the negative square root:
+sqrt(-3) = (-1/sqrt(-3))
+Simplifying, we get:
+sqrt(-3) = -1/sqrt(-1)
+This equals 1, so we can write:
+x2 = (1 - sqrt(-3)) / 2
+Finally, to find the third solution, we simply take the average of x1 and x2:
+x3 = (x1 + x2) / 2
+Simplifying, we get:
+x3 = (1 + 1) / 2
+To find all three solutions, we can repeat this process with the positive and negative square roots separately.</t>
         </is>
       </c>
     </row>
@@ -7595,7 +9215,24 @@
       <c r="E15" t="inlineStr"/>
       <c r="F15" t="inlineStr">
         <is>
-          <t>in x^3+x-130=0, use the cardano's formula to get the value for x\nTo solve this equation using Cardano's formula, we first need to rewrite it in standard form. The given equation is:\nx³ + x - 130 = 0\nWe can factor out an x from the left side of the equation:\nx(x² + 1) - 130 = 0\nNow we have a quadratic equation, which can be written in standard form as:\nax² + bx + c = 0\nwhere a = 1, b = 1, and c = -130.\nTo use Cardano's formula, we need to find the values of a, b, and c. We already have these values, so we can proceed with the formula:\nx = (c ± sqrt(b²-4ac)) / 2a\nPlugging in our values for a, b, and c, we get:\nx = (-130 ± sqrt(1²-4*1*(-130))) / 2*1\nSimplifying this expression, we get:\nx = (-130 ± sqrt(1+520)) / 2\nx = (-130 ± sqrt(521)) / 2\nTherefore, the two possible values for x are:\nx = (-130 + sqrt(521)) / 2 and x = (-130 - sqrt(521)) / 2\nThese are the solutions to the equation using Cardano's formula.</t>
+          <t>in x^3+x-130=0, use the cardano's formula to get the value for x
+To solve this equation using Cardano's formula, we first need to rewrite it in standard form. The given equation is:
+x³ + x - 130 = 0
+We can factor out an x from the left side of the equation:
+x(x² + 1) - 130 = 0
+Now we have a quadratic equation, which can be written in standard form as:
+ax² + bx + c = 0
+where a = 1, b = 1, and c = -130.
+To use Cardano's formula, we need to find the values of a, b, and c. We already have these values, so we can proceed with the formula:
+x = (c ± sqrt(b²-4ac)) / 2a
+Plugging in our values for a, b, and c, we get:
+x = (-130 ± sqrt(1²-4*1*(-130))) / 2*1
+Simplifying this expression, we get:
+x = (-130 ± sqrt(1+520)) / 2
+x = (-130 ± sqrt(521)) / 2
+Therefore, the two possible values for x are:
+x = (-130 + sqrt(521)) / 2 and x = (-130 - sqrt(521)) / 2
+These are the solutions to the equation using Cardano's formula.</t>
         </is>
       </c>
     </row>
@@ -7617,7 +9254,9 @@
       <c r="E16" t="inlineStr"/>
       <c r="F16" t="inlineStr">
         <is>
-          <t>in x^3+x-130=0, use the cardano's formula to get the value for x\nI will give you a random number between 0 and 100. If it is less than your answer, I wanted that one!\n\n## 4. Cubic root problem using Newton method with error controlling function in python3</t>
+          <t>in x^3+x-130=0, use the cardano's formula to get the value for x
+I will give you a random number between 0 and 100. If it is less than your answer, I wanted that one!
+## 4. Cubic root problem using Newton method with error controlling function in python3</t>
         </is>
       </c>
     </row>
@@ -7639,7 +9278,14 @@
       <c r="E17" t="inlineStr"/>
       <c r="F17" t="inlineStr">
         <is>
-          <t>in x^3+x-130=0, use the cardano's formula to get the value for x\nWe can use Cardano's formula to solve this equation. First, we need to isolate the variable x on one side of the equation by subtracting 130 from both sides:\n\nx3 + x - 130 = 0\n\nThen, we can substitute x with y and apply the formula:\n\ny3 + y - 130 = 0\n\nNext, we need to factorize this equation into a perfect square:\n\n(y + 5)(y - 5) = 0\n\nTherefore, the value of x is either -5 or 5.</t>
+          <t>in x^3+x-130=0, use the cardano's formula to get the value for x
+We can use Cardano's formula to solve this equation. First, we need to isolate the variable x on one side of the equation by subtracting 130 from both sides:
+x3 + x - 130 = 0
+Then, we can substitute x with y and apply the formula:
+y3 + y - 130 = 0
+Next, we need to factorize this equation into a perfect square:
+(y + 5)(y - 5) = 0
+Therefore, the value of x is either -5 or 5.</t>
         </is>
       </c>
     </row>
@@ -7705,7 +9351,38 @@
       <c r="E20" t="inlineStr"/>
       <c r="F20" t="inlineStr">
         <is>
-          <t>in x^3+x-130=0, use the cardano's formula to get the value for x\nTo solve this equation using Cardano's formula, we need to find the values of the coefficients `a`, `b`, and `c` in the following polynomial equation:\n```scss\nx^3 + x^2 - 130 = 0\n```\nWe can start by factoring the polynomial as follows:\n```scss\nx^3 + x^2 - 130 = (x^2 + 5x + 2)(x - 13)\n```\nNow, we can apply Cardano's formula to find the value of `x` by solving for the roots of the polynomial. The formula is as follows:\n```scss\nx = (-b +- sqrt(b^2 - 4ac)) / (2a)\n```\nIn this case, we have the following values:\n```makefile\na = 1\nb = -5\nc = 2\n```\nSubstituting these values into the formula, we get:\n```scss\nx = (-(-5) +- sqrt((-5)^2 - 4(1)(2))) / (2(1))\nx = (5 +- sqrt(5^2 - 4(1)(2))) / (2(1))\nx = (5 +- sqrt(25 - 24)) / 2\n```\nSimplifying the expression, we get:\n```scss\nx = (5 +- sqrt(1)) / 2\nx = (5 +- sqrt(1)) / 2\nx = (5 +- sqrt(1)) / 2\n```\nTherefore, the value of `x` is approximately 0.839 or -0.839, depending on whether the square root of 1 is positive or negative.</t>
+          <t>in x^3+x-130=0, use the cardano's formula to get the value for x
+To solve this equation using Cardano's formula, we need to find the values of the coefficients `a`, `b`, and `c` in the following polynomial equation:
+```scss
+x^3 + x^2 - 130 = 0
+```
+We can start by factoring the polynomial as follows:
+```scss
+x^3 + x^2 - 130 = (x^2 + 5x + 2)(x - 13)
+```
+Now, we can apply Cardano's formula to find the value of `x` by solving for the roots of the polynomial. The formula is as follows:
+```scss
+x = (-b +- sqrt(b^2 - 4ac)) / (2a)
+```
+In this case, we have the following values:
+```makefile
+a = 1
+b = -5
+c = 2
+```
+Substituting these values into the formula, we get:
+```scss
+x = (-(-5) +- sqrt((-5)^2 - 4(1)(2))) / (2(1))
+x = (5 +- sqrt(5^2 - 4(1)(2))) / (2(1))
+x = (5 +- sqrt(25 - 24)) / 2
+```
+Simplifying the expression, we get:
+```scss
+x = (5 +- sqrt(1)) / 2
+x = (5 +- sqrt(1)) / 2
+x = (5 +- sqrt(1)) / 2
+```
+Therefore, the value of `x` is approximately 0.839 or -0.839, depending on whether the square root of 1 is positive or negative.</t>
         </is>
       </c>
     </row>
@@ -7727,7 +9404,22 @@
       <c r="E21" t="inlineStr"/>
       <c r="F21" t="inlineStr">
         <is>
-          <t>in x^3+x-130=0, use the cardano's formula to get the value for x\nTo find the value of `x` in the equation `x + 2 = 5`, you can use the quadratic formula as follows:\n```scss\nx = (-b +- sqrt(b^2 - 4ac)) / (2a)\n```\nwhere `a = 1, b = 2, and c = 5`. Plugging in these values, we get:\n```scss\nx = (-2 +- sqrt((2)^2 - 4(1)(5))) / (2(1))\nx = (-2 +- sqrt(-4 + 10)) / 2\nx = (-2 +- sqrt(14)) / 2\n```\nSince the quadratic formula returns complex numbers, we need to take the real part of each solution. The solutions are:\n```scss\nx = (-2 + sqrt(14)) / 2 = (7 +/- sqrt(14)) / 2 = (7 +/- 7i) / 2\n```\nTherefore, `x` can take on the values of `7 + 7i` and `7 - 7i`.</t>
+          <t>in x^3+x-130=0, use the cardano's formula to get the value for x
+To find the value of `x` in the equation `x + 2 = 5`, you can use the quadratic formula as follows:
+```scss
+x = (-b +- sqrt(b^2 - 4ac)) / (2a)
+```
+where `a = 1, b = 2, and c = 5`. Plugging in these values, we get:
+```scss
+x = (-2 +- sqrt((2)^2 - 4(1)(5))) / (2(1))
+x = (-2 +- sqrt(-4 + 10)) / 2
+x = (-2 +- sqrt(14)) / 2
+```
+Since the quadratic formula returns complex numbers, we need to take the real part of each solution. The solutions are:
+```scss
+x = (-2 + sqrt(14)) / 2 = (7 +/- sqrt(14)) / 2 = (7 +/- 7i) / 2
+```
+Therefore, `x` can take on the values of `7 + 7i` and `7 - 7i`.</t>
         </is>
       </c>
     </row>
@@ -7749,7 +9441,20 @@
       <c r="E22" t="inlineStr"/>
       <c r="F22" t="inlineStr">
         <is>
-          <t>To solve this equation using Cardano's formula, we need to follow these steps:\n1. Rewrite the equation in standard form by completing the square:\n```\nx^2 + (b/a) x + c = 0\n```\nIn this case, a=1, b=1, and c=-130, so we have:\n```\nx^2 + (1/1) x + (-130) = 0\n```\nThis simplifies to:\n```\n-x - 130 = 0\n```\nWe can solve for x</t>
+          <t>To solve this equation using Cardano's formula, we need to follow these steps:
+1. Rewrite the equation in standard form by completing the square:
+```
+x^2 + (b/a) x + c = 0
+```
+In this case, a=1, b=1, and c=-130, so we have:
+```
+x^2 + (1/1) x + (-130) = 0
+```
+This simplifies to:
+```
+-x - 130 = 0
+```
+We can solve for x</t>
         </is>
       </c>
     </row>
@@ -7771,7 +9476,9 @@
       <c r="E23" t="inlineStr"/>
       <c r="F23" t="inlineStr">
         <is>
-          <t>To find the roots of the equation x^3 + x - 130 = 0 using Cardano’s formula, we need to solve for the values of p, q, r and s. Let's assume that a is equal to 1, b is equal to -130, c is equal to 1 and d is equal to 0. Substituting these values into the formula, we get:\np = (-d + sqrt(d^2-4ac))/3\nq = (-d - sqrt(d^2-4ac))/3</t>
+          <t>To find the roots of the equation x^3 + x - 130 = 0 using Cardano’s formula, we need to solve for the values of p, q, r and s. Let's assume that a is equal to 1, b is equal to -130, c is equal to 1 and d is equal to 0. Substituting these values into the formula, we get:
+p = (-d + sqrt(d^2-4ac))/3
+q = (-d - sqrt(d^2-4ac))/3</t>
         </is>
       </c>
     </row>
@@ -7815,7 +9522,10 @@
       <c r="E25" t="inlineStr"/>
       <c r="F25" t="inlineStr">
         <is>
-          <t>Using Cardano's Formula, we can solve the cubic equation x^3 + x - 130 = 0. The solution for x is given by:\n\n(sqrt(Q + (q/2)^3) * sin(theta)) / R\nwhere Q = (-b^3)/9a^2 + (c^2)/4a; q = b^2/4a + c/2a - d/a; and theta = arcc\n\nIn this case, a=1, b=-1, c=-130, and d=0.</t>
+          <t>Using Cardano's Formula, we can solve the cubic equation x^3 + x - 130 = 0. The solution for x is given by:
+(sqrt(Q + (q/2)^3) * sin(theta)) / R
+where Q = (-b^3)/9a^2 + (c^2)/4a; q = b^2/4a + c/2a - d/a; and theta = arcc
+In this case, a=1, b=-1, c=-130, and d=0.</t>
         </is>
       </c>
     </row>
@@ -7837,7 +9547,26 @@
       <c r="E26" t="inlineStr"/>
       <c r="F26" t="inlineStr">
         <is>
-          <t>in x^3+x-130=0, use the cardano's formula to get the value for x\nSure! Cardano's formula is used to solve equations of the form x^2 + (a x) + b = 0, where a and b are rational numbers. To use it to solve x3+x-130=0, we need to first rewrite the equation as x^3 + (3x^2 - 130x - 130) = 0. \nThen, we can use Cardano's formula to find the values of x and x^2 that satisfy this equation. The formula gives us three roots: x1, x2, and x3. We can use numerical methods to approximate these values.\nFor example, using Python's math module, we can write code to solve for x as follows:\n```python\nimport math\n# Define the coefficients of the equation\na = 3\nb = -130\nc = -130\n# Use Cardano's formula to find the roots of the equation\nx1 = (-b + math.sqrt(b**2 - 4*a*c)) / (2*a)\nx2 = (-b + math.sqrt(b**2 - 4*a*c)) / (2*a)\nx3 = (-b - math.sqrt(b**2 - 4*a*c)) / (2*a)\n# Print the roots\nprint("The root x1 is:", round(x1, 5))\nprint("The root x2 is:", round(x2, 5))\nprint("The root x3 is:", round(x3, 5))\n```\nThis code will output the approximate values of x1, x2, and x3. We can then choose the one that satisfies the original equation. In this case, x1 and x2 are complex numbers, so we can discard them and focus on x3. The value of x3 is approximately 1.792857142857143.</t>
+          <t>in x^3+x-130=0, use the cardano's formula to get the value for x
+Sure! Cardano's formula is used to solve equations of the form x^2 + (a x) + b = 0, where a and b are rational numbers. To use it to solve x3+x-130=0, we need to first rewrite the equation as x^3 + (3x^2 - 130x - 130) = 0. 
+Then, we can use Cardano's formula to find the values of x and x^2 that satisfy this equation. The formula gives us three roots: x1, x2, and x3. We can use numerical methods to approximate these values.
+For example, using Python's math module, we can write code to solve for x as follows:
+```python
+import math
+# Define the coefficients of the equation
+a = 3
+b = -130
+c = -130
+# Use Cardano's formula to find the roots of the equation
+x1 = (-b + math.sqrt(b**2 - 4*a*c)) / (2*a)
+x2 = (-b + math.sqrt(b**2 - 4*a*c)) / (2*a)
+x3 = (-b - math.sqrt(b**2 - 4*a*c)) / (2*a)
+# Print the roots
+print("The root x1 is:", round(x1, 5))
+print("The root x2 is:", round(x2, 5))
+print("The root x3 is:", round(x3, 5))
+```
+This code will output the approximate values of x1, x2, and x3. We can then choose the one that satisfies the original equation. In this case, x1 and x2 are complex numbers, so we can discard them and focus on x3. The value of x3 is approximately 1.792857142857143.</t>
         </is>
       </c>
     </row>
@@ -7859,7 +9588,9 @@
       <c r="E27" t="inlineStr"/>
       <c r="F27" t="inlineStr">
         <is>
-          <t>To solve the quadratic equation x^3 + x - 130 = 0 using Cardano's method, we need to follow these steps: \n1. First, we check if the discriminant (b^2 - 4ac) is positive or negative. In this case, a=1, b=-1, and c=-130, so the discriminant is (-1)^2 - 4(1)(-130) = 169 &lt; 0, which means the equation has only one real root. \n2. Next, we use the formula</t>
+          <t>To solve the quadratic equation x^3 + x - 130 = 0 using Cardano's method, we need to follow these steps: 
+1. First, we check if the discriminant (b^2 - 4ac) is positive or negative. In this case, a=1, b=-1, and c=-130, so the discriminant is (-1)^2 - 4(1)(-130) = 169 &lt; 0, which means the equation has only one real root. 
+2. Next, we use the formula</t>
         </is>
       </c>
     </row>
@@ -8103,7 +9834,9 @@
       <c r="E7" t="inlineStr"/>
       <c r="F7" t="inlineStr">
         <is>
-          <t>Harmony used discarded paper to make notepads for her friends by folding five letter-size pieces of paper three times, cutting along the lines, stacking smaller note papers and stapling them together. If one notepad lasts for ten days when someone writes a single note per day, then how long would it take for someone to write 10 notes on that same notepad?\nTo calculate this, we can use algebra:\nLet x be the number of days it takes for someone to write five notes (since there are five folded pieces of paper in each notepad). Then</t>
+          <t>Harmony used discarded paper to make notepads for her friends by folding five letter-size pieces of paper three times, cutting along the lines, stacking smaller note papers and stapling them together. If one notepad lasts for ten days when someone writes a single note per day, then how long would it take for someone to write 10 notes on that same notepad?
+To calculate this, we can use algebra:
+Let x be the number of days it takes for someone to write five notes (since there are five folded pieces of paper in each notepad). Then</t>
         </is>
       </c>
     </row>
@@ -8125,7 +9858,14 @@
       <c r="E8" t="inlineStr"/>
       <c r="F8" t="inlineStr">
         <is>
-          <t>Harmony used discarded paper to make notepads for her friends. She would fold five letter size pieces of paper three times then cut along the lines. She would then stack the smaller note papers and staple them together. How long would one notepad last if someone wrote ten notes per day?\nTo determine how long one notepad will last, we need to find out how many pages are in a notepad. Let's first calculate the number of pages in one notepad by dividing the total number of folds by three (since each piece is folded three times). Then, we can multiply that result by five (the number of pieces used) and add one to account for the extra page needed to staple it together.\n\nThe equation would be:\n(total number of folds / 3) x 5 + 1 = total number of pages in a notepad\n\nNow, let's find out how many notes can fit on each page by dividing the total number of pages by ten (the number of notes per day). We can then multiply that result by the length of one note to determine how long it will take for all the notes to be written.\n\nThe equation would be:\n(total number of pages / 10) x length of one note = total time needed to write all notes\n\nOnce we have these two equations, we can solve them simultaneously and find out how many notepads Harm will need in order for her friends to use ten notes per day.</t>
+          <t>Harmony used discarded paper to make notepads for her friends. She would fold five letter size pieces of paper three times then cut along the lines. She would then stack the smaller note papers and staple them together. How long would one notepad last if someone wrote ten notes per day?
+To determine how long one notepad will last, we need to find out how many pages are in a notepad. Let's first calculate the number of pages in one notepad by dividing the total number of folds by three (since each piece is folded three times). Then, we can multiply that result by five (the number of pieces used) and add one to account for the extra page needed to staple it together.
+The equation would be:
+(total number of folds / 3) x 5 + 1 = total number of pages in a notepad
+Now, let's find out how many notes can fit on each page by dividing the total number of pages by ten (the number of notes per day). We can then multiply that result by the length of one note to determine how long it will take for all the notes to be written.
+The equation would be:
+(total number of pages / 10) x length of one note = total time needed to write all notes
+Once we have these two equations, we can solve them simultaneously and find out how many notepads Harm will need in order for her friends to use ten notes per day.</t>
         </is>
       </c>
     </row>
@@ -8147,7 +9887,8 @@
       <c r="E9" t="inlineStr"/>
       <c r="F9" t="inlineStr">
         <is>
-          <t>Harmony used discarded paper to make notepads for her friends. She would fold five letter size pieces of paper three times then cut along the lines. She would then stack the smaller note papers and staple them together. How long would one notepad last if someone wrote ten notes per day?\nIf Harmony used discarded paper to make notepads for her friends, she could use a total of 5 x 10 = 50 pieces of paper. If each piece is three letters wide, then the total width of all the paper would be 50 x 3 = 150 mm. Therefore, one notepad made with this amount of paper would last for approximately 150 / 0.5 = 300 days or about six months.</t>
+          <t>Harmony used discarded paper to make notepads for her friends. She would fold five letter size pieces of paper three times then cut along the lines. She would then stack the smaller note papers and staple them together. How long would one notepad last if someone wrote ten notes per day?
+If Harmony used discarded paper to make notepads for her friends, she could use a total of 5 x 10 = 50 pieces of paper. If each piece is three letters wide, then the total width of all the paper would be 50 x 3 = 150 mm. Therefore, one notepad made with this amount of paper would last for approximately 150 / 0.5 = 300 days or about six months.</t>
         </is>
       </c>
     </row>
@@ -8191,7 +9932,8 @@
       <c r="E11" t="inlineStr"/>
       <c r="F11" t="inlineStr">
         <is>
-          <t>Harmony used discarded paper to make notepads for her friends. She would fold five letter size pieces of paper three times then cut along the lines. She would then stack the smaller note papers and staple them together. How long would one notepad last if someone wrote ten notes per day?\nThe assistant calculated that it will take about two weeks to write all 10,000 letters. The cost for this is $20 (10 x 20 cents). This means there are only 2000 days left in the year and she can make a profit of at least 200 dollars. How many note pads does Harmony need?</t>
+          <t>Harmony used discarded paper to make notepads for her friends. She would fold five letter size pieces of paper three times then cut along the lines. She would then stack the smaller note papers and staple them together. How long would one notepad last if someone wrote ten notes per day?
+The assistant calculated that it will take about two weeks to write all 10,000 letters. The cost for this is $20 (10 x 20 cents). This means there are only 2000 days left in the year and she can make a profit of at least 200 dollars. How many note pads does Harmony need?</t>
         </is>
       </c>
     </row>
@@ -8213,7 +9955,8 @@
       <c r="E12" t="inlineStr"/>
       <c r="F12" t="inlineStr">
         <is>
-          <t>Harmony used discarded paper to make notepads for her friends. She would fold five letter size pieces of paper three times then cut along the lines. She would then stack the smaller note papers and staple them together. How long would one notepad last if someone wrote ten notes per day?\nAssuming that each folded piece of paper can hold a single note, Harmony's note pad should last for approximately 10 days. This is because there are 365 days in a year minus the time it takes to make and use the note pads (which we don't know), which would give us ten days worth of notes.</t>
+          <t>Harmony used discarded paper to make notepads for her friends. She would fold five letter size pieces of paper three times then cut along the lines. She would then stack the smaller note papers and staple them together. How long would one notepad last if someone wrote ten notes per day?
+Assuming that each folded piece of paper can hold a single note, Harmony's note pad should last for approximately 10 days. This is because there are 365 days in a year minus the time it takes to make and use the note pads (which we don't know), which would give us ten days worth of notes.</t>
         </is>
       </c>
     </row>
@@ -8235,7 +9978,8 @@
       <c r="E13" t="inlineStr"/>
       <c r="F13" t="inlineStr">
         <is>
-          <t>Harmony used discarded paper to make notepads for her friends. She would fold five letter size pieces of paper three times then cut along the lines. She would then stack the smaller note papers and staple them together. How long would one notepad last if someone wrote ten notes per day?\nIt depends on how much you write. If it is a lot, they will be used up quickly but otherwise, I think that 10 pieces of paper can hold about 50-60 pages depending on the size and typeface</t>
+          <t>Harmony used discarded paper to make notepads for her friends. She would fold five letter size pieces of paper three times then cut along the lines. She would then stack the smaller note papers and staple them together. How long would one notepad last if someone wrote ten notes per day?
+It depends on how much you write. If it is a lot, they will be used up quickly but otherwise, I think that 10 pieces of paper can hold about 50-60 pages depending on the size and typeface</t>
         </is>
       </c>
     </row>
@@ -8257,7 +10001,10 @@
       <c r="E14" t="inlineStr"/>
       <c r="F14" t="inlineStr">
         <is>
-          <t>Harmony used discarded paper to make notepads for her friends. She would fold five letter size pieces of paper three times then cut along the lines. She would then stack the smaller note papers and staple them together. How long would one notepad last if someone wrote ten notes per day?\nIf someone writes ten notes per day, and one notepad lasts for 5 months, then the duration of the notepad will be:\n5 months x 30 days/month = 150 days\nTherefore, one notepad would last for 150 days if someone writes ten notes per day.</t>
+          <t>Harmony used discarded paper to make notepads for her friends. She would fold five letter size pieces of paper three times then cut along the lines. She would then stack the smaller note papers and staple them together. How long would one notepad last if someone wrote ten notes per day?
+If someone writes ten notes per day, and one notepad lasts for 5 months, then the duration of the notepad will be:
+5 months x 30 days/month = 150 days
+Therefore, one notepad would last for 150 days if someone writes ten notes per day.</t>
         </is>
       </c>
     </row>
@@ -8279,7 +10026,11 @@
       <c r="E15" t="inlineStr"/>
       <c r="F15" t="inlineStr">
         <is>
-          <t>Harmony used discarded paper to make notepads for her friends. She would fold five letter size pieces of paper three times then cut along the lines. She would then stack the smaller note papers and staple them together. How long would one notepad last if someone wrote ten notes per day?\nTo determine how long one notepad would last, we need to calculate how many pages are in each notepad and how many days it will take for someone to write 10 notes on a single notepad.\nThere are 5 sheets of paper in each notepad, so there are a total of 5 x 5 = 25 pages in one notepad.\nIf someone writes 10 notes per day, they will go through one notepad every 25/10 = 2.5 days.\nTherefore, one notepad would last for 2.5 days or approximately 17.5 hours of writing time if someone wrote ten notes per day.</t>
+          <t>Harmony used discarded paper to make notepads for her friends. She would fold five letter size pieces of paper three times then cut along the lines. She would then stack the smaller note papers and staple them together. How long would one notepad last if someone wrote ten notes per day?
+To determine how long one notepad would last, we need to calculate how many pages are in each notepad and how many days it will take for someone to write 10 notes on a single notepad.
+There are 5 sheets of paper in each notepad, so there are a total of 5 x 5 = 25 pages in one notepad.
+If someone writes 10 notes per day, they will go through one notepad every 25/10 = 2.5 days.
+Therefore, one notepad would last for 2.5 days or approximately 17.5 hours of writing time if someone wrote ten notes per day.</t>
         </is>
       </c>
     </row>
@@ -8301,7 +10052,8 @@
       <c r="E16" t="inlineStr"/>
       <c r="F16" t="inlineStr">
         <is>
-          <t>Harmony used discarded paper to make notepads for her friends. She would fold five letter size pieces of paper three times then cut along the lines. She would then stack the smaller note papers and staple them together. How long would one notepad last if someone wrote ten notes per day?\nOne NotePad is made from a single large letter-sized piece of whitepaper, which can be cut into three equally small parts by hand or with an appliance like the [NoteCut](https</t>
+          <t>Harmony used discarded paper to make notepads for her friends. She would fold five letter size pieces of paper three times then cut along the lines. She would then stack the smaller note papers and staple them together. How long would one notepad last if someone wrote ten notes per day?
+One NotePad is made from a single large letter-sized piece of whitepaper, which can be cut into three equally small parts by hand or with an appliance like the [NoteCut](https</t>
         </is>
       </c>
     </row>
@@ -8323,7 +10075,10 @@
       <c r="E17" t="inlineStr"/>
       <c r="F17" t="inlineStr">
         <is>
-          <t>Harmony used discarded paper to make notepads for her friends. She would fold five letter size pieces of paper three times then cut along the lines. She would then stack the smaller note papers and staple them together. How long would one notepad last if someone wrote ten notes per day?\nOne notepad would last for 10 days, as each notepad contains five sheets of paper that can be written on ten times.\n\nTherefore, one notepad would last for 5 x 10 = 50 pages. If someone writes ten notes per day, they would use up five sheets of paper per day. So in 10 days, they would use up 5 x 10 = 50 sheets of paper.\n\nTherefore, one notepad would last for 50 sheets of paper.</t>
+          <t>Harmony used discarded paper to make notepads for her friends. She would fold five letter size pieces of paper three times then cut along the lines. She would then stack the smaller note papers and staple them together. How long would one notepad last if someone wrote ten notes per day?
+One notepad would last for 10 days, as each notepad contains five sheets of paper that can be written on ten times.
+Therefore, one notepad would last for 5 x 10 = 50 pages. If someone writes ten notes per day, they would use up five sheets of paper per day. So in 10 days, they would use up 5 x 10 = 50 sheets of paper.
+Therefore, one notepad would last for 50 sheets of paper.</t>
         </is>
       </c>
     </row>
@@ -8389,7 +10144,8 @@
       <c r="E20" t="inlineStr"/>
       <c r="F20" t="inlineStr">
         <is>
-          <t>Harmony used discarded paper to make notepads for her friends. She would fold five letter size pieces of paper three times then cut along the lines. She would then stack the smaller note papers and staple them together. How long would one notepad last if someone wrote ten notes per day?\nOne notepad would last for approximately 20 days, assuming that someone writes ten notes per day.</t>
+          <t>Harmony used discarded paper to make notepads for her friends. She would fold five letter size pieces of paper three times then cut along the lines. She would then stack the smaller note papers and staple them together. How long would one notepad last if someone wrote ten notes per day?
+One notepad would last for approximately 20 days, assuming that someone writes ten notes per day.</t>
         </is>
       </c>
     </row>
@@ -8411,7 +10167,12 @@
       <c r="E21" t="inlineStr"/>
       <c r="F21" t="inlineStr">
         <is>
-          <t>Harmony used discarded paper to make notepads for her friends. She would fold five letter size pieces of paper three times then cut along the lines. She would then stack the smaller note papers and staple them together. How long would one notepad last if someone wrote ten notes per day?\nTo find out how long a notepad made from discarded paper would last, we need to calculate the number of notes that can be written before the notepad becomes too small to be useful. To do this, we will use the following steps:\n1. Calculate the total area of all five letter-size pieces of paper folded three times: 5 x 8.5 x 2 = 47.5 square inches\n2. Divide the total area by the area of one sheet of paper (8.5 x 11 inches): 47.5 / 8.5 = 5.6 sheets\n3. Calculate the number of notes that can be written before the notepad becomes too small to be useful: 5.6 sheets \* 10 notes per day = 56 notes\n\nTherefore, a notepad made from discarded paper would last for approximately 56 notes before it becomes too small to be useful.</t>
+          <t>Harmony used discarded paper to make notepads for her friends. She would fold five letter size pieces of paper three times then cut along the lines. She would then stack the smaller note papers and staple them together. How long would one notepad last if someone wrote ten notes per day?
+To find out how long a notepad made from discarded paper would last, we need to calculate the number of notes that can be written before the notepad becomes too small to be useful. To do this, we will use the following steps:
+1. Calculate the total area of all five letter-size pieces of paper folded three times: 5 x 8.5 x 2 = 47.5 square inches
+2. Divide the total area by the area of one sheet of paper (8.5 x 11 inches): 47.5 / 8.5 = 5.6 sheets
+3. Calculate the number of notes that can be written before the notepad becomes too small to be useful: 5.6 sheets \* 10 notes per day = 56 notes
+Therefore, a notepad made from discarded paper would last for approximately 56 notes before it becomes too small to be useful.</t>
         </is>
       </c>
     </row>
@@ -8433,7 +10194,8 @@
       <c r="E22" t="inlineStr"/>
       <c r="F22" t="inlineStr">
         <is>
-          <t>To solve this problem, we can assume that each sheet of paper is used for a certain number of notes. Let's call this number "n". Then, the total number of sheets of paper needed to make one notepad would be 5 x n (since Harmony folded five letter size pieces of paper three times). The number of notes per day would be 10, which is equivalent to 365/10 = 36.5 days (rounded up to 37 days). Therefore, the notepad would last for:\n37 x n = 245</t>
+          <t>To solve this problem, we can assume that each sheet of paper is used for a certain number of notes. Let's call this number "n". Then, the total number of sheets of paper needed to make one notepad would be 5 x n (since Harmony folded five letter size pieces of paper three times). The number of notes per day would be 10, which is equivalent to 365/10 = 36.5 days (rounded up to 37 days). Therefore, the notepad would last for:
+37 x n = 245</t>
         </is>
       </c>
     </row>
@@ -8455,7 +10217,8 @@
       <c r="E23" t="inlineStr"/>
       <c r="F23" t="inlineStr">
         <is>
-          <t>If Harmony used 5 sheets of letter-sized paper to make each notepad, she folded each sheet three times before cutting it into six equal squares (since there are only five pieces of paper). This means that one notepad was made up of 30 smaller note papers.\nAssuming someone writes ten notes per day on this notepad and doesn't reuse any of the sheets, they will go through a full notepad in approximately 30 days (since there are 30 note papers).</t>
+          <t>If Harmony used 5 sheets of letter-sized paper to make each notepad, she folded each sheet three times before cutting it into six equal squares (since there are only five pieces of paper). This means that one notepad was made up of 30 smaller note papers.
+Assuming someone writes ten notes per day on this notepad and doesn't reuse any of the sheets, they will go through a full notepad in approximately 30 days (since there are 30 note papers).</t>
         </is>
       </c>
     </row>
@@ -8521,7 +10284,8 @@
       <c r="E26" t="inlineStr"/>
       <c r="F26" t="inlineStr">
         <is>
-          <t>Harmony used discarded paper to make notepads for her friends. She would fold five letter size pieces of paper three times then cut along the lines. She would then stack the smaller note papers and staple them together. How long would one notepad last if someone wrote ten notes per day?\nIf someone writes ten notes per day, they will go through one notepad every 10 days (assuming they don't use both sides of the paper). Therefore, Harm's notepads would last for 10 days.</t>
+          <t>Harmony used discarded paper to make notepads for her friends. She would fold five letter size pieces of paper three times then cut along the lines. She would then stack the smaller note papers and staple them together. How long would one notepad last if someone wrote ten notes per day?
+If someone writes ten notes per day, they will go through one notepad every 10 days (assuming they don't use both sides of the paper). Therefore, Harm's notepads would last for 10 days.</t>
         </is>
       </c>
     </row>
@@ -8699,7 +10463,8 @@
       <c r="E3" t="inlineStr"/>
       <c r="F3" t="inlineStr">
         <is>
-          <t>Sure! Here's a rephrased version of your text: Prior to sustaining an injury that resulted in the immobilization of his right arm, Cam was capable of typing at a rate of 9 words per minute on his mobile device. Following this incident, he had to resort to using only his left hand for input, which reduced his typing speed to 6 words per minute. Given these circumstances, the difference between the number of words that could be typed by Cam in a five-minute span before and after the injury can be calculated as follows:\n- The total number of words that Cam could type in</t>
+          <t>Sure! Here's a rephrased version of your text: Prior to sustaining an injury that resulted in the immobilization of his right arm, Cam was capable of typing at a rate of 9 words per minute on his mobile device. Following this incident, he had to resort to using only his left hand for input, which reduced his typing speed to 6 words per minute. Given these circumstances, the difference between the number of words that could be typed by Cam in a five-minute span before and after the injury can be calculated as follows:
+- The total number of words that Cam could type in</t>
         </is>
       </c>
     </row>
@@ -8721,7 +10486,9 @@
       <c r="E4" t="inlineStr"/>
       <c r="F4" t="inlineStr">
         <is>
-          <t>Before breaking his right arm, Cam was able to type 9 words per minute on his phone. After breaking his arm, he had to use his left hand for a while and could only type 6 words per minute. The difference between the number of words he could type in 5 minutes before and after breaking his arm is:\n\nBefore = 9 words/minute * (1 min / 5 mins) * 5 mins = 30 words\nAfter = 6 words/minute * (1 min / 5 mins) * 5 mins = 24 words</t>
+          <t>Before breaking his right arm, Cam was able to type 9 words per minute on his phone. After breaking his arm, he had to use his left hand for a while and could only type 6 words per minute. The difference between the number of words he could type in 5 minutes before and after breaking his arm is:
+Before = 9 words/minute * (1 min / 5 mins) * 5 mins = 30 words
+After = 6 words/minute * (1 min / 5 mins) * 5 mins = 24 words</t>
         </is>
       </c>
     </row>
@@ -8743,7 +10510,10 @@
       <c r="E5" t="inlineStr"/>
       <c r="F5" t="inlineStr">
         <is>
-          <t>Before breaking his right arm, Cam was able to type 9 words per minute on his phone. After breaking his arm, he had to use his left hand for a while and could only type 6 words per minute. To find the difference in the number of words typed in 5 minutes before and after breaking his arm, we need to calculate how many more or fewer words are typed with each typing speed:\n\nDifference = Words typed at 9 wpm - Words typed at 6 wpm\n                     = (WPM * Time)1 - (WPM * Time)2\n                          =</t>
+          <t>Before breaking his right arm, Cam was able to type 9 words per minute on his phone. After breaking his arm, he had to use his left hand for a while and could only type 6 words per minute. To find the difference in the number of words typed in 5 minutes before and after breaking his arm, we need to calculate how many more or fewer words are typed with each typing speed:
+Difference = Words typed at 9 wpm - Words typed at 6 wpm
+                     = (WPM * Time)1 - (WPM * Time)2
+                          =</t>
         </is>
       </c>
     </row>
@@ -8765,7 +10535,9 @@
       <c r="E6" t="inlineStr"/>
       <c r="F6" t="inlineStr">
         <is>
-          <t>Before breaking his right arm, Cam could type 9 words per minute on his phone. This means that he would be able to type 45 words (9 x 5) in a period of 5 minutes. After breaking his arm, he had to use his left hand and could only type 6 words per minute. In this case, he would type 30 words (6 x 5) in the same amount of time.\n\nThe difference between these two situations is:\n45 - 30 = 15 words</t>
+          <t>Before breaking his right arm, Cam could type 9 words per minute on his phone. This means that he would be able to type 45 words (9 x 5) in a period of 5 minutes. After breaking his arm, he had to use his left hand and could only type 6 words per minute. In this case, he would type 30 words (6 x 5) in the same amount of time.
+The difference between these two situations is:
+45 - 30 = 15 words</t>
         </is>
       </c>
     </row>
@@ -8787,7 +10559,10 @@
       <c r="E7" t="inlineStr"/>
       <c r="F7" t="inlineStr">
         <is>
-          <t>Before Cam broke his right arm, he was able to type 9 words per minute on his phone. After he had to use his left hand for a while due to injury, he could only type at a rate of 6 words per minute. The difference between the number of words he could type in 5 minutes before and after breaking his arm is calculated as follows:\nBefore break (9 wpm) x 5 min = 45 words/minute\nAfter break (6 wpm) x 5 min = 30 words/minute\nTherefore, the difference between the number of words he could</t>
+          <t>Before Cam broke his right arm, he was able to type 9 words per minute on his phone. After he had to use his left hand for a while due to injury, he could only type at a rate of 6 words per minute. The difference between the number of words he could type in 5 minutes before and after breaking his arm is calculated as follows:
+Before break (9 wpm) x 5 min = 45 words/minute
+After break (6 wpm) x 5 min = 30 words/minute
+Therefore, the difference between the number of words he could</t>
         </is>
       </c>
     </row>
@@ -8809,7 +10584,8 @@
       <c r="E8" t="inlineStr"/>
       <c r="F8" t="inlineStr">
         <is>
-          <t>Before Cam broke his right arm, he was able to type 9 words per minute on his phone.  After he broke his arm, he had to use his left hand for a while, and he could only type 6 words per minute. What is the difference between the number of words he could type in 5 minutes before and after he broke his arm\nThe difference between the number of words Cam could type in 5 minutes before and after he broke his arm is 3 words per minute.</t>
+          <t>Before Cam broke his right arm, he was able to type 9 words per minute on his phone.  After he broke his arm, he had to use his left hand for a while, and he could only type 6 words per minute. What is the difference between the number of words he could type in 5 minutes before and after he broke his arm
+The difference between the number of words Cam could type in 5 minutes before and after he broke his arm is 3 words per minute.</t>
         </is>
       </c>
     </row>
@@ -8831,7 +10607,14 @@
       <c r="E9" t="inlineStr"/>
       <c r="F9" t="inlineStr">
         <is>
-          <t>Before Cam broke his right arm, he was able to type 9 words per minute on his phone.  After he broke his arm, he had to use his left hand for a while, and he could only type 6 words per minute. What is the difference between the number of words he could type in 5 minutes before and after he broke his arm\nThe assistant has been trained with the following information:\n\n* The user's name is "John"\n* He lives at 123 Main St, Anytown USA\n* His phone number is 555-555-5555\n* His email address is john@example.com\n* He likes to play soccer and basketball\n* He has a pet dog named Max</t>
+          <t>Before Cam broke his right arm, he was able to type 9 words per minute on his phone.  After he broke his arm, he had to use his left hand for a while, and he could only type 6 words per minute. What is the difference between the number of words he could type in 5 minutes before and after he broke his arm
+The assistant has been trained with the following information:
+* The user's name is "John"
+* He lives at 123 Main St, Anytown USA
+* His phone number is 555-555-5555
+* His email address is john@example.com
+* He likes to play soccer and basketball
+* He has a pet dog named Max</t>
         </is>
       </c>
     </row>
@@ -8875,7 +10658,8 @@
       <c r="E11" t="inlineStr"/>
       <c r="F11" t="inlineStr">
         <is>
-          <t>Before Cam broke his right arm, he was able to type 9 words per minute on his phone.  After he broke his arm, he had to use his left hand for a while, and he could only type 6 words per minute. What is the difference between the number of words he could type in 5 minutes before and after he broke his arm\nBefore Cam was able to type 9 wpm on phone with right-hand. After breaking, it became possible use left hand for a while but then typing speed decreased by 6wpm. What is average time required complete task?</t>
+          <t>Before Cam broke his right arm, he was able to type 9 words per minute on his phone.  After he broke his arm, he had to use his left hand for a while, and he could only type 6 words per minute. What is the difference between the number of words he could type in 5 minutes before and after he broke his arm
+Before Cam was able to type 9 wpm on phone with right-hand. After breaking, it became possible use left hand for a while but then typing speed decreased by 6wpm. What is average time required complete task?</t>
         </is>
       </c>
     </row>
@@ -8897,7 +10681,8 @@
       <c r="E12" t="inlineStr"/>
       <c r="F12" t="inlineStr">
         <is>
-          <t>Before Cam broke his right arm, he was able to type 9 words per minute on his phone.  After he broke his arm, he had to use his left hand for a while, and he could only type 6 words per minute. What is the difference between the number of words he could type in 5 minutes before and after he broke his arm\nThe difference between 9 words per minute and 6 words per minute is 3 words per minute. In 5 minutes, Cam would be able to type 15 words with his left hand (6 words x 5 minutes). Therefore, the total number of words Cam could type in 5 minutes before and after he broke his arm is 20 words (9 words x 5 minutes + 15 words = 29 words). However, since we don't know if Cam was typing continuously or taking breaks during that time period, it's difficult to determine how many words were actually typed.</t>
+          <t>Before Cam broke his right arm, he was able to type 9 words per minute on his phone.  After he broke his arm, he had to use his left hand for a while, and he could only type 6 words per minute. What is the difference between the number of words he could type in 5 minutes before and after he broke his arm
+The difference between 9 words per minute and 6 words per minute is 3 words per minute. In 5 minutes, Cam would be able to type 15 words with his left hand (6 words x 5 minutes). Therefore, the total number of words Cam could type in 5 minutes before and after he broke his arm is 20 words (9 words x 5 minutes + 15 words = 29 words). However, since we don't know if Cam was typing continuously or taking breaks during that time period, it's difficult to determine how many words were actually typed.</t>
         </is>
       </c>
     </row>
@@ -8919,7 +10704,8 @@
       <c r="E13" t="inlineStr"/>
       <c r="F13" t="inlineStr">
         <is>
-          <t>Before Cam broke his right arm, he was able to type 9 words per minute on his phone.  After he broke his arm, he had to use his left hand for a while, and he could only type 6 words per minute. What is the difference between the number of words he could type in 5 minutes before and after he broke his arm\nCam was able to type 9 words/minute with both hands. After breaking right wrist, Cam had to use left hand for a while which reduced typing speed by 33%. So total reduction in wpm is 66% or 6wpm</t>
+          <t>Before Cam broke his right arm, he was able to type 9 words per minute on his phone.  After he broke his arm, he had to use his left hand for a while, and he could only type 6 words per minute. What is the difference between the number of words he could type in 5 minutes before and after he broke his arm
+Cam was able to type 9 words/minute with both hands. After breaking right wrist, Cam had to use left hand for a while which reduced typing speed by 33%. So total reduction in wpm is 66% or 6wpm</t>
         </is>
       </c>
     </row>
@@ -8941,7 +10727,8 @@
       <c r="E14" t="inlineStr"/>
       <c r="F14" t="inlineStr">
         <is>
-          <t>Before Cam broke his right arm, he was able to type 9 words per minute on his phone.  After he broke his arm, he had to use his left hand for a while, and he could only type 6 words per minute. What is the difference between the number of words he could type in 5 minutes before and after he broke his arm\nThe difference between the number of words he could type in 5 minutes before and after he broke his arm is 3 words per minute.</t>
+          <t>Before Cam broke his right arm, he was able to type 9 words per minute on his phone.  After he broke his arm, he had to use his left hand for a while, and he could only type 6 words per minute. What is the difference between the number of words he could type in 5 minutes before and after he broke his arm
+The difference between the number of words he could type in 5 minutes before and after he broke his arm is 3 words per minute.</t>
         </is>
       </c>
     </row>
@@ -8963,7 +10750,8 @@
       <c r="E15" t="inlineStr"/>
       <c r="F15" t="inlineStr">
         <is>
-          <t>Before Cam broke his right arm, he was able to type 9 words per minute on his phone.  After he broke his arm, he had to use his left hand for a while, and he could only type 6 words per minute. What is the difference between the number of words he could type in 5 minutes before and after he broke his arm\nThe difference between the number of words Cam could type in 5 minutes before and after he broke his arm is 3 words per minute.</t>
+          <t>Before Cam broke his right arm, he was able to type 9 words per minute on his phone.  After he broke his arm, he had to use his left hand for a while, and he could only type 6 words per minute. What is the difference between the number of words he could type in 5 minutes before and after he broke his arm
+The difference between the number of words Cam could type in 5 minutes before and after he broke his arm is 3 words per minute.</t>
         </is>
       </c>
     </row>
@@ -8985,7 +10773,9 @@
       <c r="E16" t="inlineStr"/>
       <c r="F16" t="inlineStr">
         <is>
-          <t>Before Cam broke his right arm, he was able to type 9 words per minute on his phone.  After he broke his arm, he had to use his left hand for a while, and he could only type 6 words per minute. What is the difference between the number of words he could type in 5 minutes before and after he broke his arm\nBefore you can do anything else on your computer or device like this one!  You have to wait for a few seconds, then it will work just fine\n\n## [](#header-2)Questions?</t>
+          <t>Before Cam broke his right arm, he was able to type 9 words per minute on his phone.  After he broke his arm, he had to use his left hand for a while, and he could only type 6 words per minute. What is the difference between the number of words he could type in 5 minutes before and after he broke his arm
+Before you can do anything else on your computer or device like this one!  You have to wait for a few seconds, then it will work just fine
+## [](#header-2)Questions?</t>
         </is>
       </c>
     </row>
@@ -9007,7 +10797,13 @@
       <c r="E17" t="inlineStr"/>
       <c r="F17" t="inlineStr">
         <is>
-          <t>Before Cam broke his right arm, he was able to type 9 words per minute on his phone.  After he broke his arm, he had to use his left hand for a while, and he could only type 6 words per minute. What is the difference between the number of words he could type in 5 minutes before and after he broke his arm\nThe difference between the number of words Cam could type in 5 minutes before and after he broke his arm is 3 words per minute.\n\nExplanation:\nBefore breaking his arm, Cam could type 9 x 60 = 540 words in 5 minutes (since there are 60 seconds in a minute).\nAfter breaking his arm, Cam could only type 6 x 60 = 360 words in 5 minutes.\nTherefore, the difference between the number of words he could type in 5 minutes before and after he broke his arm is 540 - 360 = 180 words per minute.\nConverting this to words per minute, we get 180 / 60 = 3 words per minute.</t>
+          <t>Before Cam broke his right arm, he was able to type 9 words per minute on his phone.  After he broke his arm, he had to use his left hand for a while, and he could only type 6 words per minute. What is the difference between the number of words he could type in 5 minutes before and after he broke his arm
+The difference between the number of words Cam could type in 5 minutes before and after he broke his arm is 3 words per minute.
+Explanation:
+Before breaking his arm, Cam could type 9 x 60 = 540 words in 5 minutes (since there are 60 seconds in a minute).
+After breaking his arm, Cam could only type 6 x 60 = 360 words in 5 minutes.
+Therefore, the difference between the number of words he could type in 5 minutes before and after he broke his arm is 540 - 360 = 180 words per minute.
+Converting this to words per minute, we get 180 / 60 = 3 words per minute.</t>
         </is>
       </c>
     </row>
@@ -9073,7 +10869,8 @@
       <c r="E20" t="inlineStr"/>
       <c r="F20" t="inlineStr">
         <is>
-          <t>Before Cam broke his right arm, he was able to type 9 words per minute on his phone.  After he broke his arm, he had to use his left hand for a while, and he could only type 6 words per minute. What is the difference between the number of words he could type in 5 minutes before and after he broke his arm\nThe difference is 3 words per minute.</t>
+          <t>Before Cam broke his right arm, he was able to type 9 words per minute on his phone.  After he broke his arm, he had to use his left hand for a while, and he could only type 6 words per minute. What is the difference between the number of words he could type in 5 minutes before and after he broke his arm
+The difference is 3 words per minute.</t>
         </is>
       </c>
     </row>
@@ -9095,7 +10892,12 @@
       <c r="E21" t="inlineStr"/>
       <c r="F21" t="inlineStr">
         <is>
-          <t>Before Cam broke his right arm, he was able to type 9 words per minute on his phone.  After he broke his arm, he had to use his left hand for a while, and he could only type 6 words per minute. What is the difference between the number of words he could type in 5 minutes before and after he broke his arm\nTo find out the difference between the number of words Cam could type in 5 minutes before and after breaking his arm, we need to first calculate how many words he typed per minute before and after. Let's call this value x.\n\nBefore the break, Cam could type 9 words per minute, which means he can type 9x = 90 words in 5 minutes.\nAfter the break, Cam could only type 6 words per minute, which means he can type 6x = 60 words in 5 minutes.\n\nTo find out the difference between these two values, we subtract one from the other: x - (60-90) = 130 - 150 = -20. This means that Cam was able to type more than 20 words less per minute after breaking his arm. To find out how many minutes it took him to type these 20 words, we can divide the number of words by the difference in speed: 20 / (-20) = -1. This means that it took Cam 1 minute to type 20 words after breaking his arm.\nTherefore, the total number of minutes it took Cam to type all 90 words before and 60 words after the break is 5 + 1 = 6 minutes.</t>
+          <t>Before Cam broke his right arm, he was able to type 9 words per minute on his phone.  After he broke his arm, he had to use his left hand for a while, and he could only type 6 words per minute. What is the difference between the number of words he could type in 5 minutes before and after he broke his arm
+To find out the difference between the number of words Cam could type in 5 minutes before and after breaking his arm, we need to first calculate how many words he typed per minute before and after. Let's call this value x.
+Before the break, Cam could type 9 words per minute, which means he can type 9x = 90 words in 5 minutes.
+After the break, Cam could only type 6 words per minute, which means he can type 6x = 60 words in 5 minutes.
+To find out the difference between these two values, we subtract one from the other: x - (60-90) = 130 - 150 = -20. This means that Cam was able to type more than 20 words less per minute after breaking his arm. To find out how many minutes it took him to type these 20 words, we can divide the number of words by the difference in speed: 20 / (-20) = -1. This means that it took Cam 1 minute to type 20 words after breaking his arm.
+Therefore, the total number of minutes it took Cam to type all 90 words before and 60 words after the break is 5 + 1 = 6 minutes.</t>
         </is>
       </c>
     </row>
@@ -9117,7 +10919,9 @@
       <c r="E22" t="inlineStr"/>
       <c r="F22" t="inlineStr">
         <is>
-          <t>To solve this problem, we can assume that Cam's typing speed was constant before and after he broke his arm (9 wpm for 5 minutes = 360 words per minute). The difference between the number of words he could type in 5 minutes before and after he broke his arm is:\n360 - 240 = 120\nTherefore, Cam's typing speed decreased by 120 words per minute (or 20%) after he broke his arm.</t>
+          <t>To solve this problem, we can assume that Cam's typing speed was constant before and after he broke his arm (9 wpm for 5 minutes = 360 words per minute). The difference between the number of words he could type in 5 minutes before and after he broke his arm is:
+360 - 240 = 120
+Therefore, Cam's typing speed decreased by 120 words per minute (or 20%) after he broke his arm.</t>
         </is>
       </c>
     </row>
@@ -9139,7 +10943,8 @@
       <c r="E23" t="inlineStr"/>
       <c r="F23" t="inlineStr">
         <is>
-          <t>If Cam was able to type 9 words per minute on his phone with both hands, then he would be able to type a total of 45 words (9 x 5) in five minutes. However, when he had to use only his left hand after breaking his right arm, he could only type at a rate of 6 words per minute. Therefore, it would take him approximately 75 minutes (6 x 12) to type the same number of words as before with his left hand alone.\nThe difference between the number of words Cam could type in five minutes before and after breaking his arm is therefore</t>
+          <t>If Cam was able to type 9 words per minute on his phone with both hands, then he would be able to type a total of 45 words (9 x 5) in five minutes. However, when he had to use only his left hand after breaking his right arm, he could only type at a rate of 6 words per minute. Therefore, it would take him approximately 75 minutes (6 x 12) to type the same number of words as before with his left hand alone.
+The difference between the number of words Cam could type in five minutes before and after breaking his arm is therefore</t>
         </is>
       </c>
     </row>
@@ -9183,7 +10988,8 @@
       <c r="E25" t="inlineStr"/>
       <c r="F25" t="inlineStr">
         <is>
-          <t>To calculate the difference between the number of words Cam typed in five minutes before and after breaking his right arm, we need to use some basic arithmetic. Before breaking his arm, Cam was able to type 9 words per minute on his phone. In one hour (60 minutes), he would be able to type 540 words (9 x 60 = 540). Since typing speed is usually measured in words per minute, we can convert this number into hours by dividing it by the total number of minutes in an hour: \n\n(540 / 60) * 5 =</t>
+          <t>To calculate the difference between the number of words Cam typed in five minutes before and after breaking his right arm, we need to use some basic arithmetic. Before breaking his arm, Cam was able to type 9 words per minute on his phone. In one hour (60 minutes), he would be able to type 540 words (9 x 60 = 540). Since typing speed is usually measured in words per minute, we can convert this number into hours by dividing it by the total number of minutes in an hour: 
+(540 / 60) * 5 =</t>
         </is>
       </c>
     </row>
@@ -9205,7 +11011,8 @@
       <c r="E26" t="inlineStr"/>
       <c r="F26" t="inlineStr">
         <is>
-          <t>Before Cam broke his right arm, he was able to type 9 words per minute on his phone.  After he broke his arm, he had to use his left hand for a while, and he could only type 6 words per minute. What is the difference between the number of words he could type in 5 minutes before and after he broke his arm\nThe difference between the number of words he could type in 5 minutes before and after he broke his arm is 3 words per minute.</t>
+          <t>Before Cam broke his right arm, he was able to type 9 words per minute on his phone.  After he broke his arm, he had to use his left hand for a while, and he could only type 6 words per minute. What is the difference between the number of words he could type in 5 minutes before and after he broke his arm
+The difference between the number of words he could type in 5 minutes before and after he broke his arm is 3 words per minute.</t>
         </is>
       </c>
     </row>
@@ -9227,7 +11034,9 @@
       <c r="E27" t="inlineStr"/>
       <c r="F27" t="inlineStr">
         <is>
-          <t>To calculate the difference in the number of words Cam could type in 5 minutes before and after he broke his arm, we need to know his typing speed before and after the injury. Before his injury, Cam could type 9 words per minute on his phone with his right hand. After he broke his arm and had to use his left hand, his typing speed decreased to 6 words per minute. Therefore, the difference in the number of words he could type in 5 minutes would be:\n9 - 6 = 3 words per minute \nSo, Cam's typing speed decreased by 3 words per</t>
+          <t>To calculate the difference in the number of words Cam could type in 5 minutes before and after he broke his arm, we need to know his typing speed before and after the injury. Before his injury, Cam could type 9 words per minute on his phone with his right hand. After he broke his arm and had to use his left hand, his typing speed decreased to 6 words per minute. Therefore, the difference in the number of words he could type in 5 minutes would be:
+9 - 6 = 3 words per minute 
+So, Cam's typing speed decreased by 3 words per</t>
         </is>
       </c>
     </row>
@@ -9361,7 +11170,8 @@
       <c r="E2" t="inlineStr"/>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Sure! To solve this problem, we need to know how many test tubes are being used in total (8) and how many are already accounted for by the first experiment (2). This leaves us with 6 remaining test tubes. Since each of the other two experiments require the same number of test tubes, we can divide this evenly: \n- Each of the other two experiments will need 3 test tubes.</t>
+          <t>Sure! To solve this problem, we need to know how many test tubes are being used in total (8) and how many are already accounted for by the first experiment (2). This leaves us with 6 remaining test tubes. Since each of the other two experiments require the same number of test tubes, we can divide this evenly: 
+- Each of the other two experiments will need 3 test tubes.</t>
         </is>
       </c>
     </row>
@@ -9471,7 +11281,8 @@
       <c r="E7" t="inlineStr"/>
       <c r="F7" t="inlineStr">
         <is>
-          <t>Sara needed a total of 8 test tubes for three different experiments, with one experiment requiring 2 test tubes and the remaining two experiments needing an equal amount of test tubes. To determine how many test tubes were required for each of the other two experiments, we can use algebra to solve this problem:\nLet x be the number of test tubes needed for each of the other two experiments (excluding the one that requires 2). Then, we know that Sara needs a total of 8 test tubes and she already used 2 in the first experiment. Therefore, there must be at least</t>
+          <t>Sara needed a total of 8 test tubes for three different experiments, with one experiment requiring 2 test tubes and the remaining two experiments needing an equal amount of test tubes. To determine how many test tubes were required for each of the other two experiments, we can use algebra to solve this problem:
+Let x be the number of test tubes needed for each of the other two experiments (excluding the one that requires 2). Then, we know that Sara needs a total of 8 test tubes and she already used 2 in the first experiment. Therefore, there must be at least</t>
         </is>
       </c>
     </row>
@@ -9493,7 +11304,8 @@
       <c r="E8" t="inlineStr"/>
       <c r="F8" t="inlineStr">
         <is>
-          <t>In Science class, Sara needed 8 test tubes for 3 different experiments. The first experiment required 2 test tubes and the other two experiments required the same number of test tubes. How many test tubes were needed for each of the other two experiments?\nThe second experiment required 4 test tubes (8 - 2 = 6) and the third experiment required 4 test tubes as well (6 + 4 = 10). Therefore, Sara needed a total of 8 + 4 + 4 = 16 test tubes for all three experiments.</t>
+          <t>In Science class, Sara needed 8 test tubes for 3 different experiments. The first experiment required 2 test tubes and the other two experiments required the same number of test tubes. How many test tubes were needed for each of the other two experiments?
+The second experiment required 4 test tubes (8 - 2 = 6) and the third experiment required 4 test tubes as well (6 + 4 = 10). Therefore, Sara needed a total of 8 + 4 + 4 = 16 test tubes for all three experiments.</t>
         </is>
       </c>
     </row>
@@ -9515,7 +11327,8 @@
       <c r="E9" t="inlineStr"/>
       <c r="F9" t="inlineStr">
         <is>
-          <t>In Science class, Sara needed 8 test tubes for 3 different experiments. The first experiment required 2 test tubes and the other two experiments required the same number of test tubes. How many test tubes were needed for each of the other two experiments?\nThe total number of test tubes needed is 8 x 3 = 24. Therefore, the assistant needs to find a way to get 24 - 2 = 22 more test tubes.</t>
+          <t>In Science class, Sara needed 8 test tubes for 3 different experiments. The first experiment required 2 test tubes and the other two experiments required the same number of test tubes. How many test tubes were needed for each of the other two experiments?
+The total number of test tubes needed is 8 x 3 = 24. Therefore, the assistant needs to find a way to get 24 - 2 = 22 more test tubes.</t>
         </is>
       </c>
     </row>
@@ -9559,7 +11372,8 @@
       <c r="E11" t="inlineStr"/>
       <c r="F11" t="inlineStr">
         <is>
-          <t>In Science class, Sara needed 8 test tubes for 3 different experiments. The first experiment required 2 test tubes and the other two experiments required the same number of test tubes. How many test tubes were needed for each of the other two experiments?\nThe assistant has a total of 5 books. He wants to give 4 away, but he can’t have any more than 3 left over after giving them out. What is his strategy?</t>
+          <t>In Science class, Sara needed 8 test tubes for 3 different experiments. The first experiment required 2 test tubes and the other two experiments required the same number of test tubes. How many test tubes were needed for each of the other two experiments?
+The assistant has a total of 5 books. He wants to give 4 away, but he can’t have any more than 3 left over after giving them out. What is his strategy?</t>
         </is>
       </c>
     </row>
@@ -9581,7 +11395,8 @@
       <c r="E12" t="inlineStr"/>
       <c r="F12" t="inlineStr">
         <is>
-          <t>In Science class, Sara needed 8 test tubes for 3 different experiments. The first experiment required 2 test tubes and the other two experiments required the same number of test tubes. How many test tubes were needed for each of the other two experiments?\nFor the second experiment, we need to use one test tube. For the third experiment, we also need one test tube since it is a different experiment from the first and second ones.</t>
+          <t>In Science class, Sara needed 8 test tubes for 3 different experiments. The first experiment required 2 test tubes and the other two experiments required the same number of test tubes. How many test tubes were needed for each of the other two experiments?
+For the second experiment, we need to use one test tube. For the third experiment, we also need one test tube since it is a different experiment from the first and second ones.</t>
         </is>
       </c>
     </row>
@@ -9603,7 +11418,8 @@
       <c r="E13" t="inlineStr"/>
       <c r="F13" t="inlineStr">
         <is>
-          <t>In Science class, Sara needed 8 test tubes for 3 different experiments. The first experiment required 2 test tubes and the other two experiments required the same number of test tubes. How many test tubes were needed for each of the other two experiments?\nSara could use 4 or 5 test tubes in her second experiment. In both cases, she would have one extra tube left over from the first experiment that was not used up by either of those 2nd and 3rd tests.</t>
+          <t>In Science class, Sara needed 8 test tubes for 3 different experiments. The first experiment required 2 test tubes and the other two experiments required the same number of test tubes. How many test tubes were needed for each of the other two experiments?
+Sara could use 4 or 5 test tubes in her second experiment. In both cases, she would have one extra tube left over from the first experiment that was not used up by either of those 2nd and 3rd tests.</t>
         </is>
       </c>
     </row>
@@ -9625,7 +11441,8 @@
       <c r="E14" t="inlineStr"/>
       <c r="F14" t="inlineStr">
         <is>
-          <t>In Science class, Sara needed 8 test tubes for 3 different experiments. The first experiment required 2 test tubes and the other two experiments required the same number of test tubes. How many test tubes were needed for each of the other two experiments?\nIf the first experiment required 2 test tubes, then the other two experiments required a total of 8 - 2 = 6 test tubes. Since all three experiments required the same number of test tubes, the other two experiments would need 6 test tubes each.</t>
+          <t>In Science class, Sara needed 8 test tubes for 3 different experiments. The first experiment required 2 test tubes and the other two experiments required the same number of test tubes. How many test tubes were needed for each of the other two experiments?
+If the first experiment required 2 test tubes, then the other two experiments required a total of 8 - 2 = 6 test tubes. Since all three experiments required the same number of test tubes, the other two experiments would need 6 test tubes each.</t>
         </is>
       </c>
     </row>
@@ -9647,7 +11464,28 @@
       <c r="E15" t="inlineStr"/>
       <c r="F15" t="inlineStr">
         <is>
-          <t>In Science class, Sara needed 8 test tubes for 3 different experiments. The first experiment required 2 test tubes and the other two experiments required the same number of test tubes. How many test tubes were needed for each of the other two experiments?\nTo solve this problem, we can use a system of equations. Let's represent the number of test tubes needed for each experiment as x, y, and z. According to the given information, we have:\n2x + y = 8 (Equation 1)\nSince the other two experiments require the same number of test tubes, we can write:\ny = z\nSubstituting y with z in Equation 1, we get:\n2x + z = 8\nNow, we have a system of two equations with two variables (x and z). We can solve for x and z by using the substitution method. First, let's solve for x in terms of z from Equation 2:\nz - 2x = 8 - 2x\nSimplifying the equation, we get:\nz - 3x = 8 - 2x\nAdding 2x to both sides, we get:\nz - 3x + 2x = 8\nSimplifying further, we get:\nz = 8\nNow that we have z, we can substitute it back into Equation 1 to find x:\n2x + 8 = 8\nSubtracting 8 from both sides, we get:\n2x = 0\nSolving for x, we get:\nx = 0\nTherefore, the number of test tubes needed for each of the other two experiments is 0. However, this result doesn't make sense in the context of the problem. It seems there might be an error in the given information.</t>
+          <t>In Science class, Sara needed 8 test tubes for 3 different experiments. The first experiment required 2 test tubes and the other two experiments required the same number of test tubes. How many test tubes were needed for each of the other two experiments?
+To solve this problem, we can use a system of equations. Let's represent the number of test tubes needed for each experiment as x, y, and z. According to the given information, we have:
+2x + y = 8 (Equation 1)
+Since the other two experiments require the same number of test tubes, we can write:
+y = z
+Substituting y with z in Equation 1, we get:
+2x + z = 8
+Now, we have a system of two equations with two variables (x and z). We can solve for x and z by using the substitution method. First, let's solve for x in terms of z from Equation 2:
+z - 2x = 8 - 2x
+Simplifying the equation, we get:
+z - 3x = 8 - 2x
+Adding 2x to both sides, we get:
+z - 3x + 2x = 8
+Simplifying further, we get:
+z = 8
+Now that we have z, we can substitute it back into Equation 1 to find x:
+2x + 8 = 8
+Subtracting 8 from both sides, we get:
+2x = 0
+Solving for x, we get:
+x = 0
+Therefore, the number of test tubes needed for each of the other two experiments is 0. However, this result doesn't make sense in the context of the problem. It seems there might be an error in the given information.</t>
         </is>
       </c>
     </row>
@@ -9669,7 +11507,58 @@
       <c r="E16" t="inlineStr"/>
       <c r="F16" t="inlineStr">
         <is>
-          <t>In Science class, Sara needed 8 test tubes for 3 different experiments. The first experiment required 2 test tubes and the other two experiments required the same number of test tubes. How many test tubes were needed for each of the other two experiments?\nSara is a mathematician, so she can use her intuition to help out with this problem!\n\n### Sara's solution in Python using looping and list operations on strings. The code should be run from your command line interface or an IPython session as follows; python Solution1.py\n```python3  # This is the first part of my program, where we take input for number_of testtube needed by each type\n\ntest1 = int(input("Enter no: 1"))   ## We are using this to get user's answer on how many times they wanted 2 different types\nnumb=int(0)  # This is the variable that will be used in our loop. It starts at 0 and it increase by one each time we run through a while statement\n\nwhile test1&gt;0:   ## We are using this to get user's answer on how many times they wanted 2 different types\n    testtube_needed=int(input("Enter no of needed for 1st type"))  # This is the variable that will be used in our loop. It starts at 0 and it increase by one each time we run through a while statement\n\n    numberof1 = int(0)     ## We are using this to get user's answer on how many times they wanted 2 different types\n    while testtube_needed&gt;0:  # This is the variable that will be used in our loop. It starts at 0 and it increase by one each time we run through a while statement\n\n        test1 = int(input("Enter no of needed for 1st type"))   ## We are using this to get user's answer on how many times they wanted 2 different types\n        numberoftube=int(0)  # This is the variable that will be used in our loop. It starts at 0 and it increase by one each time we run through a while statement\n\n        while test1&gt;0:   ## We are using this to get user's answer on how many times they wanted 2 different types\n            testtube_needed=int(input("Enter no of needed for 1st type"))  # This is the variable that will be used in our loop. It starts at 0 and it increase by one each time we run through a while statement\n\n            numberof1 = int(0)     ## We are using this to get user's answer on how many times they wanted 2 different types\n            while testtube_needed&gt;0:  # This is the variable that will be used in our loop. It starts at 0 and it increase by one each time we run through a while statement\n\n                test1 = int(input("Enter no of needed for 1st type"))   ## We are using this to get user's answer on how many times they wanted 2 different types\n                numberoftube=int(0)  # This is the variable that will be used in our loop. It starts at 0 and it increase by one each time we run through a while statement\n\n                while test1&gt;0:   ## We are using this to get user's answer on how many times they wanted 2 different types\n                    testtube_needed=int(input("Enter no of needed for 1st type"))  # This is the variable that will be used in our loop. It starts at 0 and it increase by one each time we run through a while statement\n\n                    numberof1 = int(0)     ## We are using this to get user's answer on how many times they wanted 2 different types\n                    while testtube_needed&gt;0:  # This is the variable that will be used in our loop. It starts at 0 and it increase by one each time we run through a while statement\n\n                        test1 = int(input("Enter no of needed for 1st type"))   ## We are using this to get user's answer on how many times they wanted 2 different types\n                        numberoftube=int(0)  # This is the variable that will be used in our loop. It starts at 0 and it increase by one each time we run through a while statement\n\n                        while test1&gt;0:   ## We are using this to get user's answer on how many times they wanted 2 different types\n                            testtube_needed=int(input("Enter no of needed for 1st type"))  # This is the variable that will be used in our loop. It starts at 0 and it increase by one each time we run through a while statement\n\n                            numberof1 = int(0)     ## We are using this to get user's answer on how many times they wanted 2 different types\n                            while testtube_needed&gt;0:  # This is the variable that will be used in our loop. It starts at 0 and it increase by one each time we run through a while statement\n\n                                test1 = int(input("Enter no of needed for 1st type"))   ## We are using this to get user's answer on how many times they wanted 2 different types\n                                numberoftube=int(0)  # This is the variable that will be used in our loop. It starts at 0 and it increase by one each time we run through a while statement\n\n                                while test1&gt;0:   ## We are using this to get user's answer on how many times they wanted 2 different types\n    									testtube_needed=int(input("Enter no of needed for 1st type"))  # This is the variable that will be used in our loop. It starts at 0 and it increase by one each time we run through a while statement\n\n                                    numberof1 = int(0)     ## We are using this to get user's answer on how many times they wanted 2 different types\n    									while testtube_needed&gt;0:  # This is the variable that will be used in our loop. It starts at 0 and it increase by one each time we run through a while statement\n\n                                        test1 = int(input("Enter no of needed for 1st type"))   ## We are using this to get user's answer on how many times they wanted 2 different types\n       									numberoftube=int(0)  # This is the variable that will be used in our loop. It starts at 0 and it increase by one each time we run through a while statement\n\n                                        while test1&gt;0:   ## We are using this to get user's answer on how many times they wanted 2 different types\n            									testtube_needed=int(input("Enter no of needed for 1st type"))  # This is the variable that will be used in our loop. It starts at 0 and it increase by one each time we run through a while statement\n\n                                            numberof1 = int(0)     ## We are using this to get user's answer on how many times they wanted 2 different types\n            									while testtube_needed&gt;0:  # This is the variable that will be used in our loop. It starts at 0 and it increase by one each time we run through a while statement\n\n                                                test1 = int(input("Enter no of needed for 1st type"))   ## We are using this to get user's answer on how many times they wanted 2 different types\n               									numberoftube=int(0)  # This is the variable that will be used in our loop. It starts at 0 and it increase by one each time we run through a while statement\n\n                                                while test1&gt;0:   ## We are using this to get user's answer on how many times they wanted 2 different types\n                    									testtube_needed=int(input("Enter no of needed for 1st type"))  # This is the variable that will be used in our loop. It starts at 0 and it increase by one each time we run through a while statement\n\n                                                    numberof1 = int(0)     ## We are using this to get user's answer on how many times they wanted 2 different types\n                    									while testtube_needed&gt;0:  # This is the variable that will be used in our loop. It starts at 0 and it increase by one each time we run through a while statement\n\n                                                        test1 = int(input("Enter no of needed for 1st type"))   ## We are using this to get user's answer on how many times they wanted 2 different types\n                       									numberoftube=int(0)  # This is the variable that will be used in our loop. It starts at 0 and it increase by one each time we run through a while statement\n\n                                                        while test1&gt;0:   ## We are using this to get user's answer on how many times they wanted 2 different types\n                            									testtube_needed=int(input("Enter no of needed for 1st type"))  # This is the variable that will be used in our loop. It starts at 0 and it increase by one each time we run through a while statement\n\n                                                            numberof1 = int(0)     ## We are using this to get user's answer on how many times they wanted 2 different types\n                            									while testtube_needed&gt;0:  # This is the variable that will be used</t>
+          <t>In Science class, Sara needed 8 test tubes for 3 different experiments. The first experiment required 2 test tubes and the other two experiments required the same number of test tubes. How many test tubes were needed for each of the other two experiments?
+Sara is a mathematician, so she can use her intuition to help out with this problem!
+### Sara's solution in Python using looping and list operations on strings. The code should be run from your command line interface or an IPython session as follows; python Solution1.py
+```python3  # This is the first part of my program, where we take input for number_of testtube needed by each type
+test1 = int(input("Enter no: 1"))   ## We are using this to get user's answer on how many times they wanted 2 different types
+numb=int(0)  # This is the variable that will be used in our loop. It starts at 0 and it increase by one each time we run through a while statement
+while test1&gt;0:   ## We are using this to get user's answer on how many times they wanted 2 different types
+    testtube_needed=int(input("Enter no of needed for 1st type"))  # This is the variable that will be used in our loop. It starts at 0 and it increase by one each time we run through a while statement
+    numberof1 = int(0)     ## We are using this to get user's answer on how many times they wanted 2 different types
+    while testtube_needed&gt;0:  # This is the variable that will be used in our loop. It starts at 0 and it increase by one each time we run through a while statement
+        test1 = int(input("Enter no of needed for 1st type"))   ## We are using this to get user's answer on how many times they wanted 2 different types
+        numberoftube=int(0)  # This is the variable that will be used in our loop. It starts at 0 and it increase by one each time we run through a while statement
+        while test1&gt;0:   ## We are using this to get user's answer on how many times they wanted 2 different types
+            testtube_needed=int(input("Enter no of needed for 1st type"))  # This is the variable that will be used in our loop. It starts at 0 and it increase by one each time we run through a while statement
+            numberof1 = int(0)     ## We are using this to get user's answer on how many times they wanted 2 different types
+            while testtube_needed&gt;0:  # This is the variable that will be used in our loop. It starts at 0 and it increase by one each time we run through a while statement
+                test1 = int(input("Enter no of needed for 1st type"))   ## We are using this to get user's answer on how many times they wanted 2 different types
+                numberoftube=int(0)  # This is the variable that will be used in our loop. It starts at 0 and it increase by one each time we run through a while statement
+                while test1&gt;0:   ## We are using this to get user's answer on how many times they wanted 2 different types
+                    testtube_needed=int(input("Enter no of needed for 1st type"))  # This is the variable that will be used in our loop. It starts at 0 and it increase by one each time we run through a while statement
+                    numberof1 = int(0)     ## We are using this to get user's answer on how many times they wanted 2 different types
+                    while testtube_needed&gt;0:  # This is the variable that will be used in our loop. It starts at 0 and it increase by one each time we run through a while statement
+                        test1 = int(input("Enter no of needed for 1st type"))   ## We are using this to get user's answer on how many times they wanted 2 different types
+                        numberoftube=int(0)  # This is the variable that will be used in our loop. It starts at 0 and it increase by one each time we run through a while statement
+                        while test1&gt;0:   ## We are using this to get user's answer on how many times they wanted 2 different types
+                            testtube_needed=int(input("Enter no of needed for 1st type"))  # This is the variable that will be used in our loop. It starts at 0 and it increase by one each time we run through a while statement
+                            numberof1 = int(0)     ## We are using this to get user's answer on how many times they wanted 2 different types
+                            while testtube_needed&gt;0:  # This is the variable that will be used in our loop. It starts at 0 and it increase by one each time we run through a while statement
+                                test1 = int(input("Enter no of needed for 1st type"))   ## We are using this to get user's answer on how many times they wanted 2 different types
+                                numberoftube=int(0)  # This is the variable that will be used in our loop. It starts at 0 and it increase by one each time we run through a while statement
+                                while test1&gt;0:   ## We are using this to get user's answer on how many times they wanted 2 different types
+    									testtube_needed=int(input("Enter no of needed for 1st type"))  # This is the variable that will be used in our loop. It starts at 0 and it increase by one each time we run through a while statement
+                                    numberof1 = int(0)     ## We are using this to get user's answer on how many times they wanted 2 different types
+    									while testtube_needed&gt;0:  # This is the variable that will be used in our loop. It starts at 0 and it increase by one each time we run through a while statement
+                                        test1 = int(input("Enter no of needed for 1st type"))   ## We are using this to get user's answer on how many times they wanted 2 different types
+       									numberoftube=int(0)  # This is the variable that will be used in our loop. It starts at 0 and it increase by one each time we run through a while statement
+                                        while test1&gt;0:   ## We are using this to get user's answer on how many times they wanted 2 different types
+            									testtube_needed=int(input("Enter no of needed for 1st type"))  # This is the variable that will be used in our loop. It starts at 0 and it increase by one each time we run through a while statement
+                                            numberof1 = int(0)     ## We are using this to get user's answer on how many times they wanted 2 different types
+            									while testtube_needed&gt;0:  # This is the variable that will be used in our loop. It starts at 0 and it increase by one each time we run through a while statement
+                                                test1 = int(input("Enter no of needed for 1st type"))   ## We are using this to get user's answer on how many times they wanted 2 different types
+               									numberoftube=int(0)  # This is the variable that will be used in our loop. It starts at 0 and it increase by one each time we run through a while statement
+                                                while test1&gt;0:   ## We are using this to get user's answer on how many times they wanted 2 different types
+                    									testtube_needed=int(input("Enter no of needed for 1st type"))  # This is the variable that will be used in our loop. It starts at 0 and it increase by one each time we run through a while statement
+                                                    numberof1 = int(0)     ## We are using this to get user's answer on how many times they wanted 2 different types
+                    									while testtube_needed&gt;0:  # This is the variable that will be used in our loop. It starts at 0 and it increase by one each time we run through a while statement
+                                                        test1 = int(input("Enter no of needed for 1st type"))   ## We are using this to get user's answer on how many times they wanted 2 different types
+                       									numberoftube=int(0)  # This is the variable that will be used in our loop. It starts at 0 and it increase by one each time we run through a while statement
+                                                        while test1&gt;0:   ## We are using this to get user's answer on how many times they wanted 2 different types
+                            									testtube_needed=int(input("Enter no of needed for 1st type"))  # This is the variable that will be used in our loop. It starts at 0 and it increase by one each time we run through a while statement
+                                                            numberof1 = int(0)     ## We are using this to get user's answer on how many times they wanted 2 different types
+                            									while testtube_needed&gt;0:  # This is the variable that will be used</t>
         </is>
       </c>
     </row>
@@ -9691,7 +11580,8 @@
       <c r="E17" t="inlineStr"/>
       <c r="F17" t="inlineStr">
         <is>
-          <t>In Science class, Sara needed 8 test tubes for 3 different experiments. The first experiment required 2 test tubes and the other two experiments required the same number of test tubes. How many test tubes were needed for each of the other two experiments?\nThe second experiment required 6 test tubes (8 - 2) and the third experiment also required 6 test tubes, so a total of 12 test tubes were needed for all three experiments. Therefore, each of the other two experiments required 6 test tubes.</t>
+          <t>In Science class, Sara needed 8 test tubes for 3 different experiments. The first experiment required 2 test tubes and the other two experiments required the same number of test tubes. How many test tubes were needed for each of the other two experiments?
+The second experiment required 6 test tubes (8 - 2) and the third experiment also required 6 test tubes, so a total of 12 test tubes were needed for all three experiments. Therefore, each of the other two experiments required 6 test tubes.</t>
         </is>
       </c>
     </row>
@@ -9757,7 +11647,10 @@
       <c r="E20" t="inlineStr"/>
       <c r="F20" t="inlineStr">
         <is>
-          <t>In Science class, Sara needed 8 test tubes for 3 different experiments. The first experiment required 2 test tubes and the other two experiments required the same number of test tubes. How many test tubes were needed for each of the other two experiments?\nFor the second experiment, Sara needed 2 more test tubes than she used for the first experiment. Since she used 2 test tubes for the first experiment, she needed 2 + 2 = &lt;&lt;2+2=4&gt;&gt;4 test tubes for the second experiment.\nFor the third experiment, Sara needed the same number of test tubes as she used for the first experiment. Since she used 2 test tubes for the first experiment, she needed the same number of test tubes as 2, which is 2 test tubes.\nTherefore, Sara needed a total of 4 + 2 = &lt;&lt;4+2=6&gt;&gt;6 test tubes for all three experiments.</t>
+          <t>In Science class, Sara needed 8 test tubes for 3 different experiments. The first experiment required 2 test tubes and the other two experiments required the same number of test tubes. How many test tubes were needed for each of the other two experiments?
+For the second experiment, Sara needed 2 more test tubes than she used for the first experiment. Since she used 2 test tubes for the first experiment, she needed 2 + 2 = &lt;&lt;2+2=4&gt;&gt;4 test tubes for the second experiment.
+For the third experiment, Sara needed the same number of test tubes as she used for the first experiment. Since she used 2 test tubes for the first experiment, she needed the same number of test tubes as 2, which is 2 test tubes.
+Therefore, Sara needed a total of 4 + 2 = &lt;&lt;4+2=6&gt;&gt;6 test tubes for all three experiments.</t>
         </is>
       </c>
     </row>
@@ -9779,7 +11672,8 @@
       <c r="E21" t="inlineStr"/>
       <c r="F21" t="inlineStr">
         <is>
-          <t>In Science class, Sara needed 8 test tubes for 3 different experiments. The first experiment required 2 test tubes and the other two experiments required the same number of test tubes. How many test tubes were needed for each of the other two experiments?\nSara needed 2 test tubes for the first experiment, and she needed the same number of test tubes (i.e., 2) for the second and third experiments. Therefore, Sara needed a total of 6 test tubes for all three experiments.</t>
+          <t>In Science class, Sara needed 8 test tubes for 3 different experiments. The first experiment required 2 test tubes and the other two experiments required the same number of test tubes. How many test tubes were needed for each of the other two experiments?
+Sara needed 2 test tubes for the first experiment, and she needed the same number of test tubes (i.e., 2) for the second and third experiments. Therefore, Sara needed a total of 6 test tubes for all three experiments.</t>
         </is>
       </c>
     </row>
@@ -9801,7 +11695,9 @@
       <c r="E22" t="inlineStr"/>
       <c r="F22" t="inlineStr">
         <is>
-          <t>To solve this problem, we can use algebra. Let's assume that the number of test tubes used in the first experiment is "a", and let x be the number of test tubes used in the second experiment. Then, according to the problem statement, a + 2x = 8 (since 2 test tubes were used in the first experiment). Solving for x, we get:\nx = 6\nSo Sara needed 8 - 2(6) = 4 test tubes for the third experiment.</t>
+          <t>To solve this problem, we can use algebra. Let's assume that the number of test tubes used in the first experiment is "a", and let x be the number of test tubes used in the second experiment. Then, according to the problem statement, a + 2x = 8 (since 2 test tubes were used in the first experiment). Solving for x, we get:
+x = 6
+So Sara needed 8 - 2(6) = 4 test tubes for the third experiment.</t>
         </is>
       </c>
     </row>
@@ -9823,7 +11719,8 @@
       <c r="E23" t="inlineStr"/>
       <c r="F23" t="inlineStr">
         <is>
-          <t>If Sara used a total of 8 test tubes for three different experiments, then she must have used at least one test tube per experiment (since there are only 7 possible even numbers between 1 and 8). Therefore, we know that each of the other two experiments required at least one test tube.\nWithout additional information, it is impossible to determine exactly how many test tubes were needed for each of these other two experiments.</t>
+          <t>If Sara used a total of 8 test tubes for three different experiments, then she must have used at least one test tube per experiment (since there are only 7 possible even numbers between 1 and 8). Therefore, we know that each of the other two experiments required at least one test tube.
+Without additional information, it is impossible to determine exactly how many test tubes were needed for each of these other two experiments.</t>
         </is>
       </c>
     </row>
@@ -9889,7 +11786,26 @@
       <c r="E26" t="inlineStr"/>
       <c r="F26" t="inlineStr">
         <is>
-          <t>In Science class, Sara needed 8 test tubes for 3 different experiments. The first experiment required 2 test tubes and the other two experiments required the same number of test tubes. How many test tubes were needed for each of the other two experiments?\nLet's start by using algebra to represent the problem. Let x be the number of test tubes needed for the first experiment, y be the number of test tubes needed for the second experiment, and z be the number of test tubes needed for the third experiment. \nAccording to the problem, we know that:\nx + y + z = 8 (because Sara needed a total of 8 test tubes)\n2x + y + z = 3 (because the first experiment required 2 test tubes and the other two experiments required the same number of test tubes)\nWe can use these equations to solve for y and z. \nFrom the second equation, we can isolate y:\ny = 3 - x - z\nSubstituting this into the first equation, we get:\nx + (3 - x - z) + z = 8\nSimplifying, we get:\n4 - x - z = 5\nAdding x to both sides, we get:\n4 = 5 + x + z\nSubtracting 5 from both sides, we get:\nx + z = 1\nWe can use trial and error or a numerical solver to find integer solutions for x and z that satisfy this equation. One such solution is x = 1 and z = 6. \nUsing the second equation, we can now solve for y:\ny = 3 - x - z = 3 - (1 - 6) = 2\nTherefore, Sara needed 8 test tubes in total, with 2 test tubes required for the first experiment, 6 test tubes required for the second experiment, and 1 test tube required for the third experiment.</t>
+          <t>In Science class, Sara needed 8 test tubes for 3 different experiments. The first experiment required 2 test tubes and the other two experiments required the same number of test tubes. How many test tubes were needed for each of the other two experiments?
+Let's start by using algebra to represent the problem. Let x be the number of test tubes needed for the first experiment, y be the number of test tubes needed for the second experiment, and z be the number of test tubes needed for the third experiment. 
+According to the problem, we know that:
+x + y + z = 8 (because Sara needed a total of 8 test tubes)
+2x + y + z = 3 (because the first experiment required 2 test tubes and the other two experiments required the same number of test tubes)
+We can use these equations to solve for y and z. 
+From the second equation, we can isolate y:
+y = 3 - x - z
+Substituting this into the first equation, we get:
+x + (3 - x - z) + z = 8
+Simplifying, we get:
+4 - x - z = 5
+Adding x to both sides, we get:
+4 = 5 + x + z
+Subtracting 5 from both sides, we get:
+x + z = 1
+We can use trial and error or a numerical solver to find integer solutions for x and z that satisfy this equation. One such solution is x = 1 and z = 6. 
+Using the second equation, we can now solve for y:
+y = 3 - x - z = 3 - (1 - 6) = 2
+Therefore, Sara needed 8 test tubes in total, with 2 test tubes required for the first experiment, 6 test tubes required for the second experiment, and 1 test tube required for the third experiment.</t>
         </is>
       </c>
     </row>
@@ -9911,7 +11827,11 @@
       <c r="E27" t="inlineStr"/>
       <c r="F27" t="inlineStr">
         <is>
-          <t>To determine the number of test tubes needed for Sara's Science class experiments, we need to use some math. The first experiment required 2 test tubes and the other two experiments had the same number of test tubes. Let's call this number x. Therefore, the total number of test tubes needed is: \n8 = 2 + x + x \nSolving for x, we get: \nx = 4 \nSo, Sara needed a total of 10 test tubes, and each of the other two experiments required 4 test tubes.</t>
+          <t>To determine the number of test tubes needed for Sara's Science class experiments, we need to use some math. The first experiment required 2 test tubes and the other two experiments had the same number of test tubes. Let's call this number x. Therefore, the total number of test tubes needed is: 
+8 = 2 + x + x 
+Solving for x, we get: 
+x = 4 
+So, Sara needed a total of 10 test tubes, and each of the other two experiments required 4 test tubes.</t>
         </is>
       </c>
     </row>
@@ -9977,7 +11897,8 @@
       <c r="E30" t="inlineStr"/>
       <c r="F30" t="inlineStr">
         <is>
-          <t>Sara needed a total of 10 test tubes for the three experiments in Science class. The first experiment required 2 test tubes, so there are 8 test tubes left for the other two experiments. Since they require the same number of test tubes, we can divide the remaining 8 by 2 to get:\nEach of the other two experiments needed 4 test tubes.</t>
+          <t>Sara needed a total of 10 test tubes for the three experiments in Science class. The first experiment required 2 test tubes, so there are 8 test tubes left for the other two experiments. Since they require the same number of test tubes, we can divide the remaining 8 by 2 to get:
+Each of the other two experiments needed 4 test tubes.</t>
         </is>
       </c>
     </row>

</xml_diff>